<commit_message>
Updated fcerm1 spreadsheet to latest version
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipgardiner/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selks\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16524"/>
   </bookViews>
   <sheets>
     <sheet name="FCRM1" sheetId="1" r:id="rId1"/>
@@ -90,23 +90,20 @@
     <definedName name="wages_freq_int_rec" localSheetId="0">#REF!</definedName>
     <definedName name="wages_freq_int_rec">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="325">
   <si>
     <t>FCRM1 - Medium Term Plan</t>
   </si>
@@ -1117,6 +1114,9 @@
   </si>
   <si>
     <t>OM2+3 18/19 - 20/21 total</t>
+  </si>
+  <si>
+    <t>xx</t>
   </si>
 </sst>
 </file>
@@ -1124,9 +1124,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1478,7 +1478,7 @@
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -1503,7 +1503,7 @@
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1521,10 +1521,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1586,7 +1586,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1613,6 +1613,243 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1750,243 +1987,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2374,24 +2374,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:KH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="7" topLeftCell="KB8" activePane="bottomRight" state="frozen"/>
       <selection activeCell="LZ2343" sqref="LZ2343"/>
       <selection pane="topRight" activeCell="LZ2343" sqref="LZ2343"/>
       <selection pane="bottomLeft" activeCell="LZ2343" sqref="LZ2343"/>
-      <selection pane="bottomRight" activeCell="IY5" sqref="IY5:JL6"/>
+      <selection pane="bottomRight" activeCell="KH8" sqref="KH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="41.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" style="1" customWidth="1"/>
     <col min="3" max="6" width="21" style="1" customWidth="1"/>
     <col min="7" max="7" width="21" style="2" customWidth="1"/>
     <col min="8" max="8" width="21" style="1" customWidth="1"/>
@@ -2407,11 +2407,11 @@
     <col min="45" max="278" width="21" style="1" customWidth="1"/>
     <col min="279" max="285" width="21" style="35" customWidth="1"/>
     <col min="286" max="293" width="21" style="8" customWidth="1"/>
-    <col min="294" max="294" width="8.85546875" style="8"/>
-    <col min="295" max="16384" width="8.85546875" style="36"/>
+    <col min="294" max="294" width="8.81640625" style="8"/>
+    <col min="295" max="16384" width="8.81640625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:294" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:294" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CB1" s="6"/>
       <c r="CC1" s="6"/>
       <c r="CD1" s="6"/>
@@ -2424,7 +2424,7 @@
       <c r="JX1" s="7"/>
       <c r="JY1" s="7"/>
     </row>
-    <row r="2" spans="1:294" ht="28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:294" ht="28.2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -2444,7 +2444,7 @@
       <c r="JX2" s="14"/>
       <c r="JY2" s="14"/>
     </row>
-    <row r="3" spans="1:294" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:294" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>319</v>
       </c>
@@ -2484,7 +2484,7 @@
       <c r="KG3" s="16"/>
       <c r="KH3" s="16"/>
     </row>
-    <row r="4" spans="1:294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -2780,655 +2780,655 @@
       <c r="KG4" s="22"/>
       <c r="KH4" s="18"/>
     </row>
-    <row r="5" spans="1:294" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
+    <row r="5" spans="1:294" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="68" t="s">
+      <c r="B5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="147" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="96" t="s">
+      <c r="F5" s="148"/>
+      <c r="G5" s="148"/>
+      <c r="H5" s="148"/>
+      <c r="I5" s="148"/>
+      <c r="J5" s="149"/>
+      <c r="K5" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="97"/>
-      <c r="M5" s="97"/>
-      <c r="N5" s="97"/>
-      <c r="O5" s="98"/>
-      <c r="P5" s="84" t="s">
+      <c r="L5" s="111"/>
+      <c r="M5" s="111"/>
+      <c r="N5" s="111"/>
+      <c r="O5" s="112"/>
+      <c r="P5" s="163" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="85"/>
-      <c r="T5" s="86"/>
-      <c r="U5" s="56" t="s">
+      <c r="Q5" s="164"/>
+      <c r="R5" s="164"/>
+      <c r="S5" s="164"/>
+      <c r="T5" s="165"/>
+      <c r="U5" s="135" t="s">
         <v>5</v>
       </c>
-      <c r="V5" s="57"/>
-      <c r="W5" s="57"/>
-      <c r="X5" s="57"/>
-      <c r="Y5" s="57"/>
-      <c r="Z5" s="57"/>
-      <c r="AA5" s="57"/>
-      <c r="AB5" s="58"/>
-      <c r="AC5" s="62" t="s">
+      <c r="V5" s="136"/>
+      <c r="W5" s="136"/>
+      <c r="X5" s="136"/>
+      <c r="Y5" s="136"/>
+      <c r="Z5" s="136"/>
+      <c r="AA5" s="136"/>
+      <c r="AB5" s="137"/>
+      <c r="AC5" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="AD5" s="63"/>
-      <c r="AE5" s="63"/>
-      <c r="AF5" s="63"/>
-      <c r="AG5" s="63"/>
-      <c r="AH5" s="63"/>
-      <c r="AI5" s="64"/>
-      <c r="AJ5" s="102" t="s">
+      <c r="AD5" s="142"/>
+      <c r="AE5" s="142"/>
+      <c r="AF5" s="142"/>
+      <c r="AG5" s="142"/>
+      <c r="AH5" s="142"/>
+      <c r="AI5" s="143"/>
+      <c r="AJ5" s="116" t="s">
         <v>313</v>
       </c>
-      <c r="AK5" s="103"/>
-      <c r="AL5" s="104"/>
-      <c r="AM5" s="74" t="s">
+      <c r="AK5" s="117"/>
+      <c r="AL5" s="118"/>
+      <c r="AM5" s="153" t="s">
         <v>7</v>
       </c>
-      <c r="AN5" s="75"/>
-      <c r="AO5" s="50" t="s">
+      <c r="AN5" s="154"/>
+      <c r="AO5" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="AP5" s="51"/>
-      <c r="AQ5" s="51"/>
-      <c r="AR5" s="52"/>
-      <c r="AS5" s="78" t="s">
+      <c r="AP5" s="130"/>
+      <c r="AQ5" s="130"/>
+      <c r="AR5" s="131"/>
+      <c r="AS5" s="157" t="s">
         <v>9</v>
       </c>
-      <c r="AT5" s="79"/>
-      <c r="AU5" s="79"/>
-      <c r="AV5" s="79"/>
-      <c r="AW5" s="79"/>
-      <c r="AX5" s="79"/>
-      <c r="AY5" s="79"/>
-      <c r="AZ5" s="79"/>
-      <c r="BA5" s="79"/>
-      <c r="BB5" s="79"/>
-      <c r="BC5" s="79"/>
-      <c r="BD5" s="79"/>
-      <c r="BE5" s="79"/>
-      <c r="BF5" s="79"/>
-      <c r="BG5" s="79"/>
-      <c r="BH5" s="79"/>
-      <c r="BI5" s="79"/>
-      <c r="BJ5" s="80"/>
-      <c r="BK5" s="109" t="s">
+      <c r="AT5" s="158"/>
+      <c r="AU5" s="158"/>
+      <c r="AV5" s="158"/>
+      <c r="AW5" s="158"/>
+      <c r="AX5" s="158"/>
+      <c r="AY5" s="158"/>
+      <c r="AZ5" s="158"/>
+      <c r="BA5" s="158"/>
+      <c r="BB5" s="158"/>
+      <c r="BC5" s="158"/>
+      <c r="BD5" s="158"/>
+      <c r="BE5" s="158"/>
+      <c r="BF5" s="158"/>
+      <c r="BG5" s="158"/>
+      <c r="BH5" s="158"/>
+      <c r="BI5" s="158"/>
+      <c r="BJ5" s="159"/>
+      <c r="BK5" s="50" t="s">
         <v>284</v>
       </c>
-      <c r="BL5" s="110"/>
-      <c r="BM5" s="110"/>
-      <c r="BN5" s="110"/>
-      <c r="BO5" s="110"/>
-      <c r="BP5" s="110"/>
-      <c r="BQ5" s="110"/>
-      <c r="BR5" s="110"/>
-      <c r="BS5" s="110"/>
-      <c r="BT5" s="110"/>
-      <c r="BU5" s="110"/>
-      <c r="BV5" s="110"/>
-      <c r="BW5" s="110"/>
-      <c r="BX5" s="111"/>
-      <c r="BY5" s="115" t="s">
+      <c r="BL5" s="51"/>
+      <c r="BM5" s="51"/>
+      <c r="BN5" s="51"/>
+      <c r="BO5" s="51"/>
+      <c r="BP5" s="51"/>
+      <c r="BQ5" s="51"/>
+      <c r="BR5" s="51"/>
+      <c r="BS5" s="51"/>
+      <c r="BT5" s="51"/>
+      <c r="BU5" s="51"/>
+      <c r="BV5" s="51"/>
+      <c r="BW5" s="51"/>
+      <c r="BX5" s="52"/>
+      <c r="BY5" s="86" t="s">
         <v>285</v>
       </c>
-      <c r="BZ5" s="116"/>
-      <c r="CA5" s="116"/>
-      <c r="CB5" s="116"/>
-      <c r="CC5" s="116"/>
-      <c r="CD5" s="116"/>
-      <c r="CE5" s="116"/>
-      <c r="CF5" s="116"/>
-      <c r="CG5" s="116"/>
-      <c r="CH5" s="116"/>
-      <c r="CI5" s="116"/>
-      <c r="CJ5" s="116"/>
-      <c r="CK5" s="116"/>
-      <c r="CL5" s="117"/>
-      <c r="CM5" s="121" t="s">
+      <c r="BZ5" s="87"/>
+      <c r="CA5" s="87"/>
+      <c r="CB5" s="87"/>
+      <c r="CC5" s="87"/>
+      <c r="CD5" s="87"/>
+      <c r="CE5" s="87"/>
+      <c r="CF5" s="87"/>
+      <c r="CG5" s="87"/>
+      <c r="CH5" s="87"/>
+      <c r="CI5" s="87"/>
+      <c r="CJ5" s="87"/>
+      <c r="CK5" s="87"/>
+      <c r="CL5" s="88"/>
+      <c r="CM5" s="92" t="s">
         <v>286</v>
       </c>
-      <c r="CN5" s="122"/>
-      <c r="CO5" s="122"/>
-      <c r="CP5" s="122"/>
-      <c r="CQ5" s="122"/>
-      <c r="CR5" s="122"/>
-      <c r="CS5" s="122"/>
-      <c r="CT5" s="122"/>
-      <c r="CU5" s="122"/>
-      <c r="CV5" s="122"/>
-      <c r="CW5" s="122"/>
-      <c r="CX5" s="122"/>
-      <c r="CY5" s="122"/>
-      <c r="CZ5" s="123"/>
-      <c r="DA5" s="127" t="s">
+      <c r="CN5" s="93"/>
+      <c r="CO5" s="93"/>
+      <c r="CP5" s="93"/>
+      <c r="CQ5" s="93"/>
+      <c r="CR5" s="93"/>
+      <c r="CS5" s="93"/>
+      <c r="CT5" s="93"/>
+      <c r="CU5" s="93"/>
+      <c r="CV5" s="93"/>
+      <c r="CW5" s="93"/>
+      <c r="CX5" s="93"/>
+      <c r="CY5" s="93"/>
+      <c r="CZ5" s="94"/>
+      <c r="DA5" s="98" t="s">
         <v>287</v>
       </c>
-      <c r="DB5" s="128"/>
-      <c r="DC5" s="128"/>
-      <c r="DD5" s="128"/>
-      <c r="DE5" s="128"/>
-      <c r="DF5" s="128"/>
-      <c r="DG5" s="128"/>
-      <c r="DH5" s="128"/>
-      <c r="DI5" s="128"/>
-      <c r="DJ5" s="128"/>
-      <c r="DK5" s="128"/>
-      <c r="DL5" s="128"/>
-      <c r="DM5" s="128"/>
-      <c r="DN5" s="129"/>
-      <c r="DO5" s="133" t="s">
+      <c r="DB5" s="99"/>
+      <c r="DC5" s="99"/>
+      <c r="DD5" s="99"/>
+      <c r="DE5" s="99"/>
+      <c r="DF5" s="99"/>
+      <c r="DG5" s="99"/>
+      <c r="DH5" s="99"/>
+      <c r="DI5" s="99"/>
+      <c r="DJ5" s="99"/>
+      <c r="DK5" s="99"/>
+      <c r="DL5" s="99"/>
+      <c r="DM5" s="99"/>
+      <c r="DN5" s="100"/>
+      <c r="DO5" s="68" t="s">
         <v>288</v>
       </c>
-      <c r="DP5" s="134"/>
-      <c r="DQ5" s="134"/>
-      <c r="DR5" s="134"/>
-      <c r="DS5" s="134"/>
-      <c r="DT5" s="134"/>
-      <c r="DU5" s="134"/>
-      <c r="DV5" s="134"/>
-      <c r="DW5" s="134"/>
-      <c r="DX5" s="134"/>
-      <c r="DY5" s="134"/>
-      <c r="DZ5" s="134"/>
-      <c r="EA5" s="134"/>
-      <c r="EB5" s="135"/>
-      <c r="EC5" s="139" t="s">
+      <c r="DP5" s="69"/>
+      <c r="DQ5" s="69"/>
+      <c r="DR5" s="69"/>
+      <c r="DS5" s="69"/>
+      <c r="DT5" s="69"/>
+      <c r="DU5" s="69"/>
+      <c r="DV5" s="69"/>
+      <c r="DW5" s="69"/>
+      <c r="DX5" s="69"/>
+      <c r="DY5" s="69"/>
+      <c r="DZ5" s="69"/>
+      <c r="EA5" s="69"/>
+      <c r="EB5" s="70"/>
+      <c r="EC5" s="74" t="s">
         <v>289</v>
       </c>
-      <c r="ED5" s="140"/>
-      <c r="EE5" s="140"/>
-      <c r="EF5" s="140"/>
-      <c r="EG5" s="140"/>
-      <c r="EH5" s="140"/>
-      <c r="EI5" s="140"/>
-      <c r="EJ5" s="140"/>
-      <c r="EK5" s="140"/>
-      <c r="EL5" s="140"/>
-      <c r="EM5" s="140"/>
-      <c r="EN5" s="140"/>
-      <c r="EO5" s="140"/>
-      <c r="EP5" s="141"/>
-      <c r="EQ5" s="145" t="s">
+      <c r="ED5" s="75"/>
+      <c r="EE5" s="75"/>
+      <c r="EF5" s="75"/>
+      <c r="EG5" s="75"/>
+      <c r="EH5" s="75"/>
+      <c r="EI5" s="75"/>
+      <c r="EJ5" s="75"/>
+      <c r="EK5" s="75"/>
+      <c r="EL5" s="75"/>
+      <c r="EM5" s="75"/>
+      <c r="EN5" s="75"/>
+      <c r="EO5" s="75"/>
+      <c r="EP5" s="76"/>
+      <c r="EQ5" s="80" t="s">
         <v>290</v>
       </c>
-      <c r="ER5" s="146"/>
-      <c r="ES5" s="146"/>
-      <c r="ET5" s="146"/>
-      <c r="EU5" s="146"/>
-      <c r="EV5" s="146"/>
-      <c r="EW5" s="146"/>
-      <c r="EX5" s="146"/>
-      <c r="EY5" s="146"/>
-      <c r="EZ5" s="146"/>
-      <c r="FA5" s="146"/>
-      <c r="FB5" s="146"/>
-      <c r="FC5" s="146"/>
-      <c r="FD5" s="147"/>
-      <c r="FE5" s="151" t="s">
+      <c r="ER5" s="81"/>
+      <c r="ES5" s="81"/>
+      <c r="ET5" s="81"/>
+      <c r="EU5" s="81"/>
+      <c r="EV5" s="81"/>
+      <c r="EW5" s="81"/>
+      <c r="EX5" s="81"/>
+      <c r="EY5" s="81"/>
+      <c r="EZ5" s="81"/>
+      <c r="FA5" s="81"/>
+      <c r="FB5" s="81"/>
+      <c r="FC5" s="81"/>
+      <c r="FD5" s="82"/>
+      <c r="FE5" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="FF5" s="152"/>
-      <c r="FG5" s="152"/>
-      <c r="FH5" s="152"/>
-      <c r="FI5" s="152"/>
-      <c r="FJ5" s="152"/>
-      <c r="FK5" s="152"/>
-      <c r="FL5" s="152"/>
-      <c r="FM5" s="152"/>
-      <c r="FN5" s="152"/>
-      <c r="FO5" s="152"/>
-      <c r="FP5" s="152"/>
-      <c r="FQ5" s="152"/>
-      <c r="FR5" s="153"/>
-      <c r="FS5" s="157" t="s">
+      <c r="FF5" s="57"/>
+      <c r="FG5" s="57"/>
+      <c r="FH5" s="57"/>
+      <c r="FI5" s="57"/>
+      <c r="FJ5" s="57"/>
+      <c r="FK5" s="57"/>
+      <c r="FL5" s="57"/>
+      <c r="FM5" s="57"/>
+      <c r="FN5" s="57"/>
+      <c r="FO5" s="57"/>
+      <c r="FP5" s="57"/>
+      <c r="FQ5" s="57"/>
+      <c r="FR5" s="58"/>
+      <c r="FS5" s="62" t="s">
         <v>291</v>
       </c>
-      <c r="FT5" s="158"/>
-      <c r="FU5" s="158"/>
-      <c r="FV5" s="158"/>
-      <c r="FW5" s="158"/>
-      <c r="FX5" s="158"/>
-      <c r="FY5" s="158"/>
-      <c r="FZ5" s="158"/>
-      <c r="GA5" s="158"/>
-      <c r="GB5" s="158"/>
-      <c r="GC5" s="158"/>
-      <c r="GD5" s="158"/>
-      <c r="GE5" s="158"/>
-      <c r="GF5" s="159"/>
-      <c r="GG5" s="109" t="s">
+      <c r="FT5" s="63"/>
+      <c r="FU5" s="63"/>
+      <c r="FV5" s="63"/>
+      <c r="FW5" s="63"/>
+      <c r="FX5" s="63"/>
+      <c r="FY5" s="63"/>
+      <c r="FZ5" s="63"/>
+      <c r="GA5" s="63"/>
+      <c r="GB5" s="63"/>
+      <c r="GC5" s="63"/>
+      <c r="GD5" s="63"/>
+      <c r="GE5" s="63"/>
+      <c r="GF5" s="64"/>
+      <c r="GG5" s="50" t="s">
         <v>292</v>
       </c>
-      <c r="GH5" s="110"/>
-      <c r="GI5" s="110"/>
-      <c r="GJ5" s="110"/>
-      <c r="GK5" s="110"/>
-      <c r="GL5" s="110"/>
-      <c r="GM5" s="110"/>
-      <c r="GN5" s="110"/>
-      <c r="GO5" s="110"/>
-      <c r="GP5" s="110"/>
-      <c r="GQ5" s="110"/>
-      <c r="GR5" s="110"/>
-      <c r="GS5" s="110"/>
-      <c r="GT5" s="111"/>
-      <c r="GU5" s="109" t="s">
+      <c r="GH5" s="51"/>
+      <c r="GI5" s="51"/>
+      <c r="GJ5" s="51"/>
+      <c r="GK5" s="51"/>
+      <c r="GL5" s="51"/>
+      <c r="GM5" s="51"/>
+      <c r="GN5" s="51"/>
+      <c r="GO5" s="51"/>
+      <c r="GP5" s="51"/>
+      <c r="GQ5" s="51"/>
+      <c r="GR5" s="51"/>
+      <c r="GS5" s="51"/>
+      <c r="GT5" s="52"/>
+      <c r="GU5" s="50" t="s">
         <v>293</v>
       </c>
-      <c r="GV5" s="110"/>
-      <c r="GW5" s="110"/>
-      <c r="GX5" s="110"/>
-      <c r="GY5" s="110"/>
-      <c r="GZ5" s="110"/>
-      <c r="HA5" s="110"/>
-      <c r="HB5" s="110"/>
-      <c r="HC5" s="110"/>
-      <c r="HD5" s="110"/>
-      <c r="HE5" s="110"/>
-      <c r="HF5" s="110"/>
-      <c r="HG5" s="110"/>
-      <c r="HH5" s="111"/>
-      <c r="HI5" s="109" t="s">
+      <c r="GV5" s="51"/>
+      <c r="GW5" s="51"/>
+      <c r="GX5" s="51"/>
+      <c r="GY5" s="51"/>
+      <c r="GZ5" s="51"/>
+      <c r="HA5" s="51"/>
+      <c r="HB5" s="51"/>
+      <c r="HC5" s="51"/>
+      <c r="HD5" s="51"/>
+      <c r="HE5" s="51"/>
+      <c r="HF5" s="51"/>
+      <c r="HG5" s="51"/>
+      <c r="HH5" s="52"/>
+      <c r="HI5" s="50" t="s">
         <v>294</v>
       </c>
-      <c r="HJ5" s="110"/>
-      <c r="HK5" s="110"/>
-      <c r="HL5" s="110"/>
-      <c r="HM5" s="110"/>
-      <c r="HN5" s="110"/>
-      <c r="HO5" s="110"/>
-      <c r="HP5" s="110"/>
-      <c r="HQ5" s="110"/>
-      <c r="HR5" s="110"/>
-      <c r="HS5" s="110"/>
-      <c r="HT5" s="110"/>
-      <c r="HU5" s="110"/>
-      <c r="HV5" s="111"/>
-      <c r="HW5" s="163" t="s">
+      <c r="HJ5" s="51"/>
+      <c r="HK5" s="51"/>
+      <c r="HL5" s="51"/>
+      <c r="HM5" s="51"/>
+      <c r="HN5" s="51"/>
+      <c r="HO5" s="51"/>
+      <c r="HP5" s="51"/>
+      <c r="HQ5" s="51"/>
+      <c r="HR5" s="51"/>
+      <c r="HS5" s="51"/>
+      <c r="HT5" s="51"/>
+      <c r="HU5" s="51"/>
+      <c r="HV5" s="52"/>
+      <c r="HW5" s="44" t="s">
         <v>295</v>
       </c>
-      <c r="HX5" s="164"/>
-      <c r="HY5" s="164"/>
-      <c r="HZ5" s="164"/>
-      <c r="IA5" s="164"/>
-      <c r="IB5" s="164"/>
-      <c r="IC5" s="164"/>
-      <c r="ID5" s="164"/>
-      <c r="IE5" s="164"/>
-      <c r="IF5" s="164"/>
-      <c r="IG5" s="164"/>
-      <c r="IH5" s="164"/>
-      <c r="II5" s="164"/>
-      <c r="IJ5" s="165"/>
-      <c r="IK5" s="163" t="s">
+      <c r="HX5" s="45"/>
+      <c r="HY5" s="45"/>
+      <c r="HZ5" s="45"/>
+      <c r="IA5" s="45"/>
+      <c r="IB5" s="45"/>
+      <c r="IC5" s="45"/>
+      <c r="ID5" s="45"/>
+      <c r="IE5" s="45"/>
+      <c r="IF5" s="45"/>
+      <c r="IG5" s="45"/>
+      <c r="IH5" s="45"/>
+      <c r="II5" s="45"/>
+      <c r="IJ5" s="46"/>
+      <c r="IK5" s="44" t="s">
         <v>296</v>
       </c>
-      <c r="IL5" s="164"/>
-      <c r="IM5" s="164"/>
-      <c r="IN5" s="164"/>
-      <c r="IO5" s="164"/>
-      <c r="IP5" s="164"/>
-      <c r="IQ5" s="164"/>
-      <c r="IR5" s="164"/>
-      <c r="IS5" s="164"/>
-      <c r="IT5" s="164"/>
-      <c r="IU5" s="164"/>
-      <c r="IV5" s="164"/>
-      <c r="IW5" s="164"/>
-      <c r="IX5" s="165"/>
-      <c r="IY5" s="163" t="s">
+      <c r="IL5" s="45"/>
+      <c r="IM5" s="45"/>
+      <c r="IN5" s="45"/>
+      <c r="IO5" s="45"/>
+      <c r="IP5" s="45"/>
+      <c r="IQ5" s="45"/>
+      <c r="IR5" s="45"/>
+      <c r="IS5" s="45"/>
+      <c r="IT5" s="45"/>
+      <c r="IU5" s="45"/>
+      <c r="IV5" s="45"/>
+      <c r="IW5" s="45"/>
+      <c r="IX5" s="46"/>
+      <c r="IY5" s="44" t="s">
         <v>297</v>
       </c>
-      <c r="IZ5" s="164"/>
-      <c r="JA5" s="164"/>
-      <c r="JB5" s="164"/>
-      <c r="JC5" s="164"/>
-      <c r="JD5" s="164"/>
-      <c r="JE5" s="164"/>
-      <c r="JF5" s="164"/>
-      <c r="JG5" s="164"/>
-      <c r="JH5" s="164"/>
-      <c r="JI5" s="164"/>
-      <c r="JJ5" s="164"/>
-      <c r="JK5" s="164"/>
-      <c r="JL5" s="165"/>
-      <c r="JM5" s="108" t="s">
+      <c r="IZ5" s="45"/>
+      <c r="JA5" s="45"/>
+      <c r="JB5" s="45"/>
+      <c r="JC5" s="45"/>
+      <c r="JD5" s="45"/>
+      <c r="JE5" s="45"/>
+      <c r="JF5" s="45"/>
+      <c r="JG5" s="45"/>
+      <c r="JH5" s="45"/>
+      <c r="JI5" s="45"/>
+      <c r="JJ5" s="45"/>
+      <c r="JK5" s="45"/>
+      <c r="JL5" s="46"/>
+      <c r="JM5" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="JN5" s="108"/>
-      <c r="JO5" s="108"/>
-      <c r="JP5" s="108"/>
-      <c r="JQ5" s="108"/>
-      <c r="JR5" s="108"/>
-      <c r="JS5" s="108"/>
-      <c r="JT5" s="108"/>
-      <c r="JU5" s="108"/>
-      <c r="JV5" s="108"/>
-      <c r="JW5" s="108"/>
-      <c r="JX5" s="108"/>
-      <c r="JY5" s="108"/>
-      <c r="JZ5" s="93" t="s">
+      <c r="JN5" s="122"/>
+      <c r="JO5" s="122"/>
+      <c r="JP5" s="122"/>
+      <c r="JQ5" s="122"/>
+      <c r="JR5" s="122"/>
+      <c r="JS5" s="122"/>
+      <c r="JT5" s="122"/>
+      <c r="JU5" s="122"/>
+      <c r="JV5" s="122"/>
+      <c r="JW5" s="122"/>
+      <c r="JX5" s="122"/>
+      <c r="JY5" s="122"/>
+      <c r="JZ5" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="KA5" s="94"/>
-      <c r="KB5" s="94"/>
-      <c r="KC5" s="94"/>
-      <c r="KD5" s="94"/>
-      <c r="KE5" s="94"/>
-      <c r="KF5" s="94"/>
-      <c r="KG5" s="95"/>
+      <c r="KA5" s="108"/>
+      <c r="KB5" s="108"/>
+      <c r="KC5" s="108"/>
+      <c r="KD5" s="108"/>
+      <c r="KE5" s="108"/>
+      <c r="KF5" s="108"/>
+      <c r="KG5" s="109"/>
     </row>
-    <row r="6" spans="1:294" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
-      <c r="O6" s="101"/>
-      <c r="P6" s="87"/>
-      <c r="Q6" s="88"/>
-      <c r="R6" s="88"/>
-      <c r="S6" s="88"/>
-      <c r="T6" s="89"/>
-      <c r="U6" s="59"/>
-      <c r="V6" s="60"/>
-      <c r="W6" s="60"/>
-      <c r="X6" s="60"/>
-      <c r="Y6" s="60"/>
-      <c r="Z6" s="60"/>
-      <c r="AA6" s="60"/>
-      <c r="AB6" s="61"/>
-      <c r="AC6" s="65"/>
-      <c r="AD6" s="66"/>
-      <c r="AE6" s="66"/>
-      <c r="AF6" s="66"/>
-      <c r="AG6" s="66"/>
-      <c r="AH6" s="66"/>
-      <c r="AI6" s="67"/>
-      <c r="AJ6" s="105"/>
-      <c r="AK6" s="106"/>
-      <c r="AL6" s="107"/>
-      <c r="AM6" s="76"/>
-      <c r="AN6" s="77"/>
-      <c r="AO6" s="53"/>
-      <c r="AP6" s="54"/>
-      <c r="AQ6" s="54"/>
-      <c r="AR6" s="55"/>
-      <c r="AS6" s="81"/>
-      <c r="AT6" s="82"/>
-      <c r="AU6" s="82"/>
-      <c r="AV6" s="82"/>
-      <c r="AW6" s="82"/>
-      <c r="AX6" s="82"/>
-      <c r="AY6" s="82"/>
-      <c r="AZ6" s="82"/>
-      <c r="BA6" s="82"/>
-      <c r="BB6" s="82"/>
-      <c r="BC6" s="82"/>
-      <c r="BD6" s="82"/>
-      <c r="BE6" s="82"/>
-      <c r="BF6" s="82"/>
-      <c r="BG6" s="82"/>
-      <c r="BH6" s="82"/>
-      <c r="BI6" s="82"/>
-      <c r="BJ6" s="83"/>
-      <c r="BK6" s="112"/>
-      <c r="BL6" s="113"/>
-      <c r="BM6" s="113"/>
-      <c r="BN6" s="113"/>
-      <c r="BO6" s="113"/>
-      <c r="BP6" s="113"/>
-      <c r="BQ6" s="113"/>
-      <c r="BR6" s="113"/>
-      <c r="BS6" s="113"/>
-      <c r="BT6" s="113"/>
-      <c r="BU6" s="113"/>
-      <c r="BV6" s="113"/>
-      <c r="BW6" s="113"/>
-      <c r="BX6" s="114"/>
-      <c r="BY6" s="118"/>
-      <c r="BZ6" s="119"/>
-      <c r="CA6" s="119"/>
-      <c r="CB6" s="119"/>
-      <c r="CC6" s="119"/>
-      <c r="CD6" s="119"/>
-      <c r="CE6" s="119"/>
-      <c r="CF6" s="119"/>
-      <c r="CG6" s="119"/>
-      <c r="CH6" s="119"/>
-      <c r="CI6" s="119"/>
-      <c r="CJ6" s="119"/>
-      <c r="CK6" s="119"/>
-      <c r="CL6" s="120"/>
-      <c r="CM6" s="124"/>
-      <c r="CN6" s="125"/>
-      <c r="CO6" s="125"/>
-      <c r="CP6" s="125"/>
-      <c r="CQ6" s="125"/>
-      <c r="CR6" s="125"/>
-      <c r="CS6" s="125"/>
-      <c r="CT6" s="125"/>
-      <c r="CU6" s="125"/>
-      <c r="CV6" s="125"/>
-      <c r="CW6" s="125"/>
-      <c r="CX6" s="125"/>
-      <c r="CY6" s="125"/>
-      <c r="CZ6" s="126"/>
-      <c r="DA6" s="130"/>
-      <c r="DB6" s="131"/>
-      <c r="DC6" s="131"/>
-      <c r="DD6" s="131"/>
-      <c r="DE6" s="131"/>
-      <c r="DF6" s="131"/>
-      <c r="DG6" s="131"/>
-      <c r="DH6" s="131"/>
-      <c r="DI6" s="131"/>
-      <c r="DJ6" s="131"/>
-      <c r="DK6" s="131"/>
-      <c r="DL6" s="131"/>
-      <c r="DM6" s="131"/>
-      <c r="DN6" s="132"/>
-      <c r="DO6" s="136"/>
-      <c r="DP6" s="137"/>
-      <c r="DQ6" s="137"/>
-      <c r="DR6" s="137"/>
-      <c r="DS6" s="137"/>
-      <c r="DT6" s="137"/>
-      <c r="DU6" s="137"/>
-      <c r="DV6" s="137"/>
-      <c r="DW6" s="137"/>
-      <c r="DX6" s="137"/>
-      <c r="DY6" s="137"/>
-      <c r="DZ6" s="137"/>
-      <c r="EA6" s="137"/>
-      <c r="EB6" s="138"/>
-      <c r="EC6" s="142"/>
-      <c r="ED6" s="143"/>
-      <c r="EE6" s="143"/>
-      <c r="EF6" s="143"/>
-      <c r="EG6" s="143"/>
-      <c r="EH6" s="143"/>
-      <c r="EI6" s="143"/>
-      <c r="EJ6" s="143"/>
-      <c r="EK6" s="143"/>
-      <c r="EL6" s="143"/>
-      <c r="EM6" s="143"/>
-      <c r="EN6" s="143"/>
-      <c r="EO6" s="143"/>
-      <c r="EP6" s="144"/>
-      <c r="EQ6" s="148"/>
-      <c r="ER6" s="149"/>
-      <c r="ES6" s="149"/>
-      <c r="ET6" s="149"/>
-      <c r="EU6" s="149"/>
-      <c r="EV6" s="149"/>
-      <c r="EW6" s="149"/>
-      <c r="EX6" s="149"/>
-      <c r="EY6" s="149"/>
-      <c r="EZ6" s="149"/>
-      <c r="FA6" s="149"/>
-      <c r="FB6" s="149"/>
-      <c r="FC6" s="149"/>
-      <c r="FD6" s="150"/>
-      <c r="FE6" s="154"/>
-      <c r="FF6" s="155"/>
-      <c r="FG6" s="155"/>
-      <c r="FH6" s="155"/>
-      <c r="FI6" s="155"/>
-      <c r="FJ6" s="155"/>
-      <c r="FK6" s="155"/>
-      <c r="FL6" s="155"/>
-      <c r="FM6" s="155"/>
-      <c r="FN6" s="155"/>
-      <c r="FO6" s="155"/>
-      <c r="FP6" s="155"/>
-      <c r="FQ6" s="155"/>
-      <c r="FR6" s="156"/>
-      <c r="FS6" s="160"/>
-      <c r="FT6" s="161"/>
-      <c r="FU6" s="161"/>
-      <c r="FV6" s="161"/>
-      <c r="FW6" s="161"/>
-      <c r="FX6" s="161"/>
-      <c r="FY6" s="161"/>
-      <c r="FZ6" s="161"/>
-      <c r="GA6" s="161"/>
-      <c r="GB6" s="161"/>
-      <c r="GC6" s="161"/>
-      <c r="GD6" s="161"/>
-      <c r="GE6" s="161"/>
-      <c r="GF6" s="162"/>
-      <c r="GG6" s="112"/>
-      <c r="GH6" s="113"/>
-      <c r="GI6" s="113"/>
-      <c r="GJ6" s="113"/>
-      <c r="GK6" s="113"/>
-      <c r="GL6" s="113"/>
-      <c r="GM6" s="113"/>
-      <c r="GN6" s="113"/>
-      <c r="GO6" s="113"/>
-      <c r="GP6" s="113"/>
-      <c r="GQ6" s="113"/>
-      <c r="GR6" s="113"/>
-      <c r="GS6" s="113"/>
-      <c r="GT6" s="114"/>
-      <c r="GU6" s="112"/>
-      <c r="GV6" s="113"/>
-      <c r="GW6" s="113"/>
-      <c r="GX6" s="113"/>
-      <c r="GY6" s="113"/>
-      <c r="GZ6" s="113"/>
-      <c r="HA6" s="113"/>
-      <c r="HB6" s="113"/>
-      <c r="HC6" s="113"/>
-      <c r="HD6" s="113"/>
-      <c r="HE6" s="113"/>
-      <c r="HF6" s="113"/>
-      <c r="HG6" s="113"/>
-      <c r="HH6" s="114"/>
-      <c r="HI6" s="112"/>
-      <c r="HJ6" s="113"/>
-      <c r="HK6" s="113"/>
-      <c r="HL6" s="113"/>
-      <c r="HM6" s="113"/>
-      <c r="HN6" s="113"/>
-      <c r="HO6" s="113"/>
-      <c r="HP6" s="113"/>
-      <c r="HQ6" s="113"/>
-      <c r="HR6" s="113"/>
-      <c r="HS6" s="113"/>
-      <c r="HT6" s="113"/>
-      <c r="HU6" s="113"/>
-      <c r="HV6" s="114"/>
-      <c r="HW6" s="166"/>
-      <c r="HX6" s="167"/>
-      <c r="HY6" s="167"/>
-      <c r="HZ6" s="167"/>
-      <c r="IA6" s="167"/>
-      <c r="IB6" s="167"/>
-      <c r="IC6" s="167"/>
-      <c r="ID6" s="167"/>
-      <c r="IE6" s="167"/>
-      <c r="IF6" s="167"/>
-      <c r="IG6" s="167"/>
-      <c r="IH6" s="167"/>
-      <c r="II6" s="167"/>
-      <c r="IJ6" s="168"/>
-      <c r="IK6" s="166"/>
-      <c r="IL6" s="167"/>
-      <c r="IM6" s="167"/>
-      <c r="IN6" s="167"/>
-      <c r="IO6" s="167"/>
-      <c r="IP6" s="167"/>
-      <c r="IQ6" s="167"/>
-      <c r="IR6" s="167"/>
-      <c r="IS6" s="167"/>
-      <c r="IT6" s="167"/>
-      <c r="IU6" s="167"/>
-      <c r="IV6" s="167"/>
-      <c r="IW6" s="167"/>
-      <c r="IX6" s="168"/>
-      <c r="IY6" s="166"/>
-      <c r="IZ6" s="167"/>
-      <c r="JA6" s="167"/>
-      <c r="JB6" s="167"/>
-      <c r="JC6" s="167"/>
-      <c r="JD6" s="167"/>
-      <c r="JE6" s="167"/>
-      <c r="JF6" s="167"/>
-      <c r="JG6" s="167"/>
-      <c r="JH6" s="167"/>
-      <c r="JI6" s="167"/>
-      <c r="JJ6" s="167"/>
-      <c r="JK6" s="167"/>
-      <c r="JL6" s="168"/>
-      <c r="JM6" s="108"/>
-      <c r="JN6" s="108"/>
-      <c r="JO6" s="108"/>
-      <c r="JP6" s="108"/>
-      <c r="JQ6" s="108"/>
-      <c r="JR6" s="108"/>
-      <c r="JS6" s="108"/>
-      <c r="JT6" s="108"/>
-      <c r="JU6" s="108"/>
-      <c r="JV6" s="108"/>
-      <c r="JW6" s="108"/>
-      <c r="JX6" s="108"/>
-      <c r="JY6" s="108"/>
-      <c r="JZ6" s="90" t="s">
+    <row r="6" spans="1:294" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="126"/>
+      <c r="B6" s="127"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="150"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="151"/>
+      <c r="H6" s="151"/>
+      <c r="I6" s="151"/>
+      <c r="J6" s="152"/>
+      <c r="K6" s="113"/>
+      <c r="L6" s="114"/>
+      <c r="M6" s="114"/>
+      <c r="N6" s="114"/>
+      <c r="O6" s="115"/>
+      <c r="P6" s="166"/>
+      <c r="Q6" s="167"/>
+      <c r="R6" s="167"/>
+      <c r="S6" s="167"/>
+      <c r="T6" s="168"/>
+      <c r="U6" s="138"/>
+      <c r="V6" s="139"/>
+      <c r="W6" s="139"/>
+      <c r="X6" s="139"/>
+      <c r="Y6" s="139"/>
+      <c r="Z6" s="139"/>
+      <c r="AA6" s="139"/>
+      <c r="AB6" s="140"/>
+      <c r="AC6" s="144"/>
+      <c r="AD6" s="145"/>
+      <c r="AE6" s="145"/>
+      <c r="AF6" s="145"/>
+      <c r="AG6" s="145"/>
+      <c r="AH6" s="145"/>
+      <c r="AI6" s="146"/>
+      <c r="AJ6" s="119"/>
+      <c r="AK6" s="120"/>
+      <c r="AL6" s="121"/>
+      <c r="AM6" s="155"/>
+      <c r="AN6" s="156"/>
+      <c r="AO6" s="132"/>
+      <c r="AP6" s="133"/>
+      <c r="AQ6" s="133"/>
+      <c r="AR6" s="134"/>
+      <c r="AS6" s="160"/>
+      <c r="AT6" s="161"/>
+      <c r="AU6" s="161"/>
+      <c r="AV6" s="161"/>
+      <c r="AW6" s="161"/>
+      <c r="AX6" s="161"/>
+      <c r="AY6" s="161"/>
+      <c r="AZ6" s="161"/>
+      <c r="BA6" s="161"/>
+      <c r="BB6" s="161"/>
+      <c r="BC6" s="161"/>
+      <c r="BD6" s="161"/>
+      <c r="BE6" s="161"/>
+      <c r="BF6" s="161"/>
+      <c r="BG6" s="161"/>
+      <c r="BH6" s="161"/>
+      <c r="BI6" s="161"/>
+      <c r="BJ6" s="162"/>
+      <c r="BK6" s="53"/>
+      <c r="BL6" s="54"/>
+      <c r="BM6" s="54"/>
+      <c r="BN6" s="54"/>
+      <c r="BO6" s="54"/>
+      <c r="BP6" s="54"/>
+      <c r="BQ6" s="54"/>
+      <c r="BR6" s="54"/>
+      <c r="BS6" s="54"/>
+      <c r="BT6" s="54"/>
+      <c r="BU6" s="54"/>
+      <c r="BV6" s="54"/>
+      <c r="BW6" s="54"/>
+      <c r="BX6" s="55"/>
+      <c r="BY6" s="89"/>
+      <c r="BZ6" s="90"/>
+      <c r="CA6" s="90"/>
+      <c r="CB6" s="90"/>
+      <c r="CC6" s="90"/>
+      <c r="CD6" s="90"/>
+      <c r="CE6" s="90"/>
+      <c r="CF6" s="90"/>
+      <c r="CG6" s="90"/>
+      <c r="CH6" s="90"/>
+      <c r="CI6" s="90"/>
+      <c r="CJ6" s="90"/>
+      <c r="CK6" s="90"/>
+      <c r="CL6" s="91"/>
+      <c r="CM6" s="95"/>
+      <c r="CN6" s="96"/>
+      <c r="CO6" s="96"/>
+      <c r="CP6" s="96"/>
+      <c r="CQ6" s="96"/>
+      <c r="CR6" s="96"/>
+      <c r="CS6" s="96"/>
+      <c r="CT6" s="96"/>
+      <c r="CU6" s="96"/>
+      <c r="CV6" s="96"/>
+      <c r="CW6" s="96"/>
+      <c r="CX6" s="96"/>
+      <c r="CY6" s="96"/>
+      <c r="CZ6" s="97"/>
+      <c r="DA6" s="101"/>
+      <c r="DB6" s="102"/>
+      <c r="DC6" s="102"/>
+      <c r="DD6" s="102"/>
+      <c r="DE6" s="102"/>
+      <c r="DF6" s="102"/>
+      <c r="DG6" s="102"/>
+      <c r="DH6" s="102"/>
+      <c r="DI6" s="102"/>
+      <c r="DJ6" s="102"/>
+      <c r="DK6" s="102"/>
+      <c r="DL6" s="102"/>
+      <c r="DM6" s="102"/>
+      <c r="DN6" s="103"/>
+      <c r="DO6" s="71"/>
+      <c r="DP6" s="72"/>
+      <c r="DQ6" s="72"/>
+      <c r="DR6" s="72"/>
+      <c r="DS6" s="72"/>
+      <c r="DT6" s="72"/>
+      <c r="DU6" s="72"/>
+      <c r="DV6" s="72"/>
+      <c r="DW6" s="72"/>
+      <c r="DX6" s="72"/>
+      <c r="DY6" s="72"/>
+      <c r="DZ6" s="72"/>
+      <c r="EA6" s="72"/>
+      <c r="EB6" s="73"/>
+      <c r="EC6" s="77"/>
+      <c r="ED6" s="78"/>
+      <c r="EE6" s="78"/>
+      <c r="EF6" s="78"/>
+      <c r="EG6" s="78"/>
+      <c r="EH6" s="78"/>
+      <c r="EI6" s="78"/>
+      <c r="EJ6" s="78"/>
+      <c r="EK6" s="78"/>
+      <c r="EL6" s="78"/>
+      <c r="EM6" s="78"/>
+      <c r="EN6" s="78"/>
+      <c r="EO6" s="78"/>
+      <c r="EP6" s="79"/>
+      <c r="EQ6" s="83"/>
+      <c r="ER6" s="84"/>
+      <c r="ES6" s="84"/>
+      <c r="ET6" s="84"/>
+      <c r="EU6" s="84"/>
+      <c r="EV6" s="84"/>
+      <c r="EW6" s="84"/>
+      <c r="EX6" s="84"/>
+      <c r="EY6" s="84"/>
+      <c r="EZ6" s="84"/>
+      <c r="FA6" s="84"/>
+      <c r="FB6" s="84"/>
+      <c r="FC6" s="84"/>
+      <c r="FD6" s="85"/>
+      <c r="FE6" s="59"/>
+      <c r="FF6" s="60"/>
+      <c r="FG6" s="60"/>
+      <c r="FH6" s="60"/>
+      <c r="FI6" s="60"/>
+      <c r="FJ6" s="60"/>
+      <c r="FK6" s="60"/>
+      <c r="FL6" s="60"/>
+      <c r="FM6" s="60"/>
+      <c r="FN6" s="60"/>
+      <c r="FO6" s="60"/>
+      <c r="FP6" s="60"/>
+      <c r="FQ6" s="60"/>
+      <c r="FR6" s="61"/>
+      <c r="FS6" s="65"/>
+      <c r="FT6" s="66"/>
+      <c r="FU6" s="66"/>
+      <c r="FV6" s="66"/>
+      <c r="FW6" s="66"/>
+      <c r="FX6" s="66"/>
+      <c r="FY6" s="66"/>
+      <c r="FZ6" s="66"/>
+      <c r="GA6" s="66"/>
+      <c r="GB6" s="66"/>
+      <c r="GC6" s="66"/>
+      <c r="GD6" s="66"/>
+      <c r="GE6" s="66"/>
+      <c r="GF6" s="67"/>
+      <c r="GG6" s="53"/>
+      <c r="GH6" s="54"/>
+      <c r="GI6" s="54"/>
+      <c r="GJ6" s="54"/>
+      <c r="GK6" s="54"/>
+      <c r="GL6" s="54"/>
+      <c r="GM6" s="54"/>
+      <c r="GN6" s="54"/>
+      <c r="GO6" s="54"/>
+      <c r="GP6" s="54"/>
+      <c r="GQ6" s="54"/>
+      <c r="GR6" s="54"/>
+      <c r="GS6" s="54"/>
+      <c r="GT6" s="55"/>
+      <c r="GU6" s="53"/>
+      <c r="GV6" s="54"/>
+      <c r="GW6" s="54"/>
+      <c r="GX6" s="54"/>
+      <c r="GY6" s="54"/>
+      <c r="GZ6" s="54"/>
+      <c r="HA6" s="54"/>
+      <c r="HB6" s="54"/>
+      <c r="HC6" s="54"/>
+      <c r="HD6" s="54"/>
+      <c r="HE6" s="54"/>
+      <c r="HF6" s="54"/>
+      <c r="HG6" s="54"/>
+      <c r="HH6" s="55"/>
+      <c r="HI6" s="53"/>
+      <c r="HJ6" s="54"/>
+      <c r="HK6" s="54"/>
+      <c r="HL6" s="54"/>
+      <c r="HM6" s="54"/>
+      <c r="HN6" s="54"/>
+      <c r="HO6" s="54"/>
+      <c r="HP6" s="54"/>
+      <c r="HQ6" s="54"/>
+      <c r="HR6" s="54"/>
+      <c r="HS6" s="54"/>
+      <c r="HT6" s="54"/>
+      <c r="HU6" s="54"/>
+      <c r="HV6" s="55"/>
+      <c r="HW6" s="47"/>
+      <c r="HX6" s="48"/>
+      <c r="HY6" s="48"/>
+      <c r="HZ6" s="48"/>
+      <c r="IA6" s="48"/>
+      <c r="IB6" s="48"/>
+      <c r="IC6" s="48"/>
+      <c r="ID6" s="48"/>
+      <c r="IE6" s="48"/>
+      <c r="IF6" s="48"/>
+      <c r="IG6" s="48"/>
+      <c r="IH6" s="48"/>
+      <c r="II6" s="48"/>
+      <c r="IJ6" s="49"/>
+      <c r="IK6" s="47"/>
+      <c r="IL6" s="48"/>
+      <c r="IM6" s="48"/>
+      <c r="IN6" s="48"/>
+      <c r="IO6" s="48"/>
+      <c r="IP6" s="48"/>
+      <c r="IQ6" s="48"/>
+      <c r="IR6" s="48"/>
+      <c r="IS6" s="48"/>
+      <c r="IT6" s="48"/>
+      <c r="IU6" s="48"/>
+      <c r="IV6" s="48"/>
+      <c r="IW6" s="48"/>
+      <c r="IX6" s="49"/>
+      <c r="IY6" s="47"/>
+      <c r="IZ6" s="48"/>
+      <c r="JA6" s="48"/>
+      <c r="JB6" s="48"/>
+      <c r="JC6" s="48"/>
+      <c r="JD6" s="48"/>
+      <c r="JE6" s="48"/>
+      <c r="JF6" s="48"/>
+      <c r="JG6" s="48"/>
+      <c r="JH6" s="48"/>
+      <c r="JI6" s="48"/>
+      <c r="JJ6" s="48"/>
+      <c r="JK6" s="48"/>
+      <c r="JL6" s="49"/>
+      <c r="JM6" s="122"/>
+      <c r="JN6" s="122"/>
+      <c r="JO6" s="122"/>
+      <c r="JP6" s="122"/>
+      <c r="JQ6" s="122"/>
+      <c r="JR6" s="122"/>
+      <c r="JS6" s="122"/>
+      <c r="JT6" s="122"/>
+      <c r="JU6" s="122"/>
+      <c r="JV6" s="122"/>
+      <c r="JW6" s="122"/>
+      <c r="JX6" s="122"/>
+      <c r="JY6" s="122"/>
+      <c r="JZ6" s="104" t="s">
         <v>318</v>
       </c>
-      <c r="KA6" s="91"/>
-      <c r="KB6" s="91"/>
-      <c r="KC6" s="92"/>
-      <c r="KD6" s="90" t="s">
+      <c r="KA6" s="105"/>
+      <c r="KB6" s="105"/>
+      <c r="KC6" s="106"/>
+      <c r="KD6" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="KE6" s="91"/>
-      <c r="KF6" s="91"/>
-      <c r="KG6" s="92"/>
+      <c r="KE6" s="105"/>
+      <c r="KF6" s="105"/>
+      <c r="KG6" s="106"/>
     </row>
-    <row r="7" spans="1:294" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:294" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>15</v>
       </c>
@@ -4310,11 +4310,15 @@
       </c>
       <c r="KH7" s="34"/>
     </row>
-    <row r="8" spans="1:294" ht="31.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:294" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38"/>
       <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="C8" s="40" t="s">
+        <v>324</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="E8" s="38"/>
       <c r="F8" s="38"/>
       <c r="G8" s="39"/>
@@ -4324,21 +4328,33 @@
       <c r="K8" s="38"/>
       <c r="L8" s="38"/>
       <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
+      <c r="N8" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="O8" s="38"/>
       <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
+      <c r="Q8" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="R8" s="38"/>
       <c r="S8" s="38"/>
-      <c r="T8" s="38"/>
-      <c r="U8" s="38"/>
+      <c r="T8" s="40" t="s">
+        <v>324</v>
+      </c>
+      <c r="U8" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="V8" s="38"/>
-      <c r="W8" s="38"/>
+      <c r="W8" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="X8" s="41"/>
       <c r="Y8" s="41"/>
       <c r="Z8" s="38"/>
       <c r="AA8" s="38"/>
-      <c r="AB8" s="41"/>
+      <c r="AB8" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="AC8" s="38"/>
       <c r="AD8" s="41"/>
       <c r="AE8" s="41"/>
@@ -4349,7 +4365,9 @@
       <c r="AJ8" s="38"/>
       <c r="AK8" s="38"/>
       <c r="AL8" s="38"/>
-      <c r="AM8" s="38"/>
+      <c r="AM8" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="AN8" s="38"/>
       <c r="AO8" s="42"/>
       <c r="AP8" s="42"/>
@@ -4728,22 +4746,6 @@
   </sheetData>
   <autoFilter ref="B7:KH7"/>
   <mergeCells count="29">
-    <mergeCell ref="IK5:IX6"/>
-    <mergeCell ref="IY5:JL6"/>
-    <mergeCell ref="GU5:HH6"/>
-    <mergeCell ref="HI5:HV6"/>
-    <mergeCell ref="HW5:IJ6"/>
-    <mergeCell ref="FE5:FR6"/>
-    <mergeCell ref="FS5:GF6"/>
-    <mergeCell ref="GG5:GT6"/>
-    <mergeCell ref="DO5:EB6"/>
-    <mergeCell ref="EC5:EP6"/>
-    <mergeCell ref="EQ5:FD6"/>
-    <mergeCell ref="BY5:CL6"/>
-    <mergeCell ref="CM5:CZ6"/>
-    <mergeCell ref="DA5:DN6"/>
-    <mergeCell ref="KD6:KG6"/>
-    <mergeCell ref="JZ5:KG5"/>
     <mergeCell ref="K5:O6"/>
     <mergeCell ref="AJ5:AL6"/>
     <mergeCell ref="JZ6:KC6"/>
@@ -4757,6 +4759,22 @@
     <mergeCell ref="AS5:BJ6"/>
     <mergeCell ref="P5:T6"/>
     <mergeCell ref="BK5:BX6"/>
+    <mergeCell ref="BY5:CL6"/>
+    <mergeCell ref="CM5:CZ6"/>
+    <mergeCell ref="DA5:DN6"/>
+    <mergeCell ref="KD6:KG6"/>
+    <mergeCell ref="JZ5:KG5"/>
+    <mergeCell ref="FE5:FR6"/>
+    <mergeCell ref="FS5:GF6"/>
+    <mergeCell ref="GG5:GT6"/>
+    <mergeCell ref="DO5:EB6"/>
+    <mergeCell ref="EC5:EP6"/>
+    <mergeCell ref="EQ5:FD6"/>
+    <mergeCell ref="IK5:IX6"/>
+    <mergeCell ref="IY5:JL6"/>
+    <mergeCell ref="GU5:HH6"/>
+    <mergeCell ref="HI5:HV6"/>
+    <mergeCell ref="HW5:IJ6"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO1:AR6 AO8:AR1048576">

</xml_diff>

<commit_message>
Apply spreadsheet hack to fill in 'missing' formula
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MadeFiles\RubyonRails\FCRM1spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Chrome\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16524"/>
   </bookViews>
   <sheets>
     <sheet name="FCRM1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,6 @@
     <definedName name="wages_freq_int_rec">#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2249,17 +2248,17 @@
   <dimension ref="A1:KH8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="BB8" activePane="bottomRight" state="frozen"/>
       <selection activeCell="LZ2343" sqref="LZ2343"/>
       <selection pane="topRight" activeCell="LZ2343" sqref="LZ2343"/>
       <selection pane="bottomLeft" activeCell="LZ2343" sqref="LZ2343"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="BI16" sqref="BI16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.23046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="41.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" style="1" customWidth="1"/>
     <col min="3" max="6" width="21" style="1" customWidth="1"/>
     <col min="7" max="7" width="21" style="2" customWidth="1"/>
     <col min="8" max="8" width="21" style="1" customWidth="1"/>
@@ -2275,11 +2274,11 @@
     <col min="45" max="278" width="21" style="1" customWidth="1"/>
     <col min="279" max="285" width="21" style="35" customWidth="1"/>
     <col min="286" max="293" width="21" style="8" customWidth="1"/>
-    <col min="294" max="294" width="8.84375" style="8"/>
-    <col min="295" max="16384" width="8.84375" style="36"/>
+    <col min="294" max="294" width="8.81640625" style="8"/>
+    <col min="295" max="16384" width="8.81640625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:294" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:294" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CB1" s="6"/>
       <c r="CC1" s="6"/>
       <c r="CD1" s="6"/>
@@ -2292,7 +2291,7 @@
       <c r="JX1" s="7"/>
       <c r="JY1" s="7"/>
     </row>
-    <row r="2" spans="1:294" ht="28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:294" ht="28.2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -2312,7 +2311,7 @@
       <c r="JX2" s="14"/>
       <c r="JY2" s="14"/>
     </row>
-    <row r="3" spans="1:294" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:294" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>319</v>
       </c>
@@ -2352,7 +2351,7 @@
       <c r="KG3" s="16"/>
       <c r="KH3" s="16"/>
     </row>
-    <row r="4" spans="1:294" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -2648,7 +2647,7 @@
       <c r="KG4" s="22"/>
       <c r="KH4" s="18"/>
     </row>
-    <row r="5" spans="1:294" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:294" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
         <v>1</v>
       </c>
@@ -2997,7 +2996,7 @@
       <c r="KF5" s="131"/>
       <c r="KG5" s="132"/>
     </row>
-    <row r="6" spans="1:294" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:294" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="63"/>
       <c r="B6" s="64"/>
       <c r="C6" s="64"/>
@@ -3296,7 +3295,7 @@
       <c r="KF6" s="57"/>
       <c r="KG6" s="58"/>
     </row>
-    <row r="7" spans="1:294" ht="81.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:294" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>15</v>
       </c>
@@ -4178,7 +4177,7 @@
       </c>
       <c r="KH7" s="34"/>
     </row>
-    <row r="8" spans="1:294" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:294" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38"/>
       <c r="B8" s="38"/>
       <c r="C8" s="40" t="s">
@@ -4318,51 +4317,51 @@
         <v>0</v>
       </c>
       <c r="BL8" s="38">
-        <f t="shared" ref="BL8:BW8" si="1">BZ8+CN8+DB8+DP8+ED8+ER8+FF8+FT8</f>
+        <f t="shared" ref="BL8" si="1">BZ8+CN8+DB8+DP8+ED8+ER8+FF8+FT8</f>
         <v>0</v>
       </c>
       <c r="BM8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BM8" si="2">CA8+CO8+DC8+DQ8+EE8+ES8+FG8+FU8</f>
         <v>0</v>
       </c>
       <c r="BN8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BN8" si="3">CB8+CP8+DD8+DR8+EF8+ET8+FH8+FV8</f>
         <v>0</v>
       </c>
       <c r="BO8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BO8" si="4">CC8+CQ8+DE8+DS8+EG8+EU8+FI8+FW8</f>
         <v>0</v>
       </c>
       <c r="BP8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BP8" si="5">CD8+CR8+DF8+DT8+EH8+EV8+FJ8+FX8</f>
         <v>0</v>
       </c>
       <c r="BQ8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BQ8" si="6">CE8+CS8+DG8+DU8+EI8+EW8+FK8+FY8</f>
         <v>0</v>
       </c>
       <c r="BR8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BR8" si="7">CF8+CT8+DH8+DV8+EJ8+EX8+FL8+FZ8</f>
         <v>0</v>
       </c>
       <c r="BS8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BS8" si="8">CG8+CU8+DI8+DW8+EK8+EY8+FM8+GA8</f>
         <v>0</v>
       </c>
       <c r="BT8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BT8" si="9">CH8+CV8+DJ8+DX8+EL8+EZ8+FN8+GB8</f>
         <v>0</v>
       </c>
       <c r="BU8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BU8" si="10">CI8+CW8+DK8+DY8+EM8+FA8+FO8+GC8</f>
         <v>0</v>
       </c>
       <c r="BV8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BV8" si="11">CJ8+CX8+DL8+DZ8+EN8+FB8+FP8+GD8</f>
         <v>0</v>
       </c>
       <c r="BW8" s="38">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BW8" si="12">CK8+CY8+DM8+EA8+EO8+FC8+FQ8+GE8</f>
         <v>0</v>
       </c>
       <c r="BX8" s="38">

</xml_diff>

<commit_message>
Update FCERM template to resolve issue with Excel's name manager
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -5,90 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\FCRM Allocation and Programme\National FCRM Programme\System_Data Development\System Development\PAFS\17-18 improvements &amp; budget\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selks\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9024"/>
   </bookViews>
   <sheets>
     <sheet name="Master local choices" sheetId="2" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$KK$6</definedName>
-    <definedName name="AdjOMScore">'[1]PF Calculator (1-6yr Projects)'!$H$19</definedName>
-    <definedName name="Allocation" localSheetId="0">#REF!</definedName>
-    <definedName name="Allocation">#REF!</definedName>
-    <definedName name="Authority">'[1]PF Calculator (1-6yr Projects)'!$H$25</definedName>
-    <definedName name="AvCEDamages">'[1]Discount Rates &amp; Assumptions'!$K$35</definedName>
-    <definedName name="AvFloodDamages">'[1]Discount Rates &amp; Assumptions'!$K$32</definedName>
-    <definedName name="BenefitsApportioned?" localSheetId="0">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="BenefitsApportioned?">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="by_Funding_code" localSheetId="0">#REF!</definedName>
-    <definedName name="by_Funding_code">#REF!</definedName>
-    <definedName name="Construction" localSheetId="0">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="Construction">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="Contribution" localSheetId="0">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="Contribution">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="ContributionsSecured" localSheetId="0">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="ContributionsSecured">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="CostCentre" localSheetId="0">#REF!</definedName>
-    <definedName name="CostCentre">#REF!</definedName>
-    <definedName name="CostsForApproval" localSheetId="0">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="CostsForApproval">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="DeprivedAreasScalar" localSheetId="0">'[1]Discount Rates &amp; Assumptions'!#REF!</definedName>
-    <definedName name="DeprivedAreasScalar">'[1]Discount Rates &amp; Assumptions'!#REF!</definedName>
-    <definedName name="DeprivedScalar20">'[1]Discount Rates &amp; Assumptions'!$K$9</definedName>
-    <definedName name="DeprivedScalar40">'[1]Discount Rates &amp; Assumptions'!$K$10</definedName>
-    <definedName name="DeprivedScalarOther">'[1]Discount Rates &amp; Assumptions'!$K$11</definedName>
-    <definedName name="Duration">'[1]PF Calculator (1-6yr Projects)'!$H$27</definedName>
-    <definedName name="EMPLOYEE_NAME" localSheetId="0">#REF!</definedName>
-    <definedName name="EMPLOYEE_NAME">#REF!</definedName>
-    <definedName name="ExtContributionRequired" localSheetId="0">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="ExtContributionRequired">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="FDGIAContribution" localSheetId="0">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="FDGIAContribution">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="fUNDING_CODE_BY_REGION" localSheetId="0">#REF!</definedName>
-    <definedName name="fUNDING_CODE_BY_REGION">#REF!</definedName>
-    <definedName name="Maintenance" localSheetId="0">#REF!</definedName>
-    <definedName name="Maintenance">#REF!</definedName>
-    <definedName name="Maintenance_Work" localSheetId="0">#REF!</definedName>
-    <definedName name="Maintenance_Work">#REF!</definedName>
-    <definedName name="ONS_2" localSheetId="0">#REF!</definedName>
-    <definedName name="ONS_2">#REF!</definedName>
-    <definedName name="ONS_Region" localSheetId="0">#REF!</definedName>
-    <definedName name="ONS_Region">#REF!</definedName>
-    <definedName name="Ops_Delivery" localSheetId="0">#REF!</definedName>
-    <definedName name="Ops_Delivery">#REF!</definedName>
-    <definedName name="Organisation_Area" localSheetId="0">#REF!</definedName>
-    <definedName name="Organisation_Area">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Master local choices'!#REF!</definedName>
-    <definedName name="Project_Class" localSheetId="0">#REF!</definedName>
-    <definedName name="Project_Class">#REF!</definedName>
-    <definedName name="project_types" localSheetId="0">#REF!</definedName>
-    <definedName name="project_types">#REF!</definedName>
-    <definedName name="PVWLBs" localSheetId="0">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="PVWLBs">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="PVWLCs" localSheetId="0">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="PVWLCs">'[1]PF Calculator (1-6yr Projects)'!#REF!</definedName>
-    <definedName name="RawOMScore">'[1]PF Calculator (1-6yr Projects)'!$H$15</definedName>
-    <definedName name="REV_BID_v_ALLOC" localSheetId="0">#REF!</definedName>
-    <definedName name="REV_BID_v_ALLOC">#REF!</definedName>
-    <definedName name="SL_50" localSheetId="0">#REF!</definedName>
-    <definedName name="SL_50">#REF!</definedName>
-    <definedName name="SLs_by_RFDC" localSheetId="0">#REF!</definedName>
-    <definedName name="SLs_by_RFDC">#REF!</definedName>
-    <definedName name="SUMMARY_by_SLs" localSheetId="0">#REF!</definedName>
-    <definedName name="SUMMARY_by_SLs">#REF!</definedName>
-    <definedName name="TargetBCRWLBs">'[1]Discount Rates &amp; Assumptions'!$K$6</definedName>
-    <definedName name="TargetMinBCR">'[1]Discount Rates &amp; Assumptions'!$K$5</definedName>
-    <definedName name="Total_Allocation" localSheetId="0">#REF!</definedName>
-    <definedName name="Total_Allocation">#REF!</definedName>
-    <definedName name="wages_freq_int_rec" localSheetId="0">#REF!</definedName>
-    <definedName name="wages_freq_int_rec">#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -1764,6 +1691,69 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1782,74 +1772,11 @@
     <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1885,107 +1812,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Changes"/>
-      <sheetName val="User notes"/>
-      <sheetName val="Proposal Part1 (All Projects)"/>
-      <sheetName val="PF Score Estimator Tool"/>
-      <sheetName val="Proposal Part2 (1-6yr Projects)"/>
-      <sheetName val="PF Calculator (1-6yr Projects)"/>
-      <sheetName val="PV Calculator Tool"/>
-      <sheetName val="Discount Rates &amp; Assumptions"/>
-      <sheetName val="Version Control"/>
-      <sheetName val="Sensitivity 1"/>
-      <sheetName val="Sensitivity 2"/>
-      <sheetName val="Sensitivity 3"/>
-      <sheetName val="Sensitivity 4"/>
-      <sheetName val="Sensitivity 5"/>
-      <sheetName val="Urgency Moderation form"/>
-      <sheetName val="FCRM1 form"/>
-      <sheetName val="FCRM1 field descriptions"/>
-      <sheetName val="Deprived areas map"/>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
-        <row r="15">
-          <cell r="H15" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="H19" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="H25">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7">
-        <row r="5">
-          <cell r="K5">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="K6">
-            <v>18</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="K9">
-            <v>2.25</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="K10">
-            <v>1.5</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="K11">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="K32">
-            <v>30</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="K35">
-            <v>6000</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2258,16 +2084,16 @@
   <dimension ref="A1:KL7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="CE7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="CJ7" sqref="CJ7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54" style="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="3" customWidth="1"/>
     <col min="5" max="6" width="21" style="1" customWidth="1"/>
@@ -2285,17 +2111,17 @@
     <col min="45" max="278" width="21" style="1" customWidth="1"/>
     <col min="279" max="285" width="21" style="29" customWidth="1"/>
     <col min="286" max="293" width="21" style="6" customWidth="1"/>
-    <col min="294" max="296" width="22.21875" style="7" customWidth="1"/>
-    <col min="297" max="297" width="13.21875" style="7" customWidth="1"/>
+    <col min="294" max="296" width="22.1796875" style="7" customWidth="1"/>
+    <col min="297" max="297" width="13.1796875" style="7" customWidth="1"/>
     <col min="298" max="298" width="11" style="7" customWidth="1"/>
-    <col min="299" max="16384" width="8.77734375" style="7"/>
+    <col min="299" max="16384" width="8.81640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
+    <row r="1" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
+      <c r="B1" s="62"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
@@ -2588,11 +2414,11 @@
       <c r="KF1" s="23"/>
       <c r="KG1" s="23"/>
     </row>
-    <row r="2" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="82" t="s">
+    <row r="2" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="63" t="s">
         <v>320</v>
       </c>
-      <c r="B2" s="82"/>
+      <c r="B2" s="63"/>
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
       <c r="E2" s="23"/>
@@ -2885,7 +2711,7 @@
       <c r="KF2" s="42"/>
       <c r="KG2" s="42"/>
     </row>
-    <row r="3" spans="1:298" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:298" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44"/>
       <c r="B3" s="45"/>
       <c r="C3" s="44"/>
@@ -3180,423 +3006,423 @@
       <c r="KF3" s="50"/>
       <c r="KG3" s="50"/>
     </row>
-    <row r="4" spans="1:298" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="83" t="s">
+    <row r="4" spans="1:298" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="84" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="85" t="s">
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="85"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="85"/>
-      <c r="P4" s="86" t="s">
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="87" t="s">
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="87"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="88" t="s">
+      <c r="V4" s="68"/>
+      <c r="W4" s="68"/>
+      <c r="X4" s="68"/>
+      <c r="Y4" s="68"/>
+      <c r="Z4" s="68"/>
+      <c r="AA4" s="68"/>
+      <c r="AB4" s="68"/>
+      <c r="AC4" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="88"/>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
-      <c r="AH4" s="88"/>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="89" t="s">
+      <c r="AD4" s="69"/>
+      <c r="AE4" s="69"/>
+      <c r="AF4" s="69"/>
+      <c r="AG4" s="69"/>
+      <c r="AH4" s="69"/>
+      <c r="AI4" s="69"/>
+      <c r="AJ4" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="89"/>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="80" t="s">
+      <c r="AK4" s="70"/>
+      <c r="AL4" s="70"/>
+      <c r="AM4" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="80"/>
-      <c r="AO4" s="70"/>
-      <c r="AP4" s="70"/>
-      <c r="AQ4" s="70"/>
-      <c r="AR4" s="70"/>
-      <c r="AS4" s="71" t="s">
+      <c r="AN4" s="61"/>
+      <c r="AO4" s="72"/>
+      <c r="AP4" s="72"/>
+      <c r="AQ4" s="72"/>
+      <c r="AR4" s="72"/>
+      <c r="AS4" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="71"/>
-      <c r="AU4" s="71"/>
-      <c r="AV4" s="71"/>
-      <c r="AW4" s="71"/>
-      <c r="AX4" s="71"/>
-      <c r="AY4" s="71"/>
-      <c r="AZ4" s="71"/>
-      <c r="BA4" s="71"/>
-      <c r="BB4" s="71"/>
-      <c r="BC4" s="71"/>
-      <c r="BD4" s="71"/>
-      <c r="BE4" s="71"/>
-      <c r="BF4" s="71"/>
-      <c r="BG4" s="71"/>
-      <c r="BH4" s="71"/>
-      <c r="BI4" s="71"/>
-      <c r="BJ4" s="71"/>
-      <c r="BK4" s="67" t="s">
+      <c r="AT4" s="73"/>
+      <c r="AU4" s="73"/>
+      <c r="AV4" s="73"/>
+      <c r="AW4" s="73"/>
+      <c r="AX4" s="73"/>
+      <c r="AY4" s="73"/>
+      <c r="AZ4" s="73"/>
+      <c r="BA4" s="73"/>
+      <c r="BB4" s="73"/>
+      <c r="BC4" s="73"/>
+      <c r="BD4" s="73"/>
+      <c r="BE4" s="73"/>
+      <c r="BF4" s="73"/>
+      <c r="BG4" s="73"/>
+      <c r="BH4" s="73"/>
+      <c r="BI4" s="73"/>
+      <c r="BJ4" s="73"/>
+      <c r="BK4" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="BL4" s="67"/>
-      <c r="BM4" s="67"/>
-      <c r="BN4" s="67"/>
-      <c r="BO4" s="67"/>
-      <c r="BP4" s="67"/>
-      <c r="BQ4" s="67"/>
-      <c r="BR4" s="67"/>
-      <c r="BS4" s="67"/>
-      <c r="BT4" s="67"/>
-      <c r="BU4" s="67"/>
-      <c r="BV4" s="67"/>
-      <c r="BW4" s="67"/>
-      <c r="BX4" s="67"/>
-      <c r="BY4" s="72" t="s">
+      <c r="BL4" s="71"/>
+      <c r="BM4" s="71"/>
+      <c r="BN4" s="71"/>
+      <c r="BO4" s="71"/>
+      <c r="BP4" s="71"/>
+      <c r="BQ4" s="71"/>
+      <c r="BR4" s="71"/>
+      <c r="BS4" s="71"/>
+      <c r="BT4" s="71"/>
+      <c r="BU4" s="71"/>
+      <c r="BV4" s="71"/>
+      <c r="BW4" s="71"/>
+      <c r="BX4" s="71"/>
+      <c r="BY4" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="72"/>
-      <c r="CA4" s="72"/>
-      <c r="CB4" s="72"/>
-      <c r="CC4" s="72"/>
-      <c r="CD4" s="72"/>
-      <c r="CE4" s="72"/>
-      <c r="CF4" s="72"/>
-      <c r="CG4" s="72"/>
-      <c r="CH4" s="72"/>
-      <c r="CI4" s="72"/>
-      <c r="CJ4" s="72"/>
-      <c r="CK4" s="72"/>
-      <c r="CL4" s="72"/>
-      <c r="CM4" s="73" t="s">
+      <c r="BZ4" s="74"/>
+      <c r="CA4" s="74"/>
+      <c r="CB4" s="74"/>
+      <c r="CC4" s="74"/>
+      <c r="CD4" s="74"/>
+      <c r="CE4" s="74"/>
+      <c r="CF4" s="74"/>
+      <c r="CG4" s="74"/>
+      <c r="CH4" s="74"/>
+      <c r="CI4" s="74"/>
+      <c r="CJ4" s="74"/>
+      <c r="CK4" s="74"/>
+      <c r="CL4" s="74"/>
+      <c r="CM4" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="73"/>
-      <c r="CO4" s="73"/>
-      <c r="CP4" s="73"/>
-      <c r="CQ4" s="73"/>
-      <c r="CR4" s="73"/>
-      <c r="CS4" s="73"/>
-      <c r="CT4" s="73"/>
-      <c r="CU4" s="73"/>
-      <c r="CV4" s="73"/>
-      <c r="CW4" s="73"/>
-      <c r="CX4" s="73"/>
-      <c r="CY4" s="73"/>
-      <c r="CZ4" s="73"/>
-      <c r="DA4" s="74" t="s">
+      <c r="CN4" s="75"/>
+      <c r="CO4" s="75"/>
+      <c r="CP4" s="75"/>
+      <c r="CQ4" s="75"/>
+      <c r="CR4" s="75"/>
+      <c r="CS4" s="75"/>
+      <c r="CT4" s="75"/>
+      <c r="CU4" s="75"/>
+      <c r="CV4" s="75"/>
+      <c r="CW4" s="75"/>
+      <c r="CX4" s="75"/>
+      <c r="CY4" s="75"/>
+      <c r="CZ4" s="75"/>
+      <c r="DA4" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="74"/>
-      <c r="DC4" s="74"/>
-      <c r="DD4" s="74"/>
-      <c r="DE4" s="74"/>
-      <c r="DF4" s="74"/>
-      <c r="DG4" s="74"/>
-      <c r="DH4" s="74"/>
-      <c r="DI4" s="74"/>
-      <c r="DJ4" s="74"/>
-      <c r="DK4" s="74"/>
-      <c r="DL4" s="74"/>
-      <c r="DM4" s="74"/>
-      <c r="DN4" s="74"/>
-      <c r="DO4" s="75" t="s">
+      <c r="DB4" s="76"/>
+      <c r="DC4" s="76"/>
+      <c r="DD4" s="76"/>
+      <c r="DE4" s="76"/>
+      <c r="DF4" s="76"/>
+      <c r="DG4" s="76"/>
+      <c r="DH4" s="76"/>
+      <c r="DI4" s="76"/>
+      <c r="DJ4" s="76"/>
+      <c r="DK4" s="76"/>
+      <c r="DL4" s="76"/>
+      <c r="DM4" s="76"/>
+      <c r="DN4" s="76"/>
+      <c r="DO4" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="75"/>
-      <c r="DQ4" s="75"/>
-      <c r="DR4" s="75"/>
-      <c r="DS4" s="75"/>
-      <c r="DT4" s="75"/>
-      <c r="DU4" s="75"/>
-      <c r="DV4" s="75"/>
-      <c r="DW4" s="75"/>
-      <c r="DX4" s="75"/>
-      <c r="DY4" s="75"/>
-      <c r="DZ4" s="75"/>
-      <c r="EA4" s="75"/>
-      <c r="EB4" s="75"/>
-      <c r="EC4" s="76" t="s">
+      <c r="DP4" s="77"/>
+      <c r="DQ4" s="77"/>
+      <c r="DR4" s="77"/>
+      <c r="DS4" s="77"/>
+      <c r="DT4" s="77"/>
+      <c r="DU4" s="77"/>
+      <c r="DV4" s="77"/>
+      <c r="DW4" s="77"/>
+      <c r="DX4" s="77"/>
+      <c r="DY4" s="77"/>
+      <c r="DZ4" s="77"/>
+      <c r="EA4" s="77"/>
+      <c r="EB4" s="77"/>
+      <c r="EC4" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="76"/>
-      <c r="EE4" s="76"/>
-      <c r="EF4" s="76"/>
-      <c r="EG4" s="76"/>
-      <c r="EH4" s="76"/>
-      <c r="EI4" s="76"/>
-      <c r="EJ4" s="76"/>
-      <c r="EK4" s="76"/>
-      <c r="EL4" s="76"/>
-      <c r="EM4" s="76"/>
-      <c r="EN4" s="76"/>
-      <c r="EO4" s="76"/>
-      <c r="EP4" s="76"/>
-      <c r="EQ4" s="77" t="s">
+      <c r="ED4" s="78"/>
+      <c r="EE4" s="78"/>
+      <c r="EF4" s="78"/>
+      <c r="EG4" s="78"/>
+      <c r="EH4" s="78"/>
+      <c r="EI4" s="78"/>
+      <c r="EJ4" s="78"/>
+      <c r="EK4" s="78"/>
+      <c r="EL4" s="78"/>
+      <c r="EM4" s="78"/>
+      <c r="EN4" s="78"/>
+      <c r="EO4" s="78"/>
+      <c r="EP4" s="78"/>
+      <c r="EQ4" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="77"/>
-      <c r="ES4" s="77"/>
-      <c r="ET4" s="77"/>
-      <c r="EU4" s="77"/>
-      <c r="EV4" s="77"/>
-      <c r="EW4" s="77"/>
-      <c r="EX4" s="77"/>
-      <c r="EY4" s="77"/>
-      <c r="EZ4" s="77"/>
-      <c r="FA4" s="77"/>
-      <c r="FB4" s="77"/>
-      <c r="FC4" s="77"/>
-      <c r="FD4" s="77"/>
-      <c r="FE4" s="78" t="s">
+      <c r="ER4" s="79"/>
+      <c r="ES4" s="79"/>
+      <c r="ET4" s="79"/>
+      <c r="EU4" s="79"/>
+      <c r="EV4" s="79"/>
+      <c r="EW4" s="79"/>
+      <c r="EX4" s="79"/>
+      <c r="EY4" s="79"/>
+      <c r="EZ4" s="79"/>
+      <c r="FA4" s="79"/>
+      <c r="FB4" s="79"/>
+      <c r="FC4" s="79"/>
+      <c r="FD4" s="79"/>
+      <c r="FE4" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="78"/>
-      <c r="FG4" s="78"/>
-      <c r="FH4" s="78"/>
-      <c r="FI4" s="78"/>
-      <c r="FJ4" s="78"/>
-      <c r="FK4" s="78"/>
-      <c r="FL4" s="78"/>
-      <c r="FM4" s="78"/>
-      <c r="FN4" s="78"/>
-      <c r="FO4" s="78"/>
-      <c r="FP4" s="78"/>
-      <c r="FQ4" s="78"/>
-      <c r="FR4" s="78"/>
-      <c r="FS4" s="79" t="s">
+      <c r="FF4" s="80"/>
+      <c r="FG4" s="80"/>
+      <c r="FH4" s="80"/>
+      <c r="FI4" s="80"/>
+      <c r="FJ4" s="80"/>
+      <c r="FK4" s="80"/>
+      <c r="FL4" s="80"/>
+      <c r="FM4" s="80"/>
+      <c r="FN4" s="80"/>
+      <c r="FO4" s="80"/>
+      <c r="FP4" s="80"/>
+      <c r="FQ4" s="80"/>
+      <c r="FR4" s="80"/>
+      <c r="FS4" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="79"/>
-      <c r="FU4" s="79"/>
-      <c r="FV4" s="79"/>
-      <c r="FW4" s="79"/>
-      <c r="FX4" s="79"/>
-      <c r="FY4" s="79"/>
-      <c r="FZ4" s="79"/>
-      <c r="GA4" s="79"/>
-      <c r="GB4" s="79"/>
-      <c r="GC4" s="79"/>
-      <c r="GD4" s="79"/>
-      <c r="GE4" s="79"/>
-      <c r="GF4" s="79"/>
-      <c r="GG4" s="67" t="s">
+      <c r="FT4" s="81"/>
+      <c r="FU4" s="81"/>
+      <c r="FV4" s="81"/>
+      <c r="FW4" s="81"/>
+      <c r="FX4" s="81"/>
+      <c r="FY4" s="81"/>
+      <c r="FZ4" s="81"/>
+      <c r="GA4" s="81"/>
+      <c r="GB4" s="81"/>
+      <c r="GC4" s="81"/>
+      <c r="GD4" s="81"/>
+      <c r="GE4" s="81"/>
+      <c r="GF4" s="81"/>
+      <c r="GG4" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="GH4" s="67"/>
-      <c r="GI4" s="67"/>
-      <c r="GJ4" s="67"/>
-      <c r="GK4" s="67"/>
-      <c r="GL4" s="67"/>
-      <c r="GM4" s="67"/>
-      <c r="GN4" s="67"/>
-      <c r="GO4" s="67"/>
-      <c r="GP4" s="67"/>
-      <c r="GQ4" s="67"/>
-      <c r="GR4" s="67"/>
-      <c r="GS4" s="67"/>
-      <c r="GT4" s="67"/>
-      <c r="GU4" s="67" t="s">
+      <c r="GH4" s="71"/>
+      <c r="GI4" s="71"/>
+      <c r="GJ4" s="71"/>
+      <c r="GK4" s="71"/>
+      <c r="GL4" s="71"/>
+      <c r="GM4" s="71"/>
+      <c r="GN4" s="71"/>
+      <c r="GO4" s="71"/>
+      <c r="GP4" s="71"/>
+      <c r="GQ4" s="71"/>
+      <c r="GR4" s="71"/>
+      <c r="GS4" s="71"/>
+      <c r="GT4" s="71"/>
+      <c r="GU4" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="GV4" s="67"/>
-      <c r="GW4" s="67"/>
-      <c r="GX4" s="67"/>
-      <c r="GY4" s="67"/>
-      <c r="GZ4" s="67"/>
-      <c r="HA4" s="67"/>
-      <c r="HB4" s="67"/>
-      <c r="HC4" s="67"/>
-      <c r="HD4" s="67"/>
-      <c r="HE4" s="67"/>
-      <c r="HF4" s="67"/>
-      <c r="HG4" s="67"/>
-      <c r="HH4" s="67"/>
-      <c r="HI4" s="67" t="s">
+      <c r="GV4" s="71"/>
+      <c r="GW4" s="71"/>
+      <c r="GX4" s="71"/>
+      <c r="GY4" s="71"/>
+      <c r="GZ4" s="71"/>
+      <c r="HA4" s="71"/>
+      <c r="HB4" s="71"/>
+      <c r="HC4" s="71"/>
+      <c r="HD4" s="71"/>
+      <c r="HE4" s="71"/>
+      <c r="HF4" s="71"/>
+      <c r="HG4" s="71"/>
+      <c r="HH4" s="71"/>
+      <c r="HI4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="HJ4" s="67"/>
-      <c r="HK4" s="67"/>
-      <c r="HL4" s="67"/>
-      <c r="HM4" s="67"/>
-      <c r="HN4" s="67"/>
-      <c r="HO4" s="67"/>
-      <c r="HP4" s="67"/>
-      <c r="HQ4" s="67"/>
-      <c r="HR4" s="67"/>
-      <c r="HS4" s="67"/>
-      <c r="HT4" s="67"/>
-      <c r="HU4" s="67"/>
-      <c r="HV4" s="67"/>
-      <c r="HW4" s="68" t="s">
+      <c r="HJ4" s="71"/>
+      <c r="HK4" s="71"/>
+      <c r="HL4" s="71"/>
+      <c r="HM4" s="71"/>
+      <c r="HN4" s="71"/>
+      <c r="HO4" s="71"/>
+      <c r="HP4" s="71"/>
+      <c r="HQ4" s="71"/>
+      <c r="HR4" s="71"/>
+      <c r="HS4" s="71"/>
+      <c r="HT4" s="71"/>
+      <c r="HU4" s="71"/>
+      <c r="HV4" s="71"/>
+      <c r="HW4" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="68"/>
-      <c r="HY4" s="68"/>
-      <c r="HZ4" s="68"/>
-      <c r="IA4" s="68"/>
-      <c r="IB4" s="68"/>
-      <c r="IC4" s="68"/>
-      <c r="ID4" s="68"/>
-      <c r="IE4" s="68"/>
-      <c r="IF4" s="68"/>
-      <c r="IG4" s="68"/>
-      <c r="IH4" s="68"/>
-      <c r="II4" s="68"/>
-      <c r="IJ4" s="68"/>
-      <c r="IK4" s="68" t="s">
+      <c r="HX4" s="88"/>
+      <c r="HY4" s="88"/>
+      <c r="HZ4" s="88"/>
+      <c r="IA4" s="88"/>
+      <c r="IB4" s="88"/>
+      <c r="IC4" s="88"/>
+      <c r="ID4" s="88"/>
+      <c r="IE4" s="88"/>
+      <c r="IF4" s="88"/>
+      <c r="IG4" s="88"/>
+      <c r="IH4" s="88"/>
+      <c r="II4" s="88"/>
+      <c r="IJ4" s="88"/>
+      <c r="IK4" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="68"/>
-      <c r="IM4" s="68"/>
-      <c r="IN4" s="68"/>
-      <c r="IO4" s="68"/>
-      <c r="IP4" s="68"/>
-      <c r="IQ4" s="68"/>
-      <c r="IR4" s="68"/>
-      <c r="IS4" s="68"/>
-      <c r="IT4" s="68"/>
-      <c r="IU4" s="68"/>
-      <c r="IV4" s="68"/>
-      <c r="IW4" s="68"/>
-      <c r="IX4" s="68"/>
-      <c r="IY4" s="68" t="s">
+      <c r="IL4" s="88"/>
+      <c r="IM4" s="88"/>
+      <c r="IN4" s="88"/>
+      <c r="IO4" s="88"/>
+      <c r="IP4" s="88"/>
+      <c r="IQ4" s="88"/>
+      <c r="IR4" s="88"/>
+      <c r="IS4" s="88"/>
+      <c r="IT4" s="88"/>
+      <c r="IU4" s="88"/>
+      <c r="IV4" s="88"/>
+      <c r="IW4" s="88"/>
+      <c r="IX4" s="88"/>
+      <c r="IY4" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="68"/>
-      <c r="JA4" s="68"/>
-      <c r="JB4" s="68"/>
-      <c r="JC4" s="68"/>
-      <c r="JD4" s="68"/>
-      <c r="JE4" s="68"/>
-      <c r="JF4" s="68"/>
-      <c r="JG4" s="68"/>
-      <c r="JH4" s="68"/>
-      <c r="JI4" s="68"/>
-      <c r="JJ4" s="68"/>
-      <c r="JK4" s="68"/>
-      <c r="JL4" s="68"/>
-      <c r="JM4" s="69" t="s">
+      <c r="IZ4" s="88"/>
+      <c r="JA4" s="88"/>
+      <c r="JB4" s="88"/>
+      <c r="JC4" s="88"/>
+      <c r="JD4" s="88"/>
+      <c r="JE4" s="88"/>
+      <c r="JF4" s="88"/>
+      <c r="JG4" s="88"/>
+      <c r="JH4" s="88"/>
+      <c r="JI4" s="88"/>
+      <c r="JJ4" s="88"/>
+      <c r="JK4" s="88"/>
+      <c r="JL4" s="88"/>
+      <c r="JM4" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="69"/>
-      <c r="JO4" s="69"/>
-      <c r="JP4" s="69"/>
-      <c r="JQ4" s="69"/>
-      <c r="JR4" s="69"/>
-      <c r="JS4" s="69"/>
-      <c r="JT4" s="69"/>
-      <c r="JU4" s="69"/>
-      <c r="JV4" s="69"/>
-      <c r="JW4" s="69"/>
-      <c r="JX4" s="69"/>
-      <c r="JY4" s="69"/>
-      <c r="JZ4" s="65" t="s">
+      <c r="JN4" s="89"/>
+      <c r="JO4" s="89"/>
+      <c r="JP4" s="89"/>
+      <c r="JQ4" s="89"/>
+      <c r="JR4" s="89"/>
+      <c r="JS4" s="89"/>
+      <c r="JT4" s="89"/>
+      <c r="JU4" s="89"/>
+      <c r="JV4" s="89"/>
+      <c r="JW4" s="89"/>
+      <c r="JX4" s="89"/>
+      <c r="JY4" s="89"/>
+      <c r="JZ4" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="66"/>
-      <c r="KB4" s="66"/>
-      <c r="KC4" s="66"/>
-      <c r="KD4" s="66"/>
-      <c r="KE4" s="66"/>
-      <c r="KF4" s="66"/>
-      <c r="KG4" s="66"/>
-      <c r="KH4" s="61" t="s">
+      <c r="KA4" s="87"/>
+      <c r="KB4" s="87"/>
+      <c r="KC4" s="87"/>
+      <c r="KD4" s="87"/>
+      <c r="KE4" s="87"/>
+      <c r="KF4" s="87"/>
+      <c r="KG4" s="87"/>
+      <c r="KH4" s="82" t="s">
         <v>322</v>
       </c>
-      <c r="KI4" s="62"/>
-      <c r="KJ4" s="62"/>
-      <c r="KK4" s="62"/>
+      <c r="KI4" s="83"/>
+      <c r="KJ4" s="83"/>
+      <c r="KK4" s="83"/>
       <c r="KL4" s="60"/>
     </row>
-    <row r="5" spans="1:298" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="83"/>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="85"/>
-      <c r="L5" s="85"/>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="86"/>
-      <c r="Q5" s="86"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="86"/>
-      <c r="T5" s="86"/>
-      <c r="U5" s="87"/>
-      <c r="V5" s="87"/>
-      <c r="W5" s="87"/>
-      <c r="X5" s="87"/>
-      <c r="Y5" s="87"/>
-      <c r="Z5" s="87"/>
-      <c r="AA5" s="87"/>
-      <c r="AB5" s="87"/>
-      <c r="AC5" s="88"/>
-      <c r="AD5" s="88"/>
-      <c r="AE5" s="88"/>
-      <c r="AF5" s="88"/>
-      <c r="AG5" s="88"/>
-      <c r="AH5" s="88"/>
-      <c r="AI5" s="88"/>
-      <c r="AJ5" s="89"/>
-      <c r="AK5" s="89"/>
-      <c r="AL5" s="89"/>
-      <c r="AM5" s="80"/>
-      <c r="AN5" s="80"/>
-      <c r="AO5" s="70"/>
-      <c r="AP5" s="70"/>
-      <c r="AQ5" s="70"/>
-      <c r="AR5" s="70"/>
-      <c r="AS5" s="71"/>
-      <c r="AT5" s="71"/>
-      <c r="AU5" s="71"/>
-      <c r="AV5" s="71"/>
-      <c r="AW5" s="71"/>
-      <c r="AX5" s="71"/>
-      <c r="AY5" s="71"/>
-      <c r="AZ5" s="71"/>
-      <c r="BA5" s="71"/>
-      <c r="BB5" s="71"/>
-      <c r="BC5" s="71"/>
-      <c r="BD5" s="71"/>
-      <c r="BE5" s="71"/>
-      <c r="BF5" s="71"/>
-      <c r="BG5" s="71"/>
-      <c r="BH5" s="71"/>
-      <c r="BI5" s="71"/>
-      <c r="BJ5" s="71"/>
+    <row r="5" spans="1:298" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="64"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="67"/>
+      <c r="U5" s="68"/>
+      <c r="V5" s="68"/>
+      <c r="W5" s="68"/>
+      <c r="X5" s="68"/>
+      <c r="Y5" s="68"/>
+      <c r="Z5" s="68"/>
+      <c r="AA5" s="68"/>
+      <c r="AB5" s="68"/>
+      <c r="AC5" s="69"/>
+      <c r="AD5" s="69"/>
+      <c r="AE5" s="69"/>
+      <c r="AF5" s="69"/>
+      <c r="AG5" s="69"/>
+      <c r="AH5" s="69"/>
+      <c r="AI5" s="69"/>
+      <c r="AJ5" s="70"/>
+      <c r="AK5" s="70"/>
+      <c r="AL5" s="70"/>
+      <c r="AM5" s="61"/>
+      <c r="AN5" s="61"/>
+      <c r="AO5" s="72"/>
+      <c r="AP5" s="72"/>
+      <c r="AQ5" s="72"/>
+      <c r="AR5" s="72"/>
+      <c r="AS5" s="73"/>
+      <c r="AT5" s="73"/>
+      <c r="AU5" s="73"/>
+      <c r="AV5" s="73"/>
+      <c r="AW5" s="73"/>
+      <c r="AX5" s="73"/>
+      <c r="AY5" s="73"/>
+      <c r="AZ5" s="73"/>
+      <c r="BA5" s="73"/>
+      <c r="BB5" s="73"/>
+      <c r="BC5" s="73"/>
+      <c r="BD5" s="73"/>
+      <c r="BE5" s="73"/>
+      <c r="BF5" s="73"/>
+      <c r="BG5" s="73"/>
+      <c r="BH5" s="73"/>
+      <c r="BI5" s="73"/>
+      <c r="BJ5" s="73"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -4227,38 +4053,38 @@
       <c r="JL5" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="JM5" s="69"/>
-      <c r="JN5" s="69"/>
-      <c r="JO5" s="69"/>
-      <c r="JP5" s="69"/>
-      <c r="JQ5" s="69"/>
-      <c r="JR5" s="69"/>
-      <c r="JS5" s="69"/>
-      <c r="JT5" s="69"/>
-      <c r="JU5" s="69"/>
-      <c r="JV5" s="69"/>
-      <c r="JW5" s="69"/>
-      <c r="JX5" s="69"/>
-      <c r="JY5" s="69"/>
-      <c r="JZ5" s="66" t="s">
+      <c r="JM5" s="89"/>
+      <c r="JN5" s="89"/>
+      <c r="JO5" s="89"/>
+      <c r="JP5" s="89"/>
+      <c r="JQ5" s="89"/>
+      <c r="JR5" s="89"/>
+      <c r="JS5" s="89"/>
+      <c r="JT5" s="89"/>
+      <c r="JU5" s="89"/>
+      <c r="JV5" s="89"/>
+      <c r="JW5" s="89"/>
+      <c r="JX5" s="89"/>
+      <c r="JY5" s="89"/>
+      <c r="JZ5" s="87" t="s">
         <v>316</v>
       </c>
-      <c r="KA5" s="66"/>
-      <c r="KB5" s="66"/>
-      <c r="KC5" s="66"/>
-      <c r="KD5" s="66" t="s">
+      <c r="KA5" s="87"/>
+      <c r="KB5" s="87"/>
+      <c r="KC5" s="87"/>
+      <c r="KD5" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="66"/>
-      <c r="KF5" s="66"/>
-      <c r="KG5" s="66"/>
-      <c r="KH5" s="63"/>
-      <c r="KI5" s="64"/>
-      <c r="KJ5" s="64"/>
-      <c r="KK5" s="64"/>
+      <c r="KE5" s="87"/>
+      <c r="KF5" s="87"/>
+      <c r="KG5" s="87"/>
+      <c r="KH5" s="84"/>
+      <c r="KI5" s="85"/>
+      <c r="KJ5" s="85"/>
+      <c r="KK5" s="85"/>
       <c r="KL5" s="60"/>
     </row>
-    <row r="6" spans="1:298" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:298" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -5154,7 +4980,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="7" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
       <c r="C7" s="32"/>
@@ -5581,16 +5407,16 @@
     </sortState>
   </autoFilter>
   <mergeCells count="32">
-    <mergeCell ref="AM4:AN5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:D5"/>
-    <mergeCell ref="E4:J5"/>
-    <mergeCell ref="K4:O5"/>
-    <mergeCell ref="P4:T5"/>
-    <mergeCell ref="U4:AB5"/>
-    <mergeCell ref="AC4:AI5"/>
-    <mergeCell ref="AJ4:AL5"/>
+    <mergeCell ref="KH4:KK5"/>
+    <mergeCell ref="JZ4:KG4"/>
+    <mergeCell ref="JZ5:KC5"/>
+    <mergeCell ref="KD5:KG5"/>
+    <mergeCell ref="GU4:HH4"/>
+    <mergeCell ref="HI4:HV4"/>
+    <mergeCell ref="HW4:IJ4"/>
+    <mergeCell ref="IK4:IX4"/>
+    <mergeCell ref="IY4:JL4"/>
+    <mergeCell ref="JM4:JY5"/>
     <mergeCell ref="GG4:GT4"/>
     <mergeCell ref="AO4:AR5"/>
     <mergeCell ref="AS4:BJ5"/>
@@ -5603,16 +5429,16 @@
     <mergeCell ref="EQ4:FD4"/>
     <mergeCell ref="FE4:FR4"/>
     <mergeCell ref="FS4:GF4"/>
-    <mergeCell ref="KH4:KK5"/>
-    <mergeCell ref="JZ4:KG4"/>
-    <mergeCell ref="JZ5:KC5"/>
-    <mergeCell ref="KD5:KG5"/>
-    <mergeCell ref="GU4:HH4"/>
-    <mergeCell ref="HI4:HV4"/>
-    <mergeCell ref="HW4:IJ4"/>
-    <mergeCell ref="IK4:IX4"/>
-    <mergeCell ref="IY4:JL4"/>
-    <mergeCell ref="JM4:JY5"/>
+    <mergeCell ref="AM4:AN5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:D5"/>
+    <mergeCell ref="E4:J5"/>
+    <mergeCell ref="K4:O5"/>
+    <mergeCell ref="P4:T5"/>
+    <mergeCell ref="U4:AB5"/>
+    <mergeCell ref="AC4:AI5"/>
+    <mergeCell ref="AJ4:AL5"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>

</xml_diff>

<commit_message>
Update FCRM1 to include a filter for a project's status
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selks\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssargeant\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9024"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="Master local choices" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$KK$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$KL$6</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="344">
   <si>
     <t>FCRM1 - National Capital Programme</t>
   </si>
@@ -1171,6 +1171,9 @@
   </si>
   <si>
     <t>PAFS Status</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1691,6 +1694,63 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1720,63 +1780,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -2084,16 +2087,16 @@
   <dimension ref="A1:KL7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="CE7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="CJ7" sqref="CJ7"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54" style="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="3" customWidth="1"/>
     <col min="5" max="6" width="21" style="1" customWidth="1"/>
@@ -2111,17 +2114,17 @@
     <col min="45" max="278" width="21" style="1" customWidth="1"/>
     <col min="279" max="285" width="21" style="29" customWidth="1"/>
     <col min="286" max="293" width="21" style="6" customWidth="1"/>
-    <col min="294" max="296" width="22.1796875" style="7" customWidth="1"/>
-    <col min="297" max="297" width="13.1796875" style="7" customWidth="1"/>
+    <col min="294" max="296" width="22.21875" style="7" customWidth="1"/>
+    <col min="297" max="297" width="13.21875" style="7" customWidth="1"/>
     <col min="298" max="298" width="11" style="7" customWidth="1"/>
-    <col min="299" max="16384" width="8.81640625" style="7"/>
+    <col min="299" max="16384" width="8.77734375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
+      <c r="B1" s="81"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
@@ -2414,11 +2417,11 @@
       <c r="KF1" s="23"/>
       <c r="KG1" s="23"/>
     </row>
-    <row r="2" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+    <row r="2" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="82" t="s">
         <v>320</v>
       </c>
-      <c r="B2" s="63"/>
+      <c r="B2" s="82"/>
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
       <c r="E2" s="23"/>
@@ -2711,7 +2714,7 @@
       <c r="KF2" s="42"/>
       <c r="KG2" s="42"/>
     </row>
-    <row r="3" spans="1:298" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:298" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="44"/>
       <c r="B3" s="45"/>
       <c r="C3" s="44"/>
@@ -3006,423 +3009,423 @@
       <c r="KF3" s="50"/>
       <c r="KG3" s="50"/>
     </row>
-    <row r="4" spans="1:298" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+    <row r="4" spans="1:298" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="65" t="s">
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="66" t="s">
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="67" t="s">
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="68" t="s">
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="68"/>
-      <c r="W4" s="68"/>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="68"/>
-      <c r="Z4" s="68"/>
-      <c r="AA4" s="68"/>
-      <c r="AB4" s="68"/>
-      <c r="AC4" s="69" t="s">
+      <c r="V4" s="87"/>
+      <c r="W4" s="87"/>
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="87"/>
+      <c r="AA4" s="87"/>
+      <c r="AB4" s="87"/>
+      <c r="AC4" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="69"/>
-      <c r="AE4" s="69"/>
-      <c r="AF4" s="69"/>
-      <c r="AG4" s="69"/>
-      <c r="AH4" s="69"/>
-      <c r="AI4" s="69"/>
-      <c r="AJ4" s="70" t="s">
+      <c r="AD4" s="88"/>
+      <c r="AE4" s="88"/>
+      <c r="AF4" s="88"/>
+      <c r="AG4" s="88"/>
+      <c r="AH4" s="88"/>
+      <c r="AI4" s="88"/>
+      <c r="AJ4" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="70"/>
-      <c r="AL4" s="70"/>
-      <c r="AM4" s="61" t="s">
+      <c r="AK4" s="89"/>
+      <c r="AL4" s="89"/>
+      <c r="AM4" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="61"/>
-      <c r="AO4" s="72"/>
-      <c r="AP4" s="72"/>
-      <c r="AQ4" s="72"/>
-      <c r="AR4" s="72"/>
-      <c r="AS4" s="73" t="s">
+      <c r="AN4" s="80"/>
+      <c r="AO4" s="70"/>
+      <c r="AP4" s="70"/>
+      <c r="AQ4" s="70"/>
+      <c r="AR4" s="70"/>
+      <c r="AS4" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="73"/>
-      <c r="AV4" s="73"/>
-      <c r="AW4" s="73"/>
-      <c r="AX4" s="73"/>
-      <c r="AY4" s="73"/>
-      <c r="AZ4" s="73"/>
-      <c r="BA4" s="73"/>
-      <c r="BB4" s="73"/>
-      <c r="BC4" s="73"/>
-      <c r="BD4" s="73"/>
-      <c r="BE4" s="73"/>
-      <c r="BF4" s="73"/>
-      <c r="BG4" s="73"/>
-      <c r="BH4" s="73"/>
-      <c r="BI4" s="73"/>
-      <c r="BJ4" s="73"/>
-      <c r="BK4" s="71" t="s">
+      <c r="AT4" s="71"/>
+      <c r="AU4" s="71"/>
+      <c r="AV4" s="71"/>
+      <c r="AW4" s="71"/>
+      <c r="AX4" s="71"/>
+      <c r="AY4" s="71"/>
+      <c r="AZ4" s="71"/>
+      <c r="BA4" s="71"/>
+      <c r="BB4" s="71"/>
+      <c r="BC4" s="71"/>
+      <c r="BD4" s="71"/>
+      <c r="BE4" s="71"/>
+      <c r="BF4" s="71"/>
+      <c r="BG4" s="71"/>
+      <c r="BH4" s="71"/>
+      <c r="BI4" s="71"/>
+      <c r="BJ4" s="71"/>
+      <c r="BK4" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="BL4" s="71"/>
-      <c r="BM4" s="71"/>
-      <c r="BN4" s="71"/>
-      <c r="BO4" s="71"/>
-      <c r="BP4" s="71"/>
-      <c r="BQ4" s="71"/>
-      <c r="BR4" s="71"/>
-      <c r="BS4" s="71"/>
-      <c r="BT4" s="71"/>
-      <c r="BU4" s="71"/>
-      <c r="BV4" s="71"/>
-      <c r="BW4" s="71"/>
-      <c r="BX4" s="71"/>
-      <c r="BY4" s="74" t="s">
+      <c r="BL4" s="67"/>
+      <c r="BM4" s="67"/>
+      <c r="BN4" s="67"/>
+      <c r="BO4" s="67"/>
+      <c r="BP4" s="67"/>
+      <c r="BQ4" s="67"/>
+      <c r="BR4" s="67"/>
+      <c r="BS4" s="67"/>
+      <c r="BT4" s="67"/>
+      <c r="BU4" s="67"/>
+      <c r="BV4" s="67"/>
+      <c r="BW4" s="67"/>
+      <c r="BX4" s="67"/>
+      <c r="BY4" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="74"/>
-      <c r="CA4" s="74"/>
-      <c r="CB4" s="74"/>
-      <c r="CC4" s="74"/>
-      <c r="CD4" s="74"/>
-      <c r="CE4" s="74"/>
-      <c r="CF4" s="74"/>
-      <c r="CG4" s="74"/>
-      <c r="CH4" s="74"/>
-      <c r="CI4" s="74"/>
-      <c r="CJ4" s="74"/>
-      <c r="CK4" s="74"/>
-      <c r="CL4" s="74"/>
-      <c r="CM4" s="75" t="s">
+      <c r="BZ4" s="72"/>
+      <c r="CA4" s="72"/>
+      <c r="CB4" s="72"/>
+      <c r="CC4" s="72"/>
+      <c r="CD4" s="72"/>
+      <c r="CE4" s="72"/>
+      <c r="CF4" s="72"/>
+      <c r="CG4" s="72"/>
+      <c r="CH4" s="72"/>
+      <c r="CI4" s="72"/>
+      <c r="CJ4" s="72"/>
+      <c r="CK4" s="72"/>
+      <c r="CL4" s="72"/>
+      <c r="CM4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="75"/>
-      <c r="CO4" s="75"/>
-      <c r="CP4" s="75"/>
-      <c r="CQ4" s="75"/>
-      <c r="CR4" s="75"/>
-      <c r="CS4" s="75"/>
-      <c r="CT4" s="75"/>
-      <c r="CU4" s="75"/>
-      <c r="CV4" s="75"/>
-      <c r="CW4" s="75"/>
-      <c r="CX4" s="75"/>
-      <c r="CY4" s="75"/>
-      <c r="CZ4" s="75"/>
-      <c r="DA4" s="76" t="s">
+      <c r="CN4" s="73"/>
+      <c r="CO4" s="73"/>
+      <c r="CP4" s="73"/>
+      <c r="CQ4" s="73"/>
+      <c r="CR4" s="73"/>
+      <c r="CS4" s="73"/>
+      <c r="CT4" s="73"/>
+      <c r="CU4" s="73"/>
+      <c r="CV4" s="73"/>
+      <c r="CW4" s="73"/>
+      <c r="CX4" s="73"/>
+      <c r="CY4" s="73"/>
+      <c r="CZ4" s="73"/>
+      <c r="DA4" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="76"/>
-      <c r="DC4" s="76"/>
-      <c r="DD4" s="76"/>
-      <c r="DE4" s="76"/>
-      <c r="DF4" s="76"/>
-      <c r="DG4" s="76"/>
-      <c r="DH4" s="76"/>
-      <c r="DI4" s="76"/>
-      <c r="DJ4" s="76"/>
-      <c r="DK4" s="76"/>
-      <c r="DL4" s="76"/>
-      <c r="DM4" s="76"/>
-      <c r="DN4" s="76"/>
-      <c r="DO4" s="77" t="s">
+      <c r="DB4" s="74"/>
+      <c r="DC4" s="74"/>
+      <c r="DD4" s="74"/>
+      <c r="DE4" s="74"/>
+      <c r="DF4" s="74"/>
+      <c r="DG4" s="74"/>
+      <c r="DH4" s="74"/>
+      <c r="DI4" s="74"/>
+      <c r="DJ4" s="74"/>
+      <c r="DK4" s="74"/>
+      <c r="DL4" s="74"/>
+      <c r="DM4" s="74"/>
+      <c r="DN4" s="74"/>
+      <c r="DO4" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="77"/>
-      <c r="DQ4" s="77"/>
-      <c r="DR4" s="77"/>
-      <c r="DS4" s="77"/>
-      <c r="DT4" s="77"/>
-      <c r="DU4" s="77"/>
-      <c r="DV4" s="77"/>
-      <c r="DW4" s="77"/>
-      <c r="DX4" s="77"/>
-      <c r="DY4" s="77"/>
-      <c r="DZ4" s="77"/>
-      <c r="EA4" s="77"/>
-      <c r="EB4" s="77"/>
-      <c r="EC4" s="78" t="s">
+      <c r="DP4" s="75"/>
+      <c r="DQ4" s="75"/>
+      <c r="DR4" s="75"/>
+      <c r="DS4" s="75"/>
+      <c r="DT4" s="75"/>
+      <c r="DU4" s="75"/>
+      <c r="DV4" s="75"/>
+      <c r="DW4" s="75"/>
+      <c r="DX4" s="75"/>
+      <c r="DY4" s="75"/>
+      <c r="DZ4" s="75"/>
+      <c r="EA4" s="75"/>
+      <c r="EB4" s="75"/>
+      <c r="EC4" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="78"/>
-      <c r="EE4" s="78"/>
-      <c r="EF4" s="78"/>
-      <c r="EG4" s="78"/>
-      <c r="EH4" s="78"/>
-      <c r="EI4" s="78"/>
-      <c r="EJ4" s="78"/>
-      <c r="EK4" s="78"/>
-      <c r="EL4" s="78"/>
-      <c r="EM4" s="78"/>
-      <c r="EN4" s="78"/>
-      <c r="EO4" s="78"/>
-      <c r="EP4" s="78"/>
-      <c r="EQ4" s="79" t="s">
+      <c r="ED4" s="76"/>
+      <c r="EE4" s="76"/>
+      <c r="EF4" s="76"/>
+      <c r="EG4" s="76"/>
+      <c r="EH4" s="76"/>
+      <c r="EI4" s="76"/>
+      <c r="EJ4" s="76"/>
+      <c r="EK4" s="76"/>
+      <c r="EL4" s="76"/>
+      <c r="EM4" s="76"/>
+      <c r="EN4" s="76"/>
+      <c r="EO4" s="76"/>
+      <c r="EP4" s="76"/>
+      <c r="EQ4" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="79"/>
-      <c r="ES4" s="79"/>
-      <c r="ET4" s="79"/>
-      <c r="EU4" s="79"/>
-      <c r="EV4" s="79"/>
-      <c r="EW4" s="79"/>
-      <c r="EX4" s="79"/>
-      <c r="EY4" s="79"/>
-      <c r="EZ4" s="79"/>
-      <c r="FA4" s="79"/>
-      <c r="FB4" s="79"/>
-      <c r="FC4" s="79"/>
-      <c r="FD4" s="79"/>
-      <c r="FE4" s="80" t="s">
+      <c r="ER4" s="77"/>
+      <c r="ES4" s="77"/>
+      <c r="ET4" s="77"/>
+      <c r="EU4" s="77"/>
+      <c r="EV4" s="77"/>
+      <c r="EW4" s="77"/>
+      <c r="EX4" s="77"/>
+      <c r="EY4" s="77"/>
+      <c r="EZ4" s="77"/>
+      <c r="FA4" s="77"/>
+      <c r="FB4" s="77"/>
+      <c r="FC4" s="77"/>
+      <c r="FD4" s="77"/>
+      <c r="FE4" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="80"/>
-      <c r="FG4" s="80"/>
-      <c r="FH4" s="80"/>
-      <c r="FI4" s="80"/>
-      <c r="FJ4" s="80"/>
-      <c r="FK4" s="80"/>
-      <c r="FL4" s="80"/>
-      <c r="FM4" s="80"/>
-      <c r="FN4" s="80"/>
-      <c r="FO4" s="80"/>
-      <c r="FP4" s="80"/>
-      <c r="FQ4" s="80"/>
-      <c r="FR4" s="80"/>
-      <c r="FS4" s="81" t="s">
+      <c r="FF4" s="78"/>
+      <c r="FG4" s="78"/>
+      <c r="FH4" s="78"/>
+      <c r="FI4" s="78"/>
+      <c r="FJ4" s="78"/>
+      <c r="FK4" s="78"/>
+      <c r="FL4" s="78"/>
+      <c r="FM4" s="78"/>
+      <c r="FN4" s="78"/>
+      <c r="FO4" s="78"/>
+      <c r="FP4" s="78"/>
+      <c r="FQ4" s="78"/>
+      <c r="FR4" s="78"/>
+      <c r="FS4" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="81"/>
-      <c r="FU4" s="81"/>
-      <c r="FV4" s="81"/>
-      <c r="FW4" s="81"/>
-      <c r="FX4" s="81"/>
-      <c r="FY4" s="81"/>
-      <c r="FZ4" s="81"/>
-      <c r="GA4" s="81"/>
-      <c r="GB4" s="81"/>
-      <c r="GC4" s="81"/>
-      <c r="GD4" s="81"/>
-      <c r="GE4" s="81"/>
-      <c r="GF4" s="81"/>
-      <c r="GG4" s="71" t="s">
+      <c r="FT4" s="79"/>
+      <c r="FU4" s="79"/>
+      <c r="FV4" s="79"/>
+      <c r="FW4" s="79"/>
+      <c r="FX4" s="79"/>
+      <c r="FY4" s="79"/>
+      <c r="FZ4" s="79"/>
+      <c r="GA4" s="79"/>
+      <c r="GB4" s="79"/>
+      <c r="GC4" s="79"/>
+      <c r="GD4" s="79"/>
+      <c r="GE4" s="79"/>
+      <c r="GF4" s="79"/>
+      <c r="GG4" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="GH4" s="71"/>
-      <c r="GI4" s="71"/>
-      <c r="GJ4" s="71"/>
-      <c r="GK4" s="71"/>
-      <c r="GL4" s="71"/>
-      <c r="GM4" s="71"/>
-      <c r="GN4" s="71"/>
-      <c r="GO4" s="71"/>
-      <c r="GP4" s="71"/>
-      <c r="GQ4" s="71"/>
-      <c r="GR4" s="71"/>
-      <c r="GS4" s="71"/>
-      <c r="GT4" s="71"/>
-      <c r="GU4" s="71" t="s">
+      <c r="GH4" s="67"/>
+      <c r="GI4" s="67"/>
+      <c r="GJ4" s="67"/>
+      <c r="GK4" s="67"/>
+      <c r="GL4" s="67"/>
+      <c r="GM4" s="67"/>
+      <c r="GN4" s="67"/>
+      <c r="GO4" s="67"/>
+      <c r="GP4" s="67"/>
+      <c r="GQ4" s="67"/>
+      <c r="GR4" s="67"/>
+      <c r="GS4" s="67"/>
+      <c r="GT4" s="67"/>
+      <c r="GU4" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="GV4" s="71"/>
-      <c r="GW4" s="71"/>
-      <c r="GX4" s="71"/>
-      <c r="GY4" s="71"/>
-      <c r="GZ4" s="71"/>
-      <c r="HA4" s="71"/>
-      <c r="HB4" s="71"/>
-      <c r="HC4" s="71"/>
-      <c r="HD4" s="71"/>
-      <c r="HE4" s="71"/>
-      <c r="HF4" s="71"/>
-      <c r="HG4" s="71"/>
-      <c r="HH4" s="71"/>
-      <c r="HI4" s="71" t="s">
+      <c r="GV4" s="67"/>
+      <c r="GW4" s="67"/>
+      <c r="GX4" s="67"/>
+      <c r="GY4" s="67"/>
+      <c r="GZ4" s="67"/>
+      <c r="HA4" s="67"/>
+      <c r="HB4" s="67"/>
+      <c r="HC4" s="67"/>
+      <c r="HD4" s="67"/>
+      <c r="HE4" s="67"/>
+      <c r="HF4" s="67"/>
+      <c r="HG4" s="67"/>
+      <c r="HH4" s="67"/>
+      <c r="HI4" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="HJ4" s="71"/>
-      <c r="HK4" s="71"/>
-      <c r="HL4" s="71"/>
-      <c r="HM4" s="71"/>
-      <c r="HN4" s="71"/>
-      <c r="HO4" s="71"/>
-      <c r="HP4" s="71"/>
-      <c r="HQ4" s="71"/>
-      <c r="HR4" s="71"/>
-      <c r="HS4" s="71"/>
-      <c r="HT4" s="71"/>
-      <c r="HU4" s="71"/>
-      <c r="HV4" s="71"/>
-      <c r="HW4" s="88" t="s">
+      <c r="HJ4" s="67"/>
+      <c r="HK4" s="67"/>
+      <c r="HL4" s="67"/>
+      <c r="HM4" s="67"/>
+      <c r="HN4" s="67"/>
+      <c r="HO4" s="67"/>
+      <c r="HP4" s="67"/>
+      <c r="HQ4" s="67"/>
+      <c r="HR4" s="67"/>
+      <c r="HS4" s="67"/>
+      <c r="HT4" s="67"/>
+      <c r="HU4" s="67"/>
+      <c r="HV4" s="67"/>
+      <c r="HW4" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="88"/>
-      <c r="HY4" s="88"/>
-      <c r="HZ4" s="88"/>
-      <c r="IA4" s="88"/>
-      <c r="IB4" s="88"/>
-      <c r="IC4" s="88"/>
-      <c r="ID4" s="88"/>
-      <c r="IE4" s="88"/>
-      <c r="IF4" s="88"/>
-      <c r="IG4" s="88"/>
-      <c r="IH4" s="88"/>
-      <c r="II4" s="88"/>
-      <c r="IJ4" s="88"/>
-      <c r="IK4" s="88" t="s">
+      <c r="HX4" s="68"/>
+      <c r="HY4" s="68"/>
+      <c r="HZ4" s="68"/>
+      <c r="IA4" s="68"/>
+      <c r="IB4" s="68"/>
+      <c r="IC4" s="68"/>
+      <c r="ID4" s="68"/>
+      <c r="IE4" s="68"/>
+      <c r="IF4" s="68"/>
+      <c r="IG4" s="68"/>
+      <c r="IH4" s="68"/>
+      <c r="II4" s="68"/>
+      <c r="IJ4" s="68"/>
+      <c r="IK4" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="88"/>
-      <c r="IM4" s="88"/>
-      <c r="IN4" s="88"/>
-      <c r="IO4" s="88"/>
-      <c r="IP4" s="88"/>
-      <c r="IQ4" s="88"/>
-      <c r="IR4" s="88"/>
-      <c r="IS4" s="88"/>
-      <c r="IT4" s="88"/>
-      <c r="IU4" s="88"/>
-      <c r="IV4" s="88"/>
-      <c r="IW4" s="88"/>
-      <c r="IX4" s="88"/>
-      <c r="IY4" s="88" t="s">
+      <c r="IL4" s="68"/>
+      <c r="IM4" s="68"/>
+      <c r="IN4" s="68"/>
+      <c r="IO4" s="68"/>
+      <c r="IP4" s="68"/>
+      <c r="IQ4" s="68"/>
+      <c r="IR4" s="68"/>
+      <c r="IS4" s="68"/>
+      <c r="IT4" s="68"/>
+      <c r="IU4" s="68"/>
+      <c r="IV4" s="68"/>
+      <c r="IW4" s="68"/>
+      <c r="IX4" s="68"/>
+      <c r="IY4" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="88"/>
-      <c r="JA4" s="88"/>
-      <c r="JB4" s="88"/>
-      <c r="JC4" s="88"/>
-      <c r="JD4" s="88"/>
-      <c r="JE4" s="88"/>
-      <c r="JF4" s="88"/>
-      <c r="JG4" s="88"/>
-      <c r="JH4" s="88"/>
-      <c r="JI4" s="88"/>
-      <c r="JJ4" s="88"/>
-      <c r="JK4" s="88"/>
-      <c r="JL4" s="88"/>
-      <c r="JM4" s="89" t="s">
+      <c r="IZ4" s="68"/>
+      <c r="JA4" s="68"/>
+      <c r="JB4" s="68"/>
+      <c r="JC4" s="68"/>
+      <c r="JD4" s="68"/>
+      <c r="JE4" s="68"/>
+      <c r="JF4" s="68"/>
+      <c r="JG4" s="68"/>
+      <c r="JH4" s="68"/>
+      <c r="JI4" s="68"/>
+      <c r="JJ4" s="68"/>
+      <c r="JK4" s="68"/>
+      <c r="JL4" s="68"/>
+      <c r="JM4" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="89"/>
-      <c r="JO4" s="89"/>
-      <c r="JP4" s="89"/>
-      <c r="JQ4" s="89"/>
-      <c r="JR4" s="89"/>
-      <c r="JS4" s="89"/>
-      <c r="JT4" s="89"/>
-      <c r="JU4" s="89"/>
-      <c r="JV4" s="89"/>
-      <c r="JW4" s="89"/>
-      <c r="JX4" s="89"/>
-      <c r="JY4" s="89"/>
-      <c r="JZ4" s="86" t="s">
+      <c r="JN4" s="69"/>
+      <c r="JO4" s="69"/>
+      <c r="JP4" s="69"/>
+      <c r="JQ4" s="69"/>
+      <c r="JR4" s="69"/>
+      <c r="JS4" s="69"/>
+      <c r="JT4" s="69"/>
+      <c r="JU4" s="69"/>
+      <c r="JV4" s="69"/>
+      <c r="JW4" s="69"/>
+      <c r="JX4" s="69"/>
+      <c r="JY4" s="69"/>
+      <c r="JZ4" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="87"/>
-      <c r="KB4" s="87"/>
-      <c r="KC4" s="87"/>
-      <c r="KD4" s="87"/>
-      <c r="KE4" s="87"/>
-      <c r="KF4" s="87"/>
-      <c r="KG4" s="87"/>
-      <c r="KH4" s="82" t="s">
+      <c r="KA4" s="66"/>
+      <c r="KB4" s="66"/>
+      <c r="KC4" s="66"/>
+      <c r="KD4" s="66"/>
+      <c r="KE4" s="66"/>
+      <c r="KF4" s="66"/>
+      <c r="KG4" s="66"/>
+      <c r="KH4" s="61" t="s">
         <v>322</v>
       </c>
-      <c r="KI4" s="83"/>
-      <c r="KJ4" s="83"/>
-      <c r="KK4" s="83"/>
+      <c r="KI4" s="62"/>
+      <c r="KJ4" s="62"/>
+      <c r="KK4" s="62"/>
       <c r="KL4" s="60"/>
     </row>
-    <row r="5" spans="1:298" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="68"/>
-      <c r="V5" s="68"/>
-      <c r="W5" s="68"/>
-      <c r="X5" s="68"/>
-      <c r="Y5" s="68"/>
-      <c r="Z5" s="68"/>
-      <c r="AA5" s="68"/>
-      <c r="AB5" s="68"/>
-      <c r="AC5" s="69"/>
-      <c r="AD5" s="69"/>
-      <c r="AE5" s="69"/>
-      <c r="AF5" s="69"/>
-      <c r="AG5" s="69"/>
-      <c r="AH5" s="69"/>
-      <c r="AI5" s="69"/>
-      <c r="AJ5" s="70"/>
-      <c r="AK5" s="70"/>
-      <c r="AL5" s="70"/>
-      <c r="AM5" s="61"/>
-      <c r="AN5" s="61"/>
-      <c r="AO5" s="72"/>
-      <c r="AP5" s="72"/>
-      <c r="AQ5" s="72"/>
-      <c r="AR5" s="72"/>
-      <c r="AS5" s="73"/>
-      <c r="AT5" s="73"/>
-      <c r="AU5" s="73"/>
-      <c r="AV5" s="73"/>
-      <c r="AW5" s="73"/>
-      <c r="AX5" s="73"/>
-      <c r="AY5" s="73"/>
-      <c r="AZ5" s="73"/>
-      <c r="BA5" s="73"/>
-      <c r="BB5" s="73"/>
-      <c r="BC5" s="73"/>
-      <c r="BD5" s="73"/>
-      <c r="BE5" s="73"/>
-      <c r="BF5" s="73"/>
-      <c r="BG5" s="73"/>
-      <c r="BH5" s="73"/>
-      <c r="BI5" s="73"/>
-      <c r="BJ5" s="73"/>
+    <row r="5" spans="1:298" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="83"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="86"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="87"/>
+      <c r="V5" s="87"/>
+      <c r="W5" s="87"/>
+      <c r="X5" s="87"/>
+      <c r="Y5" s="87"/>
+      <c r="Z5" s="87"/>
+      <c r="AA5" s="87"/>
+      <c r="AB5" s="87"/>
+      <c r="AC5" s="88"/>
+      <c r="AD5" s="88"/>
+      <c r="AE5" s="88"/>
+      <c r="AF5" s="88"/>
+      <c r="AG5" s="88"/>
+      <c r="AH5" s="88"/>
+      <c r="AI5" s="88"/>
+      <c r="AJ5" s="89"/>
+      <c r="AK5" s="89"/>
+      <c r="AL5" s="89"/>
+      <c r="AM5" s="80"/>
+      <c r="AN5" s="80"/>
+      <c r="AO5" s="70"/>
+      <c r="AP5" s="70"/>
+      <c r="AQ5" s="70"/>
+      <c r="AR5" s="70"/>
+      <c r="AS5" s="71"/>
+      <c r="AT5" s="71"/>
+      <c r="AU5" s="71"/>
+      <c r="AV5" s="71"/>
+      <c r="AW5" s="71"/>
+      <c r="AX5" s="71"/>
+      <c r="AY5" s="71"/>
+      <c r="AZ5" s="71"/>
+      <c r="BA5" s="71"/>
+      <c r="BB5" s="71"/>
+      <c r="BC5" s="71"/>
+      <c r="BD5" s="71"/>
+      <c r="BE5" s="71"/>
+      <c r="BF5" s="71"/>
+      <c r="BG5" s="71"/>
+      <c r="BH5" s="71"/>
+      <c r="BI5" s="71"/>
+      <c r="BJ5" s="71"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -4053,38 +4056,38 @@
       <c r="JL5" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="JM5" s="89"/>
-      <c r="JN5" s="89"/>
-      <c r="JO5" s="89"/>
-      <c r="JP5" s="89"/>
-      <c r="JQ5" s="89"/>
-      <c r="JR5" s="89"/>
-      <c r="JS5" s="89"/>
-      <c r="JT5" s="89"/>
-      <c r="JU5" s="89"/>
-      <c r="JV5" s="89"/>
-      <c r="JW5" s="89"/>
-      <c r="JX5" s="89"/>
-      <c r="JY5" s="89"/>
-      <c r="JZ5" s="87" t="s">
+      <c r="JM5" s="69"/>
+      <c r="JN5" s="69"/>
+      <c r="JO5" s="69"/>
+      <c r="JP5" s="69"/>
+      <c r="JQ5" s="69"/>
+      <c r="JR5" s="69"/>
+      <c r="JS5" s="69"/>
+      <c r="JT5" s="69"/>
+      <c r="JU5" s="69"/>
+      <c r="JV5" s="69"/>
+      <c r="JW5" s="69"/>
+      <c r="JX5" s="69"/>
+      <c r="JY5" s="69"/>
+      <c r="JZ5" s="66" t="s">
         <v>316</v>
       </c>
-      <c r="KA5" s="87"/>
-      <c r="KB5" s="87"/>
-      <c r="KC5" s="87"/>
-      <c r="KD5" s="87" t="s">
+      <c r="KA5" s="66"/>
+      <c r="KB5" s="66"/>
+      <c r="KC5" s="66"/>
+      <c r="KD5" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="87"/>
-      <c r="KF5" s="87"/>
-      <c r="KG5" s="87"/>
-      <c r="KH5" s="84"/>
-      <c r="KI5" s="85"/>
-      <c r="KJ5" s="85"/>
-      <c r="KK5" s="85"/>
+      <c r="KE5" s="66"/>
+      <c r="KF5" s="66"/>
+      <c r="KG5" s="66"/>
+      <c r="KH5" s="63"/>
+      <c r="KI5" s="64"/>
+      <c r="KJ5" s="64"/>
+      <c r="KK5" s="64"/>
       <c r="KL5" s="60"/>
     </row>
-    <row r="6" spans="1:298" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:298" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -4980,12 +4983,14 @@
         <v>342</v>
       </c>
     </row>
-    <row r="7" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
+      <c r="E7" s="32" t="s">
+        <v>343</v>
+      </c>
       <c r="F7" s="32"/>
       <c r="G7" s="32"/>
       <c r="H7" s="32"/>
@@ -4998,14 +5003,22 @@
       <c r="O7" s="53"/>
       <c r="P7" s="53"/>
       <c r="Q7" s="53"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
+      <c r="R7" s="53" t="s">
+        <v>343</v>
+      </c>
+      <c r="S7" s="53" t="s">
+        <v>343</v>
+      </c>
       <c r="T7" s="53"/>
       <c r="U7" s="53"/>
       <c r="V7" s="53"/>
       <c r="W7" s="53"/>
-      <c r="X7" s="54"/>
-      <c r="Y7" s="54"/>
+      <c r="X7" s="54" t="s">
+        <v>343</v>
+      </c>
+      <c r="Y7" s="54" t="s">
+        <v>343</v>
+      </c>
       <c r="Z7" s="53"/>
       <c r="AA7" s="53"/>
       <c r="AB7" s="54"/>
@@ -5016,9 +5029,15 @@
       <c r="AG7" s="31"/>
       <c r="AH7" s="57"/>
       <c r="AI7" s="31"/>
-      <c r="AJ7" s="52"/>
-      <c r="AK7" s="52"/>
-      <c r="AL7" s="52"/>
+      <c r="AJ7" s="52" t="s">
+        <v>343</v>
+      </c>
+      <c r="AK7" s="52" t="s">
+        <v>343</v>
+      </c>
+      <c r="AL7" s="52" t="s">
+        <v>343</v>
+      </c>
       <c r="AM7" s="53"/>
       <c r="AN7" s="58"/>
       <c r="AO7" s="51"/>
@@ -5086,71 +5105,71 @@
         <v>0</v>
       </c>
       <c r="BH7" s="30">
-        <f t="shared" ref="BH7:BJ7" si="0">JM7</f>
+        <f t="shared" ref="BH7" si="0">JM7</f>
         <v>0</v>
       </c>
       <c r="BI7" s="30">
-        <f t="shared" si="0"/>
+        <f>JN7</f>
         <v>0</v>
       </c>
       <c r="BJ7" s="30">
-        <f t="shared" si="0"/>
+        <f>JO7</f>
         <v>0</v>
       </c>
       <c r="BK7" s="30">
-        <f t="shared" ref="BK7:BX7" si="1">BY7+CM7+DA7+DO7+EC7+EQ7+FE7+FS7</f>
+        <f t="shared" ref="BK7" si="1">BY7+CM7+DA7+DO7+EC7+EQ7+FE7+FS7</f>
         <v>0</v>
       </c>
       <c r="BL7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="BL7:BX7" si="2">BZ7+CN7+DB7+DP7+ED7+ER7+FF7+FT7</f>
         <v>0</v>
       </c>
       <c r="BM7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BN7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BO7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BP7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BQ7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BR7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BS7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BT7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BU7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BV7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BW7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BX7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BY7" s="31"/>
@@ -5401,22 +5420,18 @@
       <c r="KL7" s="28"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:KK6">
-    <sortState ref="A7:KK10">
-      <sortCondition ref="KK6"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A6:KL6"/>
   <mergeCells count="32">
-    <mergeCell ref="KH4:KK5"/>
-    <mergeCell ref="JZ4:KG4"/>
-    <mergeCell ref="JZ5:KC5"/>
-    <mergeCell ref="KD5:KG5"/>
-    <mergeCell ref="GU4:HH4"/>
-    <mergeCell ref="HI4:HV4"/>
-    <mergeCell ref="HW4:IJ4"/>
-    <mergeCell ref="IK4:IX4"/>
-    <mergeCell ref="IY4:JL4"/>
-    <mergeCell ref="JM4:JY5"/>
+    <mergeCell ref="AM4:AN5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:D5"/>
+    <mergeCell ref="E4:J5"/>
+    <mergeCell ref="K4:O5"/>
+    <mergeCell ref="P4:T5"/>
+    <mergeCell ref="U4:AB5"/>
+    <mergeCell ref="AC4:AI5"/>
+    <mergeCell ref="AJ4:AL5"/>
     <mergeCell ref="GG4:GT4"/>
     <mergeCell ref="AO4:AR5"/>
     <mergeCell ref="AS4:BJ5"/>
@@ -5429,16 +5444,16 @@
     <mergeCell ref="EQ4:FD4"/>
     <mergeCell ref="FE4:FR4"/>
     <mergeCell ref="FS4:GF4"/>
-    <mergeCell ref="AM4:AN5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:D5"/>
-    <mergeCell ref="E4:J5"/>
-    <mergeCell ref="K4:O5"/>
-    <mergeCell ref="P4:T5"/>
-    <mergeCell ref="U4:AB5"/>
-    <mergeCell ref="AC4:AI5"/>
-    <mergeCell ref="AJ4:AL5"/>
+    <mergeCell ref="KH4:KK5"/>
+    <mergeCell ref="JZ4:KG4"/>
+    <mergeCell ref="JZ5:KC5"/>
+    <mergeCell ref="KD5:KG5"/>
+    <mergeCell ref="GU4:HH4"/>
+    <mergeCell ref="HI4:HV4"/>
+    <mergeCell ref="HW4:IJ4"/>
+    <mergeCell ref="IK4:IX4"/>
+    <mergeCell ref="IY4:JL4"/>
+    <mergeCell ref="JM4:JY5"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>

</xml_diff>

<commit_message>
[PM-343] Update FCERM1 spreadsheet
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -1,38 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssargeant\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthall/Work/pafs/pafs_core/lib/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84F3FAD-9F25-3A49-9B3B-4E25A0E35093}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25200" windowHeight="11980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master local choices" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$KL$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$KK$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Registered User</author>
   </authors>
   <commentList>
-    <comment ref="CD6" authorId="0" shapeId="0">
+    <comment ref="CD6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="349">
   <si>
     <t>FCRM1 - National Capital Programme</t>
   </si>
@@ -1068,10 +1075,88 @@
     <t>Year 12</t>
   </si>
   <si>
-    <t>TPE 19/20 - 20/21 total</t>
-  </si>
-  <si>
-    <t>19/20-20/21</t>
+    <t>Year 13</t>
+  </si>
+  <si>
+    <t>Confidence Assessment</t>
+  </si>
+  <si>
+    <t>TPE - 2027/28 on</t>
+  </si>
+  <si>
+    <t>GiA - 2027/28 on</t>
+  </si>
+  <si>
+    <t>Growth - 2027/28 on</t>
+  </si>
+  <si>
+    <t>Local Levy - 2027/28 on</t>
+  </si>
+  <si>
+    <t>IDB - 2027/28 on</t>
+  </si>
+  <si>
+    <t>Public - 2027/28 on</t>
+  </si>
+  <si>
+    <t>Private - 2027/28 on</t>
+  </si>
+  <si>
+    <t>Other EA - 2027/28 on</t>
+  </si>
+  <si>
+    <t>Further required - 2027/28 on</t>
+  </si>
+  <si>
+    <t>OM2 - 2027/28 on</t>
+  </si>
+  <si>
+    <t>OM2b - 2027/28 on</t>
+  </si>
+  <si>
+    <t>OM2c - 2027/28 on</t>
+  </si>
+  <si>
+    <t>OM3 - 2027/28 on</t>
+  </si>
+  <si>
+    <t>OM3b - 2027/28 on</t>
+  </si>
+  <si>
+    <t>OM3c - 2027/28 on</t>
+  </si>
+  <si>
+    <t>PAFS Status</t>
+  </si>
+  <si>
+    <t>Confidence in 'Number' of homes (all scheme including post 2021)</t>
+  </si>
+  <si>
+    <t>Confidence in Homes being delivered (by specified gateway 4 date)</t>
+  </si>
+  <si>
+    <t>Confidence in Securing Partnership Funding (all schemes including post-2021)</t>
+  </si>
+  <si>
+    <t>Confidence Assessment Picklist</t>
+  </si>
+  <si>
+    <t>3. Medium High</t>
+  </si>
+  <si>
+    <t>2. Medium Low</t>
+  </si>
+  <si>
+    <t>1. Low</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>PAFS Base 2020/21</t>
   </si>
   <si>
     <r>
@@ -1094,100 +1179,37 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> 19/20 - 20/21 total</t>
+      <t xml:space="preserve"> 20/21</t>
     </r>
   </si>
   <si>
-    <t>Contributions 19/20 - 20/21 total</t>
-  </si>
-  <si>
-    <t>OM2+3 19/20 - 20/21 total</t>
-  </si>
-  <si>
-    <t>PAFS Base 2019/20</t>
-  </si>
-  <si>
-    <t>Year 13</t>
-  </si>
-  <si>
-    <t>Confidence Assessment</t>
-  </si>
-  <si>
-    <t>Confidence in 'Number' of homes</t>
-  </si>
-  <si>
-    <t>Confidence in Homes being delivered by 2021</t>
-  </si>
-  <si>
-    <t>Confidence in Securing Partnership Funding</t>
-  </si>
-  <si>
-    <t>Proposed Delivery Route</t>
-  </si>
-  <si>
-    <t>TPE - 2027/28 on</t>
-  </si>
-  <si>
-    <t>GiA - 2027/28 on</t>
-  </si>
-  <si>
-    <t>Growth - 2027/28 on</t>
-  </si>
-  <si>
-    <t>Local Levy - 2027/28 on</t>
-  </si>
-  <si>
-    <t>IDB - 2027/28 on</t>
-  </si>
-  <si>
-    <t>Public - 2027/28 on</t>
-  </si>
-  <si>
-    <t>Private - 2027/28 on</t>
-  </si>
-  <si>
-    <t>Other EA - 2027/28 on</t>
-  </si>
-  <si>
-    <t>Further required - 2027/28 on</t>
-  </si>
-  <si>
-    <t>OM2 - 2027/28 on</t>
-  </si>
-  <si>
-    <t>OM2b - 2027/28 on</t>
-  </si>
-  <si>
-    <t>OM2c - 2027/28 on</t>
-  </si>
-  <si>
-    <t>OM3 - 2027/28 on</t>
-  </si>
-  <si>
-    <t>OM3b - 2027/28 on</t>
-  </si>
-  <si>
-    <t>OM3c - 2027/28 on</t>
-  </si>
-  <si>
-    <t>PAFS Status</t>
-  </si>
-  <si>
-    <t/>
+    <t>TPE 20/21</t>
+  </si>
+  <si>
+    <t>Contributions 20/21 total</t>
+  </si>
+  <si>
+    <t>OM2+3 20/21</t>
+  </si>
+  <si>
+    <t>20/21</t>
+  </si>
+  <si>
+    <t>4. High</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="167" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="168" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1280,6 +1302,13 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1287,13 +1316,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1509,9 +1531,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -1519,8 +1541,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1585,7 +1608,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1603,97 +1626,166 @@
     <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1712,86 +1804,24 @@
     <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="%" xfId="3"/>
-    <cellStyle name="% 2 2 2" xfId="4"/>
+  <cellStyles count="10">
+    <cellStyle name="%" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% 2 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="8"/>
-    <cellStyle name="Normal 2 2" xfId="6"/>
-    <cellStyle name="Normal_RCP" xfId="5"/>
+    <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal_RCP" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Percent 11" xfId="7"/>
+    <cellStyle name="Percent 11" xfId="7" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -2079,25 +2109,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:KL7"/>
+  <dimension ref="A1:KN11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="AZ9" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98.7109375" style="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="3" customWidth="1"/>
     <col min="5" max="6" width="21" style="1" customWidth="1"/>
     <col min="7" max="7" width="21" style="2" customWidth="1"/>
@@ -2112,26 +2142,28 @@
     <col min="32" max="39" width="21" style="1" customWidth="1"/>
     <col min="40" max="44" width="21" style="5" customWidth="1"/>
     <col min="45" max="278" width="21" style="1" customWidth="1"/>
-    <col min="279" max="285" width="21" style="29" customWidth="1"/>
+    <col min="279" max="285" width="21" style="28" customWidth="1"/>
     <col min="286" max="293" width="21" style="6" customWidth="1"/>
-    <col min="294" max="296" width="22.21875" style="7" customWidth="1"/>
-    <col min="297" max="297" width="13.21875" style="7" customWidth="1"/>
-    <col min="298" max="298" width="11" style="7" customWidth="1"/>
-    <col min="299" max="16384" width="8.77734375" style="7"/>
+    <col min="294" max="296" width="22.28515625" style="7" customWidth="1"/>
+    <col min="297" max="297" width="11" style="7" customWidth="1"/>
+    <col min="298" max="298" width="12.85546875" style="7" hidden="1" customWidth="1"/>
+    <col min="299" max="299" width="8.7109375" style="7"/>
+    <col min="300" max="300" width="11" style="7" customWidth="1"/>
+    <col min="301" max="16384" width="8.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
+    <row r="1" spans="1:300" ht="28.5" customHeight="1">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
+      <c r="B1" s="66"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
       <c r="G1" s="24"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="23"/>
       <c r="K1" s="23"/>
       <c r="L1" s="23"/>
@@ -2202,16 +2234,16 @@
       <c r="BY1" s="23"/>
       <c r="BZ1" s="23"/>
       <c r="CA1" s="23"/>
-      <c r="CB1" s="38"/>
-      <c r="CC1" s="35"/>
-      <c r="CD1" s="35"/>
-      <c r="CE1" s="35"/>
+      <c r="CB1" s="33"/>
+      <c r="CC1" s="30"/>
+      <c r="CD1" s="30"/>
+      <c r="CE1" s="30"/>
       <c r="CF1" s="23"/>
       <c r="CG1" s="23"/>
       <c r="CH1" s="23"/>
       <c r="CI1" s="23"/>
-      <c r="CJ1" s="39"/>
-      <c r="CK1" s="39"/>
+      <c r="CJ1" s="34"/>
+      <c r="CK1" s="34"/>
       <c r="CL1" s="23"/>
       <c r="CM1" s="23"/>
       <c r="CN1" s="23"/>
@@ -2401,13 +2433,13 @@
       <c r="JP1" s="23"/>
       <c r="JQ1" s="23"/>
       <c r="JR1" s="23"/>
-      <c r="JS1" s="40"/>
-      <c r="JT1" s="40"/>
-      <c r="JU1" s="40"/>
-      <c r="JV1" s="40"/>
-      <c r="JW1" s="40"/>
-      <c r="JX1" s="40"/>
-      <c r="JY1" s="40"/>
+      <c r="JS1" s="35"/>
+      <c r="JT1" s="35"/>
+      <c r="JU1" s="35"/>
+      <c r="JV1" s="35"/>
+      <c r="JW1" s="35"/>
+      <c r="JX1" s="35"/>
+      <c r="JY1" s="35"/>
       <c r="JZ1" s="23"/>
       <c r="KA1" s="23"/>
       <c r="KB1" s="23"/>
@@ -2417,18 +2449,18 @@
       <c r="KF1" s="23"/>
       <c r="KG1" s="23"/>
     </row>
-    <row r="2" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="82" t="s">
-        <v>320</v>
-      </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
+    <row r="2" spans="1:300" ht="28.5" customHeight="1">
+      <c r="A2" s="67" t="s">
+        <v>342</v>
+      </c>
+      <c r="B2" s="67"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="23"/>
-      <c r="F2" s="42"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="37"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
       <c r="L2" s="23"/>
@@ -2497,18 +2529,18 @@
       <c r="BW2" s="23"/>
       <c r="BX2" s="23"/>
       <c r="BY2" s="23"/>
-      <c r="BZ2" s="43"/>
-      <c r="CA2" s="43"/>
-      <c r="CB2" s="35"/>
-      <c r="CC2" s="35"/>
-      <c r="CD2" s="35"/>
-      <c r="CE2" s="35"/>
+      <c r="BZ2" s="38"/>
+      <c r="CA2" s="38"/>
+      <c r="CB2" s="30"/>
+      <c r="CC2" s="30"/>
+      <c r="CD2" s="30"/>
+      <c r="CE2" s="30"/>
       <c r="CF2" s="23"/>
-      <c r="CG2" s="39"/>
-      <c r="CH2" s="39"/>
-      <c r="CI2" s="39"/>
-      <c r="CJ2" s="39"/>
-      <c r="CK2" s="39"/>
+      <c r="CG2" s="34"/>
+      <c r="CH2" s="34"/>
+      <c r="CI2" s="34"/>
+      <c r="CJ2" s="34"/>
+      <c r="CK2" s="34"/>
       <c r="CL2" s="23"/>
       <c r="CM2" s="23"/>
       <c r="CN2" s="23"/>
@@ -2698,734 +2730,733 @@
       <c r="JP2" s="23"/>
       <c r="JQ2" s="23"/>
       <c r="JR2" s="23"/>
-      <c r="JS2" s="42"/>
-      <c r="JT2" s="42"/>
-      <c r="JU2" s="42"/>
-      <c r="JV2" s="42"/>
-      <c r="JW2" s="42"/>
-      <c r="JX2" s="42"/>
-      <c r="JY2" s="42"/>
+      <c r="JS2" s="37"/>
+      <c r="JT2" s="37"/>
+      <c r="JU2" s="37"/>
+      <c r="JV2" s="37"/>
+      <c r="JW2" s="37"/>
+      <c r="JX2" s="37"/>
+      <c r="JY2" s="37"/>
       <c r="JZ2" s="23"/>
-      <c r="KA2" s="42"/>
-      <c r="KB2" s="42"/>
-      <c r="KC2" s="42"/>
-      <c r="KD2" s="42"/>
-      <c r="KE2" s="42"/>
-      <c r="KF2" s="42"/>
-      <c r="KG2" s="42"/>
+      <c r="KA2" s="37"/>
+      <c r="KB2" s="37"/>
+      <c r="KC2" s="37"/>
+      <c r="KD2" s="37"/>
+      <c r="KE2" s="37"/>
+      <c r="KF2" s="37"/>
+      <c r="KG2" s="37"/>
     </row>
-    <row r="3" spans="1:298" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="46"/>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="45"/>
-      <c r="AA3" s="45"/>
-      <c r="AB3" s="46"/>
-      <c r="AC3" s="45"/>
-      <c r="AD3" s="46"/>
-      <c r="AE3" s="46"/>
-      <c r="AF3" s="45"/>
-      <c r="AG3" s="45"/>
-      <c r="AH3" s="45"/>
-      <c r="AI3" s="45"/>
-      <c r="AJ3" s="45"/>
-      <c r="AK3" s="45"/>
-      <c r="AL3" s="45"/>
-      <c r="AM3" s="45"/>
-      <c r="AN3" s="47"/>
-      <c r="AO3" s="48"/>
-      <c r="AP3" s="48"/>
-      <c r="AQ3" s="48"/>
-      <c r="AR3" s="48"/>
-      <c r="AS3" s="49"/>
-      <c r="AT3" s="49"/>
-      <c r="AU3" s="49"/>
-      <c r="AV3" s="49"/>
-      <c r="AW3" s="49"/>
-      <c r="AX3" s="49"/>
-      <c r="AY3" s="49"/>
-      <c r="AZ3" s="49"/>
-      <c r="BA3" s="49"/>
-      <c r="BB3" s="49"/>
-      <c r="BC3" s="49"/>
-      <c r="BD3" s="49"/>
-      <c r="BE3" s="49"/>
-      <c r="BF3" s="49"/>
-      <c r="BG3" s="49"/>
-      <c r="BH3" s="49"/>
-      <c r="BI3" s="49"/>
-      <c r="BJ3" s="49"/>
-      <c r="BK3" s="49"/>
-      <c r="BL3" s="49"/>
-      <c r="BM3" s="49"/>
-      <c r="BN3" s="50"/>
-      <c r="BO3" s="50"/>
-      <c r="BP3" s="50"/>
-      <c r="BQ3" s="50"/>
-      <c r="BR3" s="50"/>
-      <c r="BS3" s="50"/>
-      <c r="BT3" s="50"/>
-      <c r="BU3" s="50"/>
-      <c r="BV3" s="50"/>
-      <c r="BW3" s="50"/>
-      <c r="BX3" s="50"/>
-      <c r="BY3" s="50"/>
-      <c r="BZ3" s="50"/>
-      <c r="CA3" s="50"/>
-      <c r="CB3" s="50"/>
-      <c r="CC3" s="50"/>
-      <c r="CD3" s="50"/>
-      <c r="CE3" s="50"/>
-      <c r="CF3" s="50"/>
-      <c r="CG3" s="50"/>
-      <c r="CH3" s="50"/>
-      <c r="CI3" s="50"/>
-      <c r="CJ3" s="50"/>
-      <c r="CK3" s="50"/>
-      <c r="CL3" s="50"/>
-      <c r="CM3" s="50"/>
-      <c r="CN3" s="50"/>
-      <c r="CO3" s="50"/>
-      <c r="CP3" s="50"/>
-      <c r="CQ3" s="50"/>
-      <c r="CR3" s="50"/>
-      <c r="CS3" s="50"/>
-      <c r="CT3" s="50"/>
-      <c r="CU3" s="50"/>
-      <c r="CV3" s="50"/>
-      <c r="CW3" s="50"/>
-      <c r="CX3" s="50"/>
-      <c r="CY3" s="50"/>
-      <c r="CZ3" s="50"/>
-      <c r="DA3" s="50"/>
-      <c r="DB3" s="50"/>
-      <c r="DC3" s="50"/>
-      <c r="DD3" s="50"/>
-      <c r="DE3" s="50"/>
-      <c r="DF3" s="50"/>
-      <c r="DG3" s="50"/>
-      <c r="DH3" s="50"/>
-      <c r="DI3" s="50"/>
-      <c r="DJ3" s="50"/>
-      <c r="DK3" s="50"/>
-      <c r="DL3" s="50"/>
-      <c r="DM3" s="50"/>
-      <c r="DN3" s="50"/>
-      <c r="DO3" s="50"/>
-      <c r="DP3" s="50"/>
-      <c r="DQ3" s="50"/>
-      <c r="DR3" s="50"/>
-      <c r="DS3" s="50"/>
-      <c r="DT3" s="50"/>
-      <c r="DU3" s="50"/>
-      <c r="DV3" s="50"/>
-      <c r="DW3" s="50"/>
-      <c r="DX3" s="50"/>
-      <c r="DY3" s="50"/>
-      <c r="DZ3" s="50"/>
-      <c r="EA3" s="50"/>
-      <c r="EB3" s="50"/>
-      <c r="EC3" s="50"/>
-      <c r="ED3" s="50"/>
-      <c r="EE3" s="50"/>
-      <c r="EF3" s="50"/>
-      <c r="EG3" s="50"/>
-      <c r="EH3" s="50"/>
-      <c r="EI3" s="50"/>
-      <c r="EJ3" s="50"/>
-      <c r="EK3" s="50"/>
-      <c r="EL3" s="50"/>
-      <c r="EM3" s="50"/>
-      <c r="EN3" s="50"/>
-      <c r="EO3" s="50"/>
-      <c r="EP3" s="50"/>
-      <c r="EQ3" s="50"/>
-      <c r="ER3" s="50"/>
-      <c r="ES3" s="50"/>
-      <c r="ET3" s="50"/>
-      <c r="EU3" s="50"/>
-      <c r="EV3" s="50"/>
-      <c r="EW3" s="50"/>
-      <c r="EX3" s="50"/>
-      <c r="EY3" s="50"/>
-      <c r="EZ3" s="50"/>
-      <c r="FA3" s="50"/>
-      <c r="FB3" s="50"/>
-      <c r="FC3" s="50"/>
-      <c r="FD3" s="50"/>
-      <c r="FE3" s="50"/>
-      <c r="FF3" s="50"/>
-      <c r="FG3" s="50"/>
-      <c r="FH3" s="50"/>
-      <c r="FI3" s="50"/>
-      <c r="FJ3" s="50"/>
-      <c r="FK3" s="50"/>
-      <c r="FL3" s="50"/>
-      <c r="FM3" s="50"/>
-      <c r="FN3" s="50"/>
-      <c r="FO3" s="50"/>
-      <c r="FP3" s="50"/>
-      <c r="FQ3" s="50"/>
-      <c r="FR3" s="50"/>
-      <c r="FS3" s="50"/>
-      <c r="FT3" s="50"/>
-      <c r="FU3" s="50"/>
-      <c r="FV3" s="50"/>
-      <c r="FW3" s="50"/>
-      <c r="FX3" s="50"/>
-      <c r="FY3" s="50"/>
-      <c r="FZ3" s="50"/>
-      <c r="GA3" s="50"/>
-      <c r="GB3" s="50"/>
-      <c r="GC3" s="50"/>
-      <c r="GD3" s="50"/>
-      <c r="GE3" s="50"/>
-      <c r="GF3" s="50"/>
-      <c r="GG3" s="50"/>
-      <c r="GH3" s="50"/>
-      <c r="GI3" s="50"/>
-      <c r="GJ3" s="50"/>
-      <c r="GK3" s="50"/>
-      <c r="GL3" s="50"/>
-      <c r="GM3" s="50"/>
-      <c r="GN3" s="50"/>
-      <c r="GO3" s="50"/>
-      <c r="GP3" s="50"/>
-      <c r="GQ3" s="50"/>
-      <c r="GR3" s="50"/>
-      <c r="GS3" s="50"/>
-      <c r="GT3" s="50"/>
-      <c r="GU3" s="50"/>
-      <c r="GV3" s="50"/>
-      <c r="GW3" s="50"/>
-      <c r="GX3" s="50"/>
-      <c r="GY3" s="50"/>
-      <c r="GZ3" s="50"/>
-      <c r="HA3" s="50"/>
-      <c r="HB3" s="50"/>
-      <c r="HC3" s="50"/>
-      <c r="HD3" s="50"/>
-      <c r="HE3" s="50"/>
-      <c r="HF3" s="50"/>
-      <c r="HG3" s="50"/>
-      <c r="HH3" s="50"/>
-      <c r="HI3" s="50"/>
-      <c r="HJ3" s="50"/>
-      <c r="HK3" s="50"/>
-      <c r="HL3" s="50"/>
-      <c r="HM3" s="50"/>
-      <c r="HN3" s="50"/>
-      <c r="HO3" s="50"/>
-      <c r="HP3" s="50"/>
-      <c r="HQ3" s="50"/>
-      <c r="HR3" s="50"/>
-      <c r="HS3" s="50"/>
-      <c r="HT3" s="50"/>
-      <c r="HU3" s="50"/>
-      <c r="HV3" s="50"/>
-      <c r="HW3" s="50"/>
-      <c r="HX3" s="50"/>
-      <c r="HY3" s="50"/>
-      <c r="HZ3" s="50"/>
-      <c r="IA3" s="50"/>
-      <c r="IB3" s="50"/>
-      <c r="IC3" s="50"/>
-      <c r="ID3" s="50"/>
-      <c r="IE3" s="50"/>
-      <c r="IF3" s="50"/>
-      <c r="IG3" s="50"/>
-      <c r="IH3" s="50"/>
-      <c r="II3" s="50"/>
-      <c r="IJ3" s="50"/>
-      <c r="IK3" s="50"/>
-      <c r="IL3" s="50"/>
-      <c r="IM3" s="50"/>
-      <c r="IN3" s="50"/>
-      <c r="IO3" s="50"/>
-      <c r="IP3" s="50"/>
-      <c r="IQ3" s="50"/>
-      <c r="IR3" s="50"/>
-      <c r="IS3" s="50"/>
-      <c r="IT3" s="50"/>
-      <c r="IU3" s="50"/>
-      <c r="IV3" s="50"/>
-      <c r="IW3" s="50"/>
-      <c r="IX3" s="50"/>
-      <c r="IY3" s="50"/>
-      <c r="IZ3" s="50"/>
-      <c r="JA3" s="50"/>
-      <c r="JB3" s="50"/>
-      <c r="JC3" s="50"/>
-      <c r="JD3" s="50"/>
-      <c r="JE3" s="50"/>
-      <c r="JF3" s="50"/>
-      <c r="JG3" s="50"/>
-      <c r="JH3" s="50"/>
-      <c r="JI3" s="50"/>
-      <c r="JJ3" s="50"/>
-      <c r="JK3" s="50"/>
-      <c r="JL3" s="50"/>
-      <c r="JM3" s="50"/>
-      <c r="JN3" s="50"/>
-      <c r="JO3" s="50"/>
-      <c r="JP3" s="50"/>
-      <c r="JQ3" s="50"/>
-      <c r="JR3" s="50"/>
-      <c r="JS3" s="50"/>
-      <c r="JT3" s="50"/>
-      <c r="JU3" s="50"/>
-      <c r="JV3" s="50"/>
-      <c r="JW3" s="50"/>
-      <c r="JX3" s="50"/>
-      <c r="JY3" s="50"/>
-      <c r="JZ3" s="50"/>
-      <c r="KA3" s="50"/>
-      <c r="KB3" s="50"/>
-      <c r="KC3" s="50"/>
-      <c r="KD3" s="50"/>
-      <c r="KE3" s="50"/>
-      <c r="KF3" s="50"/>
-      <c r="KG3" s="50"/>
+    <row r="3" spans="1:300" ht="25.5" customHeight="1">
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="40"/>
+      <c r="AA3" s="40"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="40"/>
+      <c r="AD3" s="41"/>
+      <c r="AE3" s="41"/>
+      <c r="AF3" s="40"/>
+      <c r="AG3" s="40"/>
+      <c r="AH3" s="40"/>
+      <c r="AI3" s="40"/>
+      <c r="AJ3" s="40"/>
+      <c r="AK3" s="40"/>
+      <c r="AL3" s="40"/>
+      <c r="AM3" s="40"/>
+      <c r="AN3" s="42"/>
+      <c r="AO3" s="43"/>
+      <c r="AP3" s="43"/>
+      <c r="AQ3" s="43"/>
+      <c r="AR3" s="43"/>
+      <c r="AS3" s="44"/>
+      <c r="AT3" s="44"/>
+      <c r="AU3" s="44"/>
+      <c r="AV3" s="44"/>
+      <c r="AW3" s="44"/>
+      <c r="AX3" s="44"/>
+      <c r="AY3" s="44"/>
+      <c r="AZ3" s="44"/>
+      <c r="BA3" s="44"/>
+      <c r="BB3" s="44"/>
+      <c r="BC3" s="44"/>
+      <c r="BD3" s="44"/>
+      <c r="BE3" s="44"/>
+      <c r="BF3" s="44"/>
+      <c r="BG3" s="44"/>
+      <c r="BH3" s="44"/>
+      <c r="BI3" s="44"/>
+      <c r="BJ3" s="44"/>
+      <c r="BK3" s="44"/>
+      <c r="BL3" s="44"/>
+      <c r="BM3" s="44"/>
+      <c r="BN3" s="45"/>
+      <c r="BO3" s="45"/>
+      <c r="BP3" s="45"/>
+      <c r="BQ3" s="45"/>
+      <c r="BR3" s="45"/>
+      <c r="BS3" s="45"/>
+      <c r="BT3" s="45"/>
+      <c r="BU3" s="45"/>
+      <c r="BV3" s="45"/>
+      <c r="BW3" s="45"/>
+      <c r="BX3" s="45"/>
+      <c r="BY3" s="45"/>
+      <c r="BZ3" s="45"/>
+      <c r="CA3" s="45"/>
+      <c r="CB3" s="45"/>
+      <c r="CC3" s="45"/>
+      <c r="CD3" s="45"/>
+      <c r="CE3" s="45"/>
+      <c r="CF3" s="45"/>
+      <c r="CG3" s="45"/>
+      <c r="CH3" s="45"/>
+      <c r="CI3" s="45"/>
+      <c r="CJ3" s="45"/>
+      <c r="CK3" s="45"/>
+      <c r="CL3" s="45"/>
+      <c r="CM3" s="45"/>
+      <c r="CN3" s="45"/>
+      <c r="CO3" s="45"/>
+      <c r="CP3" s="45"/>
+      <c r="CQ3" s="45"/>
+      <c r="CR3" s="45"/>
+      <c r="CS3" s="45"/>
+      <c r="CT3" s="45"/>
+      <c r="CU3" s="45"/>
+      <c r="CV3" s="45"/>
+      <c r="CW3" s="45"/>
+      <c r="CX3" s="45"/>
+      <c r="CY3" s="45"/>
+      <c r="CZ3" s="45"/>
+      <c r="DA3" s="45"/>
+      <c r="DB3" s="45"/>
+      <c r="DC3" s="45"/>
+      <c r="DD3" s="45"/>
+      <c r="DE3" s="45"/>
+      <c r="DF3" s="45"/>
+      <c r="DG3" s="45"/>
+      <c r="DH3" s="45"/>
+      <c r="DI3" s="45"/>
+      <c r="DJ3" s="45"/>
+      <c r="DK3" s="45"/>
+      <c r="DL3" s="45"/>
+      <c r="DM3" s="45"/>
+      <c r="DN3" s="45"/>
+      <c r="DO3" s="45"/>
+      <c r="DP3" s="45"/>
+      <c r="DQ3" s="45"/>
+      <c r="DR3" s="45"/>
+      <c r="DS3" s="45"/>
+      <c r="DT3" s="45"/>
+      <c r="DU3" s="45"/>
+      <c r="DV3" s="45"/>
+      <c r="DW3" s="45"/>
+      <c r="DX3" s="45"/>
+      <c r="DY3" s="45"/>
+      <c r="DZ3" s="45"/>
+      <c r="EA3" s="45"/>
+      <c r="EB3" s="45"/>
+      <c r="EC3" s="45"/>
+      <c r="ED3" s="45"/>
+      <c r="EE3" s="45"/>
+      <c r="EF3" s="45"/>
+      <c r="EG3" s="45"/>
+      <c r="EH3" s="45"/>
+      <c r="EI3" s="45"/>
+      <c r="EJ3" s="45"/>
+      <c r="EK3" s="45"/>
+      <c r="EL3" s="45"/>
+      <c r="EM3" s="45"/>
+      <c r="EN3" s="45"/>
+      <c r="EO3" s="45"/>
+      <c r="EP3" s="45"/>
+      <c r="EQ3" s="45"/>
+      <c r="ER3" s="45"/>
+      <c r="ES3" s="45"/>
+      <c r="ET3" s="45"/>
+      <c r="EU3" s="45"/>
+      <c r="EV3" s="45"/>
+      <c r="EW3" s="45"/>
+      <c r="EX3" s="45"/>
+      <c r="EY3" s="45"/>
+      <c r="EZ3" s="45"/>
+      <c r="FA3" s="45"/>
+      <c r="FB3" s="45"/>
+      <c r="FC3" s="45"/>
+      <c r="FD3" s="45"/>
+      <c r="FE3" s="45"/>
+      <c r="FF3" s="45"/>
+      <c r="FG3" s="45"/>
+      <c r="FH3" s="45"/>
+      <c r="FI3" s="45"/>
+      <c r="FJ3" s="45"/>
+      <c r="FK3" s="45"/>
+      <c r="FL3" s="45"/>
+      <c r="FM3" s="45"/>
+      <c r="FN3" s="45"/>
+      <c r="FO3" s="45"/>
+      <c r="FP3" s="45"/>
+      <c r="FQ3" s="45"/>
+      <c r="FR3" s="45"/>
+      <c r="FS3" s="45"/>
+      <c r="FT3" s="45"/>
+      <c r="FU3" s="45"/>
+      <c r="FV3" s="45"/>
+      <c r="FW3" s="45"/>
+      <c r="FX3" s="45"/>
+      <c r="FY3" s="45"/>
+      <c r="FZ3" s="45"/>
+      <c r="GA3" s="45"/>
+      <c r="GB3" s="45"/>
+      <c r="GC3" s="45"/>
+      <c r="GD3" s="45"/>
+      <c r="GE3" s="45"/>
+      <c r="GF3" s="45"/>
+      <c r="GG3" s="45"/>
+      <c r="GH3" s="45"/>
+      <c r="GI3" s="45"/>
+      <c r="GJ3" s="45"/>
+      <c r="GK3" s="45"/>
+      <c r="GL3" s="45"/>
+      <c r="GM3" s="45"/>
+      <c r="GN3" s="45"/>
+      <c r="GO3" s="45"/>
+      <c r="GP3" s="45"/>
+      <c r="GQ3" s="45"/>
+      <c r="GR3" s="45"/>
+      <c r="GS3" s="45"/>
+      <c r="GT3" s="45"/>
+      <c r="GU3" s="45"/>
+      <c r="GV3" s="45"/>
+      <c r="GW3" s="45"/>
+      <c r="GX3" s="45"/>
+      <c r="GY3" s="45"/>
+      <c r="GZ3" s="45"/>
+      <c r="HA3" s="45"/>
+      <c r="HB3" s="45"/>
+      <c r="HC3" s="45"/>
+      <c r="HD3" s="45"/>
+      <c r="HE3" s="45"/>
+      <c r="HF3" s="45"/>
+      <c r="HG3" s="45"/>
+      <c r="HH3" s="45"/>
+      <c r="HI3" s="45"/>
+      <c r="HJ3" s="45"/>
+      <c r="HK3" s="45"/>
+      <c r="HL3" s="45"/>
+      <c r="HM3" s="45"/>
+      <c r="HN3" s="45"/>
+      <c r="HO3" s="45"/>
+      <c r="HP3" s="45"/>
+      <c r="HQ3" s="45"/>
+      <c r="HR3" s="45"/>
+      <c r="HS3" s="45"/>
+      <c r="HT3" s="45"/>
+      <c r="HU3" s="45"/>
+      <c r="HV3" s="45"/>
+      <c r="HW3" s="45"/>
+      <c r="HX3" s="45"/>
+      <c r="HY3" s="45"/>
+      <c r="HZ3" s="45"/>
+      <c r="IA3" s="45"/>
+      <c r="IB3" s="45"/>
+      <c r="IC3" s="45"/>
+      <c r="ID3" s="45"/>
+      <c r="IE3" s="45"/>
+      <c r="IF3" s="45"/>
+      <c r="IG3" s="45"/>
+      <c r="IH3" s="45"/>
+      <c r="II3" s="45"/>
+      <c r="IJ3" s="45"/>
+      <c r="IK3" s="45"/>
+      <c r="IL3" s="45"/>
+      <c r="IM3" s="45"/>
+      <c r="IN3" s="45"/>
+      <c r="IO3" s="45"/>
+      <c r="IP3" s="45"/>
+      <c r="IQ3" s="45"/>
+      <c r="IR3" s="45"/>
+      <c r="IS3" s="45"/>
+      <c r="IT3" s="45"/>
+      <c r="IU3" s="45"/>
+      <c r="IV3" s="45"/>
+      <c r="IW3" s="45"/>
+      <c r="IX3" s="45"/>
+      <c r="IY3" s="45"/>
+      <c r="IZ3" s="45"/>
+      <c r="JA3" s="45"/>
+      <c r="JB3" s="45"/>
+      <c r="JC3" s="45"/>
+      <c r="JD3" s="45"/>
+      <c r="JE3" s="45"/>
+      <c r="JF3" s="45"/>
+      <c r="JG3" s="45"/>
+      <c r="JH3" s="45"/>
+      <c r="JI3" s="45"/>
+      <c r="JJ3" s="45"/>
+      <c r="JK3" s="45"/>
+      <c r="JL3" s="45"/>
+      <c r="JM3" s="45"/>
+      <c r="JN3" s="45"/>
+      <c r="JO3" s="45"/>
+      <c r="JP3" s="45"/>
+      <c r="JQ3" s="45"/>
+      <c r="JR3" s="45"/>
+      <c r="JS3" s="45"/>
+      <c r="JT3" s="45"/>
+      <c r="JU3" s="45"/>
+      <c r="JV3" s="45"/>
+      <c r="JW3" s="45"/>
+      <c r="JX3" s="45"/>
+      <c r="JY3" s="45"/>
+      <c r="JZ3" s="45"/>
+      <c r="KA3" s="45"/>
+      <c r="KB3" s="45"/>
+      <c r="KC3" s="45"/>
+      <c r="KD3" s="45"/>
+      <c r="KE3" s="45"/>
+      <c r="KF3" s="45"/>
+      <c r="KG3" s="45"/>
     </row>
-    <row r="4" spans="1:298" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="83" t="s">
+    <row r="4" spans="1:300" ht="46.5" customHeight="1">
+      <c r="A4" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="84" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="85" t="s">
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="85"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="85"/>
-      <c r="P4" s="86" t="s">
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
+      <c r="O4" s="70"/>
+      <c r="P4" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="87" t="s">
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="87"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="88" t="s">
+      <c r="V4" s="72"/>
+      <c r="W4" s="72"/>
+      <c r="X4" s="72"/>
+      <c r="Y4" s="72"/>
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
+      <c r="AB4" s="72"/>
+      <c r="AC4" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="88"/>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
-      <c r="AH4" s="88"/>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="89" t="s">
+      <c r="AD4" s="73"/>
+      <c r="AE4" s="73"/>
+      <c r="AF4" s="73"/>
+      <c r="AG4" s="73"/>
+      <c r="AH4" s="73"/>
+      <c r="AI4" s="73"/>
+      <c r="AJ4" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="89"/>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="80" t="s">
+      <c r="AK4" s="74"/>
+      <c r="AL4" s="74"/>
+      <c r="AM4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="80"/>
-      <c r="AO4" s="70"/>
-      <c r="AP4" s="70"/>
-      <c r="AQ4" s="70"/>
-      <c r="AR4" s="70"/>
-      <c r="AS4" s="71" t="s">
+      <c r="AN4" s="65"/>
+      <c r="AO4" s="76"/>
+      <c r="AP4" s="76"/>
+      <c r="AQ4" s="76"/>
+      <c r="AR4" s="76"/>
+      <c r="AS4" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="71"/>
-      <c r="AU4" s="71"/>
-      <c r="AV4" s="71"/>
-      <c r="AW4" s="71"/>
-      <c r="AX4" s="71"/>
-      <c r="AY4" s="71"/>
-      <c r="AZ4" s="71"/>
-      <c r="BA4" s="71"/>
-      <c r="BB4" s="71"/>
-      <c r="BC4" s="71"/>
-      <c r="BD4" s="71"/>
-      <c r="BE4" s="71"/>
-      <c r="BF4" s="71"/>
-      <c r="BG4" s="71"/>
-      <c r="BH4" s="71"/>
-      <c r="BI4" s="71"/>
-      <c r="BJ4" s="71"/>
-      <c r="BK4" s="67" t="s">
+      <c r="AT4" s="77"/>
+      <c r="AU4" s="77"/>
+      <c r="AV4" s="77"/>
+      <c r="AW4" s="77"/>
+      <c r="AX4" s="77"/>
+      <c r="AY4" s="77"/>
+      <c r="AZ4" s="77"/>
+      <c r="BA4" s="77"/>
+      <c r="BB4" s="77"/>
+      <c r="BC4" s="77"/>
+      <c r="BD4" s="77"/>
+      <c r="BE4" s="77"/>
+      <c r="BF4" s="77"/>
+      <c r="BG4" s="77"/>
+      <c r="BH4" s="77"/>
+      <c r="BI4" s="77"/>
+      <c r="BJ4" s="77"/>
+      <c r="BK4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="BL4" s="67"/>
-      <c r="BM4" s="67"/>
-      <c r="BN4" s="67"/>
-      <c r="BO4" s="67"/>
-      <c r="BP4" s="67"/>
-      <c r="BQ4" s="67"/>
-      <c r="BR4" s="67"/>
-      <c r="BS4" s="67"/>
-      <c r="BT4" s="67"/>
-      <c r="BU4" s="67"/>
-      <c r="BV4" s="67"/>
-      <c r="BW4" s="67"/>
-      <c r="BX4" s="67"/>
-      <c r="BY4" s="72" t="s">
+      <c r="BL4" s="75"/>
+      <c r="BM4" s="75"/>
+      <c r="BN4" s="75"/>
+      <c r="BO4" s="75"/>
+      <c r="BP4" s="75"/>
+      <c r="BQ4" s="75"/>
+      <c r="BR4" s="75"/>
+      <c r="BS4" s="75"/>
+      <c r="BT4" s="75"/>
+      <c r="BU4" s="75"/>
+      <c r="BV4" s="75"/>
+      <c r="BW4" s="75"/>
+      <c r="BX4" s="75"/>
+      <c r="BY4" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="72"/>
-      <c r="CA4" s="72"/>
-      <c r="CB4" s="72"/>
-      <c r="CC4" s="72"/>
-      <c r="CD4" s="72"/>
-      <c r="CE4" s="72"/>
-      <c r="CF4" s="72"/>
-      <c r="CG4" s="72"/>
-      <c r="CH4" s="72"/>
-      <c r="CI4" s="72"/>
-      <c r="CJ4" s="72"/>
-      <c r="CK4" s="72"/>
-      <c r="CL4" s="72"/>
-      <c r="CM4" s="73" t="s">
+      <c r="BZ4" s="78"/>
+      <c r="CA4" s="78"/>
+      <c r="CB4" s="78"/>
+      <c r="CC4" s="78"/>
+      <c r="CD4" s="78"/>
+      <c r="CE4" s="78"/>
+      <c r="CF4" s="78"/>
+      <c r="CG4" s="78"/>
+      <c r="CH4" s="78"/>
+      <c r="CI4" s="78"/>
+      <c r="CJ4" s="78"/>
+      <c r="CK4" s="78"/>
+      <c r="CL4" s="78"/>
+      <c r="CM4" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="73"/>
-      <c r="CO4" s="73"/>
-      <c r="CP4" s="73"/>
-      <c r="CQ4" s="73"/>
-      <c r="CR4" s="73"/>
-      <c r="CS4" s="73"/>
-      <c r="CT4" s="73"/>
-      <c r="CU4" s="73"/>
-      <c r="CV4" s="73"/>
-      <c r="CW4" s="73"/>
-      <c r="CX4" s="73"/>
-      <c r="CY4" s="73"/>
-      <c r="CZ4" s="73"/>
-      <c r="DA4" s="74" t="s">
+      <c r="CN4" s="79"/>
+      <c r="CO4" s="79"/>
+      <c r="CP4" s="79"/>
+      <c r="CQ4" s="79"/>
+      <c r="CR4" s="79"/>
+      <c r="CS4" s="79"/>
+      <c r="CT4" s="79"/>
+      <c r="CU4" s="79"/>
+      <c r="CV4" s="79"/>
+      <c r="CW4" s="79"/>
+      <c r="CX4" s="79"/>
+      <c r="CY4" s="79"/>
+      <c r="CZ4" s="79"/>
+      <c r="DA4" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="74"/>
-      <c r="DC4" s="74"/>
-      <c r="DD4" s="74"/>
-      <c r="DE4" s="74"/>
-      <c r="DF4" s="74"/>
-      <c r="DG4" s="74"/>
-      <c r="DH4" s="74"/>
-      <c r="DI4" s="74"/>
-      <c r="DJ4" s="74"/>
-      <c r="DK4" s="74"/>
-      <c r="DL4" s="74"/>
-      <c r="DM4" s="74"/>
-      <c r="DN4" s="74"/>
-      <c r="DO4" s="75" t="s">
+      <c r="DB4" s="80"/>
+      <c r="DC4" s="80"/>
+      <c r="DD4" s="80"/>
+      <c r="DE4" s="80"/>
+      <c r="DF4" s="80"/>
+      <c r="DG4" s="80"/>
+      <c r="DH4" s="80"/>
+      <c r="DI4" s="80"/>
+      <c r="DJ4" s="80"/>
+      <c r="DK4" s="80"/>
+      <c r="DL4" s="80"/>
+      <c r="DM4" s="80"/>
+      <c r="DN4" s="80"/>
+      <c r="DO4" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="75"/>
-      <c r="DQ4" s="75"/>
-      <c r="DR4" s="75"/>
-      <c r="DS4" s="75"/>
-      <c r="DT4" s="75"/>
-      <c r="DU4" s="75"/>
-      <c r="DV4" s="75"/>
-      <c r="DW4" s="75"/>
-      <c r="DX4" s="75"/>
-      <c r="DY4" s="75"/>
-      <c r="DZ4" s="75"/>
-      <c r="EA4" s="75"/>
-      <c r="EB4" s="75"/>
-      <c r="EC4" s="76" t="s">
+      <c r="DP4" s="81"/>
+      <c r="DQ4" s="81"/>
+      <c r="DR4" s="81"/>
+      <c r="DS4" s="81"/>
+      <c r="DT4" s="81"/>
+      <c r="DU4" s="81"/>
+      <c r="DV4" s="81"/>
+      <c r="DW4" s="81"/>
+      <c r="DX4" s="81"/>
+      <c r="DY4" s="81"/>
+      <c r="DZ4" s="81"/>
+      <c r="EA4" s="81"/>
+      <c r="EB4" s="81"/>
+      <c r="EC4" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="76"/>
-      <c r="EE4" s="76"/>
-      <c r="EF4" s="76"/>
-      <c r="EG4" s="76"/>
-      <c r="EH4" s="76"/>
-      <c r="EI4" s="76"/>
-      <c r="EJ4" s="76"/>
-      <c r="EK4" s="76"/>
-      <c r="EL4" s="76"/>
-      <c r="EM4" s="76"/>
-      <c r="EN4" s="76"/>
-      <c r="EO4" s="76"/>
-      <c r="EP4" s="76"/>
-      <c r="EQ4" s="77" t="s">
+      <c r="ED4" s="82"/>
+      <c r="EE4" s="82"/>
+      <c r="EF4" s="82"/>
+      <c r="EG4" s="82"/>
+      <c r="EH4" s="82"/>
+      <c r="EI4" s="82"/>
+      <c r="EJ4" s="82"/>
+      <c r="EK4" s="82"/>
+      <c r="EL4" s="82"/>
+      <c r="EM4" s="82"/>
+      <c r="EN4" s="82"/>
+      <c r="EO4" s="82"/>
+      <c r="EP4" s="82"/>
+      <c r="EQ4" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="77"/>
-      <c r="ES4" s="77"/>
-      <c r="ET4" s="77"/>
-      <c r="EU4" s="77"/>
-      <c r="EV4" s="77"/>
-      <c r="EW4" s="77"/>
-      <c r="EX4" s="77"/>
-      <c r="EY4" s="77"/>
-      <c r="EZ4" s="77"/>
-      <c r="FA4" s="77"/>
-      <c r="FB4" s="77"/>
-      <c r="FC4" s="77"/>
-      <c r="FD4" s="77"/>
-      <c r="FE4" s="78" t="s">
+      <c r="ER4" s="83"/>
+      <c r="ES4" s="83"/>
+      <c r="ET4" s="83"/>
+      <c r="EU4" s="83"/>
+      <c r="EV4" s="83"/>
+      <c r="EW4" s="83"/>
+      <c r="EX4" s="83"/>
+      <c r="EY4" s="83"/>
+      <c r="EZ4" s="83"/>
+      <c r="FA4" s="83"/>
+      <c r="FB4" s="83"/>
+      <c r="FC4" s="83"/>
+      <c r="FD4" s="83"/>
+      <c r="FE4" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="78"/>
-      <c r="FG4" s="78"/>
-      <c r="FH4" s="78"/>
-      <c r="FI4" s="78"/>
-      <c r="FJ4" s="78"/>
-      <c r="FK4" s="78"/>
-      <c r="FL4" s="78"/>
-      <c r="FM4" s="78"/>
-      <c r="FN4" s="78"/>
-      <c r="FO4" s="78"/>
-      <c r="FP4" s="78"/>
-      <c r="FQ4" s="78"/>
-      <c r="FR4" s="78"/>
-      <c r="FS4" s="79" t="s">
+      <c r="FF4" s="84"/>
+      <c r="FG4" s="84"/>
+      <c r="FH4" s="84"/>
+      <c r="FI4" s="84"/>
+      <c r="FJ4" s="84"/>
+      <c r="FK4" s="84"/>
+      <c r="FL4" s="84"/>
+      <c r="FM4" s="84"/>
+      <c r="FN4" s="84"/>
+      <c r="FO4" s="84"/>
+      <c r="FP4" s="84"/>
+      <c r="FQ4" s="84"/>
+      <c r="FR4" s="84"/>
+      <c r="FS4" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="79"/>
-      <c r="FU4" s="79"/>
-      <c r="FV4" s="79"/>
-      <c r="FW4" s="79"/>
-      <c r="FX4" s="79"/>
-      <c r="FY4" s="79"/>
-      <c r="FZ4" s="79"/>
-      <c r="GA4" s="79"/>
-      <c r="GB4" s="79"/>
-      <c r="GC4" s="79"/>
-      <c r="GD4" s="79"/>
-      <c r="GE4" s="79"/>
-      <c r="GF4" s="79"/>
-      <c r="GG4" s="67" t="s">
+      <c r="FT4" s="85"/>
+      <c r="FU4" s="85"/>
+      <c r="FV4" s="85"/>
+      <c r="FW4" s="85"/>
+      <c r="FX4" s="85"/>
+      <c r="FY4" s="85"/>
+      <c r="FZ4" s="85"/>
+      <c r="GA4" s="85"/>
+      <c r="GB4" s="85"/>
+      <c r="GC4" s="85"/>
+      <c r="GD4" s="85"/>
+      <c r="GE4" s="85"/>
+      <c r="GF4" s="85"/>
+      <c r="GG4" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="GH4" s="67"/>
-      <c r="GI4" s="67"/>
-      <c r="GJ4" s="67"/>
-      <c r="GK4" s="67"/>
-      <c r="GL4" s="67"/>
-      <c r="GM4" s="67"/>
-      <c r="GN4" s="67"/>
-      <c r="GO4" s="67"/>
-      <c r="GP4" s="67"/>
-      <c r="GQ4" s="67"/>
-      <c r="GR4" s="67"/>
-      <c r="GS4" s="67"/>
-      <c r="GT4" s="67"/>
-      <c r="GU4" s="67" t="s">
+      <c r="GH4" s="75"/>
+      <c r="GI4" s="75"/>
+      <c r="GJ4" s="75"/>
+      <c r="GK4" s="75"/>
+      <c r="GL4" s="75"/>
+      <c r="GM4" s="75"/>
+      <c r="GN4" s="75"/>
+      <c r="GO4" s="75"/>
+      <c r="GP4" s="75"/>
+      <c r="GQ4" s="75"/>
+      <c r="GR4" s="75"/>
+      <c r="GS4" s="75"/>
+      <c r="GT4" s="75"/>
+      <c r="GU4" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="GV4" s="67"/>
-      <c r="GW4" s="67"/>
-      <c r="GX4" s="67"/>
-      <c r="GY4" s="67"/>
-      <c r="GZ4" s="67"/>
-      <c r="HA4" s="67"/>
-      <c r="HB4" s="67"/>
-      <c r="HC4" s="67"/>
-      <c r="HD4" s="67"/>
-      <c r="HE4" s="67"/>
-      <c r="HF4" s="67"/>
-      <c r="HG4" s="67"/>
-      <c r="HH4" s="67"/>
-      <c r="HI4" s="67" t="s">
+      <c r="GV4" s="75"/>
+      <c r="GW4" s="75"/>
+      <c r="GX4" s="75"/>
+      <c r="GY4" s="75"/>
+      <c r="GZ4" s="75"/>
+      <c r="HA4" s="75"/>
+      <c r="HB4" s="75"/>
+      <c r="HC4" s="75"/>
+      <c r="HD4" s="75"/>
+      <c r="HE4" s="75"/>
+      <c r="HF4" s="75"/>
+      <c r="HG4" s="75"/>
+      <c r="HH4" s="75"/>
+      <c r="HI4" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="HJ4" s="67"/>
-      <c r="HK4" s="67"/>
-      <c r="HL4" s="67"/>
-      <c r="HM4" s="67"/>
-      <c r="HN4" s="67"/>
-      <c r="HO4" s="67"/>
-      <c r="HP4" s="67"/>
-      <c r="HQ4" s="67"/>
-      <c r="HR4" s="67"/>
-      <c r="HS4" s="67"/>
-      <c r="HT4" s="67"/>
-      <c r="HU4" s="67"/>
-      <c r="HV4" s="67"/>
-      <c r="HW4" s="68" t="s">
+      <c r="HJ4" s="75"/>
+      <c r="HK4" s="75"/>
+      <c r="HL4" s="75"/>
+      <c r="HM4" s="75"/>
+      <c r="HN4" s="75"/>
+      <c r="HO4" s="75"/>
+      <c r="HP4" s="75"/>
+      <c r="HQ4" s="75"/>
+      <c r="HR4" s="75"/>
+      <c r="HS4" s="75"/>
+      <c r="HT4" s="75"/>
+      <c r="HU4" s="75"/>
+      <c r="HV4" s="75"/>
+      <c r="HW4" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="68"/>
-      <c r="HY4" s="68"/>
-      <c r="HZ4" s="68"/>
-      <c r="IA4" s="68"/>
-      <c r="IB4" s="68"/>
-      <c r="IC4" s="68"/>
-      <c r="ID4" s="68"/>
-      <c r="IE4" s="68"/>
-      <c r="IF4" s="68"/>
-      <c r="IG4" s="68"/>
-      <c r="IH4" s="68"/>
-      <c r="II4" s="68"/>
-      <c r="IJ4" s="68"/>
-      <c r="IK4" s="68" t="s">
+      <c r="HX4" s="92"/>
+      <c r="HY4" s="92"/>
+      <c r="HZ4" s="92"/>
+      <c r="IA4" s="92"/>
+      <c r="IB4" s="92"/>
+      <c r="IC4" s="92"/>
+      <c r="ID4" s="92"/>
+      <c r="IE4" s="92"/>
+      <c r="IF4" s="92"/>
+      <c r="IG4" s="92"/>
+      <c r="IH4" s="92"/>
+      <c r="II4" s="92"/>
+      <c r="IJ4" s="92"/>
+      <c r="IK4" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="68"/>
-      <c r="IM4" s="68"/>
-      <c r="IN4" s="68"/>
-      <c r="IO4" s="68"/>
-      <c r="IP4" s="68"/>
-      <c r="IQ4" s="68"/>
-      <c r="IR4" s="68"/>
-      <c r="IS4" s="68"/>
-      <c r="IT4" s="68"/>
-      <c r="IU4" s="68"/>
-      <c r="IV4" s="68"/>
-      <c r="IW4" s="68"/>
-      <c r="IX4" s="68"/>
-      <c r="IY4" s="68" t="s">
+      <c r="IL4" s="92"/>
+      <c r="IM4" s="92"/>
+      <c r="IN4" s="92"/>
+      <c r="IO4" s="92"/>
+      <c r="IP4" s="92"/>
+      <c r="IQ4" s="92"/>
+      <c r="IR4" s="92"/>
+      <c r="IS4" s="92"/>
+      <c r="IT4" s="92"/>
+      <c r="IU4" s="92"/>
+      <c r="IV4" s="92"/>
+      <c r="IW4" s="92"/>
+      <c r="IX4" s="92"/>
+      <c r="IY4" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="68"/>
-      <c r="JA4" s="68"/>
-      <c r="JB4" s="68"/>
-      <c r="JC4" s="68"/>
-      <c r="JD4" s="68"/>
-      <c r="JE4" s="68"/>
-      <c r="JF4" s="68"/>
-      <c r="JG4" s="68"/>
-      <c r="JH4" s="68"/>
-      <c r="JI4" s="68"/>
-      <c r="JJ4" s="68"/>
-      <c r="JK4" s="68"/>
-      <c r="JL4" s="68"/>
-      <c r="JM4" s="69" t="s">
+      <c r="IZ4" s="92"/>
+      <c r="JA4" s="92"/>
+      <c r="JB4" s="92"/>
+      <c r="JC4" s="92"/>
+      <c r="JD4" s="92"/>
+      <c r="JE4" s="92"/>
+      <c r="JF4" s="92"/>
+      <c r="JG4" s="92"/>
+      <c r="JH4" s="92"/>
+      <c r="JI4" s="92"/>
+      <c r="JJ4" s="92"/>
+      <c r="JK4" s="92"/>
+      <c r="JL4" s="92"/>
+      <c r="JM4" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="69"/>
-      <c r="JO4" s="69"/>
-      <c r="JP4" s="69"/>
-      <c r="JQ4" s="69"/>
-      <c r="JR4" s="69"/>
-      <c r="JS4" s="69"/>
-      <c r="JT4" s="69"/>
-      <c r="JU4" s="69"/>
-      <c r="JV4" s="69"/>
-      <c r="JW4" s="69"/>
-      <c r="JX4" s="69"/>
-      <c r="JY4" s="69"/>
-      <c r="JZ4" s="65" t="s">
+      <c r="JN4" s="93"/>
+      <c r="JO4" s="93"/>
+      <c r="JP4" s="93"/>
+      <c r="JQ4" s="93"/>
+      <c r="JR4" s="93"/>
+      <c r="JS4" s="93"/>
+      <c r="JT4" s="93"/>
+      <c r="JU4" s="93"/>
+      <c r="JV4" s="93"/>
+      <c r="JW4" s="93"/>
+      <c r="JX4" s="93"/>
+      <c r="JY4" s="93"/>
+      <c r="JZ4" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="66"/>
-      <c r="KB4" s="66"/>
-      <c r="KC4" s="66"/>
-      <c r="KD4" s="66"/>
-      <c r="KE4" s="66"/>
-      <c r="KF4" s="66"/>
-      <c r="KG4" s="66"/>
-      <c r="KH4" s="61" t="s">
-        <v>322</v>
-      </c>
-      <c r="KI4" s="62"/>
-      <c r="KJ4" s="62"/>
-      <c r="KK4" s="62"/>
-      <c r="KL4" s="60"/>
+      <c r="KA4" s="91"/>
+      <c r="KB4" s="91"/>
+      <c r="KC4" s="91"/>
+      <c r="KD4" s="91"/>
+      <c r="KE4" s="91"/>
+      <c r="KF4" s="91"/>
+      <c r="KG4" s="91"/>
+      <c r="KH4" s="86" t="s">
+        <v>316</v>
+      </c>
+      <c r="KI4" s="87"/>
+      <c r="KJ4" s="87"/>
+      <c r="KK4" s="46"/>
     </row>
-    <row r="5" spans="1:298" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="83"/>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="85"/>
-      <c r="L5" s="85"/>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="86"/>
-      <c r="Q5" s="86"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="86"/>
-      <c r="T5" s="86"/>
-      <c r="U5" s="87"/>
-      <c r="V5" s="87"/>
-      <c r="W5" s="87"/>
-      <c r="X5" s="87"/>
-      <c r="Y5" s="87"/>
-      <c r="Z5" s="87"/>
-      <c r="AA5" s="87"/>
-      <c r="AB5" s="87"/>
-      <c r="AC5" s="88"/>
-      <c r="AD5" s="88"/>
-      <c r="AE5" s="88"/>
-      <c r="AF5" s="88"/>
-      <c r="AG5" s="88"/>
-      <c r="AH5" s="88"/>
-      <c r="AI5" s="88"/>
-      <c r="AJ5" s="89"/>
-      <c r="AK5" s="89"/>
-      <c r="AL5" s="89"/>
-      <c r="AM5" s="80"/>
-      <c r="AN5" s="80"/>
-      <c r="AO5" s="70"/>
-      <c r="AP5" s="70"/>
-      <c r="AQ5" s="70"/>
-      <c r="AR5" s="70"/>
-      <c r="AS5" s="71"/>
-      <c r="AT5" s="71"/>
-      <c r="AU5" s="71"/>
-      <c r="AV5" s="71"/>
-      <c r="AW5" s="71"/>
-      <c r="AX5" s="71"/>
-      <c r="AY5" s="71"/>
-      <c r="AZ5" s="71"/>
-      <c r="BA5" s="71"/>
-      <c r="BB5" s="71"/>
-      <c r="BC5" s="71"/>
-      <c r="BD5" s="71"/>
-      <c r="BE5" s="71"/>
-      <c r="BF5" s="71"/>
-      <c r="BG5" s="71"/>
-      <c r="BH5" s="71"/>
-      <c r="BI5" s="71"/>
-      <c r="BJ5" s="71"/>
+    <row r="5" spans="1:300" ht="12" customHeight="1">
+      <c r="A5" s="68"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="71"/>
+      <c r="Q5" s="71"/>
+      <c r="R5" s="71"/>
+      <c r="S5" s="71"/>
+      <c r="T5" s="71"/>
+      <c r="U5" s="72"/>
+      <c r="V5" s="72"/>
+      <c r="W5" s="72"/>
+      <c r="X5" s="72"/>
+      <c r="Y5" s="72"/>
+      <c r="Z5" s="72"/>
+      <c r="AA5" s="72"/>
+      <c r="AB5" s="72"/>
+      <c r="AC5" s="73"/>
+      <c r="AD5" s="73"/>
+      <c r="AE5" s="73"/>
+      <c r="AF5" s="73"/>
+      <c r="AG5" s="73"/>
+      <c r="AH5" s="73"/>
+      <c r="AI5" s="73"/>
+      <c r="AJ5" s="74"/>
+      <c r="AK5" s="74"/>
+      <c r="AL5" s="74"/>
+      <c r="AM5" s="65"/>
+      <c r="AN5" s="65"/>
+      <c r="AO5" s="76"/>
+      <c r="AP5" s="76"/>
+      <c r="AQ5" s="76"/>
+      <c r="AR5" s="76"/>
+      <c r="AS5" s="77"/>
+      <c r="AT5" s="77"/>
+      <c r="AU5" s="77"/>
+      <c r="AV5" s="77"/>
+      <c r="AW5" s="77"/>
+      <c r="AX5" s="77"/>
+      <c r="AY5" s="77"/>
+      <c r="AZ5" s="77"/>
+      <c r="BA5" s="77"/>
+      <c r="BB5" s="77"/>
+      <c r="BC5" s="77"/>
+      <c r="BD5" s="77"/>
+      <c r="BE5" s="77"/>
+      <c r="BF5" s="77"/>
+      <c r="BG5" s="77"/>
+      <c r="BH5" s="77"/>
+      <c r="BI5" s="77"/>
+      <c r="BJ5" s="77"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -3466,7 +3497,7 @@
         <v>314</v>
       </c>
       <c r="BX5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="BY5" s="8" t="s">
         <v>27</v>
@@ -3508,7 +3539,7 @@
         <v>314</v>
       </c>
       <c r="CL5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="CM5" s="8" t="s">
         <v>27</v>
@@ -3550,7 +3581,7 @@
         <v>314</v>
       </c>
       <c r="CZ5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="DA5" s="8" t="s">
         <v>27</v>
@@ -3592,7 +3623,7 @@
         <v>314</v>
       </c>
       <c r="DN5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="DO5" s="8" t="s">
         <v>27</v>
@@ -3634,7 +3665,7 @@
         <v>314</v>
       </c>
       <c r="EB5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="EC5" s="8" t="s">
         <v>27</v>
@@ -3676,7 +3707,7 @@
         <v>314</v>
       </c>
       <c r="EP5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="EQ5" s="8" t="s">
         <v>27</v>
@@ -3718,7 +3749,7 @@
         <v>314</v>
       </c>
       <c r="FD5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="FE5" s="8" t="s">
         <v>27</v>
@@ -3760,7 +3791,7 @@
         <v>314</v>
       </c>
       <c r="FR5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="FS5" s="8" t="s">
         <v>27</v>
@@ -3802,7 +3833,7 @@
         <v>314</v>
       </c>
       <c r="GF5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="GG5" s="8" t="s">
         <v>27</v>
@@ -3844,7 +3875,7 @@
         <v>314</v>
       </c>
       <c r="GT5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="GU5" s="8" t="s">
         <v>27</v>
@@ -3886,7 +3917,7 @@
         <v>314</v>
       </c>
       <c r="HH5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="HI5" s="8" t="s">
         <v>27</v>
@@ -3928,7 +3959,7 @@
         <v>314</v>
       </c>
       <c r="HV5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="HW5" s="8" t="s">
         <v>27</v>
@@ -3970,7 +4001,7 @@
         <v>314</v>
       </c>
       <c r="IJ5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="IK5" s="8" t="s">
         <v>27</v>
@@ -4012,7 +4043,7 @@
         <v>314</v>
       </c>
       <c r="IX5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="IY5" s="8" t="s">
         <v>27</v>
@@ -4054,40 +4085,39 @@
         <v>314</v>
       </c>
       <c r="JL5" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="JM5" s="69"/>
-      <c r="JN5" s="69"/>
-      <c r="JO5" s="69"/>
-      <c r="JP5" s="69"/>
-      <c r="JQ5" s="69"/>
-      <c r="JR5" s="69"/>
-      <c r="JS5" s="69"/>
-      <c r="JT5" s="69"/>
-      <c r="JU5" s="69"/>
-      <c r="JV5" s="69"/>
-      <c r="JW5" s="69"/>
-      <c r="JX5" s="69"/>
-      <c r="JY5" s="69"/>
-      <c r="JZ5" s="66" t="s">
-        <v>316</v>
-      </c>
-      <c r="KA5" s="66"/>
-      <c r="KB5" s="66"/>
-      <c r="KC5" s="66"/>
-      <c r="KD5" s="66" t="s">
+        <v>315</v>
+      </c>
+      <c r="JM5" s="93"/>
+      <c r="JN5" s="93"/>
+      <c r="JO5" s="93"/>
+      <c r="JP5" s="93"/>
+      <c r="JQ5" s="93"/>
+      <c r="JR5" s="93"/>
+      <c r="JS5" s="93"/>
+      <c r="JT5" s="93"/>
+      <c r="JU5" s="93"/>
+      <c r="JV5" s="93"/>
+      <c r="JW5" s="93"/>
+      <c r="JX5" s="93"/>
+      <c r="JY5" s="93"/>
+      <c r="JZ5" s="91" t="s">
+        <v>347</v>
+      </c>
+      <c r="KA5" s="91"/>
+      <c r="KB5" s="91"/>
+      <c r="KC5" s="91"/>
+      <c r="KD5" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="66"/>
-      <c r="KF5" s="66"/>
-      <c r="KG5" s="66"/>
-      <c r="KH5" s="63"/>
-      <c r="KI5" s="64"/>
-      <c r="KJ5" s="64"/>
-      <c r="KK5" s="64"/>
-      <c r="KL5" s="60"/>
+      <c r="KE5" s="91"/>
+      <c r="KF5" s="91"/>
+      <c r="KG5" s="91"/>
+      <c r="KH5" s="88"/>
+      <c r="KI5" s="89"/>
+      <c r="KJ5" s="89"/>
+      <c r="KK5" s="46"/>
     </row>
-    <row r="6" spans="1:298" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:300" ht="81.75" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -4314,7 +4344,7 @@
         <v>113</v>
       </c>
       <c r="BX6" s="22" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="BY6" s="22" t="s">
         <v>114</v>
@@ -4356,7 +4386,7 @@
         <v>126</v>
       </c>
       <c r="CL6" s="22" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="CM6" s="22" t="s">
         <v>127</v>
@@ -4398,7 +4428,7 @@
         <v>139</v>
       </c>
       <c r="CZ6" s="22" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="DA6" s="22" t="s">
         <v>140</v>
@@ -4440,7 +4470,7 @@
         <v>152</v>
       </c>
       <c r="DN6" s="22" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="DO6" s="22" t="s">
         <v>153</v>
@@ -4482,7 +4512,7 @@
         <v>165</v>
       </c>
       <c r="EB6" s="22" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="EC6" s="22" t="s">
         <v>166</v>
@@ -4524,7 +4554,7 @@
         <v>178</v>
       </c>
       <c r="EP6" s="12" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="EQ6" s="12" t="s">
         <v>179</v>
@@ -4566,7 +4596,7 @@
         <v>191</v>
       </c>
       <c r="FD6" s="12" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="FE6" s="12" t="s">
         <v>192</v>
@@ -4608,7 +4638,7 @@
         <v>204</v>
       </c>
       <c r="FR6" s="12" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="FS6" s="22" t="s">
         <v>205</v>
@@ -4650,7 +4680,7 @@
         <v>217</v>
       </c>
       <c r="GF6" s="22" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="GG6" s="22" t="s">
         <v>218</v>
@@ -4692,7 +4722,7 @@
         <v>230</v>
       </c>
       <c r="GT6" s="22" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="GU6" s="22" t="s">
         <v>231</v>
@@ -4734,7 +4764,7 @@
         <v>243</v>
       </c>
       <c r="HH6" s="22" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="HI6" s="22" t="s">
         <v>244</v>
@@ -4776,7 +4806,7 @@
         <v>256</v>
       </c>
       <c r="HV6" s="22" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="HW6" s="22" t="s">
         <v>257</v>
@@ -4818,7 +4848,7 @@
         <v>269</v>
       </c>
       <c r="IJ6" s="22" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="IK6" s="22" t="s">
         <v>270</v>
@@ -4860,7 +4890,7 @@
         <v>282</v>
       </c>
       <c r="IX6" s="22" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="IY6" s="22" t="s">
         <v>283</v>
@@ -4902,7 +4932,7 @@
         <v>295</v>
       </c>
       <c r="JL6" s="22" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="JM6" s="22" t="s">
         <v>296</v>
@@ -4944,21 +4974,21 @@
         <v>308</v>
       </c>
       <c r="JZ6" s="22" t="s">
-        <v>315</v>
-      </c>
-      <c r="KA6" s="34" t="s">
-        <v>317</v>
+        <v>344</v>
+      </c>
+      <c r="KA6" s="29" t="s">
+        <v>343</v>
       </c>
       <c r="KB6" s="22" t="s">
-        <v>318</v>
+        <v>345</v>
       </c>
       <c r="KC6" s="22" t="s">
-        <v>319</v>
+        <v>346</v>
       </c>
       <c r="KD6" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="KE6" s="34" t="s">
+      <c r="KE6" s="29" t="s">
         <v>312</v>
       </c>
       <c r="KF6" s="22" t="s">
@@ -4968,470 +4998,1682 @@
         <v>311</v>
       </c>
       <c r="KH6" s="22" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="KI6" s="22" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="KJ6" s="22" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="KK6" s="22" t="s">
-        <v>326</v>
-      </c>
-      <c r="KL6" s="22" t="s">
-        <v>342</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="KL6" s="49" t="s">
+        <v>336</v>
+      </c>
+      <c r="KM6" s="50"/>
+      <c r="KN6" s="51"/>
     </row>
-    <row r="7" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32" t="s">
-        <v>343</v>
-      </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53" t="s">
-        <v>343</v>
-      </c>
-      <c r="S7" s="53" t="s">
-        <v>343</v>
-      </c>
-      <c r="T7" s="53"/>
-      <c r="U7" s="53"/>
-      <c r="V7" s="53"/>
-      <c r="W7" s="53"/>
-      <c r="X7" s="54" t="s">
-        <v>343</v>
-      </c>
-      <c r="Y7" s="54" t="s">
-        <v>343</v>
-      </c>
-      <c r="Z7" s="53"/>
-      <c r="AA7" s="53"/>
-      <c r="AB7" s="54"/>
-      <c r="AC7" s="55"/>
-      <c r="AD7" s="56"/>
-      <c r="AE7" s="56"/>
-      <c r="AF7" s="31"/>
-      <c r="AG7" s="31"/>
-      <c r="AH7" s="57"/>
-      <c r="AI7" s="31"/>
-      <c r="AJ7" s="52" t="s">
-        <v>343</v>
-      </c>
-      <c r="AK7" s="52" t="s">
-        <v>343</v>
-      </c>
-      <c r="AL7" s="52" t="s">
-        <v>343</v>
-      </c>
-      <c r="AM7" s="53"/>
-      <c r="AN7" s="58"/>
-      <c r="AO7" s="51"/>
-      <c r="AP7" s="51"/>
-      <c r="AQ7" s="51"/>
-      <c r="AR7" s="51"/>
-      <c r="AS7" s="33">
+    <row r="7" spans="1:300" ht="15" customHeight="1">
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52" t="s">
+        <v>341</v>
+      </c>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54" t="s">
+        <v>341</v>
+      </c>
+      <c r="S7" s="54" t="s">
+        <v>341</v>
+      </c>
+      <c r="T7" s="54"/>
+      <c r="U7" s="54"/>
+      <c r="V7" s="54"/>
+      <c r="W7" s="54"/>
+      <c r="X7" s="55" t="s">
+        <v>341</v>
+      </c>
+      <c r="Y7" s="55" t="s">
+        <v>341</v>
+      </c>
+      <c r="Z7" s="54"/>
+      <c r="AA7" s="54"/>
+      <c r="AB7" s="55"/>
+      <c r="AC7" s="56"/>
+      <c r="AD7" s="57"/>
+      <c r="AE7" s="57"/>
+      <c r="AF7" s="58"/>
+      <c r="AG7" s="58"/>
+      <c r="AH7" s="59"/>
+      <c r="AI7" s="58"/>
+      <c r="AJ7" s="53" t="s">
+        <v>341</v>
+      </c>
+      <c r="AK7" s="53" t="s">
+        <v>341</v>
+      </c>
+      <c r="AL7" s="53" t="s">
+        <v>341</v>
+      </c>
+      <c r="AM7" s="54"/>
+      <c r="AN7" s="60"/>
+      <c r="AO7" s="61"/>
+      <c r="AP7" s="61"/>
+      <c r="AQ7" s="61"/>
+      <c r="AR7" s="61"/>
+      <c r="AS7" s="62">
         <f>SUM(BK7:BX7)</f>
         <v>0</v>
       </c>
-      <c r="AT7" s="30">
+      <c r="AT7" s="63">
         <f>SUM(BY7:CL7)</f>
         <v>0</v>
       </c>
-      <c r="AU7" s="30">
+      <c r="AU7" s="63">
         <f>SUM(CM7:CZ7)</f>
         <v>0</v>
       </c>
-      <c r="AV7" s="30">
+      <c r="AV7" s="63">
         <f>SUM(DA7:DN7)</f>
         <v>0</v>
       </c>
-      <c r="AW7" s="30">
+      <c r="AW7" s="63">
         <f>SUM(DO7:EB7)</f>
         <v>0</v>
       </c>
-      <c r="AX7" s="30">
+      <c r="AX7" s="63">
         <f>SUM(EC7:EP7)</f>
         <v>0</v>
       </c>
-      <c r="AY7" s="30">
+      <c r="AY7" s="63">
         <f>SUM(EQ7:FD7)</f>
         <v>0</v>
       </c>
-      <c r="AZ7" s="30">
+      <c r="AZ7" s="63">
         <f>SUM(FE7:FR7)</f>
         <v>0</v>
       </c>
-      <c r="BA7" s="30">
+      <c r="BA7" s="63">
         <f>SUM(FS7:GF7)</f>
         <v>0</v>
       </c>
-      <c r="BB7" s="30">
+      <c r="BB7" s="63">
         <f>SUM(GG7:GT7)</f>
         <v>0</v>
       </c>
-      <c r="BC7" s="30">
+      <c r="BC7" s="63">
         <f>SUM(GU7:HH7)</f>
         <v>0</v>
       </c>
-      <c r="BD7" s="30">
+      <c r="BD7" s="63">
         <f>SUM(HI7:HV7)</f>
         <v>0</v>
       </c>
-      <c r="BE7" s="30">
+      <c r="BE7" s="63">
         <f>SUM(HW7:IJ7)</f>
         <v>0</v>
       </c>
-      <c r="BF7" s="30">
+      <c r="BF7" s="63">
         <f>SUM(IK7:IX7)</f>
         <v>0</v>
       </c>
-      <c r="BG7" s="30">
+      <c r="BG7" s="63">
         <f>SUM(IY7:JL7)</f>
         <v>0</v>
       </c>
-      <c r="BH7" s="30">
+      <c r="BH7" s="63">
         <f t="shared" ref="BH7" si="0">JM7</f>
         <v>0</v>
       </c>
-      <c r="BI7" s="30">
+      <c r="BI7" s="63">
         <f>JN7</f>
         <v>0</v>
       </c>
-      <c r="BJ7" s="30">
+      <c r="BJ7" s="63">
         <f>JO7</f>
         <v>0</v>
       </c>
-      <c r="BK7" s="30">
-        <f t="shared" ref="BK7" si="1">BY7+CM7+DA7+DO7+EC7+EQ7+FE7+FS7</f>
+      <c r="BK7" s="63">
+        <f t="shared" ref="BK7:BX7" si="1">BY7+CM7+DA7+DO7+EC7+EQ7+FE7+FS7</f>
         <v>0</v>
       </c>
-      <c r="BL7" s="30">
-        <f t="shared" ref="BL7:BX7" si="2">BZ7+CN7+DB7+DP7+ED7+ER7+FF7+FT7</f>
+      <c r="BL7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BM7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BM7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BN7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BN7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BO7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BO7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BP7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BP7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BQ7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BQ7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BR7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BR7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BS7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BS7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BT7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BT7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BU7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BU7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BV7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BV7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BW7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BW7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BX7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BX7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BY7" s="31"/>
-      <c r="BZ7" s="31"/>
-      <c r="CA7" s="31"/>
-      <c r="CB7" s="31"/>
-      <c r="CC7" s="31"/>
-      <c r="CD7" s="31"/>
-      <c r="CE7" s="31"/>
-      <c r="CF7" s="31"/>
-      <c r="CG7" s="31"/>
-      <c r="CH7" s="31"/>
-      <c r="CI7" s="31"/>
-      <c r="CJ7" s="31"/>
-      <c r="CK7" s="31"/>
-      <c r="CL7" s="31"/>
-      <c r="CM7" s="31"/>
-      <c r="CN7" s="31"/>
-      <c r="CO7" s="31"/>
-      <c r="CP7" s="31"/>
-      <c r="CQ7" s="31"/>
-      <c r="CR7" s="31"/>
-      <c r="CS7" s="31"/>
-      <c r="CT7" s="31"/>
-      <c r="CU7" s="31"/>
-      <c r="CV7" s="31"/>
-      <c r="CW7" s="31"/>
-      <c r="CX7" s="31"/>
-      <c r="CY7" s="31"/>
-      <c r="CZ7" s="31"/>
-      <c r="DA7" s="31"/>
-      <c r="DB7" s="31"/>
-      <c r="DC7" s="31"/>
-      <c r="DD7" s="31"/>
-      <c r="DE7" s="31"/>
-      <c r="DF7" s="31"/>
-      <c r="DG7" s="31"/>
-      <c r="DH7" s="31"/>
-      <c r="DI7" s="31"/>
-      <c r="DJ7" s="31"/>
-      <c r="DK7" s="31"/>
-      <c r="DL7" s="31"/>
-      <c r="DM7" s="31"/>
-      <c r="DN7" s="31"/>
-      <c r="DO7" s="31"/>
-      <c r="DP7" s="31"/>
-      <c r="DQ7" s="31"/>
-      <c r="DR7" s="31"/>
-      <c r="DS7" s="31"/>
-      <c r="DT7" s="31"/>
-      <c r="DU7" s="31"/>
-      <c r="DV7" s="31"/>
-      <c r="DW7" s="31"/>
-      <c r="DX7" s="31"/>
-      <c r="DY7" s="31"/>
-      <c r="DZ7" s="31"/>
-      <c r="EA7" s="31"/>
-      <c r="EB7" s="31"/>
-      <c r="EC7" s="31"/>
-      <c r="ED7" s="31"/>
-      <c r="EE7" s="31"/>
-      <c r="EF7" s="31"/>
-      <c r="EG7" s="31"/>
-      <c r="EH7" s="31"/>
-      <c r="EI7" s="31"/>
-      <c r="EJ7" s="31"/>
-      <c r="EK7" s="31"/>
-      <c r="EL7" s="31"/>
-      <c r="EM7" s="31"/>
-      <c r="EN7" s="31"/>
-      <c r="EO7" s="31"/>
-      <c r="EP7" s="31"/>
-      <c r="EQ7" s="31"/>
-      <c r="ER7" s="31"/>
-      <c r="ES7" s="31"/>
-      <c r="ET7" s="31"/>
-      <c r="EU7" s="31"/>
-      <c r="EV7" s="31"/>
-      <c r="EW7" s="31"/>
-      <c r="EX7" s="31"/>
-      <c r="EY7" s="31"/>
-      <c r="EZ7" s="31"/>
-      <c r="FA7" s="31"/>
-      <c r="FB7" s="31"/>
-      <c r="FC7" s="31"/>
-      <c r="FD7" s="31"/>
-      <c r="FE7" s="31"/>
-      <c r="FF7" s="31"/>
-      <c r="FG7" s="31"/>
-      <c r="FH7" s="31"/>
-      <c r="FI7" s="31"/>
-      <c r="FJ7" s="31"/>
-      <c r="FK7" s="31"/>
-      <c r="FL7" s="31"/>
-      <c r="FM7" s="31"/>
-      <c r="FN7" s="31"/>
-      <c r="FO7" s="31"/>
-      <c r="FP7" s="31"/>
-      <c r="FQ7" s="31"/>
-      <c r="FR7" s="31"/>
-      <c r="FS7" s="31"/>
-      <c r="FT7" s="31"/>
-      <c r="FU7" s="31"/>
-      <c r="FV7" s="31"/>
-      <c r="FW7" s="31"/>
-      <c r="FX7" s="31"/>
-      <c r="FY7" s="31"/>
-      <c r="FZ7" s="31"/>
-      <c r="GA7" s="31"/>
-      <c r="GB7" s="31"/>
-      <c r="GC7" s="31"/>
-      <c r="GD7" s="31"/>
-      <c r="GE7" s="31"/>
-      <c r="GF7" s="31"/>
-      <c r="GG7" s="31"/>
-      <c r="GH7" s="31"/>
-      <c r="GI7" s="31"/>
-      <c r="GJ7" s="31"/>
-      <c r="GK7" s="31"/>
-      <c r="GL7" s="31"/>
-      <c r="GM7" s="31"/>
-      <c r="GN7" s="31"/>
-      <c r="GO7" s="31"/>
-      <c r="GP7" s="31"/>
-      <c r="GQ7" s="31"/>
-      <c r="GR7" s="31"/>
-      <c r="GS7" s="31"/>
-      <c r="GT7" s="31"/>
-      <c r="GU7" s="31"/>
-      <c r="GV7" s="31"/>
-      <c r="GW7" s="31"/>
-      <c r="GX7" s="31"/>
-      <c r="GY7" s="31"/>
-      <c r="GZ7" s="31"/>
-      <c r="HA7" s="31"/>
-      <c r="HB7" s="31"/>
-      <c r="HC7" s="31"/>
-      <c r="HD7" s="31"/>
-      <c r="HE7" s="31"/>
-      <c r="HF7" s="31"/>
-      <c r="HG7" s="31"/>
-      <c r="HH7" s="31"/>
-      <c r="HI7" s="31"/>
-      <c r="HJ7" s="31"/>
-      <c r="HK7" s="31"/>
-      <c r="HL7" s="31"/>
-      <c r="HM7" s="31"/>
-      <c r="HN7" s="31"/>
-      <c r="HO7" s="31"/>
-      <c r="HP7" s="31"/>
-      <c r="HQ7" s="31"/>
-      <c r="HR7" s="31"/>
-      <c r="HS7" s="31"/>
-      <c r="HT7" s="31"/>
-      <c r="HU7" s="31"/>
-      <c r="HV7" s="31"/>
-      <c r="HW7" s="31"/>
-      <c r="HX7" s="31"/>
-      <c r="HY7" s="31"/>
-      <c r="HZ7" s="31"/>
-      <c r="IA7" s="31"/>
-      <c r="IB7" s="31"/>
-      <c r="IC7" s="31"/>
-      <c r="ID7" s="31"/>
-      <c r="IE7" s="31"/>
-      <c r="IF7" s="31"/>
-      <c r="IG7" s="31"/>
-      <c r="IH7" s="31"/>
-      <c r="II7" s="31"/>
-      <c r="IJ7" s="31"/>
-      <c r="IK7" s="31"/>
-      <c r="IL7" s="31"/>
-      <c r="IM7" s="31"/>
-      <c r="IN7" s="31"/>
-      <c r="IO7" s="31"/>
-      <c r="IP7" s="31"/>
-      <c r="IQ7" s="31"/>
-      <c r="IR7" s="31"/>
-      <c r="IS7" s="31"/>
-      <c r="IT7" s="31"/>
-      <c r="IU7" s="31"/>
-      <c r="IV7" s="31"/>
-      <c r="IW7" s="31"/>
-      <c r="IX7" s="31"/>
-      <c r="IY7" s="31"/>
-      <c r="IZ7" s="31"/>
-      <c r="JA7" s="31"/>
-      <c r="JB7" s="31"/>
-      <c r="JC7" s="31"/>
-      <c r="JD7" s="31"/>
-      <c r="JE7" s="31"/>
-      <c r="JF7" s="31"/>
-      <c r="JG7" s="31"/>
-      <c r="JH7" s="31"/>
-      <c r="JI7" s="31"/>
-      <c r="JJ7" s="31"/>
-      <c r="JK7" s="31"/>
-      <c r="JL7" s="31"/>
-      <c r="JM7" s="31"/>
-      <c r="JN7" s="31"/>
-      <c r="JO7" s="31"/>
-      <c r="JP7" s="52"/>
-      <c r="JQ7" s="52"/>
-      <c r="JR7" s="52"/>
-      <c r="JS7" s="59"/>
-      <c r="JT7" s="59"/>
-      <c r="JU7" s="59"/>
-      <c r="JV7" s="59"/>
-      <c r="JW7" s="59"/>
-      <c r="JX7" s="59"/>
-      <c r="JY7" s="59"/>
-      <c r="JZ7" s="30">
-        <f>SUM(BP7:BQ7)</f>
+      <c r="BY7" s="58"/>
+      <c r="BZ7" s="58"/>
+      <c r="CA7" s="58"/>
+      <c r="CB7" s="58"/>
+      <c r="CC7" s="58"/>
+      <c r="CD7" s="58"/>
+      <c r="CE7" s="58"/>
+      <c r="CF7" s="58"/>
+      <c r="CG7" s="58"/>
+      <c r="CH7" s="58"/>
+      <c r="CI7" s="58"/>
+      <c r="CJ7" s="58"/>
+      <c r="CK7" s="58"/>
+      <c r="CL7" s="58"/>
+      <c r="CM7" s="58"/>
+      <c r="CN7" s="58"/>
+      <c r="CO7" s="58"/>
+      <c r="CP7" s="58"/>
+      <c r="CQ7" s="58"/>
+      <c r="CR7" s="58"/>
+      <c r="CS7" s="58"/>
+      <c r="CT7" s="58"/>
+      <c r="CU7" s="58"/>
+      <c r="CV7" s="58"/>
+      <c r="CW7" s="58"/>
+      <c r="CX7" s="58"/>
+      <c r="CY7" s="58"/>
+      <c r="CZ7" s="58"/>
+      <c r="DA7" s="58"/>
+      <c r="DB7" s="58"/>
+      <c r="DC7" s="58"/>
+      <c r="DD7" s="58"/>
+      <c r="DE7" s="58"/>
+      <c r="DF7" s="58"/>
+      <c r="DG7" s="58"/>
+      <c r="DH7" s="58"/>
+      <c r="DI7" s="58"/>
+      <c r="DJ7" s="58"/>
+      <c r="DK7" s="58"/>
+      <c r="DL7" s="58"/>
+      <c r="DM7" s="58"/>
+      <c r="DN7" s="58"/>
+      <c r="DO7" s="58"/>
+      <c r="DP7" s="58"/>
+      <c r="DQ7" s="58"/>
+      <c r="DR7" s="58"/>
+      <c r="DS7" s="58"/>
+      <c r="DT7" s="58"/>
+      <c r="DU7" s="58"/>
+      <c r="DV7" s="58"/>
+      <c r="DW7" s="58"/>
+      <c r="DX7" s="58"/>
+      <c r="DY7" s="58"/>
+      <c r="DZ7" s="58"/>
+      <c r="EA7" s="58"/>
+      <c r="EB7" s="58"/>
+      <c r="EC7" s="58"/>
+      <c r="ED7" s="58"/>
+      <c r="EE7" s="58"/>
+      <c r="EF7" s="58"/>
+      <c r="EG7" s="58"/>
+      <c r="EH7" s="58"/>
+      <c r="EI7" s="58"/>
+      <c r="EJ7" s="58"/>
+      <c r="EK7" s="58"/>
+      <c r="EL7" s="58"/>
+      <c r="EM7" s="58"/>
+      <c r="EN7" s="58"/>
+      <c r="EO7" s="58"/>
+      <c r="EP7" s="58"/>
+      <c r="EQ7" s="58"/>
+      <c r="ER7" s="58"/>
+      <c r="ES7" s="58"/>
+      <c r="ET7" s="58"/>
+      <c r="EU7" s="58"/>
+      <c r="EV7" s="58"/>
+      <c r="EW7" s="58"/>
+      <c r="EX7" s="58"/>
+      <c r="EY7" s="58"/>
+      <c r="EZ7" s="58"/>
+      <c r="FA7" s="58"/>
+      <c r="FB7" s="58"/>
+      <c r="FC7" s="58"/>
+      <c r="FD7" s="58"/>
+      <c r="FE7" s="58"/>
+      <c r="FF7" s="58"/>
+      <c r="FG7" s="58"/>
+      <c r="FH7" s="58"/>
+      <c r="FI7" s="58"/>
+      <c r="FJ7" s="58"/>
+      <c r="FK7" s="58"/>
+      <c r="FL7" s="58"/>
+      <c r="FM7" s="58"/>
+      <c r="FN7" s="58"/>
+      <c r="FO7" s="58"/>
+      <c r="FP7" s="58"/>
+      <c r="FQ7" s="58"/>
+      <c r="FR7" s="58"/>
+      <c r="FS7" s="58"/>
+      <c r="FT7" s="58"/>
+      <c r="FU7" s="58"/>
+      <c r="FV7" s="58"/>
+      <c r="FW7" s="58"/>
+      <c r="FX7" s="58"/>
+      <c r="FY7" s="58"/>
+      <c r="FZ7" s="58"/>
+      <c r="GA7" s="58"/>
+      <c r="GB7" s="58"/>
+      <c r="GC7" s="58"/>
+      <c r="GD7" s="58"/>
+      <c r="GE7" s="58"/>
+      <c r="GF7" s="58"/>
+      <c r="GG7" s="58"/>
+      <c r="GH7" s="58"/>
+      <c r="GI7" s="58"/>
+      <c r="GJ7" s="58"/>
+      <c r="GK7" s="58"/>
+      <c r="GL7" s="58"/>
+      <c r="GM7" s="58"/>
+      <c r="GN7" s="58"/>
+      <c r="GO7" s="58"/>
+      <c r="GP7" s="58"/>
+      <c r="GQ7" s="58"/>
+      <c r="GR7" s="58"/>
+      <c r="GS7" s="58"/>
+      <c r="GT7" s="58"/>
+      <c r="GU7" s="58"/>
+      <c r="GV7" s="58"/>
+      <c r="GW7" s="58"/>
+      <c r="GX7" s="58"/>
+      <c r="GY7" s="58"/>
+      <c r="GZ7" s="58"/>
+      <c r="HA7" s="58"/>
+      <c r="HB7" s="58"/>
+      <c r="HC7" s="58"/>
+      <c r="HD7" s="58"/>
+      <c r="HE7" s="58"/>
+      <c r="HF7" s="58"/>
+      <c r="HG7" s="58"/>
+      <c r="HH7" s="58"/>
+      <c r="HI7" s="58"/>
+      <c r="HJ7" s="58"/>
+      <c r="HK7" s="58"/>
+      <c r="HL7" s="58"/>
+      <c r="HM7" s="58"/>
+      <c r="HN7" s="58"/>
+      <c r="HO7" s="58"/>
+      <c r="HP7" s="58"/>
+      <c r="HQ7" s="58"/>
+      <c r="HR7" s="58"/>
+      <c r="HS7" s="58"/>
+      <c r="HT7" s="58"/>
+      <c r="HU7" s="58"/>
+      <c r="HV7" s="58"/>
+      <c r="HW7" s="58"/>
+      <c r="HX7" s="58"/>
+      <c r="HY7" s="58"/>
+      <c r="HZ7" s="58"/>
+      <c r="IA7" s="58"/>
+      <c r="IB7" s="58"/>
+      <c r="IC7" s="58"/>
+      <c r="ID7" s="58"/>
+      <c r="IE7" s="58"/>
+      <c r="IF7" s="58"/>
+      <c r="IG7" s="58"/>
+      <c r="IH7" s="58"/>
+      <c r="II7" s="58"/>
+      <c r="IJ7" s="58"/>
+      <c r="IK7" s="58"/>
+      <c r="IL7" s="58"/>
+      <c r="IM7" s="58"/>
+      <c r="IN7" s="58"/>
+      <c r="IO7" s="58"/>
+      <c r="IP7" s="58"/>
+      <c r="IQ7" s="58"/>
+      <c r="IR7" s="58"/>
+      <c r="IS7" s="58"/>
+      <c r="IT7" s="58"/>
+      <c r="IU7" s="58"/>
+      <c r="IV7" s="58"/>
+      <c r="IW7" s="58"/>
+      <c r="IX7" s="58"/>
+      <c r="IY7" s="58"/>
+      <c r="IZ7" s="58"/>
+      <c r="JA7" s="58"/>
+      <c r="JB7" s="58"/>
+      <c r="JC7" s="58"/>
+      <c r="JD7" s="58"/>
+      <c r="JE7" s="58"/>
+      <c r="JF7" s="58"/>
+      <c r="JG7" s="58"/>
+      <c r="JH7" s="58"/>
+      <c r="JI7" s="58"/>
+      <c r="JJ7" s="58"/>
+      <c r="JK7" s="58"/>
+      <c r="JL7" s="58"/>
+      <c r="JM7" s="58"/>
+      <c r="JN7" s="58"/>
+      <c r="JO7" s="58"/>
+      <c r="JP7" s="53"/>
+      <c r="JQ7" s="53"/>
+      <c r="JR7" s="53"/>
+      <c r="JS7" s="64"/>
+      <c r="JT7" s="64"/>
+      <c r="JU7" s="64"/>
+      <c r="JV7" s="64"/>
+      <c r="JW7" s="64"/>
+      <c r="JX7" s="64"/>
+      <c r="JY7" s="64"/>
+      <c r="JZ7" s="63">
+        <f>BQ7</f>
         <v>0</v>
       </c>
-      <c r="KA7" s="30">
-        <f>SUM(CD7:CE7)+SUM(CR7:CS7)</f>
+      <c r="KA7" s="63">
+        <f>CE7+CS7</f>
         <v>0</v>
       </c>
-      <c r="KB7" s="30">
-        <f>SUM(DF7:DG7)+SUM(DT7:DU7)+SUM(EH7:EI7)+SUM(EV7:EW7)+SUM(FJ7:FK7)+SUM(FX7:FY7)</f>
+      <c r="KB7" s="63">
+        <f>DG7+DU7+EI7+EW7+FK7+FY7</f>
         <v>0</v>
       </c>
-      <c r="KC7" s="30">
-        <f>SUM(GL7:GM7)+SUM(IB7:IC7)</f>
+      <c r="KC7" s="63">
+        <f>GM7+IC7</f>
         <v>0</v>
       </c>
-      <c r="KD7" s="30">
+      <c r="KD7" s="63">
         <f>SUM(BL7:BQ7)</f>
         <v>0</v>
       </c>
-      <c r="KE7" s="30">
+      <c r="KE7" s="63">
         <f>SUM(CN7:CS7)+SUM(BZ7:CE7)</f>
         <v>0</v>
       </c>
-      <c r="KF7" s="30">
+      <c r="KF7" s="63">
         <f>SUM(DB7:DG7)+SUM(DP7:DU7)+SUM(ED7:EI7)+SUM(ER7:EW7)+SUM(FF7:FK7)+SUM(FT7:FY7)</f>
         <v>0</v>
       </c>
-      <c r="KG7" s="30">
+      <c r="KG7" s="63">
         <f>SUM(GH7:GM7)+SUM(HX7:IC7)</f>
         <v>0</v>
       </c>
-      <c r="KH7" s="28"/>
-      <c r="KI7" s="28"/>
-      <c r="KJ7" s="28"/>
-      <c r="KK7" s="28"/>
-      <c r="KL7" s="28"/>
+      <c r="KH7" s="48"/>
+      <c r="KI7" s="48"/>
+      <c r="KJ7" s="48"/>
+      <c r="KK7" s="48"/>
+      <c r="KL7" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:300">
+      <c r="A8" s="25"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="26"/>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="23"/>
+      <c r="AB8" s="26"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="26"/>
+      <c r="AE8" s="26"/>
+      <c r="AF8" s="23"/>
+      <c r="AG8" s="23"/>
+      <c r="AH8" s="23"/>
+      <c r="AI8" s="23"/>
+      <c r="AJ8" s="23"/>
+      <c r="AK8" s="23"/>
+      <c r="AL8" s="23"/>
+      <c r="AM8" s="23"/>
+      <c r="AN8" s="27"/>
+      <c r="AO8" s="27"/>
+      <c r="AP8" s="27"/>
+      <c r="AQ8" s="27"/>
+      <c r="AR8" s="27"/>
+      <c r="AS8" s="23"/>
+      <c r="AT8" s="23"/>
+      <c r="AU8" s="23"/>
+      <c r="AV8" s="23"/>
+      <c r="AW8" s="23"/>
+      <c r="AX8" s="23"/>
+      <c r="AY8" s="23"/>
+      <c r="AZ8" s="23"/>
+      <c r="BA8" s="23"/>
+      <c r="BB8" s="23"/>
+      <c r="BC8" s="23"/>
+      <c r="BD8" s="23"/>
+      <c r="BE8" s="23"/>
+      <c r="BF8" s="23"/>
+      <c r="BG8" s="23"/>
+      <c r="BH8" s="23"/>
+      <c r="BI8" s="23"/>
+      <c r="BJ8" s="23"/>
+      <c r="BK8" s="23"/>
+      <c r="BL8" s="23"/>
+      <c r="BM8" s="23"/>
+      <c r="BN8" s="23"/>
+      <c r="BO8" s="23"/>
+      <c r="BP8" s="23"/>
+      <c r="BQ8" s="23"/>
+      <c r="BR8" s="23"/>
+      <c r="BS8" s="23"/>
+      <c r="BT8" s="23"/>
+      <c r="BU8" s="23"/>
+      <c r="BV8" s="23"/>
+      <c r="BW8" s="23"/>
+      <c r="BX8" s="23"/>
+      <c r="BY8" s="23"/>
+      <c r="BZ8" s="23"/>
+      <c r="CA8" s="23"/>
+      <c r="CB8" s="23"/>
+      <c r="CC8" s="23"/>
+      <c r="CD8" s="23"/>
+      <c r="CE8" s="23"/>
+      <c r="CF8" s="23"/>
+      <c r="CG8" s="23"/>
+      <c r="CH8" s="23"/>
+      <c r="CI8" s="23"/>
+      <c r="CJ8" s="23"/>
+      <c r="CK8" s="23"/>
+      <c r="CL8" s="23"/>
+      <c r="CM8" s="23"/>
+      <c r="CN8" s="23"/>
+      <c r="CO8" s="23"/>
+      <c r="CP8" s="23"/>
+      <c r="CQ8" s="23"/>
+      <c r="CR8" s="23"/>
+      <c r="CS8" s="23"/>
+      <c r="CT8" s="23"/>
+      <c r="CU8" s="23"/>
+      <c r="CV8" s="23"/>
+      <c r="CW8" s="23"/>
+      <c r="CX8" s="23"/>
+      <c r="CY8" s="23"/>
+      <c r="CZ8" s="23"/>
+      <c r="DA8" s="23"/>
+      <c r="DB8" s="23"/>
+      <c r="DC8" s="23"/>
+      <c r="DD8" s="23"/>
+      <c r="DE8" s="23"/>
+      <c r="DF8" s="23"/>
+      <c r="DG8" s="23"/>
+      <c r="DH8" s="23"/>
+      <c r="DI8" s="23"/>
+      <c r="DJ8" s="23"/>
+      <c r="DK8" s="23"/>
+      <c r="DL8" s="23"/>
+      <c r="DM8" s="23"/>
+      <c r="DN8" s="23"/>
+      <c r="DO8" s="23"/>
+      <c r="DP8" s="23"/>
+      <c r="DQ8" s="23"/>
+      <c r="DR8" s="23"/>
+      <c r="DS8" s="23"/>
+      <c r="DT8" s="23"/>
+      <c r="DU8" s="23"/>
+      <c r="DV8" s="23"/>
+      <c r="DW8" s="23"/>
+      <c r="DX8" s="23"/>
+      <c r="DY8" s="23"/>
+      <c r="DZ8" s="23"/>
+      <c r="EA8" s="23"/>
+      <c r="EB8" s="23"/>
+      <c r="EC8" s="23"/>
+      <c r="ED8" s="23"/>
+      <c r="EE8" s="23"/>
+      <c r="EF8" s="23"/>
+      <c r="EG8" s="23"/>
+      <c r="EH8" s="23"/>
+      <c r="EI8" s="23"/>
+      <c r="EJ8" s="23"/>
+      <c r="EK8" s="23"/>
+      <c r="EL8" s="23"/>
+      <c r="EM8" s="23"/>
+      <c r="EN8" s="23"/>
+      <c r="EO8" s="23"/>
+      <c r="EP8" s="23"/>
+      <c r="EQ8" s="23"/>
+      <c r="ER8" s="23"/>
+      <c r="ES8" s="23"/>
+      <c r="ET8" s="23"/>
+      <c r="EU8" s="23"/>
+      <c r="EV8" s="23"/>
+      <c r="EW8" s="23"/>
+      <c r="EX8" s="23"/>
+      <c r="EY8" s="23"/>
+      <c r="EZ8" s="23"/>
+      <c r="FA8" s="23"/>
+      <c r="FB8" s="23"/>
+      <c r="FC8" s="23"/>
+      <c r="FD8" s="23"/>
+      <c r="FE8" s="23"/>
+      <c r="FF8" s="23"/>
+      <c r="FG8" s="23"/>
+      <c r="FH8" s="23"/>
+      <c r="FI8" s="23"/>
+      <c r="FJ8" s="23"/>
+      <c r="FK8" s="23"/>
+      <c r="FL8" s="23"/>
+      <c r="FM8" s="23"/>
+      <c r="FN8" s="23"/>
+      <c r="FO8" s="23"/>
+      <c r="FP8" s="23"/>
+      <c r="FQ8" s="23"/>
+      <c r="FR8" s="23"/>
+      <c r="FS8" s="23"/>
+      <c r="FT8" s="23"/>
+      <c r="FU8" s="23"/>
+      <c r="FV8" s="23"/>
+      <c r="FW8" s="23"/>
+      <c r="FX8" s="23"/>
+      <c r="FY8" s="23"/>
+      <c r="FZ8" s="23"/>
+      <c r="GA8" s="23"/>
+      <c r="GB8" s="23"/>
+      <c r="GC8" s="23"/>
+      <c r="GD8" s="23"/>
+      <c r="GE8" s="23"/>
+      <c r="GF8" s="23"/>
+      <c r="GG8" s="23"/>
+      <c r="GH8" s="23"/>
+      <c r="GI8" s="23"/>
+      <c r="GJ8" s="23"/>
+      <c r="GK8" s="23"/>
+      <c r="GL8" s="23"/>
+      <c r="GM8" s="23"/>
+      <c r="GN8" s="23"/>
+      <c r="GO8" s="23"/>
+      <c r="GP8" s="23"/>
+      <c r="GQ8" s="23"/>
+      <c r="GR8" s="23"/>
+      <c r="GS8" s="23"/>
+      <c r="GT8" s="23"/>
+      <c r="GU8" s="23"/>
+      <c r="GV8" s="23"/>
+      <c r="GW8" s="23"/>
+      <c r="GX8" s="23"/>
+      <c r="GY8" s="23"/>
+      <c r="GZ8" s="23"/>
+      <c r="HA8" s="23"/>
+      <c r="HB8" s="23"/>
+      <c r="HC8" s="23"/>
+      <c r="HD8" s="23"/>
+      <c r="HE8" s="23"/>
+      <c r="HF8" s="23"/>
+      <c r="HG8" s="23"/>
+      <c r="HH8" s="23"/>
+      <c r="HI8" s="23"/>
+      <c r="HJ8" s="23"/>
+      <c r="HK8" s="23"/>
+      <c r="HL8" s="23"/>
+      <c r="HM8" s="23"/>
+      <c r="HN8" s="23"/>
+      <c r="HO8" s="23"/>
+      <c r="HP8" s="23"/>
+      <c r="HQ8" s="23"/>
+      <c r="HR8" s="23"/>
+      <c r="HS8" s="23"/>
+      <c r="HT8" s="23"/>
+      <c r="HU8" s="23"/>
+      <c r="HV8" s="23"/>
+      <c r="HW8" s="23"/>
+      <c r="HX8" s="23"/>
+      <c r="HY8" s="23"/>
+      <c r="HZ8" s="23"/>
+      <c r="IA8" s="23"/>
+      <c r="IB8" s="23"/>
+      <c r="IC8" s="23"/>
+      <c r="ID8" s="23"/>
+      <c r="IE8" s="23"/>
+      <c r="IF8" s="23"/>
+      <c r="IG8" s="23"/>
+      <c r="IH8" s="23"/>
+      <c r="II8" s="23"/>
+      <c r="IJ8" s="23"/>
+      <c r="IK8" s="23"/>
+      <c r="IL8" s="23"/>
+      <c r="IM8" s="23"/>
+      <c r="IN8" s="23"/>
+      <c r="IO8" s="23"/>
+      <c r="IP8" s="23"/>
+      <c r="IQ8" s="23"/>
+      <c r="IR8" s="23"/>
+      <c r="IS8" s="23"/>
+      <c r="IT8" s="23"/>
+      <c r="IU8" s="23"/>
+      <c r="IV8" s="23"/>
+      <c r="IW8" s="23"/>
+      <c r="IX8" s="23"/>
+      <c r="IY8" s="23"/>
+      <c r="IZ8" s="23"/>
+      <c r="JA8" s="23"/>
+      <c r="JB8" s="23"/>
+      <c r="JC8" s="23"/>
+      <c r="JD8" s="23"/>
+      <c r="JE8" s="23"/>
+      <c r="JF8" s="23"/>
+      <c r="JG8" s="23"/>
+      <c r="JH8" s="23"/>
+      <c r="JI8" s="23"/>
+      <c r="JJ8" s="23"/>
+      <c r="JK8" s="23"/>
+      <c r="JL8" s="23"/>
+      <c r="JM8" s="23"/>
+      <c r="JN8" s="23"/>
+      <c r="JO8" s="23"/>
+      <c r="JP8" s="23"/>
+      <c r="JQ8" s="23"/>
+      <c r="JR8" s="23"/>
+      <c r="JS8" s="47"/>
+      <c r="JT8" s="47"/>
+      <c r="JU8" s="47"/>
+      <c r="JV8" s="47"/>
+      <c r="JW8" s="47"/>
+      <c r="JX8" s="47"/>
+      <c r="JY8" s="47"/>
+      <c r="JZ8" s="23"/>
+      <c r="KA8" s="23"/>
+      <c r="KB8" s="23"/>
+      <c r="KC8" s="23"/>
+      <c r="KD8" s="23"/>
+      <c r="KE8" s="23"/>
+      <c r="KF8" s="23"/>
+      <c r="KG8" s="23"/>
+      <c r="KH8" s="48"/>
+      <c r="KI8" s="48"/>
+      <c r="KJ8" s="48"/>
+      <c r="KK8" s="48"/>
+      <c r="KL8" s="48" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:300">
+      <c r="A9" s="25"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="23"/>
+      <c r="AA9" s="23"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="23"/>
+      <c r="AD9" s="26"/>
+      <c r="AE9" s="26"/>
+      <c r="AF9" s="23"/>
+      <c r="AG9" s="23"/>
+      <c r="AH9" s="23"/>
+      <c r="AI9" s="23"/>
+      <c r="AJ9" s="23"/>
+      <c r="AK9" s="23"/>
+      <c r="AL9" s="23"/>
+      <c r="AM9" s="23"/>
+      <c r="AN9" s="27"/>
+      <c r="AO9" s="27"/>
+      <c r="AP9" s="27"/>
+      <c r="AQ9" s="27"/>
+      <c r="AR9" s="27"/>
+      <c r="AS9" s="23"/>
+      <c r="AT9" s="23"/>
+      <c r="AU9" s="23"/>
+      <c r="AV9" s="23"/>
+      <c r="AW9" s="23"/>
+      <c r="AX9" s="23"/>
+      <c r="AY9" s="23"/>
+      <c r="AZ9" s="23"/>
+      <c r="BA9" s="23"/>
+      <c r="BB9" s="23"/>
+      <c r="BC9" s="23"/>
+      <c r="BD9" s="23"/>
+      <c r="BE9" s="23"/>
+      <c r="BF9" s="23"/>
+      <c r="BG9" s="23"/>
+      <c r="BH9" s="23"/>
+      <c r="BI9" s="23"/>
+      <c r="BJ9" s="23"/>
+      <c r="BK9" s="23"/>
+      <c r="BL9" s="23"/>
+      <c r="BM9" s="23"/>
+      <c r="BN9" s="23"/>
+      <c r="BO9" s="23"/>
+      <c r="BP9" s="23"/>
+      <c r="BQ9" s="23"/>
+      <c r="BR9" s="23"/>
+      <c r="BS9" s="23"/>
+      <c r="BT9" s="23"/>
+      <c r="BU9" s="23"/>
+      <c r="BV9" s="23"/>
+      <c r="BW9" s="23"/>
+      <c r="BX9" s="23"/>
+      <c r="BY9" s="23"/>
+      <c r="BZ9" s="23"/>
+      <c r="CA9" s="23"/>
+      <c r="CB9" s="23"/>
+      <c r="CC9" s="23"/>
+      <c r="CD9" s="23"/>
+      <c r="CE9" s="23"/>
+      <c r="CF9" s="23"/>
+      <c r="CG9" s="23"/>
+      <c r="CH9" s="23"/>
+      <c r="CI9" s="23"/>
+      <c r="CJ9" s="23"/>
+      <c r="CK9" s="23"/>
+      <c r="CL9" s="23"/>
+      <c r="CM9" s="23"/>
+      <c r="CN9" s="23"/>
+      <c r="CO9" s="23"/>
+      <c r="CP9" s="23"/>
+      <c r="CQ9" s="23"/>
+      <c r="CR9" s="23"/>
+      <c r="CS9" s="23"/>
+      <c r="CT9" s="23"/>
+      <c r="CU9" s="23"/>
+      <c r="CV9" s="23"/>
+      <c r="CW9" s="23"/>
+      <c r="CX9" s="23"/>
+      <c r="CY9" s="23"/>
+      <c r="CZ9" s="23"/>
+      <c r="DA9" s="23"/>
+      <c r="DB9" s="23"/>
+      <c r="DC9" s="23"/>
+      <c r="DD9" s="23"/>
+      <c r="DE9" s="23"/>
+      <c r="DF9" s="23"/>
+      <c r="DG9" s="23"/>
+      <c r="DH9" s="23"/>
+      <c r="DI9" s="23"/>
+      <c r="DJ9" s="23"/>
+      <c r="DK9" s="23"/>
+      <c r="DL9" s="23"/>
+      <c r="DM9" s="23"/>
+      <c r="DN9" s="23"/>
+      <c r="DO9" s="23"/>
+      <c r="DP9" s="23"/>
+      <c r="DQ9" s="23"/>
+      <c r="DR9" s="23"/>
+      <c r="DS9" s="23"/>
+      <c r="DT9" s="23"/>
+      <c r="DU9" s="23"/>
+      <c r="DV9" s="23"/>
+      <c r="DW9" s="23"/>
+      <c r="DX9" s="23"/>
+      <c r="DY9" s="23"/>
+      <c r="DZ9" s="23"/>
+      <c r="EA9" s="23"/>
+      <c r="EB9" s="23"/>
+      <c r="EC9" s="23"/>
+      <c r="ED9" s="23"/>
+      <c r="EE9" s="23"/>
+      <c r="EF9" s="23"/>
+      <c r="EG9" s="23"/>
+      <c r="EH9" s="23"/>
+      <c r="EI9" s="23"/>
+      <c r="EJ9" s="23"/>
+      <c r="EK9" s="23"/>
+      <c r="EL9" s="23"/>
+      <c r="EM9" s="23"/>
+      <c r="EN9" s="23"/>
+      <c r="EO9" s="23"/>
+      <c r="EP9" s="23"/>
+      <c r="EQ9" s="23"/>
+      <c r="ER9" s="23"/>
+      <c r="ES9" s="23"/>
+      <c r="ET9" s="23"/>
+      <c r="EU9" s="23"/>
+      <c r="EV9" s="23"/>
+      <c r="EW9" s="23"/>
+      <c r="EX9" s="23"/>
+      <c r="EY9" s="23"/>
+      <c r="EZ9" s="23"/>
+      <c r="FA9" s="23"/>
+      <c r="FB9" s="23"/>
+      <c r="FC9" s="23"/>
+      <c r="FD9" s="23"/>
+      <c r="FE9" s="23"/>
+      <c r="FF9" s="23"/>
+      <c r="FG9" s="23"/>
+      <c r="FH9" s="23"/>
+      <c r="FI9" s="23"/>
+      <c r="FJ9" s="23"/>
+      <c r="FK9" s="23"/>
+      <c r="FL9" s="23"/>
+      <c r="FM9" s="23"/>
+      <c r="FN9" s="23"/>
+      <c r="FO9" s="23"/>
+      <c r="FP9" s="23"/>
+      <c r="FQ9" s="23"/>
+      <c r="FR9" s="23"/>
+      <c r="FS9" s="23"/>
+      <c r="FT9" s="23"/>
+      <c r="FU9" s="23"/>
+      <c r="FV9" s="23"/>
+      <c r="FW9" s="23"/>
+      <c r="FX9" s="23"/>
+      <c r="FY9" s="23"/>
+      <c r="FZ9" s="23"/>
+      <c r="GA9" s="23"/>
+      <c r="GB9" s="23"/>
+      <c r="GC9" s="23"/>
+      <c r="GD9" s="23"/>
+      <c r="GE9" s="23"/>
+      <c r="GF9" s="23"/>
+      <c r="GG9" s="23"/>
+      <c r="GH9" s="23"/>
+      <c r="GI9" s="23"/>
+      <c r="GJ9" s="23"/>
+      <c r="GK9" s="23"/>
+      <c r="GL9" s="23"/>
+      <c r="GM9" s="23"/>
+      <c r="GN9" s="23"/>
+      <c r="GO9" s="23"/>
+      <c r="GP9" s="23"/>
+      <c r="GQ9" s="23"/>
+      <c r="GR9" s="23"/>
+      <c r="GS9" s="23"/>
+      <c r="GT9" s="23"/>
+      <c r="GU9" s="23"/>
+      <c r="GV9" s="23"/>
+      <c r="GW9" s="23"/>
+      <c r="GX9" s="23"/>
+      <c r="GY9" s="23"/>
+      <c r="GZ9" s="23"/>
+      <c r="HA9" s="23"/>
+      <c r="HB9" s="23"/>
+      <c r="HC9" s="23"/>
+      <c r="HD9" s="23"/>
+      <c r="HE9" s="23"/>
+      <c r="HF9" s="23"/>
+      <c r="HG9" s="23"/>
+      <c r="HH9" s="23"/>
+      <c r="HI9" s="23"/>
+      <c r="HJ9" s="23"/>
+      <c r="HK9" s="23"/>
+      <c r="HL9" s="23"/>
+      <c r="HM9" s="23"/>
+      <c r="HN9" s="23"/>
+      <c r="HO9" s="23"/>
+      <c r="HP9" s="23"/>
+      <c r="HQ9" s="23"/>
+      <c r="HR9" s="23"/>
+      <c r="HS9" s="23"/>
+      <c r="HT9" s="23"/>
+      <c r="HU9" s="23"/>
+      <c r="HV9" s="23"/>
+      <c r="HW9" s="23"/>
+      <c r="HX9" s="23"/>
+      <c r="HY9" s="23"/>
+      <c r="HZ9" s="23"/>
+      <c r="IA9" s="23"/>
+      <c r="IB9" s="23"/>
+      <c r="IC9" s="23"/>
+      <c r="ID9" s="23"/>
+      <c r="IE9" s="23"/>
+      <c r="IF9" s="23"/>
+      <c r="IG9" s="23"/>
+      <c r="IH9" s="23"/>
+      <c r="II9" s="23"/>
+      <c r="IJ9" s="23"/>
+      <c r="IK9" s="23"/>
+      <c r="IL9" s="23"/>
+      <c r="IM9" s="23"/>
+      <c r="IN9" s="23"/>
+      <c r="IO9" s="23"/>
+      <c r="IP9" s="23"/>
+      <c r="IQ9" s="23"/>
+      <c r="IR9" s="23"/>
+      <c r="IS9" s="23"/>
+      <c r="IT9" s="23"/>
+      <c r="IU9" s="23"/>
+      <c r="IV9" s="23"/>
+      <c r="IW9" s="23"/>
+      <c r="IX9" s="23"/>
+      <c r="IY9" s="23"/>
+      <c r="IZ9" s="23"/>
+      <c r="JA9" s="23"/>
+      <c r="JB9" s="23"/>
+      <c r="JC9" s="23"/>
+      <c r="JD9" s="23"/>
+      <c r="JE9" s="23"/>
+      <c r="JF9" s="23"/>
+      <c r="JG9" s="23"/>
+      <c r="JH9" s="23"/>
+      <c r="JI9" s="23"/>
+      <c r="JJ9" s="23"/>
+      <c r="JK9" s="23"/>
+      <c r="JL9" s="23"/>
+      <c r="JM9" s="23"/>
+      <c r="JN9" s="23"/>
+      <c r="JO9" s="23"/>
+      <c r="JP9" s="23"/>
+      <c r="JQ9" s="23"/>
+      <c r="JR9" s="23"/>
+      <c r="JS9" s="47"/>
+      <c r="JT9" s="47"/>
+      <c r="JU9" s="47"/>
+      <c r="JV9" s="47"/>
+      <c r="JW9" s="47"/>
+      <c r="JX9" s="47"/>
+      <c r="JY9" s="47"/>
+      <c r="JZ9" s="23"/>
+      <c r="KA9" s="23"/>
+      <c r="KB9" s="23"/>
+      <c r="KC9" s="23"/>
+      <c r="KD9" s="23"/>
+      <c r="KE9" s="23"/>
+      <c r="KF9" s="23"/>
+      <c r="KG9" s="23"/>
+      <c r="KH9" s="48"/>
+      <c r="KI9" s="48"/>
+      <c r="KJ9" s="48"/>
+      <c r="KK9" s="48"/>
+      <c r="KL9" s="48" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:300">
+      <c r="A10" s="25"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
+      <c r="X10" s="26"/>
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="23"/>
+      <c r="AA10" s="23"/>
+      <c r="AB10" s="26"/>
+      <c r="AC10" s="23"/>
+      <c r="AD10" s="26"/>
+      <c r="AE10" s="26"/>
+      <c r="AF10" s="23"/>
+      <c r="AG10" s="23"/>
+      <c r="AH10" s="23"/>
+      <c r="AI10" s="23"/>
+      <c r="AJ10" s="23"/>
+      <c r="AK10" s="23"/>
+      <c r="AL10" s="23"/>
+      <c r="AM10" s="23"/>
+      <c r="AN10" s="27"/>
+      <c r="AO10" s="27"/>
+      <c r="AP10" s="27"/>
+      <c r="AQ10" s="27"/>
+      <c r="AR10" s="27"/>
+      <c r="AS10" s="23"/>
+      <c r="AT10" s="23"/>
+      <c r="AU10" s="23"/>
+      <c r="AV10" s="23"/>
+      <c r="AW10" s="23"/>
+      <c r="AX10" s="23"/>
+      <c r="AY10" s="23"/>
+      <c r="AZ10" s="23"/>
+      <c r="BA10" s="23"/>
+      <c r="BB10" s="23"/>
+      <c r="BC10" s="23"/>
+      <c r="BD10" s="23"/>
+      <c r="BE10" s="23"/>
+      <c r="BF10" s="23"/>
+      <c r="BG10" s="23"/>
+      <c r="BH10" s="23"/>
+      <c r="BI10" s="23"/>
+      <c r="BJ10" s="23"/>
+      <c r="BK10" s="23"/>
+      <c r="BL10" s="23"/>
+      <c r="BM10" s="23"/>
+      <c r="BN10" s="23"/>
+      <c r="BO10" s="23"/>
+      <c r="BP10" s="23"/>
+      <c r="BQ10" s="23"/>
+      <c r="BR10" s="23"/>
+      <c r="BS10" s="23"/>
+      <c r="BT10" s="23"/>
+      <c r="BU10" s="23"/>
+      <c r="BV10" s="23"/>
+      <c r="BW10" s="23"/>
+      <c r="BX10" s="23"/>
+      <c r="BY10" s="23"/>
+      <c r="BZ10" s="23"/>
+      <c r="CA10" s="23"/>
+      <c r="CB10" s="23"/>
+      <c r="CC10" s="23"/>
+      <c r="CD10" s="23"/>
+      <c r="CE10" s="23"/>
+      <c r="CF10" s="23"/>
+      <c r="CG10" s="23"/>
+      <c r="CH10" s="23"/>
+      <c r="CI10" s="23"/>
+      <c r="CJ10" s="23"/>
+      <c r="CK10" s="23"/>
+      <c r="CL10" s="23"/>
+      <c r="CM10" s="23"/>
+      <c r="CN10" s="23"/>
+      <c r="CO10" s="23"/>
+      <c r="CP10" s="23"/>
+      <c r="CQ10" s="23"/>
+      <c r="CR10" s="23"/>
+      <c r="CS10" s="23"/>
+      <c r="CT10" s="23"/>
+      <c r="CU10" s="23"/>
+      <c r="CV10" s="23"/>
+      <c r="CW10" s="23"/>
+      <c r="CX10" s="23"/>
+      <c r="CY10" s="23"/>
+      <c r="CZ10" s="23"/>
+      <c r="DA10" s="23"/>
+      <c r="DB10" s="23"/>
+      <c r="DC10" s="23"/>
+      <c r="DD10" s="23"/>
+      <c r="DE10" s="23"/>
+      <c r="DF10" s="23"/>
+      <c r="DG10" s="23"/>
+      <c r="DH10" s="23"/>
+      <c r="DI10" s="23"/>
+      <c r="DJ10" s="23"/>
+      <c r="DK10" s="23"/>
+      <c r="DL10" s="23"/>
+      <c r="DM10" s="23"/>
+      <c r="DN10" s="23"/>
+      <c r="DO10" s="23"/>
+      <c r="DP10" s="23"/>
+      <c r="DQ10" s="23"/>
+      <c r="DR10" s="23"/>
+      <c r="DS10" s="23"/>
+      <c r="DT10" s="23"/>
+      <c r="DU10" s="23"/>
+      <c r="DV10" s="23"/>
+      <c r="DW10" s="23"/>
+      <c r="DX10" s="23"/>
+      <c r="DY10" s="23"/>
+      <c r="DZ10" s="23"/>
+      <c r="EA10" s="23"/>
+      <c r="EB10" s="23"/>
+      <c r="EC10" s="23"/>
+      <c r="ED10" s="23"/>
+      <c r="EE10" s="23"/>
+      <c r="EF10" s="23"/>
+      <c r="EG10" s="23"/>
+      <c r="EH10" s="23"/>
+      <c r="EI10" s="23"/>
+      <c r="EJ10" s="23"/>
+      <c r="EK10" s="23"/>
+      <c r="EL10" s="23"/>
+      <c r="EM10" s="23"/>
+      <c r="EN10" s="23"/>
+      <c r="EO10" s="23"/>
+      <c r="EP10" s="23"/>
+      <c r="EQ10" s="23"/>
+      <c r="ER10" s="23"/>
+      <c r="ES10" s="23"/>
+      <c r="ET10" s="23"/>
+      <c r="EU10" s="23"/>
+      <c r="EV10" s="23"/>
+      <c r="EW10" s="23"/>
+      <c r="EX10" s="23"/>
+      <c r="EY10" s="23"/>
+      <c r="EZ10" s="23"/>
+      <c r="FA10" s="23"/>
+      <c r="FB10" s="23"/>
+      <c r="FC10" s="23"/>
+      <c r="FD10" s="23"/>
+      <c r="FE10" s="23"/>
+      <c r="FF10" s="23"/>
+      <c r="FG10" s="23"/>
+      <c r="FH10" s="23"/>
+      <c r="FI10" s="23"/>
+      <c r="FJ10" s="23"/>
+      <c r="FK10" s="23"/>
+      <c r="FL10" s="23"/>
+      <c r="FM10" s="23"/>
+      <c r="FN10" s="23"/>
+      <c r="FO10" s="23"/>
+      <c r="FP10" s="23"/>
+      <c r="FQ10" s="23"/>
+      <c r="FR10" s="23"/>
+      <c r="FS10" s="23"/>
+      <c r="FT10" s="23"/>
+      <c r="FU10" s="23"/>
+      <c r="FV10" s="23"/>
+      <c r="FW10" s="23"/>
+      <c r="FX10" s="23"/>
+      <c r="FY10" s="23"/>
+      <c r="FZ10" s="23"/>
+      <c r="GA10" s="23"/>
+      <c r="GB10" s="23"/>
+      <c r="GC10" s="23"/>
+      <c r="GD10" s="23"/>
+      <c r="GE10" s="23"/>
+      <c r="GF10" s="23"/>
+      <c r="GG10" s="23"/>
+      <c r="GH10" s="23"/>
+      <c r="GI10" s="23"/>
+      <c r="GJ10" s="23"/>
+      <c r="GK10" s="23"/>
+      <c r="GL10" s="23"/>
+      <c r="GM10" s="23"/>
+      <c r="GN10" s="23"/>
+      <c r="GO10" s="23"/>
+      <c r="GP10" s="23"/>
+      <c r="GQ10" s="23"/>
+      <c r="GR10" s="23"/>
+      <c r="GS10" s="23"/>
+      <c r="GT10" s="23"/>
+      <c r="GU10" s="23"/>
+      <c r="GV10" s="23"/>
+      <c r="GW10" s="23"/>
+      <c r="GX10" s="23"/>
+      <c r="GY10" s="23"/>
+      <c r="GZ10" s="23"/>
+      <c r="HA10" s="23"/>
+      <c r="HB10" s="23"/>
+      <c r="HC10" s="23"/>
+      <c r="HD10" s="23"/>
+      <c r="HE10" s="23"/>
+      <c r="HF10" s="23"/>
+      <c r="HG10" s="23"/>
+      <c r="HH10" s="23"/>
+      <c r="HI10" s="23"/>
+      <c r="HJ10" s="23"/>
+      <c r="HK10" s="23"/>
+      <c r="HL10" s="23"/>
+      <c r="HM10" s="23"/>
+      <c r="HN10" s="23"/>
+      <c r="HO10" s="23"/>
+      <c r="HP10" s="23"/>
+      <c r="HQ10" s="23"/>
+      <c r="HR10" s="23"/>
+      <c r="HS10" s="23"/>
+      <c r="HT10" s="23"/>
+      <c r="HU10" s="23"/>
+      <c r="HV10" s="23"/>
+      <c r="HW10" s="23"/>
+      <c r="HX10" s="23"/>
+      <c r="HY10" s="23"/>
+      <c r="HZ10" s="23"/>
+      <c r="IA10" s="23"/>
+      <c r="IB10" s="23"/>
+      <c r="IC10" s="23"/>
+      <c r="ID10" s="23"/>
+      <c r="IE10" s="23"/>
+      <c r="IF10" s="23"/>
+      <c r="IG10" s="23"/>
+      <c r="IH10" s="23"/>
+      <c r="II10" s="23"/>
+      <c r="IJ10" s="23"/>
+      <c r="IK10" s="23"/>
+      <c r="IL10" s="23"/>
+      <c r="IM10" s="23"/>
+      <c r="IN10" s="23"/>
+      <c r="IO10" s="23"/>
+      <c r="IP10" s="23"/>
+      <c r="IQ10" s="23"/>
+      <c r="IR10" s="23"/>
+      <c r="IS10" s="23"/>
+      <c r="IT10" s="23"/>
+      <c r="IU10" s="23"/>
+      <c r="IV10" s="23"/>
+      <c r="IW10" s="23"/>
+      <c r="IX10" s="23"/>
+      <c r="IY10" s="23"/>
+      <c r="IZ10" s="23"/>
+      <c r="JA10" s="23"/>
+      <c r="JB10" s="23"/>
+      <c r="JC10" s="23"/>
+      <c r="JD10" s="23"/>
+      <c r="JE10" s="23"/>
+      <c r="JF10" s="23"/>
+      <c r="JG10" s="23"/>
+      <c r="JH10" s="23"/>
+      <c r="JI10" s="23"/>
+      <c r="JJ10" s="23"/>
+      <c r="JK10" s="23"/>
+      <c r="JL10" s="23"/>
+      <c r="JM10" s="23"/>
+      <c r="JN10" s="23"/>
+      <c r="JO10" s="23"/>
+      <c r="JP10" s="23"/>
+      <c r="JQ10" s="23"/>
+      <c r="JR10" s="23"/>
+      <c r="JS10" s="47"/>
+      <c r="JT10" s="47"/>
+      <c r="JU10" s="47"/>
+      <c r="JV10" s="47"/>
+      <c r="JW10" s="47"/>
+      <c r="JX10" s="47"/>
+      <c r="JY10" s="47"/>
+      <c r="JZ10" s="23"/>
+      <c r="KA10" s="23"/>
+      <c r="KB10" s="23"/>
+      <c r="KC10" s="23"/>
+      <c r="KD10" s="23"/>
+      <c r="KE10" s="23"/>
+      <c r="KF10" s="23"/>
+      <c r="KG10" s="23"/>
+      <c r="KH10" s="48"/>
+      <c r="KI10" s="48"/>
+      <c r="KJ10" s="48"/>
+      <c r="KK10" s="48"/>
+      <c r="KL10" s="48" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:300">
+      <c r="A11" s="25"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="23"/>
+      <c r="AA11" s="23"/>
+      <c r="AB11" s="26"/>
+      <c r="AC11" s="23"/>
+      <c r="AD11" s="26"/>
+      <c r="AE11" s="26"/>
+      <c r="AF11" s="23"/>
+      <c r="AG11" s="23"/>
+      <c r="AH11" s="23"/>
+      <c r="AI11" s="23"/>
+      <c r="AJ11" s="23"/>
+      <c r="AK11" s="23"/>
+      <c r="AL11" s="23"/>
+      <c r="AM11" s="23"/>
+      <c r="AN11" s="27"/>
+      <c r="AO11" s="27"/>
+      <c r="AP11" s="27"/>
+      <c r="AQ11" s="27"/>
+      <c r="AR11" s="27"/>
+      <c r="AS11" s="23"/>
+      <c r="AT11" s="23"/>
+      <c r="AU11" s="23"/>
+      <c r="AV11" s="23"/>
+      <c r="AW11" s="23"/>
+      <c r="AX11" s="23"/>
+      <c r="AY11" s="23"/>
+      <c r="AZ11" s="23"/>
+      <c r="BA11" s="23"/>
+      <c r="BB11" s="23"/>
+      <c r="BC11" s="23"/>
+      <c r="BD11" s="23"/>
+      <c r="BE11" s="23"/>
+      <c r="BF11" s="23"/>
+      <c r="BG11" s="23"/>
+      <c r="BH11" s="23"/>
+      <c r="BI11" s="23"/>
+      <c r="BJ11" s="23"/>
+      <c r="BK11" s="23"/>
+      <c r="BL11" s="23"/>
+      <c r="BM11" s="23"/>
+      <c r="BN11" s="23"/>
+      <c r="BO11" s="23"/>
+      <c r="BP11" s="23"/>
+      <c r="BQ11" s="23"/>
+      <c r="BR11" s="23"/>
+      <c r="BS11" s="23"/>
+      <c r="BT11" s="23"/>
+      <c r="BU11" s="23"/>
+      <c r="BV11" s="23"/>
+      <c r="BW11" s="23"/>
+      <c r="BX11" s="23"/>
+      <c r="BY11" s="23"/>
+      <c r="BZ11" s="23"/>
+      <c r="CA11" s="23"/>
+      <c r="CB11" s="23"/>
+      <c r="CC11" s="23"/>
+      <c r="CD11" s="23"/>
+      <c r="CE11" s="23"/>
+      <c r="CF11" s="23"/>
+      <c r="CG11" s="23"/>
+      <c r="CH11" s="23"/>
+      <c r="CI11" s="23"/>
+      <c r="CJ11" s="23"/>
+      <c r="CK11" s="23"/>
+      <c r="CL11" s="23"/>
+      <c r="CM11" s="23"/>
+      <c r="CN11" s="23"/>
+      <c r="CO11" s="23"/>
+      <c r="CP11" s="23"/>
+      <c r="CQ11" s="23"/>
+      <c r="CR11" s="23"/>
+      <c r="CS11" s="23"/>
+      <c r="CT11" s="23"/>
+      <c r="CU11" s="23"/>
+      <c r="CV11" s="23"/>
+      <c r="CW11" s="23"/>
+      <c r="CX11" s="23"/>
+      <c r="CY11" s="23"/>
+      <c r="CZ11" s="23"/>
+      <c r="DA11" s="23"/>
+      <c r="DB11" s="23"/>
+      <c r="DC11" s="23"/>
+      <c r="DD11" s="23"/>
+      <c r="DE11" s="23"/>
+      <c r="DF11" s="23"/>
+      <c r="DG11" s="23"/>
+      <c r="DH11" s="23"/>
+      <c r="DI11" s="23"/>
+      <c r="DJ11" s="23"/>
+      <c r="DK11" s="23"/>
+      <c r="DL11" s="23"/>
+      <c r="DM11" s="23"/>
+      <c r="DN11" s="23"/>
+      <c r="DO11" s="23"/>
+      <c r="DP11" s="23"/>
+      <c r="DQ11" s="23"/>
+      <c r="DR11" s="23"/>
+      <c r="DS11" s="23"/>
+      <c r="DT11" s="23"/>
+      <c r="DU11" s="23"/>
+      <c r="DV11" s="23"/>
+      <c r="DW11" s="23"/>
+      <c r="DX11" s="23"/>
+      <c r="DY11" s="23"/>
+      <c r="DZ11" s="23"/>
+      <c r="EA11" s="23"/>
+      <c r="EB11" s="23"/>
+      <c r="EC11" s="23"/>
+      <c r="ED11" s="23"/>
+      <c r="EE11" s="23"/>
+      <c r="EF11" s="23"/>
+      <c r="EG11" s="23"/>
+      <c r="EH11" s="23"/>
+      <c r="EI11" s="23"/>
+      <c r="EJ11" s="23"/>
+      <c r="EK11" s="23"/>
+      <c r="EL11" s="23"/>
+      <c r="EM11" s="23"/>
+      <c r="EN11" s="23"/>
+      <c r="EO11" s="23"/>
+      <c r="EP11" s="23"/>
+      <c r="EQ11" s="23"/>
+      <c r="ER11" s="23"/>
+      <c r="ES11" s="23"/>
+      <c r="ET11" s="23"/>
+      <c r="EU11" s="23"/>
+      <c r="EV11" s="23"/>
+      <c r="EW11" s="23"/>
+      <c r="EX11" s="23"/>
+      <c r="EY11" s="23"/>
+      <c r="EZ11" s="23"/>
+      <c r="FA11" s="23"/>
+      <c r="FB11" s="23"/>
+      <c r="FC11" s="23"/>
+      <c r="FD11" s="23"/>
+      <c r="FE11" s="23"/>
+      <c r="FF11" s="23"/>
+      <c r="FG11" s="23"/>
+      <c r="FH11" s="23"/>
+      <c r="FI11" s="23"/>
+      <c r="FJ11" s="23"/>
+      <c r="FK11" s="23"/>
+      <c r="FL11" s="23"/>
+      <c r="FM11" s="23"/>
+      <c r="FN11" s="23"/>
+      <c r="FO11" s="23"/>
+      <c r="FP11" s="23"/>
+      <c r="FQ11" s="23"/>
+      <c r="FR11" s="23"/>
+      <c r="FS11" s="23"/>
+      <c r="FT11" s="23"/>
+      <c r="FU11" s="23"/>
+      <c r="FV11" s="23"/>
+      <c r="FW11" s="23"/>
+      <c r="FX11" s="23"/>
+      <c r="FY11" s="23"/>
+      <c r="FZ11" s="23"/>
+      <c r="GA11" s="23"/>
+      <c r="GB11" s="23"/>
+      <c r="GC11" s="23"/>
+      <c r="GD11" s="23"/>
+      <c r="GE11" s="23"/>
+      <c r="GF11" s="23"/>
+      <c r="GG11" s="23"/>
+      <c r="GH11" s="23"/>
+      <c r="GI11" s="23"/>
+      <c r="GJ11" s="23"/>
+      <c r="GK11" s="23"/>
+      <c r="GL11" s="23"/>
+      <c r="GM11" s="23"/>
+      <c r="GN11" s="23"/>
+      <c r="GO11" s="23"/>
+      <c r="GP11" s="23"/>
+      <c r="GQ11" s="23"/>
+      <c r="GR11" s="23"/>
+      <c r="GS11" s="23"/>
+      <c r="GT11" s="23"/>
+      <c r="GU11" s="23"/>
+      <c r="GV11" s="23"/>
+      <c r="GW11" s="23"/>
+      <c r="GX11" s="23"/>
+      <c r="GY11" s="23"/>
+      <c r="GZ11" s="23"/>
+      <c r="HA11" s="23"/>
+      <c r="HB11" s="23"/>
+      <c r="HC11" s="23"/>
+      <c r="HD11" s="23"/>
+      <c r="HE11" s="23"/>
+      <c r="HF11" s="23"/>
+      <c r="HG11" s="23"/>
+      <c r="HH11" s="23"/>
+      <c r="HI11" s="23"/>
+      <c r="HJ11" s="23"/>
+      <c r="HK11" s="23"/>
+      <c r="HL11" s="23"/>
+      <c r="HM11" s="23"/>
+      <c r="HN11" s="23"/>
+      <c r="HO11" s="23"/>
+      <c r="HP11" s="23"/>
+      <c r="HQ11" s="23"/>
+      <c r="HR11" s="23"/>
+      <c r="HS11" s="23"/>
+      <c r="HT11" s="23"/>
+      <c r="HU11" s="23"/>
+      <c r="HV11" s="23"/>
+      <c r="HW11" s="23"/>
+      <c r="HX11" s="23"/>
+      <c r="HY11" s="23"/>
+      <c r="HZ11" s="23"/>
+      <c r="IA11" s="23"/>
+      <c r="IB11" s="23"/>
+      <c r="IC11" s="23"/>
+      <c r="ID11" s="23"/>
+      <c r="IE11" s="23"/>
+      <c r="IF11" s="23"/>
+      <c r="IG11" s="23"/>
+      <c r="IH11" s="23"/>
+      <c r="II11" s="23"/>
+      <c r="IJ11" s="23"/>
+      <c r="IK11" s="23"/>
+      <c r="IL11" s="23"/>
+      <c r="IM11" s="23"/>
+      <c r="IN11" s="23"/>
+      <c r="IO11" s="23"/>
+      <c r="IP11" s="23"/>
+      <c r="IQ11" s="23"/>
+      <c r="IR11" s="23"/>
+      <c r="IS11" s="23"/>
+      <c r="IT11" s="23"/>
+      <c r="IU11" s="23"/>
+      <c r="IV11" s="23"/>
+      <c r="IW11" s="23"/>
+      <c r="IX11" s="23"/>
+      <c r="IY11" s="23"/>
+      <c r="IZ11" s="23"/>
+      <c r="JA11" s="23"/>
+      <c r="JB11" s="23"/>
+      <c r="JC11" s="23"/>
+      <c r="JD11" s="23"/>
+      <c r="JE11" s="23"/>
+      <c r="JF11" s="23"/>
+      <c r="JG11" s="23"/>
+      <c r="JH11" s="23"/>
+      <c r="JI11" s="23"/>
+      <c r="JJ11" s="23"/>
+      <c r="JK11" s="23"/>
+      <c r="JL11" s="23"/>
+      <c r="JM11" s="23"/>
+      <c r="JN11" s="23"/>
+      <c r="JO11" s="23"/>
+      <c r="JP11" s="23"/>
+      <c r="JQ11" s="23"/>
+      <c r="JR11" s="23"/>
+      <c r="JS11" s="47"/>
+      <c r="JT11" s="47"/>
+      <c r="JU11" s="47"/>
+      <c r="JV11" s="47"/>
+      <c r="JW11" s="47"/>
+      <c r="JX11" s="47"/>
+      <c r="JY11" s="47"/>
+      <c r="JZ11" s="23"/>
+      <c r="KA11" s="23"/>
+      <c r="KB11" s="23"/>
+      <c r="KC11" s="23"/>
+      <c r="KD11" s="23"/>
+      <c r="KE11" s="23"/>
+      <c r="KF11" s="23"/>
+      <c r="KG11" s="23"/>
+      <c r="KH11" s="48"/>
+      <c r="KI11" s="48"/>
+      <c r="KJ11" s="48"/>
+      <c r="KK11" s="48"/>
+      <c r="KL11" s="48" t="s">
+        <v>340</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A6:KL6"/>
+  <autoFilter ref="A6:KK6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="32">
-    <mergeCell ref="AM4:AN5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:D5"/>
-    <mergeCell ref="E4:J5"/>
-    <mergeCell ref="K4:O5"/>
-    <mergeCell ref="P4:T5"/>
-    <mergeCell ref="U4:AB5"/>
-    <mergeCell ref="AC4:AI5"/>
-    <mergeCell ref="AJ4:AL5"/>
+    <mergeCell ref="KH4:KJ5"/>
+    <mergeCell ref="JZ4:KG4"/>
+    <mergeCell ref="JZ5:KC5"/>
+    <mergeCell ref="KD5:KG5"/>
+    <mergeCell ref="GU4:HH4"/>
+    <mergeCell ref="HI4:HV4"/>
+    <mergeCell ref="HW4:IJ4"/>
+    <mergeCell ref="IK4:IX4"/>
+    <mergeCell ref="IY4:JL4"/>
+    <mergeCell ref="JM4:JY5"/>
     <mergeCell ref="GG4:GT4"/>
     <mergeCell ref="AO4:AR5"/>
     <mergeCell ref="AS4:BJ5"/>
@@ -5444,36 +6686,39 @@
     <mergeCell ref="EQ4:FD4"/>
     <mergeCell ref="FE4:FR4"/>
     <mergeCell ref="FS4:GF4"/>
-    <mergeCell ref="KH4:KK5"/>
-    <mergeCell ref="JZ4:KG4"/>
-    <mergeCell ref="JZ5:KC5"/>
-    <mergeCell ref="KD5:KG5"/>
-    <mergeCell ref="GU4:HH4"/>
-    <mergeCell ref="HI4:HV4"/>
-    <mergeCell ref="HW4:IJ4"/>
-    <mergeCell ref="IK4:IX4"/>
-    <mergeCell ref="IY4:JL4"/>
-    <mergeCell ref="JM4:JY5"/>
+    <mergeCell ref="AM4:AN5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:D5"/>
+    <mergeCell ref="E4:J5"/>
+    <mergeCell ref="K4:O5"/>
+    <mergeCell ref="P4:T5"/>
+    <mergeCell ref="U4:AB5"/>
+    <mergeCell ref="AC4:AI5"/>
+    <mergeCell ref="AJ4:AL5"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>
   </conditionalFormatting>
-  <dataValidations count="4">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR7">
+  <dataValidations count="5">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>36526</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KI7">
-      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete, No Delivery pre 2021 "</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH8:KJ11" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>$KL$7:$KL$11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KK7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH7 KJ7" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KK7" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"NGSA, WEM, FCRM Operational Framework, Other, Unknown/TBC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH7 KJ7">
-      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete,"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KI7" xr:uid="{00000000-0002-0000-0000-000004000000}">
+      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete, No Delivery pre 2021 "</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="10" orientation="landscape"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="10" orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[PM-343] Update FCERM1 spreadsheet (#235)
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -1,38 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssargeant\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthall/Work/pafs/pafs_core/lib/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84F3FAD-9F25-3A49-9B3B-4E25A0E35093}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25200" windowHeight="11980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master local choices" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$KL$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$KK$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Registered User</author>
   </authors>
   <commentList>
-    <comment ref="CD6" authorId="0" shapeId="0">
+    <comment ref="CD6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="349">
   <si>
     <t>FCRM1 - National Capital Programme</t>
   </si>
@@ -1068,10 +1075,88 @@
     <t>Year 12</t>
   </si>
   <si>
-    <t>TPE 19/20 - 20/21 total</t>
-  </si>
-  <si>
-    <t>19/20-20/21</t>
+    <t>Year 13</t>
+  </si>
+  <si>
+    <t>Confidence Assessment</t>
+  </si>
+  <si>
+    <t>TPE - 2027/28 on</t>
+  </si>
+  <si>
+    <t>GiA - 2027/28 on</t>
+  </si>
+  <si>
+    <t>Growth - 2027/28 on</t>
+  </si>
+  <si>
+    <t>Local Levy - 2027/28 on</t>
+  </si>
+  <si>
+    <t>IDB - 2027/28 on</t>
+  </si>
+  <si>
+    <t>Public - 2027/28 on</t>
+  </si>
+  <si>
+    <t>Private - 2027/28 on</t>
+  </si>
+  <si>
+    <t>Other EA - 2027/28 on</t>
+  </si>
+  <si>
+    <t>Further required - 2027/28 on</t>
+  </si>
+  <si>
+    <t>OM2 - 2027/28 on</t>
+  </si>
+  <si>
+    <t>OM2b - 2027/28 on</t>
+  </si>
+  <si>
+    <t>OM2c - 2027/28 on</t>
+  </si>
+  <si>
+    <t>OM3 - 2027/28 on</t>
+  </si>
+  <si>
+    <t>OM3b - 2027/28 on</t>
+  </si>
+  <si>
+    <t>OM3c - 2027/28 on</t>
+  </si>
+  <si>
+    <t>PAFS Status</t>
+  </si>
+  <si>
+    <t>Confidence in 'Number' of homes (all scheme including post 2021)</t>
+  </si>
+  <si>
+    <t>Confidence in Homes being delivered (by specified gateway 4 date)</t>
+  </si>
+  <si>
+    <t>Confidence in Securing Partnership Funding (all schemes including post-2021)</t>
+  </si>
+  <si>
+    <t>Confidence Assessment Picklist</t>
+  </si>
+  <si>
+    <t>3. Medium High</t>
+  </si>
+  <si>
+    <t>2. Medium Low</t>
+  </si>
+  <si>
+    <t>1. Low</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>PAFS Base 2020/21</t>
   </si>
   <si>
     <r>
@@ -1094,100 +1179,37 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> 19/20 - 20/21 total</t>
+      <t xml:space="preserve"> 20/21</t>
     </r>
   </si>
   <si>
-    <t>Contributions 19/20 - 20/21 total</t>
-  </si>
-  <si>
-    <t>OM2+3 19/20 - 20/21 total</t>
-  </si>
-  <si>
-    <t>PAFS Base 2019/20</t>
-  </si>
-  <si>
-    <t>Year 13</t>
-  </si>
-  <si>
-    <t>Confidence Assessment</t>
-  </si>
-  <si>
-    <t>Confidence in 'Number' of homes</t>
-  </si>
-  <si>
-    <t>Confidence in Homes being delivered by 2021</t>
-  </si>
-  <si>
-    <t>Confidence in Securing Partnership Funding</t>
-  </si>
-  <si>
-    <t>Proposed Delivery Route</t>
-  </si>
-  <si>
-    <t>TPE - 2027/28 on</t>
-  </si>
-  <si>
-    <t>GiA - 2027/28 on</t>
-  </si>
-  <si>
-    <t>Growth - 2027/28 on</t>
-  </si>
-  <si>
-    <t>Local Levy - 2027/28 on</t>
-  </si>
-  <si>
-    <t>IDB - 2027/28 on</t>
-  </si>
-  <si>
-    <t>Public - 2027/28 on</t>
-  </si>
-  <si>
-    <t>Private - 2027/28 on</t>
-  </si>
-  <si>
-    <t>Other EA - 2027/28 on</t>
-  </si>
-  <si>
-    <t>Further required - 2027/28 on</t>
-  </si>
-  <si>
-    <t>OM2 - 2027/28 on</t>
-  </si>
-  <si>
-    <t>OM2b - 2027/28 on</t>
-  </si>
-  <si>
-    <t>OM2c - 2027/28 on</t>
-  </si>
-  <si>
-    <t>OM3 - 2027/28 on</t>
-  </si>
-  <si>
-    <t>OM3b - 2027/28 on</t>
-  </si>
-  <si>
-    <t>OM3c - 2027/28 on</t>
-  </si>
-  <si>
-    <t>PAFS Status</t>
-  </si>
-  <si>
-    <t/>
+    <t>TPE 20/21</t>
+  </si>
+  <si>
+    <t>Contributions 20/21 total</t>
+  </si>
+  <si>
+    <t>OM2+3 20/21</t>
+  </si>
+  <si>
+    <t>20/21</t>
+  </si>
+  <si>
+    <t>4. High</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="167" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="168" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1280,6 +1302,13 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1287,13 +1316,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1509,9 +1531,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -1519,8 +1541,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1585,7 +1608,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1603,97 +1626,166 @@
     <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1712,86 +1804,24 @@
     <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="%" xfId="3"/>
-    <cellStyle name="% 2 2 2" xfId="4"/>
+  <cellStyles count="10">
+    <cellStyle name="%" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% 2 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="8"/>
-    <cellStyle name="Normal 2 2" xfId="6"/>
-    <cellStyle name="Normal_RCP" xfId="5"/>
+    <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal_RCP" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Percent 11" xfId="7"/>
+    <cellStyle name="Percent 11" xfId="7" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -2079,25 +2109,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:KL7"/>
+  <dimension ref="A1:KN11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="AZ9" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98.7109375" style="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="3" customWidth="1"/>
     <col min="5" max="6" width="21" style="1" customWidth="1"/>
     <col min="7" max="7" width="21" style="2" customWidth="1"/>
@@ -2112,26 +2142,28 @@
     <col min="32" max="39" width="21" style="1" customWidth="1"/>
     <col min="40" max="44" width="21" style="5" customWidth="1"/>
     <col min="45" max="278" width="21" style="1" customWidth="1"/>
-    <col min="279" max="285" width="21" style="29" customWidth="1"/>
+    <col min="279" max="285" width="21" style="28" customWidth="1"/>
     <col min="286" max="293" width="21" style="6" customWidth="1"/>
-    <col min="294" max="296" width="22.21875" style="7" customWidth="1"/>
-    <col min="297" max="297" width="13.21875" style="7" customWidth="1"/>
-    <col min="298" max="298" width="11" style="7" customWidth="1"/>
-    <col min="299" max="16384" width="8.77734375" style="7"/>
+    <col min="294" max="296" width="22.28515625" style="7" customWidth="1"/>
+    <col min="297" max="297" width="11" style="7" customWidth="1"/>
+    <col min="298" max="298" width="12.85546875" style="7" hidden="1" customWidth="1"/>
+    <col min="299" max="299" width="8.7109375" style="7"/>
+    <col min="300" max="300" width="11" style="7" customWidth="1"/>
+    <col min="301" max="16384" width="8.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
+    <row r="1" spans="1:300" ht="28.5" customHeight="1">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
+      <c r="B1" s="66"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
       <c r="G1" s="24"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="23"/>
       <c r="K1" s="23"/>
       <c r="L1" s="23"/>
@@ -2202,16 +2234,16 @@
       <c r="BY1" s="23"/>
       <c r="BZ1" s="23"/>
       <c r="CA1" s="23"/>
-      <c r="CB1" s="38"/>
-      <c r="CC1" s="35"/>
-      <c r="CD1" s="35"/>
-      <c r="CE1" s="35"/>
+      <c r="CB1" s="33"/>
+      <c r="CC1" s="30"/>
+      <c r="CD1" s="30"/>
+      <c r="CE1" s="30"/>
       <c r="CF1" s="23"/>
       <c r="CG1" s="23"/>
       <c r="CH1" s="23"/>
       <c r="CI1" s="23"/>
-      <c r="CJ1" s="39"/>
-      <c r="CK1" s="39"/>
+      <c r="CJ1" s="34"/>
+      <c r="CK1" s="34"/>
       <c r="CL1" s="23"/>
       <c r="CM1" s="23"/>
       <c r="CN1" s="23"/>
@@ -2401,13 +2433,13 @@
       <c r="JP1" s="23"/>
       <c r="JQ1" s="23"/>
       <c r="JR1" s="23"/>
-      <c r="JS1" s="40"/>
-      <c r="JT1" s="40"/>
-      <c r="JU1" s="40"/>
-      <c r="JV1" s="40"/>
-      <c r="JW1" s="40"/>
-      <c r="JX1" s="40"/>
-      <c r="JY1" s="40"/>
+      <c r="JS1" s="35"/>
+      <c r="JT1" s="35"/>
+      <c r="JU1" s="35"/>
+      <c r="JV1" s="35"/>
+      <c r="JW1" s="35"/>
+      <c r="JX1" s="35"/>
+      <c r="JY1" s="35"/>
       <c r="JZ1" s="23"/>
       <c r="KA1" s="23"/>
       <c r="KB1" s="23"/>
@@ -2417,18 +2449,18 @@
       <c r="KF1" s="23"/>
       <c r="KG1" s="23"/>
     </row>
-    <row r="2" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="82" t="s">
-        <v>320</v>
-      </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
+    <row r="2" spans="1:300" ht="28.5" customHeight="1">
+      <c r="A2" s="67" t="s">
+        <v>342</v>
+      </c>
+      <c r="B2" s="67"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="23"/>
-      <c r="F2" s="42"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="37"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
       <c r="L2" s="23"/>
@@ -2497,18 +2529,18 @@
       <c r="BW2" s="23"/>
       <c r="BX2" s="23"/>
       <c r="BY2" s="23"/>
-      <c r="BZ2" s="43"/>
-      <c r="CA2" s="43"/>
-      <c r="CB2" s="35"/>
-      <c r="CC2" s="35"/>
-      <c r="CD2" s="35"/>
-      <c r="CE2" s="35"/>
+      <c r="BZ2" s="38"/>
+      <c r="CA2" s="38"/>
+      <c r="CB2" s="30"/>
+      <c r="CC2" s="30"/>
+      <c r="CD2" s="30"/>
+      <c r="CE2" s="30"/>
       <c r="CF2" s="23"/>
-      <c r="CG2" s="39"/>
-      <c r="CH2" s="39"/>
-      <c r="CI2" s="39"/>
-      <c r="CJ2" s="39"/>
-      <c r="CK2" s="39"/>
+      <c r="CG2" s="34"/>
+      <c r="CH2" s="34"/>
+      <c r="CI2" s="34"/>
+      <c r="CJ2" s="34"/>
+      <c r="CK2" s="34"/>
       <c r="CL2" s="23"/>
       <c r="CM2" s="23"/>
       <c r="CN2" s="23"/>
@@ -2698,734 +2730,733 @@
       <c r="JP2" s="23"/>
       <c r="JQ2" s="23"/>
       <c r="JR2" s="23"/>
-      <c r="JS2" s="42"/>
-      <c r="JT2" s="42"/>
-      <c r="JU2" s="42"/>
-      <c r="JV2" s="42"/>
-      <c r="JW2" s="42"/>
-      <c r="JX2" s="42"/>
-      <c r="JY2" s="42"/>
+      <c r="JS2" s="37"/>
+      <c r="JT2" s="37"/>
+      <c r="JU2" s="37"/>
+      <c r="JV2" s="37"/>
+      <c r="JW2" s="37"/>
+      <c r="JX2" s="37"/>
+      <c r="JY2" s="37"/>
       <c r="JZ2" s="23"/>
-      <c r="KA2" s="42"/>
-      <c r="KB2" s="42"/>
-      <c r="KC2" s="42"/>
-      <c r="KD2" s="42"/>
-      <c r="KE2" s="42"/>
-      <c r="KF2" s="42"/>
-      <c r="KG2" s="42"/>
+      <c r="KA2" s="37"/>
+      <c r="KB2" s="37"/>
+      <c r="KC2" s="37"/>
+      <c r="KD2" s="37"/>
+      <c r="KE2" s="37"/>
+      <c r="KF2" s="37"/>
+      <c r="KG2" s="37"/>
     </row>
-    <row r="3" spans="1:298" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="46"/>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="45"/>
-      <c r="AA3" s="45"/>
-      <c r="AB3" s="46"/>
-      <c r="AC3" s="45"/>
-      <c r="AD3" s="46"/>
-      <c r="AE3" s="46"/>
-      <c r="AF3" s="45"/>
-      <c r="AG3" s="45"/>
-      <c r="AH3" s="45"/>
-      <c r="AI3" s="45"/>
-      <c r="AJ3" s="45"/>
-      <c r="AK3" s="45"/>
-      <c r="AL3" s="45"/>
-      <c r="AM3" s="45"/>
-      <c r="AN3" s="47"/>
-      <c r="AO3" s="48"/>
-      <c r="AP3" s="48"/>
-      <c r="AQ3" s="48"/>
-      <c r="AR3" s="48"/>
-      <c r="AS3" s="49"/>
-      <c r="AT3" s="49"/>
-      <c r="AU3" s="49"/>
-      <c r="AV3" s="49"/>
-      <c r="AW3" s="49"/>
-      <c r="AX3" s="49"/>
-      <c r="AY3" s="49"/>
-      <c r="AZ3" s="49"/>
-      <c r="BA3" s="49"/>
-      <c r="BB3" s="49"/>
-      <c r="BC3" s="49"/>
-      <c r="BD3" s="49"/>
-      <c r="BE3" s="49"/>
-      <c r="BF3" s="49"/>
-      <c r="BG3" s="49"/>
-      <c r="BH3" s="49"/>
-      <c r="BI3" s="49"/>
-      <c r="BJ3" s="49"/>
-      <c r="BK3" s="49"/>
-      <c r="BL3" s="49"/>
-      <c r="BM3" s="49"/>
-      <c r="BN3" s="50"/>
-      <c r="BO3" s="50"/>
-      <c r="BP3" s="50"/>
-      <c r="BQ3" s="50"/>
-      <c r="BR3" s="50"/>
-      <c r="BS3" s="50"/>
-      <c r="BT3" s="50"/>
-      <c r="BU3" s="50"/>
-      <c r="BV3" s="50"/>
-      <c r="BW3" s="50"/>
-      <c r="BX3" s="50"/>
-      <c r="BY3" s="50"/>
-      <c r="BZ3" s="50"/>
-      <c r="CA3" s="50"/>
-      <c r="CB3" s="50"/>
-      <c r="CC3" s="50"/>
-      <c r="CD3" s="50"/>
-      <c r="CE3" s="50"/>
-      <c r="CF3" s="50"/>
-      <c r="CG3" s="50"/>
-      <c r="CH3" s="50"/>
-      <c r="CI3" s="50"/>
-      <c r="CJ3" s="50"/>
-      <c r="CK3" s="50"/>
-      <c r="CL3" s="50"/>
-      <c r="CM3" s="50"/>
-      <c r="CN3" s="50"/>
-      <c r="CO3" s="50"/>
-      <c r="CP3" s="50"/>
-      <c r="CQ3" s="50"/>
-      <c r="CR3" s="50"/>
-      <c r="CS3" s="50"/>
-      <c r="CT3" s="50"/>
-      <c r="CU3" s="50"/>
-      <c r="CV3" s="50"/>
-      <c r="CW3" s="50"/>
-      <c r="CX3" s="50"/>
-      <c r="CY3" s="50"/>
-      <c r="CZ3" s="50"/>
-      <c r="DA3" s="50"/>
-      <c r="DB3" s="50"/>
-      <c r="DC3" s="50"/>
-      <c r="DD3" s="50"/>
-      <c r="DE3" s="50"/>
-      <c r="DF3" s="50"/>
-      <c r="DG3" s="50"/>
-      <c r="DH3" s="50"/>
-      <c r="DI3" s="50"/>
-      <c r="DJ3" s="50"/>
-      <c r="DK3" s="50"/>
-      <c r="DL3" s="50"/>
-      <c r="DM3" s="50"/>
-      <c r="DN3" s="50"/>
-      <c r="DO3" s="50"/>
-      <c r="DP3" s="50"/>
-      <c r="DQ3" s="50"/>
-      <c r="DR3" s="50"/>
-      <c r="DS3" s="50"/>
-      <c r="DT3" s="50"/>
-      <c r="DU3" s="50"/>
-      <c r="DV3" s="50"/>
-      <c r="DW3" s="50"/>
-      <c r="DX3" s="50"/>
-      <c r="DY3" s="50"/>
-      <c r="DZ3" s="50"/>
-      <c r="EA3" s="50"/>
-      <c r="EB3" s="50"/>
-      <c r="EC3" s="50"/>
-      <c r="ED3" s="50"/>
-      <c r="EE3" s="50"/>
-      <c r="EF3" s="50"/>
-      <c r="EG3" s="50"/>
-      <c r="EH3" s="50"/>
-      <c r="EI3" s="50"/>
-      <c r="EJ3" s="50"/>
-      <c r="EK3" s="50"/>
-      <c r="EL3" s="50"/>
-      <c r="EM3" s="50"/>
-      <c r="EN3" s="50"/>
-      <c r="EO3" s="50"/>
-      <c r="EP3" s="50"/>
-      <c r="EQ3" s="50"/>
-      <c r="ER3" s="50"/>
-      <c r="ES3" s="50"/>
-      <c r="ET3" s="50"/>
-      <c r="EU3" s="50"/>
-      <c r="EV3" s="50"/>
-      <c r="EW3" s="50"/>
-      <c r="EX3" s="50"/>
-      <c r="EY3" s="50"/>
-      <c r="EZ3" s="50"/>
-      <c r="FA3" s="50"/>
-      <c r="FB3" s="50"/>
-      <c r="FC3" s="50"/>
-      <c r="FD3" s="50"/>
-      <c r="FE3" s="50"/>
-      <c r="FF3" s="50"/>
-      <c r="FG3" s="50"/>
-      <c r="FH3" s="50"/>
-      <c r="FI3" s="50"/>
-      <c r="FJ3" s="50"/>
-      <c r="FK3" s="50"/>
-      <c r="FL3" s="50"/>
-      <c r="FM3" s="50"/>
-      <c r="FN3" s="50"/>
-      <c r="FO3" s="50"/>
-      <c r="FP3" s="50"/>
-      <c r="FQ3" s="50"/>
-      <c r="FR3" s="50"/>
-      <c r="FS3" s="50"/>
-      <c r="FT3" s="50"/>
-      <c r="FU3" s="50"/>
-      <c r="FV3" s="50"/>
-      <c r="FW3" s="50"/>
-      <c r="FX3" s="50"/>
-      <c r="FY3" s="50"/>
-      <c r="FZ3" s="50"/>
-      <c r="GA3" s="50"/>
-      <c r="GB3" s="50"/>
-      <c r="GC3" s="50"/>
-      <c r="GD3" s="50"/>
-      <c r="GE3" s="50"/>
-      <c r="GF3" s="50"/>
-      <c r="GG3" s="50"/>
-      <c r="GH3" s="50"/>
-      <c r="GI3" s="50"/>
-      <c r="GJ3" s="50"/>
-      <c r="GK3" s="50"/>
-      <c r="GL3" s="50"/>
-      <c r="GM3" s="50"/>
-      <c r="GN3" s="50"/>
-      <c r="GO3" s="50"/>
-      <c r="GP3" s="50"/>
-      <c r="GQ3" s="50"/>
-      <c r="GR3" s="50"/>
-      <c r="GS3" s="50"/>
-      <c r="GT3" s="50"/>
-      <c r="GU3" s="50"/>
-      <c r="GV3" s="50"/>
-      <c r="GW3" s="50"/>
-      <c r="GX3" s="50"/>
-      <c r="GY3" s="50"/>
-      <c r="GZ3" s="50"/>
-      <c r="HA3" s="50"/>
-      <c r="HB3" s="50"/>
-      <c r="HC3" s="50"/>
-      <c r="HD3" s="50"/>
-      <c r="HE3" s="50"/>
-      <c r="HF3" s="50"/>
-      <c r="HG3" s="50"/>
-      <c r="HH3" s="50"/>
-      <c r="HI3" s="50"/>
-      <c r="HJ3" s="50"/>
-      <c r="HK3" s="50"/>
-      <c r="HL3" s="50"/>
-      <c r="HM3" s="50"/>
-      <c r="HN3" s="50"/>
-      <c r="HO3" s="50"/>
-      <c r="HP3" s="50"/>
-      <c r="HQ3" s="50"/>
-      <c r="HR3" s="50"/>
-      <c r="HS3" s="50"/>
-      <c r="HT3" s="50"/>
-      <c r="HU3" s="50"/>
-      <c r="HV3" s="50"/>
-      <c r="HW3" s="50"/>
-      <c r="HX3" s="50"/>
-      <c r="HY3" s="50"/>
-      <c r="HZ3" s="50"/>
-      <c r="IA3" s="50"/>
-      <c r="IB3" s="50"/>
-      <c r="IC3" s="50"/>
-      <c r="ID3" s="50"/>
-      <c r="IE3" s="50"/>
-      <c r="IF3" s="50"/>
-      <c r="IG3" s="50"/>
-      <c r="IH3" s="50"/>
-      <c r="II3" s="50"/>
-      <c r="IJ3" s="50"/>
-      <c r="IK3" s="50"/>
-      <c r="IL3" s="50"/>
-      <c r="IM3" s="50"/>
-      <c r="IN3" s="50"/>
-      <c r="IO3" s="50"/>
-      <c r="IP3" s="50"/>
-      <c r="IQ3" s="50"/>
-      <c r="IR3" s="50"/>
-      <c r="IS3" s="50"/>
-      <c r="IT3" s="50"/>
-      <c r="IU3" s="50"/>
-      <c r="IV3" s="50"/>
-      <c r="IW3" s="50"/>
-      <c r="IX3" s="50"/>
-      <c r="IY3" s="50"/>
-      <c r="IZ3" s="50"/>
-      <c r="JA3" s="50"/>
-      <c r="JB3" s="50"/>
-      <c r="JC3" s="50"/>
-      <c r="JD3" s="50"/>
-      <c r="JE3" s="50"/>
-      <c r="JF3" s="50"/>
-      <c r="JG3" s="50"/>
-      <c r="JH3" s="50"/>
-      <c r="JI3" s="50"/>
-      <c r="JJ3" s="50"/>
-      <c r="JK3" s="50"/>
-      <c r="JL3" s="50"/>
-      <c r="JM3" s="50"/>
-      <c r="JN3" s="50"/>
-      <c r="JO3" s="50"/>
-      <c r="JP3" s="50"/>
-      <c r="JQ3" s="50"/>
-      <c r="JR3" s="50"/>
-      <c r="JS3" s="50"/>
-      <c r="JT3" s="50"/>
-      <c r="JU3" s="50"/>
-      <c r="JV3" s="50"/>
-      <c r="JW3" s="50"/>
-      <c r="JX3" s="50"/>
-      <c r="JY3" s="50"/>
-      <c r="JZ3" s="50"/>
-      <c r="KA3" s="50"/>
-      <c r="KB3" s="50"/>
-      <c r="KC3" s="50"/>
-      <c r="KD3" s="50"/>
-      <c r="KE3" s="50"/>
-      <c r="KF3" s="50"/>
-      <c r="KG3" s="50"/>
+    <row r="3" spans="1:300" ht="25.5" customHeight="1">
+      <c r="A3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="40"/>
+      <c r="AA3" s="40"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="40"/>
+      <c r="AD3" s="41"/>
+      <c r="AE3" s="41"/>
+      <c r="AF3" s="40"/>
+      <c r="AG3" s="40"/>
+      <c r="AH3" s="40"/>
+      <c r="AI3" s="40"/>
+      <c r="AJ3" s="40"/>
+      <c r="AK3" s="40"/>
+      <c r="AL3" s="40"/>
+      <c r="AM3" s="40"/>
+      <c r="AN3" s="42"/>
+      <c r="AO3" s="43"/>
+      <c r="AP3" s="43"/>
+      <c r="AQ3" s="43"/>
+      <c r="AR3" s="43"/>
+      <c r="AS3" s="44"/>
+      <c r="AT3" s="44"/>
+      <c r="AU3" s="44"/>
+      <c r="AV3" s="44"/>
+      <c r="AW3" s="44"/>
+      <c r="AX3" s="44"/>
+      <c r="AY3" s="44"/>
+      <c r="AZ3" s="44"/>
+      <c r="BA3" s="44"/>
+      <c r="BB3" s="44"/>
+      <c r="BC3" s="44"/>
+      <c r="BD3" s="44"/>
+      <c r="BE3" s="44"/>
+      <c r="BF3" s="44"/>
+      <c r="BG3" s="44"/>
+      <c r="BH3" s="44"/>
+      <c r="BI3" s="44"/>
+      <c r="BJ3" s="44"/>
+      <c r="BK3" s="44"/>
+      <c r="BL3" s="44"/>
+      <c r="BM3" s="44"/>
+      <c r="BN3" s="45"/>
+      <c r="BO3" s="45"/>
+      <c r="BP3" s="45"/>
+      <c r="BQ3" s="45"/>
+      <c r="BR3" s="45"/>
+      <c r="BS3" s="45"/>
+      <c r="BT3" s="45"/>
+      <c r="BU3" s="45"/>
+      <c r="BV3" s="45"/>
+      <c r="BW3" s="45"/>
+      <c r="BX3" s="45"/>
+      <c r="BY3" s="45"/>
+      <c r="BZ3" s="45"/>
+      <c r="CA3" s="45"/>
+      <c r="CB3" s="45"/>
+      <c r="CC3" s="45"/>
+      <c r="CD3" s="45"/>
+      <c r="CE3" s="45"/>
+      <c r="CF3" s="45"/>
+      <c r="CG3" s="45"/>
+      <c r="CH3" s="45"/>
+      <c r="CI3" s="45"/>
+      <c r="CJ3" s="45"/>
+      <c r="CK3" s="45"/>
+      <c r="CL3" s="45"/>
+      <c r="CM3" s="45"/>
+      <c r="CN3" s="45"/>
+      <c r="CO3" s="45"/>
+      <c r="CP3" s="45"/>
+      <c r="CQ3" s="45"/>
+      <c r="CR3" s="45"/>
+      <c r="CS3" s="45"/>
+      <c r="CT3" s="45"/>
+      <c r="CU3" s="45"/>
+      <c r="CV3" s="45"/>
+      <c r="CW3" s="45"/>
+      <c r="CX3" s="45"/>
+      <c r="CY3" s="45"/>
+      <c r="CZ3" s="45"/>
+      <c r="DA3" s="45"/>
+      <c r="DB3" s="45"/>
+      <c r="DC3" s="45"/>
+      <c r="DD3" s="45"/>
+      <c r="DE3" s="45"/>
+      <c r="DF3" s="45"/>
+      <c r="DG3" s="45"/>
+      <c r="DH3" s="45"/>
+      <c r="DI3" s="45"/>
+      <c r="DJ3" s="45"/>
+      <c r="DK3" s="45"/>
+      <c r="DL3" s="45"/>
+      <c r="DM3" s="45"/>
+      <c r="DN3" s="45"/>
+      <c r="DO3" s="45"/>
+      <c r="DP3" s="45"/>
+      <c r="DQ3" s="45"/>
+      <c r="DR3" s="45"/>
+      <c r="DS3" s="45"/>
+      <c r="DT3" s="45"/>
+      <c r="DU3" s="45"/>
+      <c r="DV3" s="45"/>
+      <c r="DW3" s="45"/>
+      <c r="DX3" s="45"/>
+      <c r="DY3" s="45"/>
+      <c r="DZ3" s="45"/>
+      <c r="EA3" s="45"/>
+      <c r="EB3" s="45"/>
+      <c r="EC3" s="45"/>
+      <c r="ED3" s="45"/>
+      <c r="EE3" s="45"/>
+      <c r="EF3" s="45"/>
+      <c r="EG3" s="45"/>
+      <c r="EH3" s="45"/>
+      <c r="EI3" s="45"/>
+      <c r="EJ3" s="45"/>
+      <c r="EK3" s="45"/>
+      <c r="EL3" s="45"/>
+      <c r="EM3" s="45"/>
+      <c r="EN3" s="45"/>
+      <c r="EO3" s="45"/>
+      <c r="EP3" s="45"/>
+      <c r="EQ3" s="45"/>
+      <c r="ER3" s="45"/>
+      <c r="ES3" s="45"/>
+      <c r="ET3" s="45"/>
+      <c r="EU3" s="45"/>
+      <c r="EV3" s="45"/>
+      <c r="EW3" s="45"/>
+      <c r="EX3" s="45"/>
+      <c r="EY3" s="45"/>
+      <c r="EZ3" s="45"/>
+      <c r="FA3" s="45"/>
+      <c r="FB3" s="45"/>
+      <c r="FC3" s="45"/>
+      <c r="FD3" s="45"/>
+      <c r="FE3" s="45"/>
+      <c r="FF3" s="45"/>
+      <c r="FG3" s="45"/>
+      <c r="FH3" s="45"/>
+      <c r="FI3" s="45"/>
+      <c r="FJ3" s="45"/>
+      <c r="FK3" s="45"/>
+      <c r="FL3" s="45"/>
+      <c r="FM3" s="45"/>
+      <c r="FN3" s="45"/>
+      <c r="FO3" s="45"/>
+      <c r="FP3" s="45"/>
+      <c r="FQ3" s="45"/>
+      <c r="FR3" s="45"/>
+      <c r="FS3" s="45"/>
+      <c r="FT3" s="45"/>
+      <c r="FU3" s="45"/>
+      <c r="FV3" s="45"/>
+      <c r="FW3" s="45"/>
+      <c r="FX3" s="45"/>
+      <c r="FY3" s="45"/>
+      <c r="FZ3" s="45"/>
+      <c r="GA3" s="45"/>
+      <c r="GB3" s="45"/>
+      <c r="GC3" s="45"/>
+      <c r="GD3" s="45"/>
+      <c r="GE3" s="45"/>
+      <c r="GF3" s="45"/>
+      <c r="GG3" s="45"/>
+      <c r="GH3" s="45"/>
+      <c r="GI3" s="45"/>
+      <c r="GJ3" s="45"/>
+      <c r="GK3" s="45"/>
+      <c r="GL3" s="45"/>
+      <c r="GM3" s="45"/>
+      <c r="GN3" s="45"/>
+      <c r="GO3" s="45"/>
+      <c r="GP3" s="45"/>
+      <c r="GQ3" s="45"/>
+      <c r="GR3" s="45"/>
+      <c r="GS3" s="45"/>
+      <c r="GT3" s="45"/>
+      <c r="GU3" s="45"/>
+      <c r="GV3" s="45"/>
+      <c r="GW3" s="45"/>
+      <c r="GX3" s="45"/>
+      <c r="GY3" s="45"/>
+      <c r="GZ3" s="45"/>
+      <c r="HA3" s="45"/>
+      <c r="HB3" s="45"/>
+      <c r="HC3" s="45"/>
+      <c r="HD3" s="45"/>
+      <c r="HE3" s="45"/>
+      <c r="HF3" s="45"/>
+      <c r="HG3" s="45"/>
+      <c r="HH3" s="45"/>
+      <c r="HI3" s="45"/>
+      <c r="HJ3" s="45"/>
+      <c r="HK3" s="45"/>
+      <c r="HL3" s="45"/>
+      <c r="HM3" s="45"/>
+      <c r="HN3" s="45"/>
+      <c r="HO3" s="45"/>
+      <c r="HP3" s="45"/>
+      <c r="HQ3" s="45"/>
+      <c r="HR3" s="45"/>
+      <c r="HS3" s="45"/>
+      <c r="HT3" s="45"/>
+      <c r="HU3" s="45"/>
+      <c r="HV3" s="45"/>
+      <c r="HW3" s="45"/>
+      <c r="HX3" s="45"/>
+      <c r="HY3" s="45"/>
+      <c r="HZ3" s="45"/>
+      <c r="IA3" s="45"/>
+      <c r="IB3" s="45"/>
+      <c r="IC3" s="45"/>
+      <c r="ID3" s="45"/>
+      <c r="IE3" s="45"/>
+      <c r="IF3" s="45"/>
+      <c r="IG3" s="45"/>
+      <c r="IH3" s="45"/>
+      <c r="II3" s="45"/>
+      <c r="IJ3" s="45"/>
+      <c r="IK3" s="45"/>
+      <c r="IL3" s="45"/>
+      <c r="IM3" s="45"/>
+      <c r="IN3" s="45"/>
+      <c r="IO3" s="45"/>
+      <c r="IP3" s="45"/>
+      <c r="IQ3" s="45"/>
+      <c r="IR3" s="45"/>
+      <c r="IS3" s="45"/>
+      <c r="IT3" s="45"/>
+      <c r="IU3" s="45"/>
+      <c r="IV3" s="45"/>
+      <c r="IW3" s="45"/>
+      <c r="IX3" s="45"/>
+      <c r="IY3" s="45"/>
+      <c r="IZ3" s="45"/>
+      <c r="JA3" s="45"/>
+      <c r="JB3" s="45"/>
+      <c r="JC3" s="45"/>
+      <c r="JD3" s="45"/>
+      <c r="JE3" s="45"/>
+      <c r="JF3" s="45"/>
+      <c r="JG3" s="45"/>
+      <c r="JH3" s="45"/>
+      <c r="JI3" s="45"/>
+      <c r="JJ3" s="45"/>
+      <c r="JK3" s="45"/>
+      <c r="JL3" s="45"/>
+      <c r="JM3" s="45"/>
+      <c r="JN3" s="45"/>
+      <c r="JO3" s="45"/>
+      <c r="JP3" s="45"/>
+      <c r="JQ3" s="45"/>
+      <c r="JR3" s="45"/>
+      <c r="JS3" s="45"/>
+      <c r="JT3" s="45"/>
+      <c r="JU3" s="45"/>
+      <c r="JV3" s="45"/>
+      <c r="JW3" s="45"/>
+      <c r="JX3" s="45"/>
+      <c r="JY3" s="45"/>
+      <c r="JZ3" s="45"/>
+      <c r="KA3" s="45"/>
+      <c r="KB3" s="45"/>
+      <c r="KC3" s="45"/>
+      <c r="KD3" s="45"/>
+      <c r="KE3" s="45"/>
+      <c r="KF3" s="45"/>
+      <c r="KG3" s="45"/>
     </row>
-    <row r="4" spans="1:298" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="83" t="s">
+    <row r="4" spans="1:300" ht="46.5" customHeight="1">
+      <c r="A4" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="84" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="85" t="s">
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="85"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="85"/>
-      <c r="P4" s="86" t="s">
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
+      <c r="O4" s="70"/>
+      <c r="P4" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="87" t="s">
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="87"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="88" t="s">
+      <c r="V4" s="72"/>
+      <c r="W4" s="72"/>
+      <c r="X4" s="72"/>
+      <c r="Y4" s="72"/>
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
+      <c r="AB4" s="72"/>
+      <c r="AC4" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="88"/>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
-      <c r="AH4" s="88"/>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="89" t="s">
+      <c r="AD4" s="73"/>
+      <c r="AE4" s="73"/>
+      <c r="AF4" s="73"/>
+      <c r="AG4" s="73"/>
+      <c r="AH4" s="73"/>
+      <c r="AI4" s="73"/>
+      <c r="AJ4" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="89"/>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="80" t="s">
+      <c r="AK4" s="74"/>
+      <c r="AL4" s="74"/>
+      <c r="AM4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="80"/>
-      <c r="AO4" s="70"/>
-      <c r="AP4" s="70"/>
-      <c r="AQ4" s="70"/>
-      <c r="AR4" s="70"/>
-      <c r="AS4" s="71" t="s">
+      <c r="AN4" s="65"/>
+      <c r="AO4" s="76"/>
+      <c r="AP4" s="76"/>
+      <c r="AQ4" s="76"/>
+      <c r="AR4" s="76"/>
+      <c r="AS4" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="71"/>
-      <c r="AU4" s="71"/>
-      <c r="AV4" s="71"/>
-      <c r="AW4" s="71"/>
-      <c r="AX4" s="71"/>
-      <c r="AY4" s="71"/>
-      <c r="AZ4" s="71"/>
-      <c r="BA4" s="71"/>
-      <c r="BB4" s="71"/>
-      <c r="BC4" s="71"/>
-      <c r="BD4" s="71"/>
-      <c r="BE4" s="71"/>
-      <c r="BF4" s="71"/>
-      <c r="BG4" s="71"/>
-      <c r="BH4" s="71"/>
-      <c r="BI4" s="71"/>
-      <c r="BJ4" s="71"/>
-      <c r="BK4" s="67" t="s">
+      <c r="AT4" s="77"/>
+      <c r="AU4" s="77"/>
+      <c r="AV4" s="77"/>
+      <c r="AW4" s="77"/>
+      <c r="AX4" s="77"/>
+      <c r="AY4" s="77"/>
+      <c r="AZ4" s="77"/>
+      <c r="BA4" s="77"/>
+      <c r="BB4" s="77"/>
+      <c r="BC4" s="77"/>
+      <c r="BD4" s="77"/>
+      <c r="BE4" s="77"/>
+      <c r="BF4" s="77"/>
+      <c r="BG4" s="77"/>
+      <c r="BH4" s="77"/>
+      <c r="BI4" s="77"/>
+      <c r="BJ4" s="77"/>
+      <c r="BK4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="BL4" s="67"/>
-      <c r="BM4" s="67"/>
-      <c r="BN4" s="67"/>
-      <c r="BO4" s="67"/>
-      <c r="BP4" s="67"/>
-      <c r="BQ4" s="67"/>
-      <c r="BR4" s="67"/>
-      <c r="BS4" s="67"/>
-      <c r="BT4" s="67"/>
-      <c r="BU4" s="67"/>
-      <c r="BV4" s="67"/>
-      <c r="BW4" s="67"/>
-      <c r="BX4" s="67"/>
-      <c r="BY4" s="72" t="s">
+      <c r="BL4" s="75"/>
+      <c r="BM4" s="75"/>
+      <c r="BN4" s="75"/>
+      <c r="BO4" s="75"/>
+      <c r="BP4" s="75"/>
+      <c r="BQ4" s="75"/>
+      <c r="BR4" s="75"/>
+      <c r="BS4" s="75"/>
+      <c r="BT4" s="75"/>
+      <c r="BU4" s="75"/>
+      <c r="BV4" s="75"/>
+      <c r="BW4" s="75"/>
+      <c r="BX4" s="75"/>
+      <c r="BY4" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="72"/>
-      <c r="CA4" s="72"/>
-      <c r="CB4" s="72"/>
-      <c r="CC4" s="72"/>
-      <c r="CD4" s="72"/>
-      <c r="CE4" s="72"/>
-      <c r="CF4" s="72"/>
-      <c r="CG4" s="72"/>
-      <c r="CH4" s="72"/>
-      <c r="CI4" s="72"/>
-      <c r="CJ4" s="72"/>
-      <c r="CK4" s="72"/>
-      <c r="CL4" s="72"/>
-      <c r="CM4" s="73" t="s">
+      <c r="BZ4" s="78"/>
+      <c r="CA4" s="78"/>
+      <c r="CB4" s="78"/>
+      <c r="CC4" s="78"/>
+      <c r="CD4" s="78"/>
+      <c r="CE4" s="78"/>
+      <c r="CF4" s="78"/>
+      <c r="CG4" s="78"/>
+      <c r="CH4" s="78"/>
+      <c r="CI4" s="78"/>
+      <c r="CJ4" s="78"/>
+      <c r="CK4" s="78"/>
+      <c r="CL4" s="78"/>
+      <c r="CM4" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="73"/>
-      <c r="CO4" s="73"/>
-      <c r="CP4" s="73"/>
-      <c r="CQ4" s="73"/>
-      <c r="CR4" s="73"/>
-      <c r="CS4" s="73"/>
-      <c r="CT4" s="73"/>
-      <c r="CU4" s="73"/>
-      <c r="CV4" s="73"/>
-      <c r="CW4" s="73"/>
-      <c r="CX4" s="73"/>
-      <c r="CY4" s="73"/>
-      <c r="CZ4" s="73"/>
-      <c r="DA4" s="74" t="s">
+      <c r="CN4" s="79"/>
+      <c r="CO4" s="79"/>
+      <c r="CP4" s="79"/>
+      <c r="CQ4" s="79"/>
+      <c r="CR4" s="79"/>
+      <c r="CS4" s="79"/>
+      <c r="CT4" s="79"/>
+      <c r="CU4" s="79"/>
+      <c r="CV4" s="79"/>
+      <c r="CW4" s="79"/>
+      <c r="CX4" s="79"/>
+      <c r="CY4" s="79"/>
+      <c r="CZ4" s="79"/>
+      <c r="DA4" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="74"/>
-      <c r="DC4" s="74"/>
-      <c r="DD4" s="74"/>
-      <c r="DE4" s="74"/>
-      <c r="DF4" s="74"/>
-      <c r="DG4" s="74"/>
-      <c r="DH4" s="74"/>
-      <c r="DI4" s="74"/>
-      <c r="DJ4" s="74"/>
-      <c r="DK4" s="74"/>
-      <c r="DL4" s="74"/>
-      <c r="DM4" s="74"/>
-      <c r="DN4" s="74"/>
-      <c r="DO4" s="75" t="s">
+      <c r="DB4" s="80"/>
+      <c r="DC4" s="80"/>
+      <c r="DD4" s="80"/>
+      <c r="DE4" s="80"/>
+      <c r="DF4" s="80"/>
+      <c r="DG4" s="80"/>
+      <c r="DH4" s="80"/>
+      <c r="DI4" s="80"/>
+      <c r="DJ4" s="80"/>
+      <c r="DK4" s="80"/>
+      <c r="DL4" s="80"/>
+      <c r="DM4" s="80"/>
+      <c r="DN4" s="80"/>
+      <c r="DO4" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="75"/>
-      <c r="DQ4" s="75"/>
-      <c r="DR4" s="75"/>
-      <c r="DS4" s="75"/>
-      <c r="DT4" s="75"/>
-      <c r="DU4" s="75"/>
-      <c r="DV4" s="75"/>
-      <c r="DW4" s="75"/>
-      <c r="DX4" s="75"/>
-      <c r="DY4" s="75"/>
-      <c r="DZ4" s="75"/>
-      <c r="EA4" s="75"/>
-      <c r="EB4" s="75"/>
-      <c r="EC4" s="76" t="s">
+      <c r="DP4" s="81"/>
+      <c r="DQ4" s="81"/>
+      <c r="DR4" s="81"/>
+      <c r="DS4" s="81"/>
+      <c r="DT4" s="81"/>
+      <c r="DU4" s="81"/>
+      <c r="DV4" s="81"/>
+      <c r="DW4" s="81"/>
+      <c r="DX4" s="81"/>
+      <c r="DY4" s="81"/>
+      <c r="DZ4" s="81"/>
+      <c r="EA4" s="81"/>
+      <c r="EB4" s="81"/>
+      <c r="EC4" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="76"/>
-      <c r="EE4" s="76"/>
-      <c r="EF4" s="76"/>
-      <c r="EG4" s="76"/>
-      <c r="EH4" s="76"/>
-      <c r="EI4" s="76"/>
-      <c r="EJ4" s="76"/>
-      <c r="EK4" s="76"/>
-      <c r="EL4" s="76"/>
-      <c r="EM4" s="76"/>
-      <c r="EN4" s="76"/>
-      <c r="EO4" s="76"/>
-      <c r="EP4" s="76"/>
-      <c r="EQ4" s="77" t="s">
+      <c r="ED4" s="82"/>
+      <c r="EE4" s="82"/>
+      <c r="EF4" s="82"/>
+      <c r="EG4" s="82"/>
+      <c r="EH4" s="82"/>
+      <c r="EI4" s="82"/>
+      <c r="EJ4" s="82"/>
+      <c r="EK4" s="82"/>
+      <c r="EL4" s="82"/>
+      <c r="EM4" s="82"/>
+      <c r="EN4" s="82"/>
+      <c r="EO4" s="82"/>
+      <c r="EP4" s="82"/>
+      <c r="EQ4" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="77"/>
-      <c r="ES4" s="77"/>
-      <c r="ET4" s="77"/>
-      <c r="EU4" s="77"/>
-      <c r="EV4" s="77"/>
-      <c r="EW4" s="77"/>
-      <c r="EX4" s="77"/>
-      <c r="EY4" s="77"/>
-      <c r="EZ4" s="77"/>
-      <c r="FA4" s="77"/>
-      <c r="FB4" s="77"/>
-      <c r="FC4" s="77"/>
-      <c r="FD4" s="77"/>
-      <c r="FE4" s="78" t="s">
+      <c r="ER4" s="83"/>
+      <c r="ES4" s="83"/>
+      <c r="ET4" s="83"/>
+      <c r="EU4" s="83"/>
+      <c r="EV4" s="83"/>
+      <c r="EW4" s="83"/>
+      <c r="EX4" s="83"/>
+      <c r="EY4" s="83"/>
+      <c r="EZ4" s="83"/>
+      <c r="FA4" s="83"/>
+      <c r="FB4" s="83"/>
+      <c r="FC4" s="83"/>
+      <c r="FD4" s="83"/>
+      <c r="FE4" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="78"/>
-      <c r="FG4" s="78"/>
-      <c r="FH4" s="78"/>
-      <c r="FI4" s="78"/>
-      <c r="FJ4" s="78"/>
-      <c r="FK4" s="78"/>
-      <c r="FL4" s="78"/>
-      <c r="FM4" s="78"/>
-      <c r="FN4" s="78"/>
-      <c r="FO4" s="78"/>
-      <c r="FP4" s="78"/>
-      <c r="FQ4" s="78"/>
-      <c r="FR4" s="78"/>
-      <c r="FS4" s="79" t="s">
+      <c r="FF4" s="84"/>
+      <c r="FG4" s="84"/>
+      <c r="FH4" s="84"/>
+      <c r="FI4" s="84"/>
+      <c r="FJ4" s="84"/>
+      <c r="FK4" s="84"/>
+      <c r="FL4" s="84"/>
+      <c r="FM4" s="84"/>
+      <c r="FN4" s="84"/>
+      <c r="FO4" s="84"/>
+      <c r="FP4" s="84"/>
+      <c r="FQ4" s="84"/>
+      <c r="FR4" s="84"/>
+      <c r="FS4" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="79"/>
-      <c r="FU4" s="79"/>
-      <c r="FV4" s="79"/>
-      <c r="FW4" s="79"/>
-      <c r="FX4" s="79"/>
-      <c r="FY4" s="79"/>
-      <c r="FZ4" s="79"/>
-      <c r="GA4" s="79"/>
-      <c r="GB4" s="79"/>
-      <c r="GC4" s="79"/>
-      <c r="GD4" s="79"/>
-      <c r="GE4" s="79"/>
-      <c r="GF4" s="79"/>
-      <c r="GG4" s="67" t="s">
+      <c r="FT4" s="85"/>
+      <c r="FU4" s="85"/>
+      <c r="FV4" s="85"/>
+      <c r="FW4" s="85"/>
+      <c r="FX4" s="85"/>
+      <c r="FY4" s="85"/>
+      <c r="FZ4" s="85"/>
+      <c r="GA4" s="85"/>
+      <c r="GB4" s="85"/>
+      <c r="GC4" s="85"/>
+      <c r="GD4" s="85"/>
+      <c r="GE4" s="85"/>
+      <c r="GF4" s="85"/>
+      <c r="GG4" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="GH4" s="67"/>
-      <c r="GI4" s="67"/>
-      <c r="GJ4" s="67"/>
-      <c r="GK4" s="67"/>
-      <c r="GL4" s="67"/>
-      <c r="GM4" s="67"/>
-      <c r="GN4" s="67"/>
-      <c r="GO4" s="67"/>
-      <c r="GP4" s="67"/>
-      <c r="GQ4" s="67"/>
-      <c r="GR4" s="67"/>
-      <c r="GS4" s="67"/>
-      <c r="GT4" s="67"/>
-      <c r="GU4" s="67" t="s">
+      <c r="GH4" s="75"/>
+      <c r="GI4" s="75"/>
+      <c r="GJ4" s="75"/>
+      <c r="GK4" s="75"/>
+      <c r="GL4" s="75"/>
+      <c r="GM4" s="75"/>
+      <c r="GN4" s="75"/>
+      <c r="GO4" s="75"/>
+      <c r="GP4" s="75"/>
+      <c r="GQ4" s="75"/>
+      <c r="GR4" s="75"/>
+      <c r="GS4" s="75"/>
+      <c r="GT4" s="75"/>
+      <c r="GU4" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="GV4" s="67"/>
-      <c r="GW4" s="67"/>
-      <c r="GX4" s="67"/>
-      <c r="GY4" s="67"/>
-      <c r="GZ4" s="67"/>
-      <c r="HA4" s="67"/>
-      <c r="HB4" s="67"/>
-      <c r="HC4" s="67"/>
-      <c r="HD4" s="67"/>
-      <c r="HE4" s="67"/>
-      <c r="HF4" s="67"/>
-      <c r="HG4" s="67"/>
-      <c r="HH4" s="67"/>
-      <c r="HI4" s="67" t="s">
+      <c r="GV4" s="75"/>
+      <c r="GW4" s="75"/>
+      <c r="GX4" s="75"/>
+      <c r="GY4" s="75"/>
+      <c r="GZ4" s="75"/>
+      <c r="HA4" s="75"/>
+      <c r="HB4" s="75"/>
+      <c r="HC4" s="75"/>
+      <c r="HD4" s="75"/>
+      <c r="HE4" s="75"/>
+      <c r="HF4" s="75"/>
+      <c r="HG4" s="75"/>
+      <c r="HH4" s="75"/>
+      <c r="HI4" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="HJ4" s="67"/>
-      <c r="HK4" s="67"/>
-      <c r="HL4" s="67"/>
-      <c r="HM4" s="67"/>
-      <c r="HN4" s="67"/>
-      <c r="HO4" s="67"/>
-      <c r="HP4" s="67"/>
-      <c r="HQ4" s="67"/>
-      <c r="HR4" s="67"/>
-      <c r="HS4" s="67"/>
-      <c r="HT4" s="67"/>
-      <c r="HU4" s="67"/>
-      <c r="HV4" s="67"/>
-      <c r="HW4" s="68" t="s">
+      <c r="HJ4" s="75"/>
+      <c r="HK4" s="75"/>
+      <c r="HL4" s="75"/>
+      <c r="HM4" s="75"/>
+      <c r="HN4" s="75"/>
+      <c r="HO4" s="75"/>
+      <c r="HP4" s="75"/>
+      <c r="HQ4" s="75"/>
+      <c r="HR4" s="75"/>
+      <c r="HS4" s="75"/>
+      <c r="HT4" s="75"/>
+      <c r="HU4" s="75"/>
+      <c r="HV4" s="75"/>
+      <c r="HW4" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="68"/>
-      <c r="HY4" s="68"/>
-      <c r="HZ4" s="68"/>
-      <c r="IA4" s="68"/>
-      <c r="IB4" s="68"/>
-      <c r="IC4" s="68"/>
-      <c r="ID4" s="68"/>
-      <c r="IE4" s="68"/>
-      <c r="IF4" s="68"/>
-      <c r="IG4" s="68"/>
-      <c r="IH4" s="68"/>
-      <c r="II4" s="68"/>
-      <c r="IJ4" s="68"/>
-      <c r="IK4" s="68" t="s">
+      <c r="HX4" s="92"/>
+      <c r="HY4" s="92"/>
+      <c r="HZ4" s="92"/>
+      <c r="IA4" s="92"/>
+      <c r="IB4" s="92"/>
+      <c r="IC4" s="92"/>
+      <c r="ID4" s="92"/>
+      <c r="IE4" s="92"/>
+      <c r="IF4" s="92"/>
+      <c r="IG4" s="92"/>
+      <c r="IH4" s="92"/>
+      <c r="II4" s="92"/>
+      <c r="IJ4" s="92"/>
+      <c r="IK4" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="68"/>
-      <c r="IM4" s="68"/>
-      <c r="IN4" s="68"/>
-      <c r="IO4" s="68"/>
-      <c r="IP4" s="68"/>
-      <c r="IQ4" s="68"/>
-      <c r="IR4" s="68"/>
-      <c r="IS4" s="68"/>
-      <c r="IT4" s="68"/>
-      <c r="IU4" s="68"/>
-      <c r="IV4" s="68"/>
-      <c r="IW4" s="68"/>
-      <c r="IX4" s="68"/>
-      <c r="IY4" s="68" t="s">
+      <c r="IL4" s="92"/>
+      <c r="IM4" s="92"/>
+      <c r="IN4" s="92"/>
+      <c r="IO4" s="92"/>
+      <c r="IP4" s="92"/>
+      <c r="IQ4" s="92"/>
+      <c r="IR4" s="92"/>
+      <c r="IS4" s="92"/>
+      <c r="IT4" s="92"/>
+      <c r="IU4" s="92"/>
+      <c r="IV4" s="92"/>
+      <c r="IW4" s="92"/>
+      <c r="IX4" s="92"/>
+      <c r="IY4" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="68"/>
-      <c r="JA4" s="68"/>
-      <c r="JB4" s="68"/>
-      <c r="JC4" s="68"/>
-      <c r="JD4" s="68"/>
-      <c r="JE4" s="68"/>
-      <c r="JF4" s="68"/>
-      <c r="JG4" s="68"/>
-      <c r="JH4" s="68"/>
-      <c r="JI4" s="68"/>
-      <c r="JJ4" s="68"/>
-      <c r="JK4" s="68"/>
-      <c r="JL4" s="68"/>
-      <c r="JM4" s="69" t="s">
+      <c r="IZ4" s="92"/>
+      <c r="JA4" s="92"/>
+      <c r="JB4" s="92"/>
+      <c r="JC4" s="92"/>
+      <c r="JD4" s="92"/>
+      <c r="JE4" s="92"/>
+      <c r="JF4" s="92"/>
+      <c r="JG4" s="92"/>
+      <c r="JH4" s="92"/>
+      <c r="JI4" s="92"/>
+      <c r="JJ4" s="92"/>
+      <c r="JK4" s="92"/>
+      <c r="JL4" s="92"/>
+      <c r="JM4" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="69"/>
-      <c r="JO4" s="69"/>
-      <c r="JP4" s="69"/>
-      <c r="JQ4" s="69"/>
-      <c r="JR4" s="69"/>
-      <c r="JS4" s="69"/>
-      <c r="JT4" s="69"/>
-      <c r="JU4" s="69"/>
-      <c r="JV4" s="69"/>
-      <c r="JW4" s="69"/>
-      <c r="JX4" s="69"/>
-      <c r="JY4" s="69"/>
-      <c r="JZ4" s="65" t="s">
+      <c r="JN4" s="93"/>
+      <c r="JO4" s="93"/>
+      <c r="JP4" s="93"/>
+      <c r="JQ4" s="93"/>
+      <c r="JR4" s="93"/>
+      <c r="JS4" s="93"/>
+      <c r="JT4" s="93"/>
+      <c r="JU4" s="93"/>
+      <c r="JV4" s="93"/>
+      <c r="JW4" s="93"/>
+      <c r="JX4" s="93"/>
+      <c r="JY4" s="93"/>
+      <c r="JZ4" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="66"/>
-      <c r="KB4" s="66"/>
-      <c r="KC4" s="66"/>
-      <c r="KD4" s="66"/>
-      <c r="KE4" s="66"/>
-      <c r="KF4" s="66"/>
-      <c r="KG4" s="66"/>
-      <c r="KH4" s="61" t="s">
-        <v>322</v>
-      </c>
-      <c r="KI4" s="62"/>
-      <c r="KJ4" s="62"/>
-      <c r="KK4" s="62"/>
-      <c r="KL4" s="60"/>
+      <c r="KA4" s="91"/>
+      <c r="KB4" s="91"/>
+      <c r="KC4" s="91"/>
+      <c r="KD4" s="91"/>
+      <c r="KE4" s="91"/>
+      <c r="KF4" s="91"/>
+      <c r="KG4" s="91"/>
+      <c r="KH4" s="86" t="s">
+        <v>316</v>
+      </c>
+      <c r="KI4" s="87"/>
+      <c r="KJ4" s="87"/>
+      <c r="KK4" s="46"/>
     </row>
-    <row r="5" spans="1:298" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="83"/>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="85"/>
-      <c r="L5" s="85"/>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="86"/>
-      <c r="Q5" s="86"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="86"/>
-      <c r="T5" s="86"/>
-      <c r="U5" s="87"/>
-      <c r="V5" s="87"/>
-      <c r="W5" s="87"/>
-      <c r="X5" s="87"/>
-      <c r="Y5" s="87"/>
-      <c r="Z5" s="87"/>
-      <c r="AA5" s="87"/>
-      <c r="AB5" s="87"/>
-      <c r="AC5" s="88"/>
-      <c r="AD5" s="88"/>
-      <c r="AE5" s="88"/>
-      <c r="AF5" s="88"/>
-      <c r="AG5" s="88"/>
-      <c r="AH5" s="88"/>
-      <c r="AI5" s="88"/>
-      <c r="AJ5" s="89"/>
-      <c r="AK5" s="89"/>
-      <c r="AL5" s="89"/>
-      <c r="AM5" s="80"/>
-      <c r="AN5" s="80"/>
-      <c r="AO5" s="70"/>
-      <c r="AP5" s="70"/>
-      <c r="AQ5" s="70"/>
-      <c r="AR5" s="70"/>
-      <c r="AS5" s="71"/>
-      <c r="AT5" s="71"/>
-      <c r="AU5" s="71"/>
-      <c r="AV5" s="71"/>
-      <c r="AW5" s="71"/>
-      <c r="AX5" s="71"/>
-      <c r="AY5" s="71"/>
-      <c r="AZ5" s="71"/>
-      <c r="BA5" s="71"/>
-      <c r="BB5" s="71"/>
-      <c r="BC5" s="71"/>
-      <c r="BD5" s="71"/>
-      <c r="BE5" s="71"/>
-      <c r="BF5" s="71"/>
-      <c r="BG5" s="71"/>
-      <c r="BH5" s="71"/>
-      <c r="BI5" s="71"/>
-      <c r="BJ5" s="71"/>
+    <row r="5" spans="1:300" ht="12" customHeight="1">
+      <c r="A5" s="68"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="71"/>
+      <c r="Q5" s="71"/>
+      <c r="R5" s="71"/>
+      <c r="S5" s="71"/>
+      <c r="T5" s="71"/>
+      <c r="U5" s="72"/>
+      <c r="V5" s="72"/>
+      <c r="W5" s="72"/>
+      <c r="X5" s="72"/>
+      <c r="Y5" s="72"/>
+      <c r="Z5" s="72"/>
+      <c r="AA5" s="72"/>
+      <c r="AB5" s="72"/>
+      <c r="AC5" s="73"/>
+      <c r="AD5" s="73"/>
+      <c r="AE5" s="73"/>
+      <c r="AF5" s="73"/>
+      <c r="AG5" s="73"/>
+      <c r="AH5" s="73"/>
+      <c r="AI5" s="73"/>
+      <c r="AJ5" s="74"/>
+      <c r="AK5" s="74"/>
+      <c r="AL5" s="74"/>
+      <c r="AM5" s="65"/>
+      <c r="AN5" s="65"/>
+      <c r="AO5" s="76"/>
+      <c r="AP5" s="76"/>
+      <c r="AQ5" s="76"/>
+      <c r="AR5" s="76"/>
+      <c r="AS5" s="77"/>
+      <c r="AT5" s="77"/>
+      <c r="AU5" s="77"/>
+      <c r="AV5" s="77"/>
+      <c r="AW5" s="77"/>
+      <c r="AX5" s="77"/>
+      <c r="AY5" s="77"/>
+      <c r="AZ5" s="77"/>
+      <c r="BA5" s="77"/>
+      <c r="BB5" s="77"/>
+      <c r="BC5" s="77"/>
+      <c r="BD5" s="77"/>
+      <c r="BE5" s="77"/>
+      <c r="BF5" s="77"/>
+      <c r="BG5" s="77"/>
+      <c r="BH5" s="77"/>
+      <c r="BI5" s="77"/>
+      <c r="BJ5" s="77"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -3466,7 +3497,7 @@
         <v>314</v>
       </c>
       <c r="BX5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="BY5" s="8" t="s">
         <v>27</v>
@@ -3508,7 +3539,7 @@
         <v>314</v>
       </c>
       <c r="CL5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="CM5" s="8" t="s">
         <v>27</v>
@@ -3550,7 +3581,7 @@
         <v>314</v>
       </c>
       <c r="CZ5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="DA5" s="8" t="s">
         <v>27</v>
@@ -3592,7 +3623,7 @@
         <v>314</v>
       </c>
       <c r="DN5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="DO5" s="8" t="s">
         <v>27</v>
@@ -3634,7 +3665,7 @@
         <v>314</v>
       </c>
       <c r="EB5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="EC5" s="8" t="s">
         <v>27</v>
@@ -3676,7 +3707,7 @@
         <v>314</v>
       </c>
       <c r="EP5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="EQ5" s="8" t="s">
         <v>27</v>
@@ -3718,7 +3749,7 @@
         <v>314</v>
       </c>
       <c r="FD5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="FE5" s="8" t="s">
         <v>27</v>
@@ -3760,7 +3791,7 @@
         <v>314</v>
       </c>
       <c r="FR5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="FS5" s="8" t="s">
         <v>27</v>
@@ -3802,7 +3833,7 @@
         <v>314</v>
       </c>
       <c r="GF5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="GG5" s="8" t="s">
         <v>27</v>
@@ -3844,7 +3875,7 @@
         <v>314</v>
       </c>
       <c r="GT5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="GU5" s="8" t="s">
         <v>27</v>
@@ -3886,7 +3917,7 @@
         <v>314</v>
       </c>
       <c r="HH5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="HI5" s="8" t="s">
         <v>27</v>
@@ -3928,7 +3959,7 @@
         <v>314</v>
       </c>
       <c r="HV5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="HW5" s="8" t="s">
         <v>27</v>
@@ -3970,7 +4001,7 @@
         <v>314</v>
       </c>
       <c r="IJ5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="IK5" s="8" t="s">
         <v>27</v>
@@ -4012,7 +4043,7 @@
         <v>314</v>
       </c>
       <c r="IX5" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="IY5" s="8" t="s">
         <v>27</v>
@@ -4054,40 +4085,39 @@
         <v>314</v>
       </c>
       <c r="JL5" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="JM5" s="69"/>
-      <c r="JN5" s="69"/>
-      <c r="JO5" s="69"/>
-      <c r="JP5" s="69"/>
-      <c r="JQ5" s="69"/>
-      <c r="JR5" s="69"/>
-      <c r="JS5" s="69"/>
-      <c r="JT5" s="69"/>
-      <c r="JU5" s="69"/>
-      <c r="JV5" s="69"/>
-      <c r="JW5" s="69"/>
-      <c r="JX5" s="69"/>
-      <c r="JY5" s="69"/>
-      <c r="JZ5" s="66" t="s">
-        <v>316</v>
-      </c>
-      <c r="KA5" s="66"/>
-      <c r="KB5" s="66"/>
-      <c r="KC5" s="66"/>
-      <c r="KD5" s="66" t="s">
+        <v>315</v>
+      </c>
+      <c r="JM5" s="93"/>
+      <c r="JN5" s="93"/>
+      <c r="JO5" s="93"/>
+      <c r="JP5" s="93"/>
+      <c r="JQ5" s="93"/>
+      <c r="JR5" s="93"/>
+      <c r="JS5" s="93"/>
+      <c r="JT5" s="93"/>
+      <c r="JU5" s="93"/>
+      <c r="JV5" s="93"/>
+      <c r="JW5" s="93"/>
+      <c r="JX5" s="93"/>
+      <c r="JY5" s="93"/>
+      <c r="JZ5" s="91" t="s">
+        <v>347</v>
+      </c>
+      <c r="KA5" s="91"/>
+      <c r="KB5" s="91"/>
+      <c r="KC5" s="91"/>
+      <c r="KD5" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="66"/>
-      <c r="KF5" s="66"/>
-      <c r="KG5" s="66"/>
-      <c r="KH5" s="63"/>
-      <c r="KI5" s="64"/>
-      <c r="KJ5" s="64"/>
-      <c r="KK5" s="64"/>
-      <c r="KL5" s="60"/>
+      <c r="KE5" s="91"/>
+      <c r="KF5" s="91"/>
+      <c r="KG5" s="91"/>
+      <c r="KH5" s="88"/>
+      <c r="KI5" s="89"/>
+      <c r="KJ5" s="89"/>
+      <c r="KK5" s="46"/>
     </row>
-    <row r="6" spans="1:298" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:300" ht="81.75" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -4314,7 +4344,7 @@
         <v>113</v>
       </c>
       <c r="BX6" s="22" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="BY6" s="22" t="s">
         <v>114</v>
@@ -4356,7 +4386,7 @@
         <v>126</v>
       </c>
       <c r="CL6" s="22" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="CM6" s="22" t="s">
         <v>127</v>
@@ -4398,7 +4428,7 @@
         <v>139</v>
       </c>
       <c r="CZ6" s="22" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="DA6" s="22" t="s">
         <v>140</v>
@@ -4440,7 +4470,7 @@
         <v>152</v>
       </c>
       <c r="DN6" s="22" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="DO6" s="22" t="s">
         <v>153</v>
@@ -4482,7 +4512,7 @@
         <v>165</v>
       </c>
       <c r="EB6" s="22" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="EC6" s="22" t="s">
         <v>166</v>
@@ -4524,7 +4554,7 @@
         <v>178</v>
       </c>
       <c r="EP6" s="12" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="EQ6" s="12" t="s">
         <v>179</v>
@@ -4566,7 +4596,7 @@
         <v>191</v>
       </c>
       <c r="FD6" s="12" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="FE6" s="12" t="s">
         <v>192</v>
@@ -4608,7 +4638,7 @@
         <v>204</v>
       </c>
       <c r="FR6" s="12" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="FS6" s="22" t="s">
         <v>205</v>
@@ -4650,7 +4680,7 @@
         <v>217</v>
       </c>
       <c r="GF6" s="22" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="GG6" s="22" t="s">
         <v>218</v>
@@ -4692,7 +4722,7 @@
         <v>230</v>
       </c>
       <c r="GT6" s="22" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="GU6" s="22" t="s">
         <v>231</v>
@@ -4734,7 +4764,7 @@
         <v>243</v>
       </c>
       <c r="HH6" s="22" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="HI6" s="22" t="s">
         <v>244</v>
@@ -4776,7 +4806,7 @@
         <v>256</v>
       </c>
       <c r="HV6" s="22" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="HW6" s="22" t="s">
         <v>257</v>
@@ -4818,7 +4848,7 @@
         <v>269</v>
       </c>
       <c r="IJ6" s="22" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="IK6" s="22" t="s">
         <v>270</v>
@@ -4860,7 +4890,7 @@
         <v>282</v>
       </c>
       <c r="IX6" s="22" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="IY6" s="22" t="s">
         <v>283</v>
@@ -4902,7 +4932,7 @@
         <v>295</v>
       </c>
       <c r="JL6" s="22" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="JM6" s="22" t="s">
         <v>296</v>
@@ -4944,21 +4974,21 @@
         <v>308</v>
       </c>
       <c r="JZ6" s="22" t="s">
-        <v>315</v>
-      </c>
-      <c r="KA6" s="34" t="s">
-        <v>317</v>
+        <v>344</v>
+      </c>
+      <c r="KA6" s="29" t="s">
+        <v>343</v>
       </c>
       <c r="KB6" s="22" t="s">
-        <v>318</v>
+        <v>345</v>
       </c>
       <c r="KC6" s="22" t="s">
-        <v>319</v>
+        <v>346</v>
       </c>
       <c r="KD6" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="KE6" s="34" t="s">
+      <c r="KE6" s="29" t="s">
         <v>312</v>
       </c>
       <c r="KF6" s="22" t="s">
@@ -4968,470 +4998,1682 @@
         <v>311</v>
       </c>
       <c r="KH6" s="22" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="KI6" s="22" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="KJ6" s="22" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="KK6" s="22" t="s">
-        <v>326</v>
-      </c>
-      <c r="KL6" s="22" t="s">
-        <v>342</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="KL6" s="49" t="s">
+        <v>336</v>
+      </c>
+      <c r="KM6" s="50"/>
+      <c r="KN6" s="51"/>
     </row>
-    <row r="7" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32" t="s">
-        <v>343</v>
-      </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53" t="s">
-        <v>343</v>
-      </c>
-      <c r="S7" s="53" t="s">
-        <v>343</v>
-      </c>
-      <c r="T7" s="53"/>
-      <c r="U7" s="53"/>
-      <c r="V7" s="53"/>
-      <c r="W7" s="53"/>
-      <c r="X7" s="54" t="s">
-        <v>343</v>
-      </c>
-      <c r="Y7" s="54" t="s">
-        <v>343</v>
-      </c>
-      <c r="Z7" s="53"/>
-      <c r="AA7" s="53"/>
-      <c r="AB7" s="54"/>
-      <c r="AC7" s="55"/>
-      <c r="AD7" s="56"/>
-      <c r="AE7" s="56"/>
-      <c r="AF7" s="31"/>
-      <c r="AG7" s="31"/>
-      <c r="AH7" s="57"/>
-      <c r="AI7" s="31"/>
-      <c r="AJ7" s="52" t="s">
-        <v>343</v>
-      </c>
-      <c r="AK7" s="52" t="s">
-        <v>343</v>
-      </c>
-      <c r="AL7" s="52" t="s">
-        <v>343</v>
-      </c>
-      <c r="AM7" s="53"/>
-      <c r="AN7" s="58"/>
-      <c r="AO7" s="51"/>
-      <c r="AP7" s="51"/>
-      <c r="AQ7" s="51"/>
-      <c r="AR7" s="51"/>
-      <c r="AS7" s="33">
+    <row r="7" spans="1:300" ht="15" customHeight="1">
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52" t="s">
+        <v>341</v>
+      </c>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54" t="s">
+        <v>341</v>
+      </c>
+      <c r="S7" s="54" t="s">
+        <v>341</v>
+      </c>
+      <c r="T7" s="54"/>
+      <c r="U7" s="54"/>
+      <c r="V7" s="54"/>
+      <c r="W7" s="54"/>
+      <c r="X7" s="55" t="s">
+        <v>341</v>
+      </c>
+      <c r="Y7" s="55" t="s">
+        <v>341</v>
+      </c>
+      <c r="Z7" s="54"/>
+      <c r="AA7" s="54"/>
+      <c r="AB7" s="55"/>
+      <c r="AC7" s="56"/>
+      <c r="AD7" s="57"/>
+      <c r="AE7" s="57"/>
+      <c r="AF7" s="58"/>
+      <c r="AG7" s="58"/>
+      <c r="AH7" s="59"/>
+      <c r="AI7" s="58"/>
+      <c r="AJ7" s="53" t="s">
+        <v>341</v>
+      </c>
+      <c r="AK7" s="53" t="s">
+        <v>341</v>
+      </c>
+      <c r="AL7" s="53" t="s">
+        <v>341</v>
+      </c>
+      <c r="AM7" s="54"/>
+      <c r="AN7" s="60"/>
+      <c r="AO7" s="61"/>
+      <c r="AP7" s="61"/>
+      <c r="AQ7" s="61"/>
+      <c r="AR7" s="61"/>
+      <c r="AS7" s="62">
         <f>SUM(BK7:BX7)</f>
         <v>0</v>
       </c>
-      <c r="AT7" s="30">
+      <c r="AT7" s="63">
         <f>SUM(BY7:CL7)</f>
         <v>0</v>
       </c>
-      <c r="AU7" s="30">
+      <c r="AU7" s="63">
         <f>SUM(CM7:CZ7)</f>
         <v>0</v>
       </c>
-      <c r="AV7" s="30">
+      <c r="AV7" s="63">
         <f>SUM(DA7:DN7)</f>
         <v>0</v>
       </c>
-      <c r="AW7" s="30">
+      <c r="AW7" s="63">
         <f>SUM(DO7:EB7)</f>
         <v>0</v>
       </c>
-      <c r="AX7" s="30">
+      <c r="AX7" s="63">
         <f>SUM(EC7:EP7)</f>
         <v>0</v>
       </c>
-      <c r="AY7" s="30">
+      <c r="AY7" s="63">
         <f>SUM(EQ7:FD7)</f>
         <v>0</v>
       </c>
-      <c r="AZ7" s="30">
+      <c r="AZ7" s="63">
         <f>SUM(FE7:FR7)</f>
         <v>0</v>
       </c>
-      <c r="BA7" s="30">
+      <c r="BA7" s="63">
         <f>SUM(FS7:GF7)</f>
         <v>0</v>
       </c>
-      <c r="BB7" s="30">
+      <c r="BB7" s="63">
         <f>SUM(GG7:GT7)</f>
         <v>0</v>
       </c>
-      <c r="BC7" s="30">
+      <c r="BC7" s="63">
         <f>SUM(GU7:HH7)</f>
         <v>0</v>
       </c>
-      <c r="BD7" s="30">
+      <c r="BD7" s="63">
         <f>SUM(HI7:HV7)</f>
         <v>0</v>
       </c>
-      <c r="BE7" s="30">
+      <c r="BE7" s="63">
         <f>SUM(HW7:IJ7)</f>
         <v>0</v>
       </c>
-      <c r="BF7" s="30">
+      <c r="BF7" s="63">
         <f>SUM(IK7:IX7)</f>
         <v>0</v>
       </c>
-      <c r="BG7" s="30">
+      <c r="BG7" s="63">
         <f>SUM(IY7:JL7)</f>
         <v>0</v>
       </c>
-      <c r="BH7" s="30">
+      <c r="BH7" s="63">
         <f t="shared" ref="BH7" si="0">JM7</f>
         <v>0</v>
       </c>
-      <c r="BI7" s="30">
+      <c r="BI7" s="63">
         <f>JN7</f>
         <v>0</v>
       </c>
-      <c r="BJ7" s="30">
+      <c r="BJ7" s="63">
         <f>JO7</f>
         <v>0</v>
       </c>
-      <c r="BK7" s="30">
-        <f t="shared" ref="BK7" si="1">BY7+CM7+DA7+DO7+EC7+EQ7+FE7+FS7</f>
+      <c r="BK7" s="63">
+        <f t="shared" ref="BK7:BX7" si="1">BY7+CM7+DA7+DO7+EC7+EQ7+FE7+FS7</f>
         <v>0</v>
       </c>
-      <c r="BL7" s="30">
-        <f t="shared" ref="BL7:BX7" si="2">BZ7+CN7+DB7+DP7+ED7+ER7+FF7+FT7</f>
+      <c r="BL7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BM7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BM7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BN7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BN7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BO7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BO7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BP7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BP7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BQ7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BQ7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BR7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BR7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BS7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BS7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BT7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BT7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BU7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BU7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BV7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BV7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BW7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BW7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BX7" s="30">
-        <f t="shared" si="2"/>
+      <c r="BX7" s="63">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BY7" s="31"/>
-      <c r="BZ7" s="31"/>
-      <c r="CA7" s="31"/>
-      <c r="CB7" s="31"/>
-      <c r="CC7" s="31"/>
-      <c r="CD7" s="31"/>
-      <c r="CE7" s="31"/>
-      <c r="CF7" s="31"/>
-      <c r="CG7" s="31"/>
-      <c r="CH7" s="31"/>
-      <c r="CI7" s="31"/>
-      <c r="CJ7" s="31"/>
-      <c r="CK7" s="31"/>
-      <c r="CL7" s="31"/>
-      <c r="CM7" s="31"/>
-      <c r="CN7" s="31"/>
-      <c r="CO7" s="31"/>
-      <c r="CP7" s="31"/>
-      <c r="CQ7" s="31"/>
-      <c r="CR7" s="31"/>
-      <c r="CS7" s="31"/>
-      <c r="CT7" s="31"/>
-      <c r="CU7" s="31"/>
-      <c r="CV7" s="31"/>
-      <c r="CW7" s="31"/>
-      <c r="CX7" s="31"/>
-      <c r="CY7" s="31"/>
-      <c r="CZ7" s="31"/>
-      <c r="DA7" s="31"/>
-      <c r="DB7" s="31"/>
-      <c r="DC7" s="31"/>
-      <c r="DD7" s="31"/>
-      <c r="DE7" s="31"/>
-      <c r="DF7" s="31"/>
-      <c r="DG7" s="31"/>
-      <c r="DH7" s="31"/>
-      <c r="DI7" s="31"/>
-      <c r="DJ7" s="31"/>
-      <c r="DK7" s="31"/>
-      <c r="DL7" s="31"/>
-      <c r="DM7" s="31"/>
-      <c r="DN7" s="31"/>
-      <c r="DO7" s="31"/>
-      <c r="DP7" s="31"/>
-      <c r="DQ7" s="31"/>
-      <c r="DR7" s="31"/>
-      <c r="DS7" s="31"/>
-      <c r="DT7" s="31"/>
-      <c r="DU7" s="31"/>
-      <c r="DV7" s="31"/>
-      <c r="DW7" s="31"/>
-      <c r="DX7" s="31"/>
-      <c r="DY7" s="31"/>
-      <c r="DZ7" s="31"/>
-      <c r="EA7" s="31"/>
-      <c r="EB7" s="31"/>
-      <c r="EC7" s="31"/>
-      <c r="ED7" s="31"/>
-      <c r="EE7" s="31"/>
-      <c r="EF7" s="31"/>
-      <c r="EG7" s="31"/>
-      <c r="EH7" s="31"/>
-      <c r="EI7" s="31"/>
-      <c r="EJ7" s="31"/>
-      <c r="EK7" s="31"/>
-      <c r="EL7" s="31"/>
-      <c r="EM7" s="31"/>
-      <c r="EN7" s="31"/>
-      <c r="EO7" s="31"/>
-      <c r="EP7" s="31"/>
-      <c r="EQ7" s="31"/>
-      <c r="ER7" s="31"/>
-      <c r="ES7" s="31"/>
-      <c r="ET7" s="31"/>
-      <c r="EU7" s="31"/>
-      <c r="EV7" s="31"/>
-      <c r="EW7" s="31"/>
-      <c r="EX7" s="31"/>
-      <c r="EY7" s="31"/>
-      <c r="EZ7" s="31"/>
-      <c r="FA7" s="31"/>
-      <c r="FB7" s="31"/>
-      <c r="FC7" s="31"/>
-      <c r="FD7" s="31"/>
-      <c r="FE7" s="31"/>
-      <c r="FF7" s="31"/>
-      <c r="FG7" s="31"/>
-      <c r="FH7" s="31"/>
-      <c r="FI7" s="31"/>
-      <c r="FJ7" s="31"/>
-      <c r="FK7" s="31"/>
-      <c r="FL7" s="31"/>
-      <c r="FM7" s="31"/>
-      <c r="FN7" s="31"/>
-      <c r="FO7" s="31"/>
-      <c r="FP7" s="31"/>
-      <c r="FQ7" s="31"/>
-      <c r="FR7" s="31"/>
-      <c r="FS7" s="31"/>
-      <c r="FT7" s="31"/>
-      <c r="FU7" s="31"/>
-      <c r="FV7" s="31"/>
-      <c r="FW7" s="31"/>
-      <c r="FX7" s="31"/>
-      <c r="FY7" s="31"/>
-      <c r="FZ7" s="31"/>
-      <c r="GA7" s="31"/>
-      <c r="GB7" s="31"/>
-      <c r="GC7" s="31"/>
-      <c r="GD7" s="31"/>
-      <c r="GE7" s="31"/>
-      <c r="GF7" s="31"/>
-      <c r="GG7" s="31"/>
-      <c r="GH7" s="31"/>
-      <c r="GI7" s="31"/>
-      <c r="GJ7" s="31"/>
-      <c r="GK7" s="31"/>
-      <c r="GL7" s="31"/>
-      <c r="GM7" s="31"/>
-      <c r="GN7" s="31"/>
-      <c r="GO7" s="31"/>
-      <c r="GP7" s="31"/>
-      <c r="GQ7" s="31"/>
-      <c r="GR7" s="31"/>
-      <c r="GS7" s="31"/>
-      <c r="GT7" s="31"/>
-      <c r="GU7" s="31"/>
-      <c r="GV7" s="31"/>
-      <c r="GW7" s="31"/>
-      <c r="GX7" s="31"/>
-      <c r="GY7" s="31"/>
-      <c r="GZ7" s="31"/>
-      <c r="HA7" s="31"/>
-      <c r="HB7" s="31"/>
-      <c r="HC7" s="31"/>
-      <c r="HD7" s="31"/>
-      <c r="HE7" s="31"/>
-      <c r="HF7" s="31"/>
-      <c r="HG7" s="31"/>
-      <c r="HH7" s="31"/>
-      <c r="HI7" s="31"/>
-      <c r="HJ7" s="31"/>
-      <c r="HK7" s="31"/>
-      <c r="HL7" s="31"/>
-      <c r="HM7" s="31"/>
-      <c r="HN7" s="31"/>
-      <c r="HO7" s="31"/>
-      <c r="HP7" s="31"/>
-      <c r="HQ7" s="31"/>
-      <c r="HR7" s="31"/>
-      <c r="HS7" s="31"/>
-      <c r="HT7" s="31"/>
-      <c r="HU7" s="31"/>
-      <c r="HV7" s="31"/>
-      <c r="HW7" s="31"/>
-      <c r="HX7" s="31"/>
-      <c r="HY7" s="31"/>
-      <c r="HZ7" s="31"/>
-      <c r="IA7" s="31"/>
-      <c r="IB7" s="31"/>
-      <c r="IC7" s="31"/>
-      <c r="ID7" s="31"/>
-      <c r="IE7" s="31"/>
-      <c r="IF7" s="31"/>
-      <c r="IG7" s="31"/>
-      <c r="IH7" s="31"/>
-      <c r="II7" s="31"/>
-      <c r="IJ7" s="31"/>
-      <c r="IK7" s="31"/>
-      <c r="IL7" s="31"/>
-      <c r="IM7" s="31"/>
-      <c r="IN7" s="31"/>
-      <c r="IO7" s="31"/>
-      <c r="IP7" s="31"/>
-      <c r="IQ7" s="31"/>
-      <c r="IR7" s="31"/>
-      <c r="IS7" s="31"/>
-      <c r="IT7" s="31"/>
-      <c r="IU7" s="31"/>
-      <c r="IV7" s="31"/>
-      <c r="IW7" s="31"/>
-      <c r="IX7" s="31"/>
-      <c r="IY7" s="31"/>
-      <c r="IZ7" s="31"/>
-      <c r="JA7" s="31"/>
-      <c r="JB7" s="31"/>
-      <c r="JC7" s="31"/>
-      <c r="JD7" s="31"/>
-      <c r="JE7" s="31"/>
-      <c r="JF7" s="31"/>
-      <c r="JG7" s="31"/>
-      <c r="JH7" s="31"/>
-      <c r="JI7" s="31"/>
-      <c r="JJ7" s="31"/>
-      <c r="JK7" s="31"/>
-      <c r="JL7" s="31"/>
-      <c r="JM7" s="31"/>
-      <c r="JN7" s="31"/>
-      <c r="JO7" s="31"/>
-      <c r="JP7" s="52"/>
-      <c r="JQ7" s="52"/>
-      <c r="JR7" s="52"/>
-      <c r="JS7" s="59"/>
-      <c r="JT7" s="59"/>
-      <c r="JU7" s="59"/>
-      <c r="JV7" s="59"/>
-      <c r="JW7" s="59"/>
-      <c r="JX7" s="59"/>
-      <c r="JY7" s="59"/>
-      <c r="JZ7" s="30">
-        <f>SUM(BP7:BQ7)</f>
+      <c r="BY7" s="58"/>
+      <c r="BZ7" s="58"/>
+      <c r="CA7" s="58"/>
+      <c r="CB7" s="58"/>
+      <c r="CC7" s="58"/>
+      <c r="CD7" s="58"/>
+      <c r="CE7" s="58"/>
+      <c r="CF7" s="58"/>
+      <c r="CG7" s="58"/>
+      <c r="CH7" s="58"/>
+      <c r="CI7" s="58"/>
+      <c r="CJ7" s="58"/>
+      <c r="CK7" s="58"/>
+      <c r="CL7" s="58"/>
+      <c r="CM7" s="58"/>
+      <c r="CN7" s="58"/>
+      <c r="CO7" s="58"/>
+      <c r="CP7" s="58"/>
+      <c r="CQ7" s="58"/>
+      <c r="CR7" s="58"/>
+      <c r="CS7" s="58"/>
+      <c r="CT7" s="58"/>
+      <c r="CU7" s="58"/>
+      <c r="CV7" s="58"/>
+      <c r="CW7" s="58"/>
+      <c r="CX7" s="58"/>
+      <c r="CY7" s="58"/>
+      <c r="CZ7" s="58"/>
+      <c r="DA7" s="58"/>
+      <c r="DB7" s="58"/>
+      <c r="DC7" s="58"/>
+      <c r="DD7" s="58"/>
+      <c r="DE7" s="58"/>
+      <c r="DF7" s="58"/>
+      <c r="DG7" s="58"/>
+      <c r="DH7" s="58"/>
+      <c r="DI7" s="58"/>
+      <c r="DJ7" s="58"/>
+      <c r="DK7" s="58"/>
+      <c r="DL7" s="58"/>
+      <c r="DM7" s="58"/>
+      <c r="DN7" s="58"/>
+      <c r="DO7" s="58"/>
+      <c r="DP7" s="58"/>
+      <c r="DQ7" s="58"/>
+      <c r="DR7" s="58"/>
+      <c r="DS7" s="58"/>
+      <c r="DT7" s="58"/>
+      <c r="DU7" s="58"/>
+      <c r="DV7" s="58"/>
+      <c r="DW7" s="58"/>
+      <c r="DX7" s="58"/>
+      <c r="DY7" s="58"/>
+      <c r="DZ7" s="58"/>
+      <c r="EA7" s="58"/>
+      <c r="EB7" s="58"/>
+      <c r="EC7" s="58"/>
+      <c r="ED7" s="58"/>
+      <c r="EE7" s="58"/>
+      <c r="EF7" s="58"/>
+      <c r="EG7" s="58"/>
+      <c r="EH7" s="58"/>
+      <c r="EI7" s="58"/>
+      <c r="EJ7" s="58"/>
+      <c r="EK7" s="58"/>
+      <c r="EL7" s="58"/>
+      <c r="EM7" s="58"/>
+      <c r="EN7" s="58"/>
+      <c r="EO7" s="58"/>
+      <c r="EP7" s="58"/>
+      <c r="EQ7" s="58"/>
+      <c r="ER7" s="58"/>
+      <c r="ES7" s="58"/>
+      <c r="ET7" s="58"/>
+      <c r="EU7" s="58"/>
+      <c r="EV7" s="58"/>
+      <c r="EW7" s="58"/>
+      <c r="EX7" s="58"/>
+      <c r="EY7" s="58"/>
+      <c r="EZ7" s="58"/>
+      <c r="FA7" s="58"/>
+      <c r="FB7" s="58"/>
+      <c r="FC7" s="58"/>
+      <c r="FD7" s="58"/>
+      <c r="FE7" s="58"/>
+      <c r="FF7" s="58"/>
+      <c r="FG7" s="58"/>
+      <c r="FH7" s="58"/>
+      <c r="FI7" s="58"/>
+      <c r="FJ7" s="58"/>
+      <c r="FK7" s="58"/>
+      <c r="FL7" s="58"/>
+      <c r="FM7" s="58"/>
+      <c r="FN7" s="58"/>
+      <c r="FO7" s="58"/>
+      <c r="FP7" s="58"/>
+      <c r="FQ7" s="58"/>
+      <c r="FR7" s="58"/>
+      <c r="FS7" s="58"/>
+      <c r="FT7" s="58"/>
+      <c r="FU7" s="58"/>
+      <c r="FV7" s="58"/>
+      <c r="FW7" s="58"/>
+      <c r="FX7" s="58"/>
+      <c r="FY7" s="58"/>
+      <c r="FZ7" s="58"/>
+      <c r="GA7" s="58"/>
+      <c r="GB7" s="58"/>
+      <c r="GC7" s="58"/>
+      <c r="GD7" s="58"/>
+      <c r="GE7" s="58"/>
+      <c r="GF7" s="58"/>
+      <c r="GG7" s="58"/>
+      <c r="GH7" s="58"/>
+      <c r="GI7" s="58"/>
+      <c r="GJ7" s="58"/>
+      <c r="GK7" s="58"/>
+      <c r="GL7" s="58"/>
+      <c r="GM7" s="58"/>
+      <c r="GN7" s="58"/>
+      <c r="GO7" s="58"/>
+      <c r="GP7" s="58"/>
+      <c r="GQ7" s="58"/>
+      <c r="GR7" s="58"/>
+      <c r="GS7" s="58"/>
+      <c r="GT7" s="58"/>
+      <c r="GU7" s="58"/>
+      <c r="GV7" s="58"/>
+      <c r="GW7" s="58"/>
+      <c r="GX7" s="58"/>
+      <c r="GY7" s="58"/>
+      <c r="GZ7" s="58"/>
+      <c r="HA7" s="58"/>
+      <c r="HB7" s="58"/>
+      <c r="HC7" s="58"/>
+      <c r="HD7" s="58"/>
+      <c r="HE7" s="58"/>
+      <c r="HF7" s="58"/>
+      <c r="HG7" s="58"/>
+      <c r="HH7" s="58"/>
+      <c r="HI7" s="58"/>
+      <c r="HJ7" s="58"/>
+      <c r="HK7" s="58"/>
+      <c r="HL7" s="58"/>
+      <c r="HM7" s="58"/>
+      <c r="HN7" s="58"/>
+      <c r="HO7" s="58"/>
+      <c r="HP7" s="58"/>
+      <c r="HQ7" s="58"/>
+      <c r="HR7" s="58"/>
+      <c r="HS7" s="58"/>
+      <c r="HT7" s="58"/>
+      <c r="HU7" s="58"/>
+      <c r="HV7" s="58"/>
+      <c r="HW7" s="58"/>
+      <c r="HX7" s="58"/>
+      <c r="HY7" s="58"/>
+      <c r="HZ7" s="58"/>
+      <c r="IA7" s="58"/>
+      <c r="IB7" s="58"/>
+      <c r="IC7" s="58"/>
+      <c r="ID7" s="58"/>
+      <c r="IE7" s="58"/>
+      <c r="IF7" s="58"/>
+      <c r="IG7" s="58"/>
+      <c r="IH7" s="58"/>
+      <c r="II7" s="58"/>
+      <c r="IJ7" s="58"/>
+      <c r="IK7" s="58"/>
+      <c r="IL7" s="58"/>
+      <c r="IM7" s="58"/>
+      <c r="IN7" s="58"/>
+      <c r="IO7" s="58"/>
+      <c r="IP7" s="58"/>
+      <c r="IQ7" s="58"/>
+      <c r="IR7" s="58"/>
+      <c r="IS7" s="58"/>
+      <c r="IT7" s="58"/>
+      <c r="IU7" s="58"/>
+      <c r="IV7" s="58"/>
+      <c r="IW7" s="58"/>
+      <c r="IX7" s="58"/>
+      <c r="IY7" s="58"/>
+      <c r="IZ7" s="58"/>
+      <c r="JA7" s="58"/>
+      <c r="JB7" s="58"/>
+      <c r="JC7" s="58"/>
+      <c r="JD7" s="58"/>
+      <c r="JE7" s="58"/>
+      <c r="JF7" s="58"/>
+      <c r="JG7" s="58"/>
+      <c r="JH7" s="58"/>
+      <c r="JI7" s="58"/>
+      <c r="JJ7" s="58"/>
+      <c r="JK7" s="58"/>
+      <c r="JL7" s="58"/>
+      <c r="JM7" s="58"/>
+      <c r="JN7" s="58"/>
+      <c r="JO7" s="58"/>
+      <c r="JP7" s="53"/>
+      <c r="JQ7" s="53"/>
+      <c r="JR7" s="53"/>
+      <c r="JS7" s="64"/>
+      <c r="JT7" s="64"/>
+      <c r="JU7" s="64"/>
+      <c r="JV7" s="64"/>
+      <c r="JW7" s="64"/>
+      <c r="JX7" s="64"/>
+      <c r="JY7" s="64"/>
+      <c r="JZ7" s="63">
+        <f>BQ7</f>
         <v>0</v>
       </c>
-      <c r="KA7" s="30">
-        <f>SUM(CD7:CE7)+SUM(CR7:CS7)</f>
+      <c r="KA7" s="63">
+        <f>CE7+CS7</f>
         <v>0</v>
       </c>
-      <c r="KB7" s="30">
-        <f>SUM(DF7:DG7)+SUM(DT7:DU7)+SUM(EH7:EI7)+SUM(EV7:EW7)+SUM(FJ7:FK7)+SUM(FX7:FY7)</f>
+      <c r="KB7" s="63">
+        <f>DG7+DU7+EI7+EW7+FK7+FY7</f>
         <v>0</v>
       </c>
-      <c r="KC7" s="30">
-        <f>SUM(GL7:GM7)+SUM(IB7:IC7)</f>
+      <c r="KC7" s="63">
+        <f>GM7+IC7</f>
         <v>0</v>
       </c>
-      <c r="KD7" s="30">
+      <c r="KD7" s="63">
         <f>SUM(BL7:BQ7)</f>
         <v>0</v>
       </c>
-      <c r="KE7" s="30">
+      <c r="KE7" s="63">
         <f>SUM(CN7:CS7)+SUM(BZ7:CE7)</f>
         <v>0</v>
       </c>
-      <c r="KF7" s="30">
+      <c r="KF7" s="63">
         <f>SUM(DB7:DG7)+SUM(DP7:DU7)+SUM(ED7:EI7)+SUM(ER7:EW7)+SUM(FF7:FK7)+SUM(FT7:FY7)</f>
         <v>0</v>
       </c>
-      <c r="KG7" s="30">
+      <c r="KG7" s="63">
         <f>SUM(GH7:GM7)+SUM(HX7:IC7)</f>
         <v>0</v>
       </c>
-      <c r="KH7" s="28"/>
-      <c r="KI7" s="28"/>
-      <c r="KJ7" s="28"/>
-      <c r="KK7" s="28"/>
-      <c r="KL7" s="28"/>
+      <c r="KH7" s="48"/>
+      <c r="KI7" s="48"/>
+      <c r="KJ7" s="48"/>
+      <c r="KK7" s="48"/>
+      <c r="KL7" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:300">
+      <c r="A8" s="25"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="26"/>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="23"/>
+      <c r="AB8" s="26"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="26"/>
+      <c r="AE8" s="26"/>
+      <c r="AF8" s="23"/>
+      <c r="AG8" s="23"/>
+      <c r="AH8" s="23"/>
+      <c r="AI8" s="23"/>
+      <c r="AJ8" s="23"/>
+      <c r="AK8" s="23"/>
+      <c r="AL8" s="23"/>
+      <c r="AM8" s="23"/>
+      <c r="AN8" s="27"/>
+      <c r="AO8" s="27"/>
+      <c r="AP8" s="27"/>
+      <c r="AQ8" s="27"/>
+      <c r="AR8" s="27"/>
+      <c r="AS8" s="23"/>
+      <c r="AT8" s="23"/>
+      <c r="AU8" s="23"/>
+      <c r="AV8" s="23"/>
+      <c r="AW8" s="23"/>
+      <c r="AX8" s="23"/>
+      <c r="AY8" s="23"/>
+      <c r="AZ8" s="23"/>
+      <c r="BA8" s="23"/>
+      <c r="BB8" s="23"/>
+      <c r="BC8" s="23"/>
+      <c r="BD8" s="23"/>
+      <c r="BE8" s="23"/>
+      <c r="BF8" s="23"/>
+      <c r="BG8" s="23"/>
+      <c r="BH8" s="23"/>
+      <c r="BI8" s="23"/>
+      <c r="BJ8" s="23"/>
+      <c r="BK8" s="23"/>
+      <c r="BL8" s="23"/>
+      <c r="BM8" s="23"/>
+      <c r="BN8" s="23"/>
+      <c r="BO8" s="23"/>
+      <c r="BP8" s="23"/>
+      <c r="BQ8" s="23"/>
+      <c r="BR8" s="23"/>
+      <c r="BS8" s="23"/>
+      <c r="BT8" s="23"/>
+      <c r="BU8" s="23"/>
+      <c r="BV8" s="23"/>
+      <c r="BW8" s="23"/>
+      <c r="BX8" s="23"/>
+      <c r="BY8" s="23"/>
+      <c r="BZ8" s="23"/>
+      <c r="CA8" s="23"/>
+      <c r="CB8" s="23"/>
+      <c r="CC8" s="23"/>
+      <c r="CD8" s="23"/>
+      <c r="CE8" s="23"/>
+      <c r="CF8" s="23"/>
+      <c r="CG8" s="23"/>
+      <c r="CH8" s="23"/>
+      <c r="CI8" s="23"/>
+      <c r="CJ8" s="23"/>
+      <c r="CK8" s="23"/>
+      <c r="CL8" s="23"/>
+      <c r="CM8" s="23"/>
+      <c r="CN8" s="23"/>
+      <c r="CO8" s="23"/>
+      <c r="CP8" s="23"/>
+      <c r="CQ8" s="23"/>
+      <c r="CR8" s="23"/>
+      <c r="CS8" s="23"/>
+      <c r="CT8" s="23"/>
+      <c r="CU8" s="23"/>
+      <c r="CV8" s="23"/>
+      <c r="CW8" s="23"/>
+      <c r="CX8" s="23"/>
+      <c r="CY8" s="23"/>
+      <c r="CZ8" s="23"/>
+      <c r="DA8" s="23"/>
+      <c r="DB8" s="23"/>
+      <c r="DC8" s="23"/>
+      <c r="DD8" s="23"/>
+      <c r="DE8" s="23"/>
+      <c r="DF8" s="23"/>
+      <c r="DG8" s="23"/>
+      <c r="DH8" s="23"/>
+      <c r="DI8" s="23"/>
+      <c r="DJ8" s="23"/>
+      <c r="DK8" s="23"/>
+      <c r="DL8" s="23"/>
+      <c r="DM8" s="23"/>
+      <c r="DN8" s="23"/>
+      <c r="DO8" s="23"/>
+      <c r="DP8" s="23"/>
+      <c r="DQ8" s="23"/>
+      <c r="DR8" s="23"/>
+      <c r="DS8" s="23"/>
+      <c r="DT8" s="23"/>
+      <c r="DU8" s="23"/>
+      <c r="DV8" s="23"/>
+      <c r="DW8" s="23"/>
+      <c r="DX8" s="23"/>
+      <c r="DY8" s="23"/>
+      <c r="DZ8" s="23"/>
+      <c r="EA8" s="23"/>
+      <c r="EB8" s="23"/>
+      <c r="EC8" s="23"/>
+      <c r="ED8" s="23"/>
+      <c r="EE8" s="23"/>
+      <c r="EF8" s="23"/>
+      <c r="EG8" s="23"/>
+      <c r="EH8" s="23"/>
+      <c r="EI8" s="23"/>
+      <c r="EJ8" s="23"/>
+      <c r="EK8" s="23"/>
+      <c r="EL8" s="23"/>
+      <c r="EM8" s="23"/>
+      <c r="EN8" s="23"/>
+      <c r="EO8" s="23"/>
+      <c r="EP8" s="23"/>
+      <c r="EQ8" s="23"/>
+      <c r="ER8" s="23"/>
+      <c r="ES8" s="23"/>
+      <c r="ET8" s="23"/>
+      <c r="EU8" s="23"/>
+      <c r="EV8" s="23"/>
+      <c r="EW8" s="23"/>
+      <c r="EX8" s="23"/>
+      <c r="EY8" s="23"/>
+      <c r="EZ8" s="23"/>
+      <c r="FA8" s="23"/>
+      <c r="FB8" s="23"/>
+      <c r="FC8" s="23"/>
+      <c r="FD8" s="23"/>
+      <c r="FE8" s="23"/>
+      <c r="FF8" s="23"/>
+      <c r="FG8" s="23"/>
+      <c r="FH8" s="23"/>
+      <c r="FI8" s="23"/>
+      <c r="FJ8" s="23"/>
+      <c r="FK8" s="23"/>
+      <c r="FL8" s="23"/>
+      <c r="FM8" s="23"/>
+      <c r="FN8" s="23"/>
+      <c r="FO8" s="23"/>
+      <c r="FP8" s="23"/>
+      <c r="FQ8" s="23"/>
+      <c r="FR8" s="23"/>
+      <c r="FS8" s="23"/>
+      <c r="FT8" s="23"/>
+      <c r="FU8" s="23"/>
+      <c r="FV8" s="23"/>
+      <c r="FW8" s="23"/>
+      <c r="FX8" s="23"/>
+      <c r="FY8" s="23"/>
+      <c r="FZ8" s="23"/>
+      <c r="GA8" s="23"/>
+      <c r="GB8" s="23"/>
+      <c r="GC8" s="23"/>
+      <c r="GD8" s="23"/>
+      <c r="GE8" s="23"/>
+      <c r="GF8" s="23"/>
+      <c r="GG8" s="23"/>
+      <c r="GH8" s="23"/>
+      <c r="GI8" s="23"/>
+      <c r="GJ8" s="23"/>
+      <c r="GK8" s="23"/>
+      <c r="GL8" s="23"/>
+      <c r="GM8" s="23"/>
+      <c r="GN8" s="23"/>
+      <c r="GO8" s="23"/>
+      <c r="GP8" s="23"/>
+      <c r="GQ8" s="23"/>
+      <c r="GR8" s="23"/>
+      <c r="GS8" s="23"/>
+      <c r="GT8" s="23"/>
+      <c r="GU8" s="23"/>
+      <c r="GV8" s="23"/>
+      <c r="GW8" s="23"/>
+      <c r="GX8" s="23"/>
+      <c r="GY8" s="23"/>
+      <c r="GZ8" s="23"/>
+      <c r="HA8" s="23"/>
+      <c r="HB8" s="23"/>
+      <c r="HC8" s="23"/>
+      <c r="HD8" s="23"/>
+      <c r="HE8" s="23"/>
+      <c r="HF8" s="23"/>
+      <c r="HG8" s="23"/>
+      <c r="HH8" s="23"/>
+      <c r="HI8" s="23"/>
+      <c r="HJ8" s="23"/>
+      <c r="HK8" s="23"/>
+      <c r="HL8" s="23"/>
+      <c r="HM8" s="23"/>
+      <c r="HN8" s="23"/>
+      <c r="HO8" s="23"/>
+      <c r="HP8" s="23"/>
+      <c r="HQ8" s="23"/>
+      <c r="HR8" s="23"/>
+      <c r="HS8" s="23"/>
+      <c r="HT8" s="23"/>
+      <c r="HU8" s="23"/>
+      <c r="HV8" s="23"/>
+      <c r="HW8" s="23"/>
+      <c r="HX8" s="23"/>
+      <c r="HY8" s="23"/>
+      <c r="HZ8" s="23"/>
+      <c r="IA8" s="23"/>
+      <c r="IB8" s="23"/>
+      <c r="IC8" s="23"/>
+      <c r="ID8" s="23"/>
+      <c r="IE8" s="23"/>
+      <c r="IF8" s="23"/>
+      <c r="IG8" s="23"/>
+      <c r="IH8" s="23"/>
+      <c r="II8" s="23"/>
+      <c r="IJ8" s="23"/>
+      <c r="IK8" s="23"/>
+      <c r="IL8" s="23"/>
+      <c r="IM8" s="23"/>
+      <c r="IN8" s="23"/>
+      <c r="IO8" s="23"/>
+      <c r="IP8" s="23"/>
+      <c r="IQ8" s="23"/>
+      <c r="IR8" s="23"/>
+      <c r="IS8" s="23"/>
+      <c r="IT8" s="23"/>
+      <c r="IU8" s="23"/>
+      <c r="IV8" s="23"/>
+      <c r="IW8" s="23"/>
+      <c r="IX8" s="23"/>
+      <c r="IY8" s="23"/>
+      <c r="IZ8" s="23"/>
+      <c r="JA8" s="23"/>
+      <c r="JB8" s="23"/>
+      <c r="JC8" s="23"/>
+      <c r="JD8" s="23"/>
+      <c r="JE8" s="23"/>
+      <c r="JF8" s="23"/>
+      <c r="JG8" s="23"/>
+      <c r="JH8" s="23"/>
+      <c r="JI8" s="23"/>
+      <c r="JJ8" s="23"/>
+      <c r="JK8" s="23"/>
+      <c r="JL8" s="23"/>
+      <c r="JM8" s="23"/>
+      <c r="JN8" s="23"/>
+      <c r="JO8" s="23"/>
+      <c r="JP8" s="23"/>
+      <c r="JQ8" s="23"/>
+      <c r="JR8" s="23"/>
+      <c r="JS8" s="47"/>
+      <c r="JT8" s="47"/>
+      <c r="JU8" s="47"/>
+      <c r="JV8" s="47"/>
+      <c r="JW8" s="47"/>
+      <c r="JX8" s="47"/>
+      <c r="JY8" s="47"/>
+      <c r="JZ8" s="23"/>
+      <c r="KA8" s="23"/>
+      <c r="KB8" s="23"/>
+      <c r="KC8" s="23"/>
+      <c r="KD8" s="23"/>
+      <c r="KE8" s="23"/>
+      <c r="KF8" s="23"/>
+      <c r="KG8" s="23"/>
+      <c r="KH8" s="48"/>
+      <c r="KI8" s="48"/>
+      <c r="KJ8" s="48"/>
+      <c r="KK8" s="48"/>
+      <c r="KL8" s="48" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:300">
+      <c r="A9" s="25"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="23"/>
+      <c r="AA9" s="23"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="23"/>
+      <c r="AD9" s="26"/>
+      <c r="AE9" s="26"/>
+      <c r="AF9" s="23"/>
+      <c r="AG9" s="23"/>
+      <c r="AH9" s="23"/>
+      <c r="AI9" s="23"/>
+      <c r="AJ9" s="23"/>
+      <c r="AK9" s="23"/>
+      <c r="AL9" s="23"/>
+      <c r="AM9" s="23"/>
+      <c r="AN9" s="27"/>
+      <c r="AO9" s="27"/>
+      <c r="AP9" s="27"/>
+      <c r="AQ9" s="27"/>
+      <c r="AR9" s="27"/>
+      <c r="AS9" s="23"/>
+      <c r="AT9" s="23"/>
+      <c r="AU9" s="23"/>
+      <c r="AV9" s="23"/>
+      <c r="AW9" s="23"/>
+      <c r="AX9" s="23"/>
+      <c r="AY9" s="23"/>
+      <c r="AZ9" s="23"/>
+      <c r="BA9" s="23"/>
+      <c r="BB9" s="23"/>
+      <c r="BC9" s="23"/>
+      <c r="BD9" s="23"/>
+      <c r="BE9" s="23"/>
+      <c r="BF9" s="23"/>
+      <c r="BG9" s="23"/>
+      <c r="BH9" s="23"/>
+      <c r="BI9" s="23"/>
+      <c r="BJ9" s="23"/>
+      <c r="BK9" s="23"/>
+      <c r="BL9" s="23"/>
+      <c r="BM9" s="23"/>
+      <c r="BN9" s="23"/>
+      <c r="BO9" s="23"/>
+      <c r="BP9" s="23"/>
+      <c r="BQ9" s="23"/>
+      <c r="BR9" s="23"/>
+      <c r="BS9" s="23"/>
+      <c r="BT9" s="23"/>
+      <c r="BU9" s="23"/>
+      <c r="BV9" s="23"/>
+      <c r="BW9" s="23"/>
+      <c r="BX9" s="23"/>
+      <c r="BY9" s="23"/>
+      <c r="BZ9" s="23"/>
+      <c r="CA9" s="23"/>
+      <c r="CB9" s="23"/>
+      <c r="CC9" s="23"/>
+      <c r="CD9" s="23"/>
+      <c r="CE9" s="23"/>
+      <c r="CF9" s="23"/>
+      <c r="CG9" s="23"/>
+      <c r="CH9" s="23"/>
+      <c r="CI9" s="23"/>
+      <c r="CJ9" s="23"/>
+      <c r="CK9" s="23"/>
+      <c r="CL9" s="23"/>
+      <c r="CM9" s="23"/>
+      <c r="CN9" s="23"/>
+      <c r="CO9" s="23"/>
+      <c r="CP9" s="23"/>
+      <c r="CQ9" s="23"/>
+      <c r="CR9" s="23"/>
+      <c r="CS9" s="23"/>
+      <c r="CT9" s="23"/>
+      <c r="CU9" s="23"/>
+      <c r="CV9" s="23"/>
+      <c r="CW9" s="23"/>
+      <c r="CX9" s="23"/>
+      <c r="CY9" s="23"/>
+      <c r="CZ9" s="23"/>
+      <c r="DA9" s="23"/>
+      <c r="DB9" s="23"/>
+      <c r="DC9" s="23"/>
+      <c r="DD9" s="23"/>
+      <c r="DE9" s="23"/>
+      <c r="DF9" s="23"/>
+      <c r="DG9" s="23"/>
+      <c r="DH9" s="23"/>
+      <c r="DI9" s="23"/>
+      <c r="DJ9" s="23"/>
+      <c r="DK9" s="23"/>
+      <c r="DL9" s="23"/>
+      <c r="DM9" s="23"/>
+      <c r="DN9" s="23"/>
+      <c r="DO9" s="23"/>
+      <c r="DP9" s="23"/>
+      <c r="DQ9" s="23"/>
+      <c r="DR9" s="23"/>
+      <c r="DS9" s="23"/>
+      <c r="DT9" s="23"/>
+      <c r="DU9" s="23"/>
+      <c r="DV9" s="23"/>
+      <c r="DW9" s="23"/>
+      <c r="DX9" s="23"/>
+      <c r="DY9" s="23"/>
+      <c r="DZ9" s="23"/>
+      <c r="EA9" s="23"/>
+      <c r="EB9" s="23"/>
+      <c r="EC9" s="23"/>
+      <c r="ED9" s="23"/>
+      <c r="EE9" s="23"/>
+      <c r="EF9" s="23"/>
+      <c r="EG9" s="23"/>
+      <c r="EH9" s="23"/>
+      <c r="EI9" s="23"/>
+      <c r="EJ9" s="23"/>
+      <c r="EK9" s="23"/>
+      <c r="EL9" s="23"/>
+      <c r="EM9" s="23"/>
+      <c r="EN9" s="23"/>
+      <c r="EO9" s="23"/>
+      <c r="EP9" s="23"/>
+      <c r="EQ9" s="23"/>
+      <c r="ER9" s="23"/>
+      <c r="ES9" s="23"/>
+      <c r="ET9" s="23"/>
+      <c r="EU9" s="23"/>
+      <c r="EV9" s="23"/>
+      <c r="EW9" s="23"/>
+      <c r="EX9" s="23"/>
+      <c r="EY9" s="23"/>
+      <c r="EZ9" s="23"/>
+      <c r="FA9" s="23"/>
+      <c r="FB9" s="23"/>
+      <c r="FC9" s="23"/>
+      <c r="FD9" s="23"/>
+      <c r="FE9" s="23"/>
+      <c r="FF9" s="23"/>
+      <c r="FG9" s="23"/>
+      <c r="FH9" s="23"/>
+      <c r="FI9" s="23"/>
+      <c r="FJ9" s="23"/>
+      <c r="FK9" s="23"/>
+      <c r="FL9" s="23"/>
+      <c r="FM9" s="23"/>
+      <c r="FN9" s="23"/>
+      <c r="FO9" s="23"/>
+      <c r="FP9" s="23"/>
+      <c r="FQ9" s="23"/>
+      <c r="FR9" s="23"/>
+      <c r="FS9" s="23"/>
+      <c r="FT9" s="23"/>
+      <c r="FU9" s="23"/>
+      <c r="FV9" s="23"/>
+      <c r="FW9" s="23"/>
+      <c r="FX9" s="23"/>
+      <c r="FY9" s="23"/>
+      <c r="FZ9" s="23"/>
+      <c r="GA9" s="23"/>
+      <c r="GB9" s="23"/>
+      <c r="GC9" s="23"/>
+      <c r="GD9" s="23"/>
+      <c r="GE9" s="23"/>
+      <c r="GF9" s="23"/>
+      <c r="GG9" s="23"/>
+      <c r="GH9" s="23"/>
+      <c r="GI9" s="23"/>
+      <c r="GJ9" s="23"/>
+      <c r="GK9" s="23"/>
+      <c r="GL9" s="23"/>
+      <c r="GM9" s="23"/>
+      <c r="GN9" s="23"/>
+      <c r="GO9" s="23"/>
+      <c r="GP9" s="23"/>
+      <c r="GQ9" s="23"/>
+      <c r="GR9" s="23"/>
+      <c r="GS9" s="23"/>
+      <c r="GT9" s="23"/>
+      <c r="GU9" s="23"/>
+      <c r="GV9" s="23"/>
+      <c r="GW9" s="23"/>
+      <c r="GX9" s="23"/>
+      <c r="GY9" s="23"/>
+      <c r="GZ9" s="23"/>
+      <c r="HA9" s="23"/>
+      <c r="HB9" s="23"/>
+      <c r="HC9" s="23"/>
+      <c r="HD9" s="23"/>
+      <c r="HE9" s="23"/>
+      <c r="HF9" s="23"/>
+      <c r="HG9" s="23"/>
+      <c r="HH9" s="23"/>
+      <c r="HI9" s="23"/>
+      <c r="HJ9" s="23"/>
+      <c r="HK9" s="23"/>
+      <c r="HL9" s="23"/>
+      <c r="HM9" s="23"/>
+      <c r="HN9" s="23"/>
+      <c r="HO9" s="23"/>
+      <c r="HP9" s="23"/>
+      <c r="HQ9" s="23"/>
+      <c r="HR9" s="23"/>
+      <c r="HS9" s="23"/>
+      <c r="HT9" s="23"/>
+      <c r="HU9" s="23"/>
+      <c r="HV9" s="23"/>
+      <c r="HW9" s="23"/>
+      <c r="HX9" s="23"/>
+      <c r="HY9" s="23"/>
+      <c r="HZ9" s="23"/>
+      <c r="IA9" s="23"/>
+      <c r="IB9" s="23"/>
+      <c r="IC9" s="23"/>
+      <c r="ID9" s="23"/>
+      <c r="IE9" s="23"/>
+      <c r="IF9" s="23"/>
+      <c r="IG9" s="23"/>
+      <c r="IH9" s="23"/>
+      <c r="II9" s="23"/>
+      <c r="IJ9" s="23"/>
+      <c r="IK9" s="23"/>
+      <c r="IL9" s="23"/>
+      <c r="IM9" s="23"/>
+      <c r="IN9" s="23"/>
+      <c r="IO9" s="23"/>
+      <c r="IP9" s="23"/>
+      <c r="IQ9" s="23"/>
+      <c r="IR9" s="23"/>
+      <c r="IS9" s="23"/>
+      <c r="IT9" s="23"/>
+      <c r="IU9" s="23"/>
+      <c r="IV9" s="23"/>
+      <c r="IW9" s="23"/>
+      <c r="IX9" s="23"/>
+      <c r="IY9" s="23"/>
+      <c r="IZ9" s="23"/>
+      <c r="JA9" s="23"/>
+      <c r="JB9" s="23"/>
+      <c r="JC9" s="23"/>
+      <c r="JD9" s="23"/>
+      <c r="JE9" s="23"/>
+      <c r="JF9" s="23"/>
+      <c r="JG9" s="23"/>
+      <c r="JH9" s="23"/>
+      <c r="JI9" s="23"/>
+      <c r="JJ9" s="23"/>
+      <c r="JK9" s="23"/>
+      <c r="JL9" s="23"/>
+      <c r="JM9" s="23"/>
+      <c r="JN9" s="23"/>
+      <c r="JO9" s="23"/>
+      <c r="JP9" s="23"/>
+      <c r="JQ9" s="23"/>
+      <c r="JR9" s="23"/>
+      <c r="JS9" s="47"/>
+      <c r="JT9" s="47"/>
+      <c r="JU9" s="47"/>
+      <c r="JV9" s="47"/>
+      <c r="JW9" s="47"/>
+      <c r="JX9" s="47"/>
+      <c r="JY9" s="47"/>
+      <c r="JZ9" s="23"/>
+      <c r="KA9" s="23"/>
+      <c r="KB9" s="23"/>
+      <c r="KC9" s="23"/>
+      <c r="KD9" s="23"/>
+      <c r="KE9" s="23"/>
+      <c r="KF9" s="23"/>
+      <c r="KG9" s="23"/>
+      <c r="KH9" s="48"/>
+      <c r="KI9" s="48"/>
+      <c r="KJ9" s="48"/>
+      <c r="KK9" s="48"/>
+      <c r="KL9" s="48" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:300">
+      <c r="A10" s="25"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
+      <c r="X10" s="26"/>
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="23"/>
+      <c r="AA10" s="23"/>
+      <c r="AB10" s="26"/>
+      <c r="AC10" s="23"/>
+      <c r="AD10" s="26"/>
+      <c r="AE10" s="26"/>
+      <c r="AF10" s="23"/>
+      <c r="AG10" s="23"/>
+      <c r="AH10" s="23"/>
+      <c r="AI10" s="23"/>
+      <c r="AJ10" s="23"/>
+      <c r="AK10" s="23"/>
+      <c r="AL10" s="23"/>
+      <c r="AM10" s="23"/>
+      <c r="AN10" s="27"/>
+      <c r="AO10" s="27"/>
+      <c r="AP10" s="27"/>
+      <c r="AQ10" s="27"/>
+      <c r="AR10" s="27"/>
+      <c r="AS10" s="23"/>
+      <c r="AT10" s="23"/>
+      <c r="AU10" s="23"/>
+      <c r="AV10" s="23"/>
+      <c r="AW10" s="23"/>
+      <c r="AX10" s="23"/>
+      <c r="AY10" s="23"/>
+      <c r="AZ10" s="23"/>
+      <c r="BA10" s="23"/>
+      <c r="BB10" s="23"/>
+      <c r="BC10" s="23"/>
+      <c r="BD10" s="23"/>
+      <c r="BE10" s="23"/>
+      <c r="BF10" s="23"/>
+      <c r="BG10" s="23"/>
+      <c r="BH10" s="23"/>
+      <c r="BI10" s="23"/>
+      <c r="BJ10" s="23"/>
+      <c r="BK10" s="23"/>
+      <c r="BL10" s="23"/>
+      <c r="BM10" s="23"/>
+      <c r="BN10" s="23"/>
+      <c r="BO10" s="23"/>
+      <c r="BP10" s="23"/>
+      <c r="BQ10" s="23"/>
+      <c r="BR10" s="23"/>
+      <c r="BS10" s="23"/>
+      <c r="BT10" s="23"/>
+      <c r="BU10" s="23"/>
+      <c r="BV10" s="23"/>
+      <c r="BW10" s="23"/>
+      <c r="BX10" s="23"/>
+      <c r="BY10" s="23"/>
+      <c r="BZ10" s="23"/>
+      <c r="CA10" s="23"/>
+      <c r="CB10" s="23"/>
+      <c r="CC10" s="23"/>
+      <c r="CD10" s="23"/>
+      <c r="CE10" s="23"/>
+      <c r="CF10" s="23"/>
+      <c r="CG10" s="23"/>
+      <c r="CH10" s="23"/>
+      <c r="CI10" s="23"/>
+      <c r="CJ10" s="23"/>
+      <c r="CK10" s="23"/>
+      <c r="CL10" s="23"/>
+      <c r="CM10" s="23"/>
+      <c r="CN10" s="23"/>
+      <c r="CO10" s="23"/>
+      <c r="CP10" s="23"/>
+      <c r="CQ10" s="23"/>
+      <c r="CR10" s="23"/>
+      <c r="CS10" s="23"/>
+      <c r="CT10" s="23"/>
+      <c r="CU10" s="23"/>
+      <c r="CV10" s="23"/>
+      <c r="CW10" s="23"/>
+      <c r="CX10" s="23"/>
+      <c r="CY10" s="23"/>
+      <c r="CZ10" s="23"/>
+      <c r="DA10" s="23"/>
+      <c r="DB10" s="23"/>
+      <c r="DC10" s="23"/>
+      <c r="DD10" s="23"/>
+      <c r="DE10" s="23"/>
+      <c r="DF10" s="23"/>
+      <c r="DG10" s="23"/>
+      <c r="DH10" s="23"/>
+      <c r="DI10" s="23"/>
+      <c r="DJ10" s="23"/>
+      <c r="DK10" s="23"/>
+      <c r="DL10" s="23"/>
+      <c r="DM10" s="23"/>
+      <c r="DN10" s="23"/>
+      <c r="DO10" s="23"/>
+      <c r="DP10" s="23"/>
+      <c r="DQ10" s="23"/>
+      <c r="DR10" s="23"/>
+      <c r="DS10" s="23"/>
+      <c r="DT10" s="23"/>
+      <c r="DU10" s="23"/>
+      <c r="DV10" s="23"/>
+      <c r="DW10" s="23"/>
+      <c r="DX10" s="23"/>
+      <c r="DY10" s="23"/>
+      <c r="DZ10" s="23"/>
+      <c r="EA10" s="23"/>
+      <c r="EB10" s="23"/>
+      <c r="EC10" s="23"/>
+      <c r="ED10" s="23"/>
+      <c r="EE10" s="23"/>
+      <c r="EF10" s="23"/>
+      <c r="EG10" s="23"/>
+      <c r="EH10" s="23"/>
+      <c r="EI10" s="23"/>
+      <c r="EJ10" s="23"/>
+      <c r="EK10" s="23"/>
+      <c r="EL10" s="23"/>
+      <c r="EM10" s="23"/>
+      <c r="EN10" s="23"/>
+      <c r="EO10" s="23"/>
+      <c r="EP10" s="23"/>
+      <c r="EQ10" s="23"/>
+      <c r="ER10" s="23"/>
+      <c r="ES10" s="23"/>
+      <c r="ET10" s="23"/>
+      <c r="EU10" s="23"/>
+      <c r="EV10" s="23"/>
+      <c r="EW10" s="23"/>
+      <c r="EX10" s="23"/>
+      <c r="EY10" s="23"/>
+      <c r="EZ10" s="23"/>
+      <c r="FA10" s="23"/>
+      <c r="FB10" s="23"/>
+      <c r="FC10" s="23"/>
+      <c r="FD10" s="23"/>
+      <c r="FE10" s="23"/>
+      <c r="FF10" s="23"/>
+      <c r="FG10" s="23"/>
+      <c r="FH10" s="23"/>
+      <c r="FI10" s="23"/>
+      <c r="FJ10" s="23"/>
+      <c r="FK10" s="23"/>
+      <c r="FL10" s="23"/>
+      <c r="FM10" s="23"/>
+      <c r="FN10" s="23"/>
+      <c r="FO10" s="23"/>
+      <c r="FP10" s="23"/>
+      <c r="FQ10" s="23"/>
+      <c r="FR10" s="23"/>
+      <c r="FS10" s="23"/>
+      <c r="FT10" s="23"/>
+      <c r="FU10" s="23"/>
+      <c r="FV10" s="23"/>
+      <c r="FW10" s="23"/>
+      <c r="FX10" s="23"/>
+      <c r="FY10" s="23"/>
+      <c r="FZ10" s="23"/>
+      <c r="GA10" s="23"/>
+      <c r="GB10" s="23"/>
+      <c r="GC10" s="23"/>
+      <c r="GD10" s="23"/>
+      <c r="GE10" s="23"/>
+      <c r="GF10" s="23"/>
+      <c r="GG10" s="23"/>
+      <c r="GH10" s="23"/>
+      <c r="GI10" s="23"/>
+      <c r="GJ10" s="23"/>
+      <c r="GK10" s="23"/>
+      <c r="GL10" s="23"/>
+      <c r="GM10" s="23"/>
+      <c r="GN10" s="23"/>
+      <c r="GO10" s="23"/>
+      <c r="GP10" s="23"/>
+      <c r="GQ10" s="23"/>
+      <c r="GR10" s="23"/>
+      <c r="GS10" s="23"/>
+      <c r="GT10" s="23"/>
+      <c r="GU10" s="23"/>
+      <c r="GV10" s="23"/>
+      <c r="GW10" s="23"/>
+      <c r="GX10" s="23"/>
+      <c r="GY10" s="23"/>
+      <c r="GZ10" s="23"/>
+      <c r="HA10" s="23"/>
+      <c r="HB10" s="23"/>
+      <c r="HC10" s="23"/>
+      <c r="HD10" s="23"/>
+      <c r="HE10" s="23"/>
+      <c r="HF10" s="23"/>
+      <c r="HG10" s="23"/>
+      <c r="HH10" s="23"/>
+      <c r="HI10" s="23"/>
+      <c r="HJ10" s="23"/>
+      <c r="HK10" s="23"/>
+      <c r="HL10" s="23"/>
+      <c r="HM10" s="23"/>
+      <c r="HN10" s="23"/>
+      <c r="HO10" s="23"/>
+      <c r="HP10" s="23"/>
+      <c r="HQ10" s="23"/>
+      <c r="HR10" s="23"/>
+      <c r="HS10" s="23"/>
+      <c r="HT10" s="23"/>
+      <c r="HU10" s="23"/>
+      <c r="HV10" s="23"/>
+      <c r="HW10" s="23"/>
+      <c r="HX10" s="23"/>
+      <c r="HY10" s="23"/>
+      <c r="HZ10" s="23"/>
+      <c r="IA10" s="23"/>
+      <c r="IB10" s="23"/>
+      <c r="IC10" s="23"/>
+      <c r="ID10" s="23"/>
+      <c r="IE10" s="23"/>
+      <c r="IF10" s="23"/>
+      <c r="IG10" s="23"/>
+      <c r="IH10" s="23"/>
+      <c r="II10" s="23"/>
+      <c r="IJ10" s="23"/>
+      <c r="IK10" s="23"/>
+      <c r="IL10" s="23"/>
+      <c r="IM10" s="23"/>
+      <c r="IN10" s="23"/>
+      <c r="IO10" s="23"/>
+      <c r="IP10" s="23"/>
+      <c r="IQ10" s="23"/>
+      <c r="IR10" s="23"/>
+      <c r="IS10" s="23"/>
+      <c r="IT10" s="23"/>
+      <c r="IU10" s="23"/>
+      <c r="IV10" s="23"/>
+      <c r="IW10" s="23"/>
+      <c r="IX10" s="23"/>
+      <c r="IY10" s="23"/>
+      <c r="IZ10" s="23"/>
+      <c r="JA10" s="23"/>
+      <c r="JB10" s="23"/>
+      <c r="JC10" s="23"/>
+      <c r="JD10" s="23"/>
+      <c r="JE10" s="23"/>
+      <c r="JF10" s="23"/>
+      <c r="JG10" s="23"/>
+      <c r="JH10" s="23"/>
+      <c r="JI10" s="23"/>
+      <c r="JJ10" s="23"/>
+      <c r="JK10" s="23"/>
+      <c r="JL10" s="23"/>
+      <c r="JM10" s="23"/>
+      <c r="JN10" s="23"/>
+      <c r="JO10" s="23"/>
+      <c r="JP10" s="23"/>
+      <c r="JQ10" s="23"/>
+      <c r="JR10" s="23"/>
+      <c r="JS10" s="47"/>
+      <c r="JT10" s="47"/>
+      <c r="JU10" s="47"/>
+      <c r="JV10" s="47"/>
+      <c r="JW10" s="47"/>
+      <c r="JX10" s="47"/>
+      <c r="JY10" s="47"/>
+      <c r="JZ10" s="23"/>
+      <c r="KA10" s="23"/>
+      <c r="KB10" s="23"/>
+      <c r="KC10" s="23"/>
+      <c r="KD10" s="23"/>
+      <c r="KE10" s="23"/>
+      <c r="KF10" s="23"/>
+      <c r="KG10" s="23"/>
+      <c r="KH10" s="48"/>
+      <c r="KI10" s="48"/>
+      <c r="KJ10" s="48"/>
+      <c r="KK10" s="48"/>
+      <c r="KL10" s="48" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:300">
+      <c r="A11" s="25"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="23"/>
+      <c r="AA11" s="23"/>
+      <c r="AB11" s="26"/>
+      <c r="AC11" s="23"/>
+      <c r="AD11" s="26"/>
+      <c r="AE11" s="26"/>
+      <c r="AF11" s="23"/>
+      <c r="AG11" s="23"/>
+      <c r="AH11" s="23"/>
+      <c r="AI11" s="23"/>
+      <c r="AJ11" s="23"/>
+      <c r="AK11" s="23"/>
+      <c r="AL11" s="23"/>
+      <c r="AM11" s="23"/>
+      <c r="AN11" s="27"/>
+      <c r="AO11" s="27"/>
+      <c r="AP11" s="27"/>
+      <c r="AQ11" s="27"/>
+      <c r="AR11" s="27"/>
+      <c r="AS11" s="23"/>
+      <c r="AT11" s="23"/>
+      <c r="AU11" s="23"/>
+      <c r="AV11" s="23"/>
+      <c r="AW11" s="23"/>
+      <c r="AX11" s="23"/>
+      <c r="AY11" s="23"/>
+      <c r="AZ11" s="23"/>
+      <c r="BA11" s="23"/>
+      <c r="BB11" s="23"/>
+      <c r="BC11" s="23"/>
+      <c r="BD11" s="23"/>
+      <c r="BE11" s="23"/>
+      <c r="BF11" s="23"/>
+      <c r="BG11" s="23"/>
+      <c r="BH11" s="23"/>
+      <c r="BI11" s="23"/>
+      <c r="BJ11" s="23"/>
+      <c r="BK11" s="23"/>
+      <c r="BL11" s="23"/>
+      <c r="BM11" s="23"/>
+      <c r="BN11" s="23"/>
+      <c r="BO11" s="23"/>
+      <c r="BP11" s="23"/>
+      <c r="BQ11" s="23"/>
+      <c r="BR11" s="23"/>
+      <c r="BS11" s="23"/>
+      <c r="BT11" s="23"/>
+      <c r="BU11" s="23"/>
+      <c r="BV11" s="23"/>
+      <c r="BW11" s="23"/>
+      <c r="BX11" s="23"/>
+      <c r="BY11" s="23"/>
+      <c r="BZ11" s="23"/>
+      <c r="CA11" s="23"/>
+      <c r="CB11" s="23"/>
+      <c r="CC11" s="23"/>
+      <c r="CD11" s="23"/>
+      <c r="CE11" s="23"/>
+      <c r="CF11" s="23"/>
+      <c r="CG11" s="23"/>
+      <c r="CH11" s="23"/>
+      <c r="CI11" s="23"/>
+      <c r="CJ11" s="23"/>
+      <c r="CK11" s="23"/>
+      <c r="CL11" s="23"/>
+      <c r="CM11" s="23"/>
+      <c r="CN11" s="23"/>
+      <c r="CO11" s="23"/>
+      <c r="CP11" s="23"/>
+      <c r="CQ11" s="23"/>
+      <c r="CR11" s="23"/>
+      <c r="CS11" s="23"/>
+      <c r="CT11" s="23"/>
+      <c r="CU11" s="23"/>
+      <c r="CV11" s="23"/>
+      <c r="CW11" s="23"/>
+      <c r="CX11" s="23"/>
+      <c r="CY11" s="23"/>
+      <c r="CZ11" s="23"/>
+      <c r="DA11" s="23"/>
+      <c r="DB11" s="23"/>
+      <c r="DC11" s="23"/>
+      <c r="DD11" s="23"/>
+      <c r="DE11" s="23"/>
+      <c r="DF11" s="23"/>
+      <c r="DG11" s="23"/>
+      <c r="DH11" s="23"/>
+      <c r="DI11" s="23"/>
+      <c r="DJ11" s="23"/>
+      <c r="DK11" s="23"/>
+      <c r="DL11" s="23"/>
+      <c r="DM11" s="23"/>
+      <c r="DN11" s="23"/>
+      <c r="DO11" s="23"/>
+      <c r="DP11" s="23"/>
+      <c r="DQ11" s="23"/>
+      <c r="DR11" s="23"/>
+      <c r="DS11" s="23"/>
+      <c r="DT11" s="23"/>
+      <c r="DU11" s="23"/>
+      <c r="DV11" s="23"/>
+      <c r="DW11" s="23"/>
+      <c r="DX11" s="23"/>
+      <c r="DY11" s="23"/>
+      <c r="DZ11" s="23"/>
+      <c r="EA11" s="23"/>
+      <c r="EB11" s="23"/>
+      <c r="EC11" s="23"/>
+      <c r="ED11" s="23"/>
+      <c r="EE11" s="23"/>
+      <c r="EF11" s="23"/>
+      <c r="EG11" s="23"/>
+      <c r="EH11" s="23"/>
+      <c r="EI11" s="23"/>
+      <c r="EJ11" s="23"/>
+      <c r="EK11" s="23"/>
+      <c r="EL11" s="23"/>
+      <c r="EM11" s="23"/>
+      <c r="EN11" s="23"/>
+      <c r="EO11" s="23"/>
+      <c r="EP11" s="23"/>
+      <c r="EQ11" s="23"/>
+      <c r="ER11" s="23"/>
+      <c r="ES11" s="23"/>
+      <c r="ET11" s="23"/>
+      <c r="EU11" s="23"/>
+      <c r="EV11" s="23"/>
+      <c r="EW11" s="23"/>
+      <c r="EX11" s="23"/>
+      <c r="EY11" s="23"/>
+      <c r="EZ11" s="23"/>
+      <c r="FA11" s="23"/>
+      <c r="FB11" s="23"/>
+      <c r="FC11" s="23"/>
+      <c r="FD11" s="23"/>
+      <c r="FE11" s="23"/>
+      <c r="FF11" s="23"/>
+      <c r="FG11" s="23"/>
+      <c r="FH11" s="23"/>
+      <c r="FI11" s="23"/>
+      <c r="FJ11" s="23"/>
+      <c r="FK11" s="23"/>
+      <c r="FL11" s="23"/>
+      <c r="FM11" s="23"/>
+      <c r="FN11" s="23"/>
+      <c r="FO11" s="23"/>
+      <c r="FP11" s="23"/>
+      <c r="FQ11" s="23"/>
+      <c r="FR11" s="23"/>
+      <c r="FS11" s="23"/>
+      <c r="FT11" s="23"/>
+      <c r="FU11" s="23"/>
+      <c r="FV11" s="23"/>
+      <c r="FW11" s="23"/>
+      <c r="FX11" s="23"/>
+      <c r="FY11" s="23"/>
+      <c r="FZ11" s="23"/>
+      <c r="GA11" s="23"/>
+      <c r="GB11" s="23"/>
+      <c r="GC11" s="23"/>
+      <c r="GD11" s="23"/>
+      <c r="GE11" s="23"/>
+      <c r="GF11" s="23"/>
+      <c r="GG11" s="23"/>
+      <c r="GH11" s="23"/>
+      <c r="GI11" s="23"/>
+      <c r="GJ11" s="23"/>
+      <c r="GK11" s="23"/>
+      <c r="GL11" s="23"/>
+      <c r="GM11" s="23"/>
+      <c r="GN11" s="23"/>
+      <c r="GO11" s="23"/>
+      <c r="GP11" s="23"/>
+      <c r="GQ11" s="23"/>
+      <c r="GR11" s="23"/>
+      <c r="GS11" s="23"/>
+      <c r="GT11" s="23"/>
+      <c r="GU11" s="23"/>
+      <c r="GV11" s="23"/>
+      <c r="GW11" s="23"/>
+      <c r="GX11" s="23"/>
+      <c r="GY11" s="23"/>
+      <c r="GZ11" s="23"/>
+      <c r="HA11" s="23"/>
+      <c r="HB11" s="23"/>
+      <c r="HC11" s="23"/>
+      <c r="HD11" s="23"/>
+      <c r="HE11" s="23"/>
+      <c r="HF11" s="23"/>
+      <c r="HG11" s="23"/>
+      <c r="HH11" s="23"/>
+      <c r="HI11" s="23"/>
+      <c r="HJ11" s="23"/>
+      <c r="HK11" s="23"/>
+      <c r="HL11" s="23"/>
+      <c r="HM11" s="23"/>
+      <c r="HN11" s="23"/>
+      <c r="HO11" s="23"/>
+      <c r="HP11" s="23"/>
+      <c r="HQ11" s="23"/>
+      <c r="HR11" s="23"/>
+      <c r="HS11" s="23"/>
+      <c r="HT11" s="23"/>
+      <c r="HU11" s="23"/>
+      <c r="HV11" s="23"/>
+      <c r="HW11" s="23"/>
+      <c r="HX11" s="23"/>
+      <c r="HY11" s="23"/>
+      <c r="HZ11" s="23"/>
+      <c r="IA11" s="23"/>
+      <c r="IB11" s="23"/>
+      <c r="IC11" s="23"/>
+      <c r="ID11" s="23"/>
+      <c r="IE11" s="23"/>
+      <c r="IF11" s="23"/>
+      <c r="IG11" s="23"/>
+      <c r="IH11" s="23"/>
+      <c r="II11" s="23"/>
+      <c r="IJ11" s="23"/>
+      <c r="IK11" s="23"/>
+      <c r="IL11" s="23"/>
+      <c r="IM11" s="23"/>
+      <c r="IN11" s="23"/>
+      <c r="IO11" s="23"/>
+      <c r="IP11" s="23"/>
+      <c r="IQ11" s="23"/>
+      <c r="IR11" s="23"/>
+      <c r="IS11" s="23"/>
+      <c r="IT11" s="23"/>
+      <c r="IU11" s="23"/>
+      <c r="IV11" s="23"/>
+      <c r="IW11" s="23"/>
+      <c r="IX11" s="23"/>
+      <c r="IY11" s="23"/>
+      <c r="IZ11" s="23"/>
+      <c r="JA11" s="23"/>
+      <c r="JB11" s="23"/>
+      <c r="JC11" s="23"/>
+      <c r="JD11" s="23"/>
+      <c r="JE11" s="23"/>
+      <c r="JF11" s="23"/>
+      <c r="JG11" s="23"/>
+      <c r="JH11" s="23"/>
+      <c r="JI11" s="23"/>
+      <c r="JJ11" s="23"/>
+      <c r="JK11" s="23"/>
+      <c r="JL11" s="23"/>
+      <c r="JM11" s="23"/>
+      <c r="JN11" s="23"/>
+      <c r="JO11" s="23"/>
+      <c r="JP11" s="23"/>
+      <c r="JQ11" s="23"/>
+      <c r="JR11" s="23"/>
+      <c r="JS11" s="47"/>
+      <c r="JT11" s="47"/>
+      <c r="JU11" s="47"/>
+      <c r="JV11" s="47"/>
+      <c r="JW11" s="47"/>
+      <c r="JX11" s="47"/>
+      <c r="JY11" s="47"/>
+      <c r="JZ11" s="23"/>
+      <c r="KA11" s="23"/>
+      <c r="KB11" s="23"/>
+      <c r="KC11" s="23"/>
+      <c r="KD11" s="23"/>
+      <c r="KE11" s="23"/>
+      <c r="KF11" s="23"/>
+      <c r="KG11" s="23"/>
+      <c r="KH11" s="48"/>
+      <c r="KI11" s="48"/>
+      <c r="KJ11" s="48"/>
+      <c r="KK11" s="48"/>
+      <c r="KL11" s="48" t="s">
+        <v>340</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A6:KL6"/>
+  <autoFilter ref="A6:KK6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="32">
-    <mergeCell ref="AM4:AN5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:D5"/>
-    <mergeCell ref="E4:J5"/>
-    <mergeCell ref="K4:O5"/>
-    <mergeCell ref="P4:T5"/>
-    <mergeCell ref="U4:AB5"/>
-    <mergeCell ref="AC4:AI5"/>
-    <mergeCell ref="AJ4:AL5"/>
+    <mergeCell ref="KH4:KJ5"/>
+    <mergeCell ref="JZ4:KG4"/>
+    <mergeCell ref="JZ5:KC5"/>
+    <mergeCell ref="KD5:KG5"/>
+    <mergeCell ref="GU4:HH4"/>
+    <mergeCell ref="HI4:HV4"/>
+    <mergeCell ref="HW4:IJ4"/>
+    <mergeCell ref="IK4:IX4"/>
+    <mergeCell ref="IY4:JL4"/>
+    <mergeCell ref="JM4:JY5"/>
     <mergeCell ref="GG4:GT4"/>
     <mergeCell ref="AO4:AR5"/>
     <mergeCell ref="AS4:BJ5"/>
@@ -5444,36 +6686,39 @@
     <mergeCell ref="EQ4:FD4"/>
     <mergeCell ref="FE4:FR4"/>
     <mergeCell ref="FS4:GF4"/>
-    <mergeCell ref="KH4:KK5"/>
-    <mergeCell ref="JZ4:KG4"/>
-    <mergeCell ref="JZ5:KC5"/>
-    <mergeCell ref="KD5:KG5"/>
-    <mergeCell ref="GU4:HH4"/>
-    <mergeCell ref="HI4:HV4"/>
-    <mergeCell ref="HW4:IJ4"/>
-    <mergeCell ref="IK4:IX4"/>
-    <mergeCell ref="IY4:JL4"/>
-    <mergeCell ref="JM4:JY5"/>
+    <mergeCell ref="AM4:AN5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:D5"/>
+    <mergeCell ref="E4:J5"/>
+    <mergeCell ref="K4:O5"/>
+    <mergeCell ref="P4:T5"/>
+    <mergeCell ref="U4:AB5"/>
+    <mergeCell ref="AC4:AI5"/>
+    <mergeCell ref="AJ4:AL5"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>
   </conditionalFormatting>
-  <dataValidations count="4">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR7">
+  <dataValidations count="5">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>36526</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KI7">
-      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete, No Delivery pre 2021 "</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH8:KJ11" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>$KL$7:$KL$11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KK7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH7 KJ7" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KK7" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"NGSA, WEM, FCRM Operational Framework, Other, Unknown/TBC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH7 KJ7">
-      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete,"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KI7" xr:uid="{00000000-0002-0000-0000-000004000000}">
+      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete, No Delivery pre 2021 "</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="10" orientation="landscape"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="10" orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[PM-343] Correct range on data validations
* Update fcerm1 spreadsheet template to correct data validation range so
all cells in the KH-KJ include the dropdown
* Remove redundant values for dropdown from sheet
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthall/Work/pafs/pafs_core/lib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84F3FAD-9F25-3A49-9B3B-4E25A0E35093}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C15B4C-59E1-924E-A5D8-DB6E776B46C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25200" windowHeight="11980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="343">
   <si>
     <t>FCRM1 - National Capital Programme</t>
   </si>
@@ -1138,21 +1138,6 @@
     <t>Confidence in Securing Partnership Funding (all schemes including post-2021)</t>
   </si>
   <si>
-    <t>Confidence Assessment Picklist</t>
-  </si>
-  <si>
-    <t>3. Medium High</t>
-  </si>
-  <si>
-    <t>2. Medium Low</t>
-  </si>
-  <si>
-    <t>1. Low</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -1194,9 +1179,6 @@
   <si>
     <t>20/21</t>
   </si>
-  <si>
-    <t>4. High</t>
-  </si>
 </sst>
 </file>
 
@@ -1209,7 +1191,7 @@
     <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     <numFmt numFmtId="168" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1543,7 +1525,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1679,11 +1661,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1969,23 +1947,23 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="67000"/>
+                <a:satMod val="105000"/>
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:tint val="73000"/>
+                <a:satMod val="103000"/>
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="81000"/>
+                <a:satMod val="109000"/>
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1995,23 +1973,23 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="94000"/>
                 <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:shade val="100000"/>
                 <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:shade val="78000"/>
+                <a:satMod val="120000"/>
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -2073,16 +2051,16 @@
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
+                <a:shade val="98000"/>
                 <a:satMod val="150000"/>
-                <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
+                <a:shade val="90000"/>
                 <a:satMod val="130000"/>
-                <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
@@ -2114,17 +2092,17 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:KN11"/>
+  <dimension ref="A1:KM7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="AZ9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="KI7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="KN6" sqref="KN6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98.7109375" style="1" customWidth="1"/>
@@ -2145,18 +2123,17 @@
     <col min="279" max="285" width="21" style="28" customWidth="1"/>
     <col min="286" max="293" width="21" style="6" customWidth="1"/>
     <col min="294" max="296" width="22.28515625" style="7" customWidth="1"/>
-    <col min="297" max="297" width="11" style="7" customWidth="1"/>
-    <col min="298" max="298" width="12.85546875" style="7" hidden="1" customWidth="1"/>
-    <col min="299" max="299" width="8.7109375" style="7"/>
-    <col min="300" max="300" width="11" style="7" customWidth="1"/>
-    <col min="301" max="16384" width="8.7109375" style="7"/>
+    <col min="297" max="297" width="17.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="298" max="298" width="8.7109375" style="7"/>
+    <col min="299" max="299" width="11" style="7" customWidth="1"/>
+    <col min="300" max="16384" width="8.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:300" ht="28.5" customHeight="1">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:299" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="64"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
@@ -2449,11 +2426,11 @@
       <c r="KF1" s="23"/>
       <c r="KG1" s="23"/>
     </row>
-    <row r="2" spans="1:300" ht="28.5" customHeight="1">
-      <c r="A2" s="67" t="s">
-        <v>342</v>
-      </c>
-      <c r="B2" s="67"/>
+    <row r="2" spans="1:299" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="65" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2" s="65"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="23"/>
@@ -2746,7 +2723,7 @@
       <c r="KF2" s="37"/>
       <c r="KG2" s="37"/>
     </row>
-    <row r="3" spans="1:300" ht="25.5" customHeight="1">
+    <row r="3" spans="1:299" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="39"/>
@@ -3041,422 +3018,422 @@
       <c r="KF3" s="45"/>
       <c r="KG3" s="45"/>
     </row>
-    <row r="4" spans="1:300" ht="46.5" customHeight="1">
-      <c r="A4" s="68" t="s">
+    <row r="4" spans="1:299" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="69" t="s">
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="70" t="s">
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="70"/>
-      <c r="P4" s="71" t="s">
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="71"/>
-      <c r="S4" s="71"/>
-      <c r="T4" s="71"/>
-      <c r="U4" s="72" t="s">
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="69"/>
+      <c r="T4" s="69"/>
+      <c r="U4" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="72"/>
-      <c r="W4" s="72"/>
-      <c r="X4" s="72"/>
-      <c r="Y4" s="72"/>
-      <c r="Z4" s="72"/>
-      <c r="AA4" s="72"/>
-      <c r="AB4" s="72"/>
-      <c r="AC4" s="73" t="s">
+      <c r="V4" s="70"/>
+      <c r="W4" s="70"/>
+      <c r="X4" s="70"/>
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="70"/>
+      <c r="AA4" s="70"/>
+      <c r="AB4" s="70"/>
+      <c r="AC4" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="73"/>
-      <c r="AE4" s="73"/>
-      <c r="AF4" s="73"/>
-      <c r="AG4" s="73"/>
-      <c r="AH4" s="73"/>
-      <c r="AI4" s="73"/>
-      <c r="AJ4" s="74" t="s">
+      <c r="AD4" s="71"/>
+      <c r="AE4" s="71"/>
+      <c r="AF4" s="71"/>
+      <c r="AG4" s="71"/>
+      <c r="AH4" s="71"/>
+      <c r="AI4" s="71"/>
+      <c r="AJ4" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="74"/>
-      <c r="AL4" s="74"/>
-      <c r="AM4" s="65" t="s">
+      <c r="AK4" s="72"/>
+      <c r="AL4" s="72"/>
+      <c r="AM4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="65"/>
-      <c r="AO4" s="76"/>
-      <c r="AP4" s="76"/>
-      <c r="AQ4" s="76"/>
-      <c r="AR4" s="76"/>
-      <c r="AS4" s="77" t="s">
+      <c r="AN4" s="63"/>
+      <c r="AO4" s="74"/>
+      <c r="AP4" s="74"/>
+      <c r="AQ4" s="74"/>
+      <c r="AR4" s="74"/>
+      <c r="AS4" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="77"/>
-      <c r="AU4" s="77"/>
-      <c r="AV4" s="77"/>
-      <c r="AW4" s="77"/>
-      <c r="AX4" s="77"/>
-      <c r="AY4" s="77"/>
-      <c r="AZ4" s="77"/>
-      <c r="BA4" s="77"/>
-      <c r="BB4" s="77"/>
-      <c r="BC4" s="77"/>
-      <c r="BD4" s="77"/>
-      <c r="BE4" s="77"/>
-      <c r="BF4" s="77"/>
-      <c r="BG4" s="77"/>
-      <c r="BH4" s="77"/>
-      <c r="BI4" s="77"/>
-      <c r="BJ4" s="77"/>
-      <c r="BK4" s="75" t="s">
+      <c r="AT4" s="75"/>
+      <c r="AU4" s="75"/>
+      <c r="AV4" s="75"/>
+      <c r="AW4" s="75"/>
+      <c r="AX4" s="75"/>
+      <c r="AY4" s="75"/>
+      <c r="AZ4" s="75"/>
+      <c r="BA4" s="75"/>
+      <c r="BB4" s="75"/>
+      <c r="BC4" s="75"/>
+      <c r="BD4" s="75"/>
+      <c r="BE4" s="75"/>
+      <c r="BF4" s="75"/>
+      <c r="BG4" s="75"/>
+      <c r="BH4" s="75"/>
+      <c r="BI4" s="75"/>
+      <c r="BJ4" s="75"/>
+      <c r="BK4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="BL4" s="75"/>
-      <c r="BM4" s="75"/>
-      <c r="BN4" s="75"/>
-      <c r="BO4" s="75"/>
-      <c r="BP4" s="75"/>
-      <c r="BQ4" s="75"/>
-      <c r="BR4" s="75"/>
-      <c r="BS4" s="75"/>
-      <c r="BT4" s="75"/>
-      <c r="BU4" s="75"/>
-      <c r="BV4" s="75"/>
-      <c r="BW4" s="75"/>
-      <c r="BX4" s="75"/>
-      <c r="BY4" s="78" t="s">
+      <c r="BL4" s="73"/>
+      <c r="BM4" s="73"/>
+      <c r="BN4" s="73"/>
+      <c r="BO4" s="73"/>
+      <c r="BP4" s="73"/>
+      <c r="BQ4" s="73"/>
+      <c r="BR4" s="73"/>
+      <c r="BS4" s="73"/>
+      <c r="BT4" s="73"/>
+      <c r="BU4" s="73"/>
+      <c r="BV4" s="73"/>
+      <c r="BW4" s="73"/>
+      <c r="BX4" s="73"/>
+      <c r="BY4" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="78"/>
-      <c r="CA4" s="78"/>
-      <c r="CB4" s="78"/>
-      <c r="CC4" s="78"/>
-      <c r="CD4" s="78"/>
-      <c r="CE4" s="78"/>
-      <c r="CF4" s="78"/>
-      <c r="CG4" s="78"/>
-      <c r="CH4" s="78"/>
-      <c r="CI4" s="78"/>
-      <c r="CJ4" s="78"/>
-      <c r="CK4" s="78"/>
-      <c r="CL4" s="78"/>
-      <c r="CM4" s="79" t="s">
+      <c r="BZ4" s="76"/>
+      <c r="CA4" s="76"/>
+      <c r="CB4" s="76"/>
+      <c r="CC4" s="76"/>
+      <c r="CD4" s="76"/>
+      <c r="CE4" s="76"/>
+      <c r="CF4" s="76"/>
+      <c r="CG4" s="76"/>
+      <c r="CH4" s="76"/>
+      <c r="CI4" s="76"/>
+      <c r="CJ4" s="76"/>
+      <c r="CK4" s="76"/>
+      <c r="CL4" s="76"/>
+      <c r="CM4" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="79"/>
-      <c r="CO4" s="79"/>
-      <c r="CP4" s="79"/>
-      <c r="CQ4" s="79"/>
-      <c r="CR4" s="79"/>
-      <c r="CS4" s="79"/>
-      <c r="CT4" s="79"/>
-      <c r="CU4" s="79"/>
-      <c r="CV4" s="79"/>
-      <c r="CW4" s="79"/>
-      <c r="CX4" s="79"/>
-      <c r="CY4" s="79"/>
-      <c r="CZ4" s="79"/>
-      <c r="DA4" s="80" t="s">
+      <c r="CN4" s="77"/>
+      <c r="CO4" s="77"/>
+      <c r="CP4" s="77"/>
+      <c r="CQ4" s="77"/>
+      <c r="CR4" s="77"/>
+      <c r="CS4" s="77"/>
+      <c r="CT4" s="77"/>
+      <c r="CU4" s="77"/>
+      <c r="CV4" s="77"/>
+      <c r="CW4" s="77"/>
+      <c r="CX4" s="77"/>
+      <c r="CY4" s="77"/>
+      <c r="CZ4" s="77"/>
+      <c r="DA4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="80"/>
-      <c r="DC4" s="80"/>
-      <c r="DD4" s="80"/>
-      <c r="DE4" s="80"/>
-      <c r="DF4" s="80"/>
-      <c r="DG4" s="80"/>
-      <c r="DH4" s="80"/>
-      <c r="DI4" s="80"/>
-      <c r="DJ4" s="80"/>
-      <c r="DK4" s="80"/>
-      <c r="DL4" s="80"/>
-      <c r="DM4" s="80"/>
-      <c r="DN4" s="80"/>
-      <c r="DO4" s="81" t="s">
+      <c r="DB4" s="78"/>
+      <c r="DC4" s="78"/>
+      <c r="DD4" s="78"/>
+      <c r="DE4" s="78"/>
+      <c r="DF4" s="78"/>
+      <c r="DG4" s="78"/>
+      <c r="DH4" s="78"/>
+      <c r="DI4" s="78"/>
+      <c r="DJ4" s="78"/>
+      <c r="DK4" s="78"/>
+      <c r="DL4" s="78"/>
+      <c r="DM4" s="78"/>
+      <c r="DN4" s="78"/>
+      <c r="DO4" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="81"/>
-      <c r="DQ4" s="81"/>
-      <c r="DR4" s="81"/>
-      <c r="DS4" s="81"/>
-      <c r="DT4" s="81"/>
-      <c r="DU4" s="81"/>
-      <c r="DV4" s="81"/>
-      <c r="DW4" s="81"/>
-      <c r="DX4" s="81"/>
-      <c r="DY4" s="81"/>
-      <c r="DZ4" s="81"/>
-      <c r="EA4" s="81"/>
-      <c r="EB4" s="81"/>
-      <c r="EC4" s="82" t="s">
+      <c r="DP4" s="79"/>
+      <c r="DQ4" s="79"/>
+      <c r="DR4" s="79"/>
+      <c r="DS4" s="79"/>
+      <c r="DT4" s="79"/>
+      <c r="DU4" s="79"/>
+      <c r="DV4" s="79"/>
+      <c r="DW4" s="79"/>
+      <c r="DX4" s="79"/>
+      <c r="DY4" s="79"/>
+      <c r="DZ4" s="79"/>
+      <c r="EA4" s="79"/>
+      <c r="EB4" s="79"/>
+      <c r="EC4" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="82"/>
-      <c r="EE4" s="82"/>
-      <c r="EF4" s="82"/>
-      <c r="EG4" s="82"/>
-      <c r="EH4" s="82"/>
-      <c r="EI4" s="82"/>
-      <c r="EJ4" s="82"/>
-      <c r="EK4" s="82"/>
-      <c r="EL4" s="82"/>
-      <c r="EM4" s="82"/>
-      <c r="EN4" s="82"/>
-      <c r="EO4" s="82"/>
-      <c r="EP4" s="82"/>
-      <c r="EQ4" s="83" t="s">
+      <c r="ED4" s="80"/>
+      <c r="EE4" s="80"/>
+      <c r="EF4" s="80"/>
+      <c r="EG4" s="80"/>
+      <c r="EH4" s="80"/>
+      <c r="EI4" s="80"/>
+      <c r="EJ4" s="80"/>
+      <c r="EK4" s="80"/>
+      <c r="EL4" s="80"/>
+      <c r="EM4" s="80"/>
+      <c r="EN4" s="80"/>
+      <c r="EO4" s="80"/>
+      <c r="EP4" s="80"/>
+      <c r="EQ4" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="83"/>
-      <c r="ES4" s="83"/>
-      <c r="ET4" s="83"/>
-      <c r="EU4" s="83"/>
-      <c r="EV4" s="83"/>
-      <c r="EW4" s="83"/>
-      <c r="EX4" s="83"/>
-      <c r="EY4" s="83"/>
-      <c r="EZ4" s="83"/>
-      <c r="FA4" s="83"/>
-      <c r="FB4" s="83"/>
-      <c r="FC4" s="83"/>
-      <c r="FD4" s="83"/>
-      <c r="FE4" s="84" t="s">
+      <c r="ER4" s="81"/>
+      <c r="ES4" s="81"/>
+      <c r="ET4" s="81"/>
+      <c r="EU4" s="81"/>
+      <c r="EV4" s="81"/>
+      <c r="EW4" s="81"/>
+      <c r="EX4" s="81"/>
+      <c r="EY4" s="81"/>
+      <c r="EZ4" s="81"/>
+      <c r="FA4" s="81"/>
+      <c r="FB4" s="81"/>
+      <c r="FC4" s="81"/>
+      <c r="FD4" s="81"/>
+      <c r="FE4" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="84"/>
-      <c r="FG4" s="84"/>
-      <c r="FH4" s="84"/>
-      <c r="FI4" s="84"/>
-      <c r="FJ4" s="84"/>
-      <c r="FK4" s="84"/>
-      <c r="FL4" s="84"/>
-      <c r="FM4" s="84"/>
-      <c r="FN4" s="84"/>
-      <c r="FO4" s="84"/>
-      <c r="FP4" s="84"/>
-      <c r="FQ4" s="84"/>
-      <c r="FR4" s="84"/>
-      <c r="FS4" s="85" t="s">
+      <c r="FF4" s="82"/>
+      <c r="FG4" s="82"/>
+      <c r="FH4" s="82"/>
+      <c r="FI4" s="82"/>
+      <c r="FJ4" s="82"/>
+      <c r="FK4" s="82"/>
+      <c r="FL4" s="82"/>
+      <c r="FM4" s="82"/>
+      <c r="FN4" s="82"/>
+      <c r="FO4" s="82"/>
+      <c r="FP4" s="82"/>
+      <c r="FQ4" s="82"/>
+      <c r="FR4" s="82"/>
+      <c r="FS4" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="85"/>
-      <c r="FU4" s="85"/>
-      <c r="FV4" s="85"/>
-      <c r="FW4" s="85"/>
-      <c r="FX4" s="85"/>
-      <c r="FY4" s="85"/>
-      <c r="FZ4" s="85"/>
-      <c r="GA4" s="85"/>
-      <c r="GB4" s="85"/>
-      <c r="GC4" s="85"/>
-      <c r="GD4" s="85"/>
-      <c r="GE4" s="85"/>
-      <c r="GF4" s="85"/>
-      <c r="GG4" s="75" t="s">
+      <c r="FT4" s="83"/>
+      <c r="FU4" s="83"/>
+      <c r="FV4" s="83"/>
+      <c r="FW4" s="83"/>
+      <c r="FX4" s="83"/>
+      <c r="FY4" s="83"/>
+      <c r="FZ4" s="83"/>
+      <c r="GA4" s="83"/>
+      <c r="GB4" s="83"/>
+      <c r="GC4" s="83"/>
+      <c r="GD4" s="83"/>
+      <c r="GE4" s="83"/>
+      <c r="GF4" s="83"/>
+      <c r="GG4" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="GH4" s="75"/>
-      <c r="GI4" s="75"/>
-      <c r="GJ4" s="75"/>
-      <c r="GK4" s="75"/>
-      <c r="GL4" s="75"/>
-      <c r="GM4" s="75"/>
-      <c r="GN4" s="75"/>
-      <c r="GO4" s="75"/>
-      <c r="GP4" s="75"/>
-      <c r="GQ4" s="75"/>
-      <c r="GR4" s="75"/>
-      <c r="GS4" s="75"/>
-      <c r="GT4" s="75"/>
-      <c r="GU4" s="75" t="s">
+      <c r="GH4" s="73"/>
+      <c r="GI4" s="73"/>
+      <c r="GJ4" s="73"/>
+      <c r="GK4" s="73"/>
+      <c r="GL4" s="73"/>
+      <c r="GM4" s="73"/>
+      <c r="GN4" s="73"/>
+      <c r="GO4" s="73"/>
+      <c r="GP4" s="73"/>
+      <c r="GQ4" s="73"/>
+      <c r="GR4" s="73"/>
+      <c r="GS4" s="73"/>
+      <c r="GT4" s="73"/>
+      <c r="GU4" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="GV4" s="75"/>
-      <c r="GW4" s="75"/>
-      <c r="GX4" s="75"/>
-      <c r="GY4" s="75"/>
-      <c r="GZ4" s="75"/>
-      <c r="HA4" s="75"/>
-      <c r="HB4" s="75"/>
-      <c r="HC4" s="75"/>
-      <c r="HD4" s="75"/>
-      <c r="HE4" s="75"/>
-      <c r="HF4" s="75"/>
-      <c r="HG4" s="75"/>
-      <c r="HH4" s="75"/>
-      <c r="HI4" s="75" t="s">
+      <c r="GV4" s="73"/>
+      <c r="GW4" s="73"/>
+      <c r="GX4" s="73"/>
+      <c r="GY4" s="73"/>
+      <c r="GZ4" s="73"/>
+      <c r="HA4" s="73"/>
+      <c r="HB4" s="73"/>
+      <c r="HC4" s="73"/>
+      <c r="HD4" s="73"/>
+      <c r="HE4" s="73"/>
+      <c r="HF4" s="73"/>
+      <c r="HG4" s="73"/>
+      <c r="HH4" s="73"/>
+      <c r="HI4" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="HJ4" s="75"/>
-      <c r="HK4" s="75"/>
-      <c r="HL4" s="75"/>
-      <c r="HM4" s="75"/>
-      <c r="HN4" s="75"/>
-      <c r="HO4" s="75"/>
-      <c r="HP4" s="75"/>
-      <c r="HQ4" s="75"/>
-      <c r="HR4" s="75"/>
-      <c r="HS4" s="75"/>
-      <c r="HT4" s="75"/>
-      <c r="HU4" s="75"/>
-      <c r="HV4" s="75"/>
-      <c r="HW4" s="92" t="s">
+      <c r="HJ4" s="73"/>
+      <c r="HK4" s="73"/>
+      <c r="HL4" s="73"/>
+      <c r="HM4" s="73"/>
+      <c r="HN4" s="73"/>
+      <c r="HO4" s="73"/>
+      <c r="HP4" s="73"/>
+      <c r="HQ4" s="73"/>
+      <c r="HR4" s="73"/>
+      <c r="HS4" s="73"/>
+      <c r="HT4" s="73"/>
+      <c r="HU4" s="73"/>
+      <c r="HV4" s="73"/>
+      <c r="HW4" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="92"/>
-      <c r="HY4" s="92"/>
-      <c r="HZ4" s="92"/>
-      <c r="IA4" s="92"/>
-      <c r="IB4" s="92"/>
-      <c r="IC4" s="92"/>
-      <c r="ID4" s="92"/>
-      <c r="IE4" s="92"/>
-      <c r="IF4" s="92"/>
-      <c r="IG4" s="92"/>
-      <c r="IH4" s="92"/>
-      <c r="II4" s="92"/>
-      <c r="IJ4" s="92"/>
-      <c r="IK4" s="92" t="s">
+      <c r="HX4" s="90"/>
+      <c r="HY4" s="90"/>
+      <c r="HZ4" s="90"/>
+      <c r="IA4" s="90"/>
+      <c r="IB4" s="90"/>
+      <c r="IC4" s="90"/>
+      <c r="ID4" s="90"/>
+      <c r="IE4" s="90"/>
+      <c r="IF4" s="90"/>
+      <c r="IG4" s="90"/>
+      <c r="IH4" s="90"/>
+      <c r="II4" s="90"/>
+      <c r="IJ4" s="90"/>
+      <c r="IK4" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="92"/>
-      <c r="IM4" s="92"/>
-      <c r="IN4" s="92"/>
-      <c r="IO4" s="92"/>
-      <c r="IP4" s="92"/>
-      <c r="IQ4" s="92"/>
-      <c r="IR4" s="92"/>
-      <c r="IS4" s="92"/>
-      <c r="IT4" s="92"/>
-      <c r="IU4" s="92"/>
-      <c r="IV4" s="92"/>
-      <c r="IW4" s="92"/>
-      <c r="IX4" s="92"/>
-      <c r="IY4" s="92" t="s">
+      <c r="IL4" s="90"/>
+      <c r="IM4" s="90"/>
+      <c r="IN4" s="90"/>
+      <c r="IO4" s="90"/>
+      <c r="IP4" s="90"/>
+      <c r="IQ4" s="90"/>
+      <c r="IR4" s="90"/>
+      <c r="IS4" s="90"/>
+      <c r="IT4" s="90"/>
+      <c r="IU4" s="90"/>
+      <c r="IV4" s="90"/>
+      <c r="IW4" s="90"/>
+      <c r="IX4" s="90"/>
+      <c r="IY4" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="92"/>
-      <c r="JA4" s="92"/>
-      <c r="JB4" s="92"/>
-      <c r="JC4" s="92"/>
-      <c r="JD4" s="92"/>
-      <c r="JE4" s="92"/>
-      <c r="JF4" s="92"/>
-      <c r="JG4" s="92"/>
-      <c r="JH4" s="92"/>
-      <c r="JI4" s="92"/>
-      <c r="JJ4" s="92"/>
-      <c r="JK4" s="92"/>
-      <c r="JL4" s="92"/>
-      <c r="JM4" s="93" t="s">
+      <c r="IZ4" s="90"/>
+      <c r="JA4" s="90"/>
+      <c r="JB4" s="90"/>
+      <c r="JC4" s="90"/>
+      <c r="JD4" s="90"/>
+      <c r="JE4" s="90"/>
+      <c r="JF4" s="90"/>
+      <c r="JG4" s="90"/>
+      <c r="JH4" s="90"/>
+      <c r="JI4" s="90"/>
+      <c r="JJ4" s="90"/>
+      <c r="JK4" s="90"/>
+      <c r="JL4" s="90"/>
+      <c r="JM4" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="93"/>
-      <c r="JO4" s="93"/>
-      <c r="JP4" s="93"/>
-      <c r="JQ4" s="93"/>
-      <c r="JR4" s="93"/>
-      <c r="JS4" s="93"/>
-      <c r="JT4" s="93"/>
-      <c r="JU4" s="93"/>
-      <c r="JV4" s="93"/>
-      <c r="JW4" s="93"/>
-      <c r="JX4" s="93"/>
-      <c r="JY4" s="93"/>
-      <c r="JZ4" s="90" t="s">
+      <c r="JN4" s="91"/>
+      <c r="JO4" s="91"/>
+      <c r="JP4" s="91"/>
+      <c r="JQ4" s="91"/>
+      <c r="JR4" s="91"/>
+      <c r="JS4" s="91"/>
+      <c r="JT4" s="91"/>
+      <c r="JU4" s="91"/>
+      <c r="JV4" s="91"/>
+      <c r="JW4" s="91"/>
+      <c r="JX4" s="91"/>
+      <c r="JY4" s="91"/>
+      <c r="JZ4" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="91"/>
-      <c r="KB4" s="91"/>
-      <c r="KC4" s="91"/>
-      <c r="KD4" s="91"/>
-      <c r="KE4" s="91"/>
-      <c r="KF4" s="91"/>
-      <c r="KG4" s="91"/>
-      <c r="KH4" s="86" t="s">
+      <c r="KA4" s="89"/>
+      <c r="KB4" s="89"/>
+      <c r="KC4" s="89"/>
+      <c r="KD4" s="89"/>
+      <c r="KE4" s="89"/>
+      <c r="KF4" s="89"/>
+      <c r="KG4" s="89"/>
+      <c r="KH4" s="84" t="s">
         <v>316</v>
       </c>
-      <c r="KI4" s="87"/>
-      <c r="KJ4" s="87"/>
+      <c r="KI4" s="85"/>
+      <c r="KJ4" s="85"/>
       <c r="KK4" s="46"/>
     </row>
-    <row r="5" spans="1:300" ht="12" customHeight="1">
-      <c r="A5" s="68"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="71"/>
-      <c r="R5" s="71"/>
-      <c r="S5" s="71"/>
-      <c r="T5" s="71"/>
-      <c r="U5" s="72"/>
-      <c r="V5" s="72"/>
-      <c r="W5" s="72"/>
-      <c r="X5" s="72"/>
-      <c r="Y5" s="72"/>
-      <c r="Z5" s="72"/>
-      <c r="AA5" s="72"/>
-      <c r="AB5" s="72"/>
-      <c r="AC5" s="73"/>
-      <c r="AD5" s="73"/>
-      <c r="AE5" s="73"/>
-      <c r="AF5" s="73"/>
-      <c r="AG5" s="73"/>
-      <c r="AH5" s="73"/>
-      <c r="AI5" s="73"/>
-      <c r="AJ5" s="74"/>
-      <c r="AK5" s="74"/>
-      <c r="AL5" s="74"/>
-      <c r="AM5" s="65"/>
-      <c r="AN5" s="65"/>
-      <c r="AO5" s="76"/>
-      <c r="AP5" s="76"/>
-      <c r="AQ5" s="76"/>
-      <c r="AR5" s="76"/>
-      <c r="AS5" s="77"/>
-      <c r="AT5" s="77"/>
-      <c r="AU5" s="77"/>
-      <c r="AV5" s="77"/>
-      <c r="AW5" s="77"/>
-      <c r="AX5" s="77"/>
-      <c r="AY5" s="77"/>
-      <c r="AZ5" s="77"/>
-      <c r="BA5" s="77"/>
-      <c r="BB5" s="77"/>
-      <c r="BC5" s="77"/>
-      <c r="BD5" s="77"/>
-      <c r="BE5" s="77"/>
-      <c r="BF5" s="77"/>
-      <c r="BG5" s="77"/>
-      <c r="BH5" s="77"/>
-      <c r="BI5" s="77"/>
-      <c r="BJ5" s="77"/>
+    <row r="5" spans="1:299" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="66"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="70"/>
+      <c r="X5" s="70"/>
+      <c r="Y5" s="70"/>
+      <c r="Z5" s="70"/>
+      <c r="AA5" s="70"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="71"/>
+      <c r="AD5" s="71"/>
+      <c r="AE5" s="71"/>
+      <c r="AF5" s="71"/>
+      <c r="AG5" s="71"/>
+      <c r="AH5" s="71"/>
+      <c r="AI5" s="71"/>
+      <c r="AJ5" s="72"/>
+      <c r="AK5" s="72"/>
+      <c r="AL5" s="72"/>
+      <c r="AM5" s="63"/>
+      <c r="AN5" s="63"/>
+      <c r="AO5" s="74"/>
+      <c r="AP5" s="74"/>
+      <c r="AQ5" s="74"/>
+      <c r="AR5" s="74"/>
+      <c r="AS5" s="75"/>
+      <c r="AT5" s="75"/>
+      <c r="AU5" s="75"/>
+      <c r="AV5" s="75"/>
+      <c r="AW5" s="75"/>
+      <c r="AX5" s="75"/>
+      <c r="AY5" s="75"/>
+      <c r="AZ5" s="75"/>
+      <c r="BA5" s="75"/>
+      <c r="BB5" s="75"/>
+      <c r="BC5" s="75"/>
+      <c r="BD5" s="75"/>
+      <c r="BE5" s="75"/>
+      <c r="BF5" s="75"/>
+      <c r="BG5" s="75"/>
+      <c r="BH5" s="75"/>
+      <c r="BI5" s="75"/>
+      <c r="BJ5" s="75"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -4087,37 +4064,37 @@
       <c r="JL5" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="JM5" s="93"/>
-      <c r="JN5" s="93"/>
-      <c r="JO5" s="93"/>
-      <c r="JP5" s="93"/>
-      <c r="JQ5" s="93"/>
-      <c r="JR5" s="93"/>
-      <c r="JS5" s="93"/>
-      <c r="JT5" s="93"/>
-      <c r="JU5" s="93"/>
-      <c r="JV5" s="93"/>
-      <c r="JW5" s="93"/>
-      <c r="JX5" s="93"/>
-      <c r="JY5" s="93"/>
-      <c r="JZ5" s="91" t="s">
-        <v>347</v>
-      </c>
-      <c r="KA5" s="91"/>
-      <c r="KB5" s="91"/>
-      <c r="KC5" s="91"/>
-      <c r="KD5" s="91" t="s">
+      <c r="JM5" s="91"/>
+      <c r="JN5" s="91"/>
+      <c r="JO5" s="91"/>
+      <c r="JP5" s="91"/>
+      <c r="JQ5" s="91"/>
+      <c r="JR5" s="91"/>
+      <c r="JS5" s="91"/>
+      <c r="JT5" s="91"/>
+      <c r="JU5" s="91"/>
+      <c r="JV5" s="91"/>
+      <c r="JW5" s="91"/>
+      <c r="JX5" s="91"/>
+      <c r="JY5" s="91"/>
+      <c r="JZ5" s="89" t="s">
+        <v>342</v>
+      </c>
+      <c r="KA5" s="89"/>
+      <c r="KB5" s="89"/>
+      <c r="KC5" s="89"/>
+      <c r="KD5" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="91"/>
-      <c r="KF5" s="91"/>
-      <c r="KG5" s="91"/>
-      <c r="KH5" s="88"/>
-      <c r="KI5" s="89"/>
-      <c r="KJ5" s="89"/>
+      <c r="KE5" s="89"/>
+      <c r="KF5" s="89"/>
+      <c r="KG5" s="89"/>
+      <c r="KH5" s="86"/>
+      <c r="KI5" s="87"/>
+      <c r="KJ5" s="87"/>
       <c r="KK5" s="46"/>
     </row>
-    <row r="6" spans="1:300" ht="81.75" customHeight="1">
+    <row r="6" spans="1:299" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -4974,16 +4951,16 @@
         <v>308</v>
       </c>
       <c r="JZ6" s="22" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="KA6" s="29" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="KB6" s="22" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="KC6" s="22" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="KD6" s="22" t="s">
         <v>309</v>
@@ -5009,1657 +4986,443 @@
       <c r="KK6" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="KL6" s="49" t="s">
+      <c r="KL6" s="48"/>
+      <c r="KM6" s="49"/>
+    </row>
+    <row r="7" spans="1:299" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50" t="s">
         <v>336</v>
       </c>
-      <c r="KM6" s="50"/>
-      <c r="KN6" s="51"/>
-    </row>
-    <row r="7" spans="1:300" ht="15" customHeight="1">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52" t="s">
-        <v>341</v>
-      </c>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="54" t="s">
-        <v>341</v>
-      </c>
-      <c r="S7" s="54" t="s">
-        <v>341</v>
-      </c>
-      <c r="T7" s="54"/>
-      <c r="U7" s="54"/>
-      <c r="V7" s="54"/>
-      <c r="W7" s="54"/>
-      <c r="X7" s="55" t="s">
-        <v>341</v>
-      </c>
-      <c r="Y7" s="55" t="s">
-        <v>341</v>
-      </c>
-      <c r="Z7" s="54"/>
-      <c r="AA7" s="54"/>
-      <c r="AB7" s="55"/>
-      <c r="AC7" s="56"/>
-      <c r="AD7" s="57"/>
-      <c r="AE7" s="57"/>
-      <c r="AF7" s="58"/>
-      <c r="AG7" s="58"/>
-      <c r="AH7" s="59"/>
-      <c r="AI7" s="58"/>
-      <c r="AJ7" s="53" t="s">
-        <v>341</v>
-      </c>
-      <c r="AK7" s="53" t="s">
-        <v>341</v>
-      </c>
-      <c r="AL7" s="53" t="s">
-        <v>341</v>
-      </c>
-      <c r="AM7" s="54"/>
-      <c r="AN7" s="60"/>
-      <c r="AO7" s="61"/>
-      <c r="AP7" s="61"/>
-      <c r="AQ7" s="61"/>
-      <c r="AR7" s="61"/>
-      <c r="AS7" s="62">
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="52" t="s">
+        <v>336</v>
+      </c>
+      <c r="S7" s="52" t="s">
+        <v>336</v>
+      </c>
+      <c r="T7" s="52"/>
+      <c r="U7" s="52"/>
+      <c r="V7" s="52"/>
+      <c r="W7" s="52"/>
+      <c r="X7" s="53" t="s">
+        <v>336</v>
+      </c>
+      <c r="Y7" s="53" t="s">
+        <v>336</v>
+      </c>
+      <c r="Z7" s="52"/>
+      <c r="AA7" s="52"/>
+      <c r="AB7" s="53"/>
+      <c r="AC7" s="54"/>
+      <c r="AD7" s="55"/>
+      <c r="AE7" s="55"/>
+      <c r="AF7" s="56"/>
+      <c r="AG7" s="56"/>
+      <c r="AH7" s="57"/>
+      <c r="AI7" s="56"/>
+      <c r="AJ7" s="51" t="s">
+        <v>336</v>
+      </c>
+      <c r="AK7" s="51" t="s">
+        <v>336</v>
+      </c>
+      <c r="AL7" s="51" t="s">
+        <v>336</v>
+      </c>
+      <c r="AM7" s="52"/>
+      <c r="AN7" s="58"/>
+      <c r="AO7" s="59"/>
+      <c r="AP7" s="59"/>
+      <c r="AQ7" s="59"/>
+      <c r="AR7" s="59"/>
+      <c r="AS7" s="60">
         <f>SUM(BK7:BX7)</f>
         <v>0</v>
       </c>
-      <c r="AT7" s="63">
+      <c r="AT7" s="61">
         <f>SUM(BY7:CL7)</f>
         <v>0</v>
       </c>
-      <c r="AU7" s="63">
+      <c r="AU7" s="61">
         <f>SUM(CM7:CZ7)</f>
         <v>0</v>
       </c>
-      <c r="AV7" s="63">
+      <c r="AV7" s="61">
         <f>SUM(DA7:DN7)</f>
         <v>0</v>
       </c>
-      <c r="AW7" s="63">
+      <c r="AW7" s="61">
         <f>SUM(DO7:EB7)</f>
         <v>0</v>
       </c>
-      <c r="AX7" s="63">
+      <c r="AX7" s="61">
         <f>SUM(EC7:EP7)</f>
         <v>0</v>
       </c>
-      <c r="AY7" s="63">
+      <c r="AY7" s="61">
         <f>SUM(EQ7:FD7)</f>
         <v>0</v>
       </c>
-      <c r="AZ7" s="63">
+      <c r="AZ7" s="61">
         <f>SUM(FE7:FR7)</f>
         <v>0</v>
       </c>
-      <c r="BA7" s="63">
+      <c r="BA7" s="61">
         <f>SUM(FS7:GF7)</f>
         <v>0</v>
       </c>
-      <c r="BB7" s="63">
+      <c r="BB7" s="61">
         <f>SUM(GG7:GT7)</f>
         <v>0</v>
       </c>
-      <c r="BC7" s="63">
+      <c r="BC7" s="61">
         <f>SUM(GU7:HH7)</f>
         <v>0</v>
       </c>
-      <c r="BD7" s="63">
+      <c r="BD7" s="61">
         <f>SUM(HI7:HV7)</f>
         <v>0</v>
       </c>
-      <c r="BE7" s="63">
+      <c r="BE7" s="61">
         <f>SUM(HW7:IJ7)</f>
         <v>0</v>
       </c>
-      <c r="BF7" s="63">
+      <c r="BF7" s="61">
         <f>SUM(IK7:IX7)</f>
         <v>0</v>
       </c>
-      <c r="BG7" s="63">
+      <c r="BG7" s="61">
         <f>SUM(IY7:JL7)</f>
         <v>0</v>
       </c>
-      <c r="BH7" s="63">
+      <c r="BH7" s="61">
         <f t="shared" ref="BH7" si="0">JM7</f>
         <v>0</v>
       </c>
-      <c r="BI7" s="63">
+      <c r="BI7" s="61">
         <f>JN7</f>
         <v>0</v>
       </c>
-      <c r="BJ7" s="63">
+      <c r="BJ7" s="61">
         <f>JO7</f>
         <v>0</v>
       </c>
-      <c r="BK7" s="63">
+      <c r="BK7" s="61">
         <f t="shared" ref="BK7:BX7" si="1">BY7+CM7+DA7+DO7+EC7+EQ7+FE7+FS7</f>
         <v>0</v>
       </c>
-      <c r="BL7" s="63">
+      <c r="BL7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BM7" s="63">
+      <c r="BM7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BN7" s="63">
+      <c r="BN7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BO7" s="63">
+      <c r="BO7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BP7" s="63">
+      <c r="BP7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BQ7" s="63">
+      <c r="BQ7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BR7" s="63">
+      <c r="BR7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BS7" s="63">
+      <c r="BS7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BT7" s="63">
+      <c r="BT7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BU7" s="63">
+      <c r="BU7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BV7" s="63">
+      <c r="BV7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BW7" s="63">
+      <c r="BW7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BX7" s="63">
+      <c r="BX7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BY7" s="58"/>
-      <c r="BZ7" s="58"/>
-      <c r="CA7" s="58"/>
-      <c r="CB7" s="58"/>
-      <c r="CC7" s="58"/>
-      <c r="CD7" s="58"/>
-      <c r="CE7" s="58"/>
-      <c r="CF7" s="58"/>
-      <c r="CG7" s="58"/>
-      <c r="CH7" s="58"/>
-      <c r="CI7" s="58"/>
-      <c r="CJ7" s="58"/>
-      <c r="CK7" s="58"/>
-      <c r="CL7" s="58"/>
-      <c r="CM7" s="58"/>
-      <c r="CN7" s="58"/>
-      <c r="CO7" s="58"/>
-      <c r="CP7" s="58"/>
-      <c r="CQ7" s="58"/>
-      <c r="CR7" s="58"/>
-      <c r="CS7" s="58"/>
-      <c r="CT7" s="58"/>
-      <c r="CU7" s="58"/>
-      <c r="CV7" s="58"/>
-      <c r="CW7" s="58"/>
-      <c r="CX7" s="58"/>
-      <c r="CY7" s="58"/>
-      <c r="CZ7" s="58"/>
-      <c r="DA7" s="58"/>
-      <c r="DB7" s="58"/>
-      <c r="DC7" s="58"/>
-      <c r="DD7" s="58"/>
-      <c r="DE7" s="58"/>
-      <c r="DF7" s="58"/>
-      <c r="DG7" s="58"/>
-      <c r="DH7" s="58"/>
-      <c r="DI7" s="58"/>
-      <c r="DJ7" s="58"/>
-      <c r="DK7" s="58"/>
-      <c r="DL7" s="58"/>
-      <c r="DM7" s="58"/>
-      <c r="DN7" s="58"/>
-      <c r="DO7" s="58"/>
-      <c r="DP7" s="58"/>
-      <c r="DQ7" s="58"/>
-      <c r="DR7" s="58"/>
-      <c r="DS7" s="58"/>
-      <c r="DT7" s="58"/>
-      <c r="DU7" s="58"/>
-      <c r="DV7" s="58"/>
-      <c r="DW7" s="58"/>
-      <c r="DX7" s="58"/>
-      <c r="DY7" s="58"/>
-      <c r="DZ7" s="58"/>
-      <c r="EA7" s="58"/>
-      <c r="EB7" s="58"/>
-      <c r="EC7" s="58"/>
-      <c r="ED7" s="58"/>
-      <c r="EE7" s="58"/>
-      <c r="EF7" s="58"/>
-      <c r="EG7" s="58"/>
-      <c r="EH7" s="58"/>
-      <c r="EI7" s="58"/>
-      <c r="EJ7" s="58"/>
-      <c r="EK7" s="58"/>
-      <c r="EL7" s="58"/>
-      <c r="EM7" s="58"/>
-      <c r="EN7" s="58"/>
-      <c r="EO7" s="58"/>
-      <c r="EP7" s="58"/>
-      <c r="EQ7" s="58"/>
-      <c r="ER7" s="58"/>
-      <c r="ES7" s="58"/>
-      <c r="ET7" s="58"/>
-      <c r="EU7" s="58"/>
-      <c r="EV7" s="58"/>
-      <c r="EW7" s="58"/>
-      <c r="EX7" s="58"/>
-      <c r="EY7" s="58"/>
-      <c r="EZ7" s="58"/>
-      <c r="FA7" s="58"/>
-      <c r="FB7" s="58"/>
-      <c r="FC7" s="58"/>
-      <c r="FD7" s="58"/>
-      <c r="FE7" s="58"/>
-      <c r="FF7" s="58"/>
-      <c r="FG7" s="58"/>
-      <c r="FH7" s="58"/>
-      <c r="FI7" s="58"/>
-      <c r="FJ7" s="58"/>
-      <c r="FK7" s="58"/>
-      <c r="FL7" s="58"/>
-      <c r="FM7" s="58"/>
-      <c r="FN7" s="58"/>
-      <c r="FO7" s="58"/>
-      <c r="FP7" s="58"/>
-      <c r="FQ7" s="58"/>
-      <c r="FR7" s="58"/>
-      <c r="FS7" s="58"/>
-      <c r="FT7" s="58"/>
-      <c r="FU7" s="58"/>
-      <c r="FV7" s="58"/>
-      <c r="FW7" s="58"/>
-      <c r="FX7" s="58"/>
-      <c r="FY7" s="58"/>
-      <c r="FZ7" s="58"/>
-      <c r="GA7" s="58"/>
-      <c r="GB7" s="58"/>
-      <c r="GC7" s="58"/>
-      <c r="GD7" s="58"/>
-      <c r="GE7" s="58"/>
-      <c r="GF7" s="58"/>
-      <c r="GG7" s="58"/>
-      <c r="GH7" s="58"/>
-      <c r="GI7" s="58"/>
-      <c r="GJ7" s="58"/>
-      <c r="GK7" s="58"/>
-      <c r="GL7" s="58"/>
-      <c r="GM7" s="58"/>
-      <c r="GN7" s="58"/>
-      <c r="GO7" s="58"/>
-      <c r="GP7" s="58"/>
-      <c r="GQ7" s="58"/>
-      <c r="GR7" s="58"/>
-      <c r="GS7" s="58"/>
-      <c r="GT7" s="58"/>
-      <c r="GU7" s="58"/>
-      <c r="GV7" s="58"/>
-      <c r="GW7" s="58"/>
-      <c r="GX7" s="58"/>
-      <c r="GY7" s="58"/>
-      <c r="GZ7" s="58"/>
-      <c r="HA7" s="58"/>
-      <c r="HB7" s="58"/>
-      <c r="HC7" s="58"/>
-      <c r="HD7" s="58"/>
-      <c r="HE7" s="58"/>
-      <c r="HF7" s="58"/>
-      <c r="HG7" s="58"/>
-      <c r="HH7" s="58"/>
-      <c r="HI7" s="58"/>
-      <c r="HJ7" s="58"/>
-      <c r="HK7" s="58"/>
-      <c r="HL7" s="58"/>
-      <c r="HM7" s="58"/>
-      <c r="HN7" s="58"/>
-      <c r="HO7" s="58"/>
-      <c r="HP7" s="58"/>
-      <c r="HQ7" s="58"/>
-      <c r="HR7" s="58"/>
-      <c r="HS7" s="58"/>
-      <c r="HT7" s="58"/>
-      <c r="HU7" s="58"/>
-      <c r="HV7" s="58"/>
-      <c r="HW7" s="58"/>
-      <c r="HX7" s="58"/>
-      <c r="HY7" s="58"/>
-      <c r="HZ7" s="58"/>
-      <c r="IA7" s="58"/>
-      <c r="IB7" s="58"/>
-      <c r="IC7" s="58"/>
-      <c r="ID7" s="58"/>
-      <c r="IE7" s="58"/>
-      <c r="IF7" s="58"/>
-      <c r="IG7" s="58"/>
-      <c r="IH7" s="58"/>
-      <c r="II7" s="58"/>
-      <c r="IJ7" s="58"/>
-      <c r="IK7" s="58"/>
-      <c r="IL7" s="58"/>
-      <c r="IM7" s="58"/>
-      <c r="IN7" s="58"/>
-      <c r="IO7" s="58"/>
-      <c r="IP7" s="58"/>
-      <c r="IQ7" s="58"/>
-      <c r="IR7" s="58"/>
-      <c r="IS7" s="58"/>
-      <c r="IT7" s="58"/>
-      <c r="IU7" s="58"/>
-      <c r="IV7" s="58"/>
-      <c r="IW7" s="58"/>
-      <c r="IX7" s="58"/>
-      <c r="IY7" s="58"/>
-      <c r="IZ7" s="58"/>
-      <c r="JA7" s="58"/>
-      <c r="JB7" s="58"/>
-      <c r="JC7" s="58"/>
-      <c r="JD7" s="58"/>
-      <c r="JE7" s="58"/>
-      <c r="JF7" s="58"/>
-      <c r="JG7" s="58"/>
-      <c r="JH7" s="58"/>
-      <c r="JI7" s="58"/>
-      <c r="JJ7" s="58"/>
-      <c r="JK7" s="58"/>
-      <c r="JL7" s="58"/>
-      <c r="JM7" s="58"/>
-      <c r="JN7" s="58"/>
-      <c r="JO7" s="58"/>
-      <c r="JP7" s="53"/>
-      <c r="JQ7" s="53"/>
-      <c r="JR7" s="53"/>
-      <c r="JS7" s="64"/>
-      <c r="JT7" s="64"/>
-      <c r="JU7" s="64"/>
-      <c r="JV7" s="64"/>
-      <c r="JW7" s="64"/>
-      <c r="JX7" s="64"/>
-      <c r="JY7" s="64"/>
-      <c r="JZ7" s="63">
+      <c r="BY7" s="56"/>
+      <c r="BZ7" s="56"/>
+      <c r="CA7" s="56"/>
+      <c r="CB7" s="56"/>
+      <c r="CC7" s="56"/>
+      <c r="CD7" s="56"/>
+      <c r="CE7" s="56"/>
+      <c r="CF7" s="56"/>
+      <c r="CG7" s="56"/>
+      <c r="CH7" s="56"/>
+      <c r="CI7" s="56"/>
+      <c r="CJ7" s="56"/>
+      <c r="CK7" s="56"/>
+      <c r="CL7" s="56"/>
+      <c r="CM7" s="56"/>
+      <c r="CN7" s="56"/>
+      <c r="CO7" s="56"/>
+      <c r="CP7" s="56"/>
+      <c r="CQ7" s="56"/>
+      <c r="CR7" s="56"/>
+      <c r="CS7" s="56"/>
+      <c r="CT7" s="56"/>
+      <c r="CU7" s="56"/>
+      <c r="CV7" s="56"/>
+      <c r="CW7" s="56"/>
+      <c r="CX7" s="56"/>
+      <c r="CY7" s="56"/>
+      <c r="CZ7" s="56"/>
+      <c r="DA7" s="56"/>
+      <c r="DB7" s="56"/>
+      <c r="DC7" s="56"/>
+      <c r="DD7" s="56"/>
+      <c r="DE7" s="56"/>
+      <c r="DF7" s="56"/>
+      <c r="DG7" s="56"/>
+      <c r="DH7" s="56"/>
+      <c r="DI7" s="56"/>
+      <c r="DJ7" s="56"/>
+      <c r="DK7" s="56"/>
+      <c r="DL7" s="56"/>
+      <c r="DM7" s="56"/>
+      <c r="DN7" s="56"/>
+      <c r="DO7" s="56"/>
+      <c r="DP7" s="56"/>
+      <c r="DQ7" s="56"/>
+      <c r="DR7" s="56"/>
+      <c r="DS7" s="56"/>
+      <c r="DT7" s="56"/>
+      <c r="DU7" s="56"/>
+      <c r="DV7" s="56"/>
+      <c r="DW7" s="56"/>
+      <c r="DX7" s="56"/>
+      <c r="DY7" s="56"/>
+      <c r="DZ7" s="56"/>
+      <c r="EA7" s="56"/>
+      <c r="EB7" s="56"/>
+      <c r="EC7" s="56"/>
+      <c r="ED7" s="56"/>
+      <c r="EE7" s="56"/>
+      <c r="EF7" s="56"/>
+      <c r="EG7" s="56"/>
+      <c r="EH7" s="56"/>
+      <c r="EI7" s="56"/>
+      <c r="EJ7" s="56"/>
+      <c r="EK7" s="56"/>
+      <c r="EL7" s="56"/>
+      <c r="EM7" s="56"/>
+      <c r="EN7" s="56"/>
+      <c r="EO7" s="56"/>
+      <c r="EP7" s="56"/>
+      <c r="EQ7" s="56"/>
+      <c r="ER7" s="56"/>
+      <c r="ES7" s="56"/>
+      <c r="ET7" s="56"/>
+      <c r="EU7" s="56"/>
+      <c r="EV7" s="56"/>
+      <c r="EW7" s="56"/>
+      <c r="EX7" s="56"/>
+      <c r="EY7" s="56"/>
+      <c r="EZ7" s="56"/>
+      <c r="FA7" s="56"/>
+      <c r="FB7" s="56"/>
+      <c r="FC7" s="56"/>
+      <c r="FD7" s="56"/>
+      <c r="FE7" s="56"/>
+      <c r="FF7" s="56"/>
+      <c r="FG7" s="56"/>
+      <c r="FH7" s="56"/>
+      <c r="FI7" s="56"/>
+      <c r="FJ7" s="56"/>
+      <c r="FK7" s="56"/>
+      <c r="FL7" s="56"/>
+      <c r="FM7" s="56"/>
+      <c r="FN7" s="56"/>
+      <c r="FO7" s="56"/>
+      <c r="FP7" s="56"/>
+      <c r="FQ7" s="56"/>
+      <c r="FR7" s="56"/>
+      <c r="FS7" s="56"/>
+      <c r="FT7" s="56"/>
+      <c r="FU7" s="56"/>
+      <c r="FV7" s="56"/>
+      <c r="FW7" s="56"/>
+      <c r="FX7" s="56"/>
+      <c r="FY7" s="56"/>
+      <c r="FZ7" s="56"/>
+      <c r="GA7" s="56"/>
+      <c r="GB7" s="56"/>
+      <c r="GC7" s="56"/>
+      <c r="GD7" s="56"/>
+      <c r="GE7" s="56"/>
+      <c r="GF7" s="56"/>
+      <c r="GG7" s="56"/>
+      <c r="GH7" s="56"/>
+      <c r="GI7" s="56"/>
+      <c r="GJ7" s="56"/>
+      <c r="GK7" s="56"/>
+      <c r="GL7" s="56"/>
+      <c r="GM7" s="56"/>
+      <c r="GN7" s="56"/>
+      <c r="GO7" s="56"/>
+      <c r="GP7" s="56"/>
+      <c r="GQ7" s="56"/>
+      <c r="GR7" s="56"/>
+      <c r="GS7" s="56"/>
+      <c r="GT7" s="56"/>
+      <c r="GU7" s="56"/>
+      <c r="GV7" s="56"/>
+      <c r="GW7" s="56"/>
+      <c r="GX7" s="56"/>
+      <c r="GY7" s="56"/>
+      <c r="GZ7" s="56"/>
+      <c r="HA7" s="56"/>
+      <c r="HB7" s="56"/>
+      <c r="HC7" s="56"/>
+      <c r="HD7" s="56"/>
+      <c r="HE7" s="56"/>
+      <c r="HF7" s="56"/>
+      <c r="HG7" s="56"/>
+      <c r="HH7" s="56"/>
+      <c r="HI7" s="56"/>
+      <c r="HJ7" s="56"/>
+      <c r="HK7" s="56"/>
+      <c r="HL7" s="56"/>
+      <c r="HM7" s="56"/>
+      <c r="HN7" s="56"/>
+      <c r="HO7" s="56"/>
+      <c r="HP7" s="56"/>
+      <c r="HQ7" s="56"/>
+      <c r="HR7" s="56"/>
+      <c r="HS7" s="56"/>
+      <c r="HT7" s="56"/>
+      <c r="HU7" s="56"/>
+      <c r="HV7" s="56"/>
+      <c r="HW7" s="56"/>
+      <c r="HX7" s="56"/>
+      <c r="HY7" s="56"/>
+      <c r="HZ7" s="56"/>
+      <c r="IA7" s="56"/>
+      <c r="IB7" s="56"/>
+      <c r="IC7" s="56"/>
+      <c r="ID7" s="56"/>
+      <c r="IE7" s="56"/>
+      <c r="IF7" s="56"/>
+      <c r="IG7" s="56"/>
+      <c r="IH7" s="56"/>
+      <c r="II7" s="56"/>
+      <c r="IJ7" s="56"/>
+      <c r="IK7" s="56"/>
+      <c r="IL7" s="56"/>
+      <c r="IM7" s="56"/>
+      <c r="IN7" s="56"/>
+      <c r="IO7" s="56"/>
+      <c r="IP7" s="56"/>
+      <c r="IQ7" s="56"/>
+      <c r="IR7" s="56"/>
+      <c r="IS7" s="56"/>
+      <c r="IT7" s="56"/>
+      <c r="IU7" s="56"/>
+      <c r="IV7" s="56"/>
+      <c r="IW7" s="56"/>
+      <c r="IX7" s="56"/>
+      <c r="IY7" s="56"/>
+      <c r="IZ7" s="56"/>
+      <c r="JA7" s="56"/>
+      <c r="JB7" s="56"/>
+      <c r="JC7" s="56"/>
+      <c r="JD7" s="56"/>
+      <c r="JE7" s="56"/>
+      <c r="JF7" s="56"/>
+      <c r="JG7" s="56"/>
+      <c r="JH7" s="56"/>
+      <c r="JI7" s="56"/>
+      <c r="JJ7" s="56"/>
+      <c r="JK7" s="56"/>
+      <c r="JL7" s="56"/>
+      <c r="JM7" s="56"/>
+      <c r="JN7" s="56"/>
+      <c r="JO7" s="56"/>
+      <c r="JP7" s="51"/>
+      <c r="JQ7" s="51"/>
+      <c r="JR7" s="51"/>
+      <c r="JS7" s="62"/>
+      <c r="JT7" s="62"/>
+      <c r="JU7" s="62"/>
+      <c r="JV7" s="62"/>
+      <c r="JW7" s="62"/>
+      <c r="JX7" s="62"/>
+      <c r="JY7" s="62"/>
+      <c r="JZ7" s="61">
         <f>BQ7</f>
         <v>0</v>
       </c>
-      <c r="KA7" s="63">
+      <c r="KA7" s="61">
         <f>CE7+CS7</f>
         <v>0</v>
       </c>
-      <c r="KB7" s="63">
+      <c r="KB7" s="61">
         <f>DG7+DU7+EI7+EW7+FK7+FY7</f>
         <v>0</v>
       </c>
-      <c r="KC7" s="63">
+      <c r="KC7" s="61">
         <f>GM7+IC7</f>
         <v>0</v>
       </c>
-      <c r="KD7" s="63">
+      <c r="KD7" s="61">
         <f>SUM(BL7:BQ7)</f>
         <v>0</v>
       </c>
-      <c r="KE7" s="63">
+      <c r="KE7" s="61">
         <f>SUM(CN7:CS7)+SUM(BZ7:CE7)</f>
         <v>0</v>
       </c>
-      <c r="KF7" s="63">
+      <c r="KF7" s="61">
         <f>SUM(DB7:DG7)+SUM(DP7:DU7)+SUM(ED7:EI7)+SUM(ER7:EW7)+SUM(FF7:FK7)+SUM(FT7:FY7)</f>
         <v>0</v>
       </c>
-      <c r="KG7" s="63">
+      <c r="KG7" s="61">
         <f>SUM(GH7:GM7)+SUM(HX7:IC7)</f>
         <v>0</v>
       </c>
-      <c r="KH7" s="48"/>
-      <c r="KI7" s="48"/>
-      <c r="KJ7" s="48"/>
-      <c r="KK7" s="48"/>
-      <c r="KL7" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="8" spans="1:300">
-      <c r="A8" s="25"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="26"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="26"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="26"/>
-      <c r="AE8" s="26"/>
-      <c r="AF8" s="23"/>
-      <c r="AG8" s="23"/>
-      <c r="AH8" s="23"/>
-      <c r="AI8" s="23"/>
-      <c r="AJ8" s="23"/>
-      <c r="AK8" s="23"/>
-      <c r="AL8" s="23"/>
-      <c r="AM8" s="23"/>
-      <c r="AN8" s="27"/>
-      <c r="AO8" s="27"/>
-      <c r="AP8" s="27"/>
-      <c r="AQ8" s="27"/>
-      <c r="AR8" s="27"/>
-      <c r="AS8" s="23"/>
-      <c r="AT8" s="23"/>
-      <c r="AU8" s="23"/>
-      <c r="AV8" s="23"/>
-      <c r="AW8" s="23"/>
-      <c r="AX8" s="23"/>
-      <c r="AY8" s="23"/>
-      <c r="AZ8" s="23"/>
-      <c r="BA8" s="23"/>
-      <c r="BB8" s="23"/>
-      <c r="BC8" s="23"/>
-      <c r="BD8" s="23"/>
-      <c r="BE8" s="23"/>
-      <c r="BF8" s="23"/>
-      <c r="BG8" s="23"/>
-      <c r="BH8" s="23"/>
-      <c r="BI8" s="23"/>
-      <c r="BJ8" s="23"/>
-      <c r="BK8" s="23"/>
-      <c r="BL8" s="23"/>
-      <c r="BM8" s="23"/>
-      <c r="BN8" s="23"/>
-      <c r="BO8" s="23"/>
-      <c r="BP8" s="23"/>
-      <c r="BQ8" s="23"/>
-      <c r="BR8" s="23"/>
-      <c r="BS8" s="23"/>
-      <c r="BT8" s="23"/>
-      <c r="BU8" s="23"/>
-      <c r="BV8" s="23"/>
-      <c r="BW8" s="23"/>
-      <c r="BX8" s="23"/>
-      <c r="BY8" s="23"/>
-      <c r="BZ8" s="23"/>
-      <c r="CA8" s="23"/>
-      <c r="CB8" s="23"/>
-      <c r="CC8" s="23"/>
-      <c r="CD8" s="23"/>
-      <c r="CE8" s="23"/>
-      <c r="CF8" s="23"/>
-      <c r="CG8" s="23"/>
-      <c r="CH8" s="23"/>
-      <c r="CI8" s="23"/>
-      <c r="CJ8" s="23"/>
-      <c r="CK8" s="23"/>
-      <c r="CL8" s="23"/>
-      <c r="CM8" s="23"/>
-      <c r="CN8" s="23"/>
-      <c r="CO8" s="23"/>
-      <c r="CP8" s="23"/>
-      <c r="CQ8" s="23"/>
-      <c r="CR8" s="23"/>
-      <c r="CS8" s="23"/>
-      <c r="CT8" s="23"/>
-      <c r="CU8" s="23"/>
-      <c r="CV8" s="23"/>
-      <c r="CW8" s="23"/>
-      <c r="CX8" s="23"/>
-      <c r="CY8" s="23"/>
-      <c r="CZ8" s="23"/>
-      <c r="DA8" s="23"/>
-      <c r="DB8" s="23"/>
-      <c r="DC8" s="23"/>
-      <c r="DD8" s="23"/>
-      <c r="DE8" s="23"/>
-      <c r="DF8" s="23"/>
-      <c r="DG8" s="23"/>
-      <c r="DH8" s="23"/>
-      <c r="DI8" s="23"/>
-      <c r="DJ8" s="23"/>
-      <c r="DK8" s="23"/>
-      <c r="DL8" s="23"/>
-      <c r="DM8" s="23"/>
-      <c r="DN8" s="23"/>
-      <c r="DO8" s="23"/>
-      <c r="DP8" s="23"/>
-      <c r="DQ8" s="23"/>
-      <c r="DR8" s="23"/>
-      <c r="DS8" s="23"/>
-      <c r="DT8" s="23"/>
-      <c r="DU8" s="23"/>
-      <c r="DV8" s="23"/>
-      <c r="DW8" s="23"/>
-      <c r="DX8" s="23"/>
-      <c r="DY8" s="23"/>
-      <c r="DZ8" s="23"/>
-      <c r="EA8" s="23"/>
-      <c r="EB8" s="23"/>
-      <c r="EC8" s="23"/>
-      <c r="ED8" s="23"/>
-      <c r="EE8" s="23"/>
-      <c r="EF8" s="23"/>
-      <c r="EG8" s="23"/>
-      <c r="EH8" s="23"/>
-      <c r="EI8" s="23"/>
-      <c r="EJ8" s="23"/>
-      <c r="EK8" s="23"/>
-      <c r="EL8" s="23"/>
-      <c r="EM8" s="23"/>
-      <c r="EN8" s="23"/>
-      <c r="EO8" s="23"/>
-      <c r="EP8" s="23"/>
-      <c r="EQ8" s="23"/>
-      <c r="ER8" s="23"/>
-      <c r="ES8" s="23"/>
-      <c r="ET8" s="23"/>
-      <c r="EU8" s="23"/>
-      <c r="EV8" s="23"/>
-      <c r="EW8" s="23"/>
-      <c r="EX8" s="23"/>
-      <c r="EY8" s="23"/>
-      <c r="EZ8" s="23"/>
-      <c r="FA8" s="23"/>
-      <c r="FB8" s="23"/>
-      <c r="FC8" s="23"/>
-      <c r="FD8" s="23"/>
-      <c r="FE8" s="23"/>
-      <c r="FF8" s="23"/>
-      <c r="FG8" s="23"/>
-      <c r="FH8" s="23"/>
-      <c r="FI8" s="23"/>
-      <c r="FJ8" s="23"/>
-      <c r="FK8" s="23"/>
-      <c r="FL8" s="23"/>
-      <c r="FM8" s="23"/>
-      <c r="FN8" s="23"/>
-      <c r="FO8" s="23"/>
-      <c r="FP8" s="23"/>
-      <c r="FQ8" s="23"/>
-      <c r="FR8" s="23"/>
-      <c r="FS8" s="23"/>
-      <c r="FT8" s="23"/>
-      <c r="FU8" s="23"/>
-      <c r="FV8" s="23"/>
-      <c r="FW8" s="23"/>
-      <c r="FX8" s="23"/>
-      <c r="FY8" s="23"/>
-      <c r="FZ8" s="23"/>
-      <c r="GA8" s="23"/>
-      <c r="GB8" s="23"/>
-      <c r="GC8" s="23"/>
-      <c r="GD8" s="23"/>
-      <c r="GE8" s="23"/>
-      <c r="GF8" s="23"/>
-      <c r="GG8" s="23"/>
-      <c r="GH8" s="23"/>
-      <c r="GI8" s="23"/>
-      <c r="GJ8" s="23"/>
-      <c r="GK8" s="23"/>
-      <c r="GL8" s="23"/>
-      <c r="GM8" s="23"/>
-      <c r="GN8" s="23"/>
-      <c r="GO8" s="23"/>
-      <c r="GP8" s="23"/>
-      <c r="GQ8" s="23"/>
-      <c r="GR8" s="23"/>
-      <c r="GS8" s="23"/>
-      <c r="GT8" s="23"/>
-      <c r="GU8" s="23"/>
-      <c r="GV8" s="23"/>
-      <c r="GW8" s="23"/>
-      <c r="GX8" s="23"/>
-      <c r="GY8" s="23"/>
-      <c r="GZ8" s="23"/>
-      <c r="HA8" s="23"/>
-      <c r="HB8" s="23"/>
-      <c r="HC8" s="23"/>
-      <c r="HD8" s="23"/>
-      <c r="HE8" s="23"/>
-      <c r="HF8" s="23"/>
-      <c r="HG8" s="23"/>
-      <c r="HH8" s="23"/>
-      <c r="HI8" s="23"/>
-      <c r="HJ8" s="23"/>
-      <c r="HK8" s="23"/>
-      <c r="HL8" s="23"/>
-      <c r="HM8" s="23"/>
-      <c r="HN8" s="23"/>
-      <c r="HO8" s="23"/>
-      <c r="HP8" s="23"/>
-      <c r="HQ8" s="23"/>
-      <c r="HR8" s="23"/>
-      <c r="HS8" s="23"/>
-      <c r="HT8" s="23"/>
-      <c r="HU8" s="23"/>
-      <c r="HV8" s="23"/>
-      <c r="HW8" s="23"/>
-      <c r="HX8" s="23"/>
-      <c r="HY8" s="23"/>
-      <c r="HZ8" s="23"/>
-      <c r="IA8" s="23"/>
-      <c r="IB8" s="23"/>
-      <c r="IC8" s="23"/>
-      <c r="ID8" s="23"/>
-      <c r="IE8" s="23"/>
-      <c r="IF8" s="23"/>
-      <c r="IG8" s="23"/>
-      <c r="IH8" s="23"/>
-      <c r="II8" s="23"/>
-      <c r="IJ8" s="23"/>
-      <c r="IK8" s="23"/>
-      <c r="IL8" s="23"/>
-      <c r="IM8" s="23"/>
-      <c r="IN8" s="23"/>
-      <c r="IO8" s="23"/>
-      <c r="IP8" s="23"/>
-      <c r="IQ8" s="23"/>
-      <c r="IR8" s="23"/>
-      <c r="IS8" s="23"/>
-      <c r="IT8" s="23"/>
-      <c r="IU8" s="23"/>
-      <c r="IV8" s="23"/>
-      <c r="IW8" s="23"/>
-      <c r="IX8" s="23"/>
-      <c r="IY8" s="23"/>
-      <c r="IZ8" s="23"/>
-      <c r="JA8" s="23"/>
-      <c r="JB8" s="23"/>
-      <c r="JC8" s="23"/>
-      <c r="JD8" s="23"/>
-      <c r="JE8" s="23"/>
-      <c r="JF8" s="23"/>
-      <c r="JG8" s="23"/>
-      <c r="JH8" s="23"/>
-      <c r="JI8" s="23"/>
-      <c r="JJ8" s="23"/>
-      <c r="JK8" s="23"/>
-      <c r="JL8" s="23"/>
-      <c r="JM8" s="23"/>
-      <c r="JN8" s="23"/>
-      <c r="JO8" s="23"/>
-      <c r="JP8" s="23"/>
-      <c r="JQ8" s="23"/>
-      <c r="JR8" s="23"/>
-      <c r="JS8" s="47"/>
-      <c r="JT8" s="47"/>
-      <c r="JU8" s="47"/>
-      <c r="JV8" s="47"/>
-      <c r="JW8" s="47"/>
-      <c r="JX8" s="47"/>
-      <c r="JY8" s="47"/>
-      <c r="JZ8" s="23"/>
-      <c r="KA8" s="23"/>
-      <c r="KB8" s="23"/>
-      <c r="KC8" s="23"/>
-      <c r="KD8" s="23"/>
-      <c r="KE8" s="23"/>
-      <c r="KF8" s="23"/>
-      <c r="KG8" s="23"/>
-      <c r="KH8" s="48"/>
-      <c r="KI8" s="48"/>
-      <c r="KJ8" s="48"/>
-      <c r="KK8" s="48"/>
-      <c r="KL8" s="48" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="9" spans="1:300">
-      <c r="A9" s="25"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="26"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="23"/>
-      <c r="AD9" s="26"/>
-      <c r="AE9" s="26"/>
-      <c r="AF9" s="23"/>
-      <c r="AG9" s="23"/>
-      <c r="AH9" s="23"/>
-      <c r="AI9" s="23"/>
-      <c r="AJ9" s="23"/>
-      <c r="AK9" s="23"/>
-      <c r="AL9" s="23"/>
-      <c r="AM9" s="23"/>
-      <c r="AN9" s="27"/>
-      <c r="AO9" s="27"/>
-      <c r="AP9" s="27"/>
-      <c r="AQ9" s="27"/>
-      <c r="AR9" s="27"/>
-      <c r="AS9" s="23"/>
-      <c r="AT9" s="23"/>
-      <c r="AU9" s="23"/>
-      <c r="AV9" s="23"/>
-      <c r="AW9" s="23"/>
-      <c r="AX9" s="23"/>
-      <c r="AY9" s="23"/>
-      <c r="AZ9" s="23"/>
-      <c r="BA9" s="23"/>
-      <c r="BB9" s="23"/>
-      <c r="BC9" s="23"/>
-      <c r="BD9" s="23"/>
-      <c r="BE9" s="23"/>
-      <c r="BF9" s="23"/>
-      <c r="BG9" s="23"/>
-      <c r="BH9" s="23"/>
-      <c r="BI9" s="23"/>
-      <c r="BJ9" s="23"/>
-      <c r="BK9" s="23"/>
-      <c r="BL9" s="23"/>
-      <c r="BM9" s="23"/>
-      <c r="BN9" s="23"/>
-      <c r="BO9" s="23"/>
-      <c r="BP9" s="23"/>
-      <c r="BQ9" s="23"/>
-      <c r="BR9" s="23"/>
-      <c r="BS9" s="23"/>
-      <c r="BT9" s="23"/>
-      <c r="BU9" s="23"/>
-      <c r="BV9" s="23"/>
-      <c r="BW9" s="23"/>
-      <c r="BX9" s="23"/>
-      <c r="BY9" s="23"/>
-      <c r="BZ9" s="23"/>
-      <c r="CA9" s="23"/>
-      <c r="CB9" s="23"/>
-      <c r="CC9" s="23"/>
-      <c r="CD9" s="23"/>
-      <c r="CE9" s="23"/>
-      <c r="CF9" s="23"/>
-      <c r="CG9" s="23"/>
-      <c r="CH9" s="23"/>
-      <c r="CI9" s="23"/>
-      <c r="CJ9" s="23"/>
-      <c r="CK9" s="23"/>
-      <c r="CL9" s="23"/>
-      <c r="CM9" s="23"/>
-      <c r="CN9" s="23"/>
-      <c r="CO9" s="23"/>
-      <c r="CP9" s="23"/>
-      <c r="CQ9" s="23"/>
-      <c r="CR9" s="23"/>
-      <c r="CS9" s="23"/>
-      <c r="CT9" s="23"/>
-      <c r="CU9" s="23"/>
-      <c r="CV9" s="23"/>
-      <c r="CW9" s="23"/>
-      <c r="CX9" s="23"/>
-      <c r="CY9" s="23"/>
-      <c r="CZ9" s="23"/>
-      <c r="DA9" s="23"/>
-      <c r="DB9" s="23"/>
-      <c r="DC9" s="23"/>
-      <c r="DD9" s="23"/>
-      <c r="DE9" s="23"/>
-      <c r="DF9" s="23"/>
-      <c r="DG9" s="23"/>
-      <c r="DH9" s="23"/>
-      <c r="DI9" s="23"/>
-      <c r="DJ9" s="23"/>
-      <c r="DK9" s="23"/>
-      <c r="DL9" s="23"/>
-      <c r="DM9" s="23"/>
-      <c r="DN9" s="23"/>
-      <c r="DO9" s="23"/>
-      <c r="DP9" s="23"/>
-      <c r="DQ9" s="23"/>
-      <c r="DR9" s="23"/>
-      <c r="DS9" s="23"/>
-      <c r="DT9" s="23"/>
-      <c r="DU9" s="23"/>
-      <c r="DV9" s="23"/>
-      <c r="DW9" s="23"/>
-      <c r="DX9" s="23"/>
-      <c r="DY9" s="23"/>
-      <c r="DZ9" s="23"/>
-      <c r="EA9" s="23"/>
-      <c r="EB9" s="23"/>
-      <c r="EC9" s="23"/>
-      <c r="ED9" s="23"/>
-      <c r="EE9" s="23"/>
-      <c r="EF9" s="23"/>
-      <c r="EG9" s="23"/>
-      <c r="EH9" s="23"/>
-      <c r="EI9" s="23"/>
-      <c r="EJ9" s="23"/>
-      <c r="EK9" s="23"/>
-      <c r="EL9" s="23"/>
-      <c r="EM9" s="23"/>
-      <c r="EN9" s="23"/>
-      <c r="EO9" s="23"/>
-      <c r="EP9" s="23"/>
-      <c r="EQ9" s="23"/>
-      <c r="ER9" s="23"/>
-      <c r="ES9" s="23"/>
-      <c r="ET9" s="23"/>
-      <c r="EU9" s="23"/>
-      <c r="EV9" s="23"/>
-      <c r="EW9" s="23"/>
-      <c r="EX9" s="23"/>
-      <c r="EY9" s="23"/>
-      <c r="EZ9" s="23"/>
-      <c r="FA9" s="23"/>
-      <c r="FB9" s="23"/>
-      <c r="FC9" s="23"/>
-      <c r="FD9" s="23"/>
-      <c r="FE9" s="23"/>
-      <c r="FF9" s="23"/>
-      <c r="FG9" s="23"/>
-      <c r="FH9" s="23"/>
-      <c r="FI9" s="23"/>
-      <c r="FJ9" s="23"/>
-      <c r="FK9" s="23"/>
-      <c r="FL9" s="23"/>
-      <c r="FM9" s="23"/>
-      <c r="FN9" s="23"/>
-      <c r="FO9" s="23"/>
-      <c r="FP9" s="23"/>
-      <c r="FQ9" s="23"/>
-      <c r="FR9" s="23"/>
-      <c r="FS9" s="23"/>
-      <c r="FT9" s="23"/>
-      <c r="FU9" s="23"/>
-      <c r="FV9" s="23"/>
-      <c r="FW9" s="23"/>
-      <c r="FX9" s="23"/>
-      <c r="FY9" s="23"/>
-      <c r="FZ9" s="23"/>
-      <c r="GA9" s="23"/>
-      <c r="GB9" s="23"/>
-      <c r="GC9" s="23"/>
-      <c r="GD9" s="23"/>
-      <c r="GE9" s="23"/>
-      <c r="GF9" s="23"/>
-      <c r="GG9" s="23"/>
-      <c r="GH9" s="23"/>
-      <c r="GI9" s="23"/>
-      <c r="GJ9" s="23"/>
-      <c r="GK9" s="23"/>
-      <c r="GL9" s="23"/>
-      <c r="GM9" s="23"/>
-      <c r="GN9" s="23"/>
-      <c r="GO9" s="23"/>
-      <c r="GP9" s="23"/>
-      <c r="GQ9" s="23"/>
-      <c r="GR9" s="23"/>
-      <c r="GS9" s="23"/>
-      <c r="GT9" s="23"/>
-      <c r="GU9" s="23"/>
-      <c r="GV9" s="23"/>
-      <c r="GW9" s="23"/>
-      <c r="GX9" s="23"/>
-      <c r="GY9" s="23"/>
-      <c r="GZ9" s="23"/>
-      <c r="HA9" s="23"/>
-      <c r="HB9" s="23"/>
-      <c r="HC9" s="23"/>
-      <c r="HD9" s="23"/>
-      <c r="HE9" s="23"/>
-      <c r="HF9" s="23"/>
-      <c r="HG9" s="23"/>
-      <c r="HH9" s="23"/>
-      <c r="HI9" s="23"/>
-      <c r="HJ9" s="23"/>
-      <c r="HK9" s="23"/>
-      <c r="HL9" s="23"/>
-      <c r="HM9" s="23"/>
-      <c r="HN9" s="23"/>
-      <c r="HO9" s="23"/>
-      <c r="HP9" s="23"/>
-      <c r="HQ9" s="23"/>
-      <c r="HR9" s="23"/>
-      <c r="HS9" s="23"/>
-      <c r="HT9" s="23"/>
-      <c r="HU9" s="23"/>
-      <c r="HV9" s="23"/>
-      <c r="HW9" s="23"/>
-      <c r="HX9" s="23"/>
-      <c r="HY9" s="23"/>
-      <c r="HZ9" s="23"/>
-      <c r="IA9" s="23"/>
-      <c r="IB9" s="23"/>
-      <c r="IC9" s="23"/>
-      <c r="ID9" s="23"/>
-      <c r="IE9" s="23"/>
-      <c r="IF9" s="23"/>
-      <c r="IG9" s="23"/>
-      <c r="IH9" s="23"/>
-      <c r="II9" s="23"/>
-      <c r="IJ9" s="23"/>
-      <c r="IK9" s="23"/>
-      <c r="IL9" s="23"/>
-      <c r="IM9" s="23"/>
-      <c r="IN9" s="23"/>
-      <c r="IO9" s="23"/>
-      <c r="IP9" s="23"/>
-      <c r="IQ9" s="23"/>
-      <c r="IR9" s="23"/>
-      <c r="IS9" s="23"/>
-      <c r="IT9" s="23"/>
-      <c r="IU9" s="23"/>
-      <c r="IV9" s="23"/>
-      <c r="IW9" s="23"/>
-      <c r="IX9" s="23"/>
-      <c r="IY9" s="23"/>
-      <c r="IZ9" s="23"/>
-      <c r="JA9" s="23"/>
-      <c r="JB9" s="23"/>
-      <c r="JC9" s="23"/>
-      <c r="JD9" s="23"/>
-      <c r="JE9" s="23"/>
-      <c r="JF9" s="23"/>
-      <c r="JG9" s="23"/>
-      <c r="JH9" s="23"/>
-      <c r="JI9" s="23"/>
-      <c r="JJ9" s="23"/>
-      <c r="JK9" s="23"/>
-      <c r="JL9" s="23"/>
-      <c r="JM9" s="23"/>
-      <c r="JN9" s="23"/>
-      <c r="JO9" s="23"/>
-      <c r="JP9" s="23"/>
-      <c r="JQ9" s="23"/>
-      <c r="JR9" s="23"/>
-      <c r="JS9" s="47"/>
-      <c r="JT9" s="47"/>
-      <c r="JU9" s="47"/>
-      <c r="JV9" s="47"/>
-      <c r="JW9" s="47"/>
-      <c r="JX9" s="47"/>
-      <c r="JY9" s="47"/>
-      <c r="JZ9" s="23"/>
-      <c r="KA9" s="23"/>
-      <c r="KB9" s="23"/>
-      <c r="KC9" s="23"/>
-      <c r="KD9" s="23"/>
-      <c r="KE9" s="23"/>
-      <c r="KF9" s="23"/>
-      <c r="KG9" s="23"/>
-      <c r="KH9" s="48"/>
-      <c r="KI9" s="48"/>
-      <c r="KJ9" s="48"/>
-      <c r="KK9" s="48"/>
-      <c r="KL9" s="48" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="10" spans="1:300">
-      <c r="A10" s="25"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="26"/>
-      <c r="Y10" s="26"/>
-      <c r="Z10" s="23"/>
-      <c r="AA10" s="23"/>
-      <c r="AB10" s="26"/>
-      <c r="AC10" s="23"/>
-      <c r="AD10" s="26"/>
-      <c r="AE10" s="26"/>
-      <c r="AF10" s="23"/>
-      <c r="AG10" s="23"/>
-      <c r="AH10" s="23"/>
-      <c r="AI10" s="23"/>
-      <c r="AJ10" s="23"/>
-      <c r="AK10" s="23"/>
-      <c r="AL10" s="23"/>
-      <c r="AM10" s="23"/>
-      <c r="AN10" s="27"/>
-      <c r="AO10" s="27"/>
-      <c r="AP10" s="27"/>
-      <c r="AQ10" s="27"/>
-      <c r="AR10" s="27"/>
-      <c r="AS10" s="23"/>
-      <c r="AT10" s="23"/>
-      <c r="AU10" s="23"/>
-      <c r="AV10" s="23"/>
-      <c r="AW10" s="23"/>
-      <c r="AX10" s="23"/>
-      <c r="AY10" s="23"/>
-      <c r="AZ10" s="23"/>
-      <c r="BA10" s="23"/>
-      <c r="BB10" s="23"/>
-      <c r="BC10" s="23"/>
-      <c r="BD10" s="23"/>
-      <c r="BE10" s="23"/>
-      <c r="BF10" s="23"/>
-      <c r="BG10" s="23"/>
-      <c r="BH10" s="23"/>
-      <c r="BI10" s="23"/>
-      <c r="BJ10" s="23"/>
-      <c r="BK10" s="23"/>
-      <c r="BL10" s="23"/>
-      <c r="BM10" s="23"/>
-      <c r="BN10" s="23"/>
-      <c r="BO10" s="23"/>
-      <c r="BP10" s="23"/>
-      <c r="BQ10" s="23"/>
-      <c r="BR10" s="23"/>
-      <c r="BS10" s="23"/>
-      <c r="BT10" s="23"/>
-      <c r="BU10" s="23"/>
-      <c r="BV10" s="23"/>
-      <c r="BW10" s="23"/>
-      <c r="BX10" s="23"/>
-      <c r="BY10" s="23"/>
-      <c r="BZ10" s="23"/>
-      <c r="CA10" s="23"/>
-      <c r="CB10" s="23"/>
-      <c r="CC10" s="23"/>
-      <c r="CD10" s="23"/>
-      <c r="CE10" s="23"/>
-      <c r="CF10" s="23"/>
-      <c r="CG10" s="23"/>
-      <c r="CH10" s="23"/>
-      <c r="CI10" s="23"/>
-      <c r="CJ10" s="23"/>
-      <c r="CK10" s="23"/>
-      <c r="CL10" s="23"/>
-      <c r="CM10" s="23"/>
-      <c r="CN10" s="23"/>
-      <c r="CO10" s="23"/>
-      <c r="CP10" s="23"/>
-      <c r="CQ10" s="23"/>
-      <c r="CR10" s="23"/>
-      <c r="CS10" s="23"/>
-      <c r="CT10" s="23"/>
-      <c r="CU10" s="23"/>
-      <c r="CV10" s="23"/>
-      <c r="CW10" s="23"/>
-      <c r="CX10" s="23"/>
-      <c r="CY10" s="23"/>
-      <c r="CZ10" s="23"/>
-      <c r="DA10" s="23"/>
-      <c r="DB10" s="23"/>
-      <c r="DC10" s="23"/>
-      <c r="DD10" s="23"/>
-      <c r="DE10" s="23"/>
-      <c r="DF10" s="23"/>
-      <c r="DG10" s="23"/>
-      <c r="DH10" s="23"/>
-      <c r="DI10" s="23"/>
-      <c r="DJ10" s="23"/>
-      <c r="DK10" s="23"/>
-      <c r="DL10" s="23"/>
-      <c r="DM10" s="23"/>
-      <c r="DN10" s="23"/>
-      <c r="DO10" s="23"/>
-      <c r="DP10" s="23"/>
-      <c r="DQ10" s="23"/>
-      <c r="DR10" s="23"/>
-      <c r="DS10" s="23"/>
-      <c r="DT10" s="23"/>
-      <c r="DU10" s="23"/>
-      <c r="DV10" s="23"/>
-      <c r="DW10" s="23"/>
-      <c r="DX10" s="23"/>
-      <c r="DY10" s="23"/>
-      <c r="DZ10" s="23"/>
-      <c r="EA10" s="23"/>
-      <c r="EB10" s="23"/>
-      <c r="EC10" s="23"/>
-      <c r="ED10" s="23"/>
-      <c r="EE10" s="23"/>
-      <c r="EF10" s="23"/>
-      <c r="EG10" s="23"/>
-      <c r="EH10" s="23"/>
-      <c r="EI10" s="23"/>
-      <c r="EJ10" s="23"/>
-      <c r="EK10" s="23"/>
-      <c r="EL10" s="23"/>
-      <c r="EM10" s="23"/>
-      <c r="EN10" s="23"/>
-      <c r="EO10" s="23"/>
-      <c r="EP10" s="23"/>
-      <c r="EQ10" s="23"/>
-      <c r="ER10" s="23"/>
-      <c r="ES10" s="23"/>
-      <c r="ET10" s="23"/>
-      <c r="EU10" s="23"/>
-      <c r="EV10" s="23"/>
-      <c r="EW10" s="23"/>
-      <c r="EX10" s="23"/>
-      <c r="EY10" s="23"/>
-      <c r="EZ10" s="23"/>
-      <c r="FA10" s="23"/>
-      <c r="FB10" s="23"/>
-      <c r="FC10" s="23"/>
-      <c r="FD10" s="23"/>
-      <c r="FE10" s="23"/>
-      <c r="FF10" s="23"/>
-      <c r="FG10" s="23"/>
-      <c r="FH10" s="23"/>
-      <c r="FI10" s="23"/>
-      <c r="FJ10" s="23"/>
-      <c r="FK10" s="23"/>
-      <c r="FL10" s="23"/>
-      <c r="FM10" s="23"/>
-      <c r="FN10" s="23"/>
-      <c r="FO10" s="23"/>
-      <c r="FP10" s="23"/>
-      <c r="FQ10" s="23"/>
-      <c r="FR10" s="23"/>
-      <c r="FS10" s="23"/>
-      <c r="FT10" s="23"/>
-      <c r="FU10" s="23"/>
-      <c r="FV10" s="23"/>
-      <c r="FW10" s="23"/>
-      <c r="FX10" s="23"/>
-      <c r="FY10" s="23"/>
-      <c r="FZ10" s="23"/>
-      <c r="GA10" s="23"/>
-      <c r="GB10" s="23"/>
-      <c r="GC10" s="23"/>
-      <c r="GD10" s="23"/>
-      <c r="GE10" s="23"/>
-      <c r="GF10" s="23"/>
-      <c r="GG10" s="23"/>
-      <c r="GH10" s="23"/>
-      <c r="GI10" s="23"/>
-      <c r="GJ10" s="23"/>
-      <c r="GK10" s="23"/>
-      <c r="GL10" s="23"/>
-      <c r="GM10" s="23"/>
-      <c r="GN10" s="23"/>
-      <c r="GO10" s="23"/>
-      <c r="GP10" s="23"/>
-      <c r="GQ10" s="23"/>
-      <c r="GR10" s="23"/>
-      <c r="GS10" s="23"/>
-      <c r="GT10" s="23"/>
-      <c r="GU10" s="23"/>
-      <c r="GV10" s="23"/>
-      <c r="GW10" s="23"/>
-      <c r="GX10" s="23"/>
-      <c r="GY10" s="23"/>
-      <c r="GZ10" s="23"/>
-      <c r="HA10" s="23"/>
-      <c r="HB10" s="23"/>
-      <c r="HC10" s="23"/>
-      <c r="HD10" s="23"/>
-      <c r="HE10" s="23"/>
-      <c r="HF10" s="23"/>
-      <c r="HG10" s="23"/>
-      <c r="HH10" s="23"/>
-      <c r="HI10" s="23"/>
-      <c r="HJ10" s="23"/>
-      <c r="HK10" s="23"/>
-      <c r="HL10" s="23"/>
-      <c r="HM10" s="23"/>
-      <c r="HN10" s="23"/>
-      <c r="HO10" s="23"/>
-      <c r="HP10" s="23"/>
-      <c r="HQ10" s="23"/>
-      <c r="HR10" s="23"/>
-      <c r="HS10" s="23"/>
-      <c r="HT10" s="23"/>
-      <c r="HU10" s="23"/>
-      <c r="HV10" s="23"/>
-      <c r="HW10" s="23"/>
-      <c r="HX10" s="23"/>
-      <c r="HY10" s="23"/>
-      <c r="HZ10" s="23"/>
-      <c r="IA10" s="23"/>
-      <c r="IB10" s="23"/>
-      <c r="IC10" s="23"/>
-      <c r="ID10" s="23"/>
-      <c r="IE10" s="23"/>
-      <c r="IF10" s="23"/>
-      <c r="IG10" s="23"/>
-      <c r="IH10" s="23"/>
-      <c r="II10" s="23"/>
-      <c r="IJ10" s="23"/>
-      <c r="IK10" s="23"/>
-      <c r="IL10" s="23"/>
-      <c r="IM10" s="23"/>
-      <c r="IN10" s="23"/>
-      <c r="IO10" s="23"/>
-      <c r="IP10" s="23"/>
-      <c r="IQ10" s="23"/>
-      <c r="IR10" s="23"/>
-      <c r="IS10" s="23"/>
-      <c r="IT10" s="23"/>
-      <c r="IU10" s="23"/>
-      <c r="IV10" s="23"/>
-      <c r="IW10" s="23"/>
-      <c r="IX10" s="23"/>
-      <c r="IY10" s="23"/>
-      <c r="IZ10" s="23"/>
-      <c r="JA10" s="23"/>
-      <c r="JB10" s="23"/>
-      <c r="JC10" s="23"/>
-      <c r="JD10" s="23"/>
-      <c r="JE10" s="23"/>
-      <c r="JF10" s="23"/>
-      <c r="JG10" s="23"/>
-      <c r="JH10" s="23"/>
-      <c r="JI10" s="23"/>
-      <c r="JJ10" s="23"/>
-      <c r="JK10" s="23"/>
-      <c r="JL10" s="23"/>
-      <c r="JM10" s="23"/>
-      <c r="JN10" s="23"/>
-      <c r="JO10" s="23"/>
-      <c r="JP10" s="23"/>
-      <c r="JQ10" s="23"/>
-      <c r="JR10" s="23"/>
-      <c r="JS10" s="47"/>
-      <c r="JT10" s="47"/>
-      <c r="JU10" s="47"/>
-      <c r="JV10" s="47"/>
-      <c r="JW10" s="47"/>
-      <c r="JX10" s="47"/>
-      <c r="JY10" s="47"/>
-      <c r="JZ10" s="23"/>
-      <c r="KA10" s="23"/>
-      <c r="KB10" s="23"/>
-      <c r="KC10" s="23"/>
-      <c r="KD10" s="23"/>
-      <c r="KE10" s="23"/>
-      <c r="KF10" s="23"/>
-      <c r="KG10" s="23"/>
-      <c r="KH10" s="48"/>
-      <c r="KI10" s="48"/>
-      <c r="KJ10" s="48"/>
-      <c r="KK10" s="48"/>
-      <c r="KL10" s="48" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="11" spans="1:300">
-      <c r="A11" s="25"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="26"/>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="26"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="26"/>
-      <c r="AE11" s="26"/>
-      <c r="AF11" s="23"/>
-      <c r="AG11" s="23"/>
-      <c r="AH11" s="23"/>
-      <c r="AI11" s="23"/>
-      <c r="AJ11" s="23"/>
-      <c r="AK11" s="23"/>
-      <c r="AL11" s="23"/>
-      <c r="AM11" s="23"/>
-      <c r="AN11" s="27"/>
-      <c r="AO11" s="27"/>
-      <c r="AP11" s="27"/>
-      <c r="AQ11" s="27"/>
-      <c r="AR11" s="27"/>
-      <c r="AS11" s="23"/>
-      <c r="AT11" s="23"/>
-      <c r="AU11" s="23"/>
-      <c r="AV11" s="23"/>
-      <c r="AW11" s="23"/>
-      <c r="AX11" s="23"/>
-      <c r="AY11" s="23"/>
-      <c r="AZ11" s="23"/>
-      <c r="BA11" s="23"/>
-      <c r="BB11" s="23"/>
-      <c r="BC11" s="23"/>
-      <c r="BD11" s="23"/>
-      <c r="BE11" s="23"/>
-      <c r="BF11" s="23"/>
-      <c r="BG11" s="23"/>
-      <c r="BH11" s="23"/>
-      <c r="BI11" s="23"/>
-      <c r="BJ11" s="23"/>
-      <c r="BK11" s="23"/>
-      <c r="BL11" s="23"/>
-      <c r="BM11" s="23"/>
-      <c r="BN11" s="23"/>
-      <c r="BO11" s="23"/>
-      <c r="BP11" s="23"/>
-      <c r="BQ11" s="23"/>
-      <c r="BR11" s="23"/>
-      <c r="BS11" s="23"/>
-      <c r="BT11" s="23"/>
-      <c r="BU11" s="23"/>
-      <c r="BV11" s="23"/>
-      <c r="BW11" s="23"/>
-      <c r="BX11" s="23"/>
-      <c r="BY11" s="23"/>
-      <c r="BZ11" s="23"/>
-      <c r="CA11" s="23"/>
-      <c r="CB11" s="23"/>
-      <c r="CC11" s="23"/>
-      <c r="CD11" s="23"/>
-      <c r="CE11" s="23"/>
-      <c r="CF11" s="23"/>
-      <c r="CG11" s="23"/>
-      <c r="CH11" s="23"/>
-      <c r="CI11" s="23"/>
-      <c r="CJ11" s="23"/>
-      <c r="CK11" s="23"/>
-      <c r="CL11" s="23"/>
-      <c r="CM11" s="23"/>
-      <c r="CN11" s="23"/>
-      <c r="CO11" s="23"/>
-      <c r="CP11" s="23"/>
-      <c r="CQ11" s="23"/>
-      <c r="CR11" s="23"/>
-      <c r="CS11" s="23"/>
-      <c r="CT11" s="23"/>
-      <c r="CU11" s="23"/>
-      <c r="CV11" s="23"/>
-      <c r="CW11" s="23"/>
-      <c r="CX11" s="23"/>
-      <c r="CY11" s="23"/>
-      <c r="CZ11" s="23"/>
-      <c r="DA11" s="23"/>
-      <c r="DB11" s="23"/>
-      <c r="DC11" s="23"/>
-      <c r="DD11" s="23"/>
-      <c r="DE11" s="23"/>
-      <c r="DF11" s="23"/>
-      <c r="DG11" s="23"/>
-      <c r="DH11" s="23"/>
-      <c r="DI11" s="23"/>
-      <c r="DJ11" s="23"/>
-      <c r="DK11" s="23"/>
-      <c r="DL11" s="23"/>
-      <c r="DM11" s="23"/>
-      <c r="DN11" s="23"/>
-      <c r="DO11" s="23"/>
-      <c r="DP11" s="23"/>
-      <c r="DQ11" s="23"/>
-      <c r="DR11" s="23"/>
-      <c r="DS11" s="23"/>
-      <c r="DT11" s="23"/>
-      <c r="DU11" s="23"/>
-      <c r="DV11" s="23"/>
-      <c r="DW11" s="23"/>
-      <c r="DX11" s="23"/>
-      <c r="DY11" s="23"/>
-      <c r="DZ11" s="23"/>
-      <c r="EA11" s="23"/>
-      <c r="EB11" s="23"/>
-      <c r="EC11" s="23"/>
-      <c r="ED11" s="23"/>
-      <c r="EE11" s="23"/>
-      <c r="EF11" s="23"/>
-      <c r="EG11" s="23"/>
-      <c r="EH11" s="23"/>
-      <c r="EI11" s="23"/>
-      <c r="EJ11" s="23"/>
-      <c r="EK11" s="23"/>
-      <c r="EL11" s="23"/>
-      <c r="EM11" s="23"/>
-      <c r="EN11" s="23"/>
-      <c r="EO11" s="23"/>
-      <c r="EP11" s="23"/>
-      <c r="EQ11" s="23"/>
-      <c r="ER11" s="23"/>
-      <c r="ES11" s="23"/>
-      <c r="ET11" s="23"/>
-      <c r="EU11" s="23"/>
-      <c r="EV11" s="23"/>
-      <c r="EW11" s="23"/>
-      <c r="EX11" s="23"/>
-      <c r="EY11" s="23"/>
-      <c r="EZ11" s="23"/>
-      <c r="FA11" s="23"/>
-      <c r="FB11" s="23"/>
-      <c r="FC11" s="23"/>
-      <c r="FD11" s="23"/>
-      <c r="FE11" s="23"/>
-      <c r="FF11" s="23"/>
-      <c r="FG11" s="23"/>
-      <c r="FH11" s="23"/>
-      <c r="FI11" s="23"/>
-      <c r="FJ11" s="23"/>
-      <c r="FK11" s="23"/>
-      <c r="FL11" s="23"/>
-      <c r="FM11" s="23"/>
-      <c r="FN11" s="23"/>
-      <c r="FO11" s="23"/>
-      <c r="FP11" s="23"/>
-      <c r="FQ11" s="23"/>
-      <c r="FR11" s="23"/>
-      <c r="FS11" s="23"/>
-      <c r="FT11" s="23"/>
-      <c r="FU11" s="23"/>
-      <c r="FV11" s="23"/>
-      <c r="FW11" s="23"/>
-      <c r="FX11" s="23"/>
-      <c r="FY11" s="23"/>
-      <c r="FZ11" s="23"/>
-      <c r="GA11" s="23"/>
-      <c r="GB11" s="23"/>
-      <c r="GC11" s="23"/>
-      <c r="GD11" s="23"/>
-      <c r="GE11" s="23"/>
-      <c r="GF11" s="23"/>
-      <c r="GG11" s="23"/>
-      <c r="GH11" s="23"/>
-      <c r="GI11" s="23"/>
-      <c r="GJ11" s="23"/>
-      <c r="GK11" s="23"/>
-      <c r="GL11" s="23"/>
-      <c r="GM11" s="23"/>
-      <c r="GN11" s="23"/>
-      <c r="GO11" s="23"/>
-      <c r="GP11" s="23"/>
-      <c r="GQ11" s="23"/>
-      <c r="GR11" s="23"/>
-      <c r="GS11" s="23"/>
-      <c r="GT11" s="23"/>
-      <c r="GU11" s="23"/>
-      <c r="GV11" s="23"/>
-      <c r="GW11" s="23"/>
-      <c r="GX11" s="23"/>
-      <c r="GY11" s="23"/>
-      <c r="GZ11" s="23"/>
-      <c r="HA11" s="23"/>
-      <c r="HB11" s="23"/>
-      <c r="HC11" s="23"/>
-      <c r="HD11" s="23"/>
-      <c r="HE11" s="23"/>
-      <c r="HF11" s="23"/>
-      <c r="HG11" s="23"/>
-      <c r="HH11" s="23"/>
-      <c r="HI11" s="23"/>
-      <c r="HJ11" s="23"/>
-      <c r="HK11" s="23"/>
-      <c r="HL11" s="23"/>
-      <c r="HM11" s="23"/>
-      <c r="HN11" s="23"/>
-      <c r="HO11" s="23"/>
-      <c r="HP11" s="23"/>
-      <c r="HQ11" s="23"/>
-      <c r="HR11" s="23"/>
-      <c r="HS11" s="23"/>
-      <c r="HT11" s="23"/>
-      <c r="HU11" s="23"/>
-      <c r="HV11" s="23"/>
-      <c r="HW11" s="23"/>
-      <c r="HX11" s="23"/>
-      <c r="HY11" s="23"/>
-      <c r="HZ11" s="23"/>
-      <c r="IA11" s="23"/>
-      <c r="IB11" s="23"/>
-      <c r="IC11" s="23"/>
-      <c r="ID11" s="23"/>
-      <c r="IE11" s="23"/>
-      <c r="IF11" s="23"/>
-      <c r="IG11" s="23"/>
-      <c r="IH11" s="23"/>
-      <c r="II11" s="23"/>
-      <c r="IJ11" s="23"/>
-      <c r="IK11" s="23"/>
-      <c r="IL11" s="23"/>
-      <c r="IM11" s="23"/>
-      <c r="IN11" s="23"/>
-      <c r="IO11" s="23"/>
-      <c r="IP11" s="23"/>
-      <c r="IQ11" s="23"/>
-      <c r="IR11" s="23"/>
-      <c r="IS11" s="23"/>
-      <c r="IT11" s="23"/>
-      <c r="IU11" s="23"/>
-      <c r="IV11" s="23"/>
-      <c r="IW11" s="23"/>
-      <c r="IX11" s="23"/>
-      <c r="IY11" s="23"/>
-      <c r="IZ11" s="23"/>
-      <c r="JA11" s="23"/>
-      <c r="JB11" s="23"/>
-      <c r="JC11" s="23"/>
-      <c r="JD11" s="23"/>
-      <c r="JE11" s="23"/>
-      <c r="JF11" s="23"/>
-      <c r="JG11" s="23"/>
-      <c r="JH11" s="23"/>
-      <c r="JI11" s="23"/>
-      <c r="JJ11" s="23"/>
-      <c r="JK11" s="23"/>
-      <c r="JL11" s="23"/>
-      <c r="JM11" s="23"/>
-      <c r="JN11" s="23"/>
-      <c r="JO11" s="23"/>
-      <c r="JP11" s="23"/>
-      <c r="JQ11" s="23"/>
-      <c r="JR11" s="23"/>
-      <c r="JS11" s="47"/>
-      <c r="JT11" s="47"/>
-      <c r="JU11" s="47"/>
-      <c r="JV11" s="47"/>
-      <c r="JW11" s="47"/>
-      <c r="JX11" s="47"/>
-      <c r="JY11" s="47"/>
-      <c r="JZ11" s="23"/>
-      <c r="KA11" s="23"/>
-      <c r="KB11" s="23"/>
-      <c r="KC11" s="23"/>
-      <c r="KD11" s="23"/>
-      <c r="KE11" s="23"/>
-      <c r="KF11" s="23"/>
-      <c r="KG11" s="23"/>
-      <c r="KH11" s="48"/>
-      <c r="KI11" s="48"/>
-      <c r="KJ11" s="48"/>
-      <c r="KK11" s="48"/>
-      <c r="KL11" s="48" t="s">
-        <v>340</v>
-      </c>
+      <c r="KH7" s="47"/>
+      <c r="KI7" s="47"/>
+      <c r="KJ7" s="47"/>
+      <c r="KK7" s="47"/>
     </row>
   </sheetData>
   <autoFilter ref="A6:KK6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -6700,15 +5463,9 @@
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>
   </conditionalFormatting>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>36526</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH8:KJ11" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>$KL$7:$KL$11</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH7 KJ7" xr:uid="{00000000-0002-0000-0000-000002000000}">
-      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete,"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KK7" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"NGSA, WEM, FCRM Operational Framework, Other, Unknown/TBC"</formula1>
@@ -6716,6 +5473,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KI7" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete, No Delivery pre 2021 "</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH6:KJ999996" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete,"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="10" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
[PM-343] Remove spurious data validation from KK
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthall/Work/pafs/pafs_core/lib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C15B4C-59E1-924E-A5D8-DB6E776B46C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DAC8F2-0DFE-7347-99E2-9CC799A05998}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25200" windowHeight="11980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1701,6 +1701,63 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1730,63 +1787,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2095,11 +2095,11 @@
   <dimension ref="A1:KM7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="KI7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="KG7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="KN6" sqref="KN6"/>
+      <selection pane="bottomRight" activeCell="KH7" sqref="KH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2130,10 +2130,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:299" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
+      <c r="B1" s="83"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
@@ -2427,10 +2427,10 @@
       <c r="KG1" s="23"/>
     </row>
     <row r="2" spans="1:299" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="84" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="84"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="23"/>
@@ -3019,421 +3019,421 @@
       <c r="KG3" s="45"/>
     </row>
     <row r="4" spans="1:299" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="67" t="s">
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="68" t="s">
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="69" t="s">
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="70" t="s">
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="70"/>
-      <c r="W4" s="70"/>
-      <c r="X4" s="70"/>
-      <c r="Y4" s="70"/>
-      <c r="Z4" s="70"/>
-      <c r="AA4" s="70"/>
-      <c r="AB4" s="70"/>
-      <c r="AC4" s="71" t="s">
+      <c r="V4" s="89"/>
+      <c r="W4" s="89"/>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="89"/>
+      <c r="AC4" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="71"/>
-      <c r="AE4" s="71"/>
-      <c r="AF4" s="71"/>
-      <c r="AG4" s="71"/>
-      <c r="AH4" s="71"/>
-      <c r="AI4" s="71"/>
-      <c r="AJ4" s="72" t="s">
+      <c r="AD4" s="90"/>
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="90"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="90"/>
+      <c r="AI4" s="90"/>
+      <c r="AJ4" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="72"/>
-      <c r="AL4" s="72"/>
-      <c r="AM4" s="63" t="s">
+      <c r="AK4" s="91"/>
+      <c r="AL4" s="91"/>
+      <c r="AM4" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="63"/>
-      <c r="AO4" s="74"/>
-      <c r="AP4" s="74"/>
-      <c r="AQ4" s="74"/>
-      <c r="AR4" s="74"/>
-      <c r="AS4" s="75" t="s">
+      <c r="AN4" s="82"/>
+      <c r="AO4" s="72"/>
+      <c r="AP4" s="72"/>
+      <c r="AQ4" s="72"/>
+      <c r="AR4" s="72"/>
+      <c r="AS4" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="75"/>
-      <c r="AU4" s="75"/>
-      <c r="AV4" s="75"/>
-      <c r="AW4" s="75"/>
-      <c r="AX4" s="75"/>
-      <c r="AY4" s="75"/>
-      <c r="AZ4" s="75"/>
-      <c r="BA4" s="75"/>
-      <c r="BB4" s="75"/>
-      <c r="BC4" s="75"/>
-      <c r="BD4" s="75"/>
-      <c r="BE4" s="75"/>
-      <c r="BF4" s="75"/>
-      <c r="BG4" s="75"/>
-      <c r="BH4" s="75"/>
-      <c r="BI4" s="75"/>
-      <c r="BJ4" s="75"/>
-      <c r="BK4" s="73" t="s">
+      <c r="AT4" s="73"/>
+      <c r="AU4" s="73"/>
+      <c r="AV4" s="73"/>
+      <c r="AW4" s="73"/>
+      <c r="AX4" s="73"/>
+      <c r="AY4" s="73"/>
+      <c r="AZ4" s="73"/>
+      <c r="BA4" s="73"/>
+      <c r="BB4" s="73"/>
+      <c r="BC4" s="73"/>
+      <c r="BD4" s="73"/>
+      <c r="BE4" s="73"/>
+      <c r="BF4" s="73"/>
+      <c r="BG4" s="73"/>
+      <c r="BH4" s="73"/>
+      <c r="BI4" s="73"/>
+      <c r="BJ4" s="73"/>
+      <c r="BK4" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="BL4" s="73"/>
-      <c r="BM4" s="73"/>
-      <c r="BN4" s="73"/>
-      <c r="BO4" s="73"/>
-      <c r="BP4" s="73"/>
-      <c r="BQ4" s="73"/>
-      <c r="BR4" s="73"/>
-      <c r="BS4" s="73"/>
-      <c r="BT4" s="73"/>
-      <c r="BU4" s="73"/>
-      <c r="BV4" s="73"/>
-      <c r="BW4" s="73"/>
-      <c r="BX4" s="73"/>
-      <c r="BY4" s="76" t="s">
+      <c r="BL4" s="69"/>
+      <c r="BM4" s="69"/>
+      <c r="BN4" s="69"/>
+      <c r="BO4" s="69"/>
+      <c r="BP4" s="69"/>
+      <c r="BQ4" s="69"/>
+      <c r="BR4" s="69"/>
+      <c r="BS4" s="69"/>
+      <c r="BT4" s="69"/>
+      <c r="BU4" s="69"/>
+      <c r="BV4" s="69"/>
+      <c r="BW4" s="69"/>
+      <c r="BX4" s="69"/>
+      <c r="BY4" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="76"/>
-      <c r="CA4" s="76"/>
-      <c r="CB4" s="76"/>
-      <c r="CC4" s="76"/>
-      <c r="CD4" s="76"/>
-      <c r="CE4" s="76"/>
-      <c r="CF4" s="76"/>
-      <c r="CG4" s="76"/>
-      <c r="CH4" s="76"/>
-      <c r="CI4" s="76"/>
-      <c r="CJ4" s="76"/>
-      <c r="CK4" s="76"/>
-      <c r="CL4" s="76"/>
-      <c r="CM4" s="77" t="s">
+      <c r="BZ4" s="74"/>
+      <c r="CA4" s="74"/>
+      <c r="CB4" s="74"/>
+      <c r="CC4" s="74"/>
+      <c r="CD4" s="74"/>
+      <c r="CE4" s="74"/>
+      <c r="CF4" s="74"/>
+      <c r="CG4" s="74"/>
+      <c r="CH4" s="74"/>
+      <c r="CI4" s="74"/>
+      <c r="CJ4" s="74"/>
+      <c r="CK4" s="74"/>
+      <c r="CL4" s="74"/>
+      <c r="CM4" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="77"/>
-      <c r="CO4" s="77"/>
-      <c r="CP4" s="77"/>
-      <c r="CQ4" s="77"/>
-      <c r="CR4" s="77"/>
-      <c r="CS4" s="77"/>
-      <c r="CT4" s="77"/>
-      <c r="CU4" s="77"/>
-      <c r="CV4" s="77"/>
-      <c r="CW4" s="77"/>
-      <c r="CX4" s="77"/>
-      <c r="CY4" s="77"/>
-      <c r="CZ4" s="77"/>
-      <c r="DA4" s="78" t="s">
+      <c r="CN4" s="75"/>
+      <c r="CO4" s="75"/>
+      <c r="CP4" s="75"/>
+      <c r="CQ4" s="75"/>
+      <c r="CR4" s="75"/>
+      <c r="CS4" s="75"/>
+      <c r="CT4" s="75"/>
+      <c r="CU4" s="75"/>
+      <c r="CV4" s="75"/>
+      <c r="CW4" s="75"/>
+      <c r="CX4" s="75"/>
+      <c r="CY4" s="75"/>
+      <c r="CZ4" s="75"/>
+      <c r="DA4" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="78"/>
-      <c r="DC4" s="78"/>
-      <c r="DD4" s="78"/>
-      <c r="DE4" s="78"/>
-      <c r="DF4" s="78"/>
-      <c r="DG4" s="78"/>
-      <c r="DH4" s="78"/>
-      <c r="DI4" s="78"/>
-      <c r="DJ4" s="78"/>
-      <c r="DK4" s="78"/>
-      <c r="DL4" s="78"/>
-      <c r="DM4" s="78"/>
-      <c r="DN4" s="78"/>
-      <c r="DO4" s="79" t="s">
+      <c r="DB4" s="76"/>
+      <c r="DC4" s="76"/>
+      <c r="DD4" s="76"/>
+      <c r="DE4" s="76"/>
+      <c r="DF4" s="76"/>
+      <c r="DG4" s="76"/>
+      <c r="DH4" s="76"/>
+      <c r="DI4" s="76"/>
+      <c r="DJ4" s="76"/>
+      <c r="DK4" s="76"/>
+      <c r="DL4" s="76"/>
+      <c r="DM4" s="76"/>
+      <c r="DN4" s="76"/>
+      <c r="DO4" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="79"/>
-      <c r="DQ4" s="79"/>
-      <c r="DR4" s="79"/>
-      <c r="DS4" s="79"/>
-      <c r="DT4" s="79"/>
-      <c r="DU4" s="79"/>
-      <c r="DV4" s="79"/>
-      <c r="DW4" s="79"/>
-      <c r="DX4" s="79"/>
-      <c r="DY4" s="79"/>
-      <c r="DZ4" s="79"/>
-      <c r="EA4" s="79"/>
-      <c r="EB4" s="79"/>
-      <c r="EC4" s="80" t="s">
+      <c r="DP4" s="77"/>
+      <c r="DQ4" s="77"/>
+      <c r="DR4" s="77"/>
+      <c r="DS4" s="77"/>
+      <c r="DT4" s="77"/>
+      <c r="DU4" s="77"/>
+      <c r="DV4" s="77"/>
+      <c r="DW4" s="77"/>
+      <c r="DX4" s="77"/>
+      <c r="DY4" s="77"/>
+      <c r="DZ4" s="77"/>
+      <c r="EA4" s="77"/>
+      <c r="EB4" s="77"/>
+      <c r="EC4" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="80"/>
-      <c r="EE4" s="80"/>
-      <c r="EF4" s="80"/>
-      <c r="EG4" s="80"/>
-      <c r="EH4" s="80"/>
-      <c r="EI4" s="80"/>
-      <c r="EJ4" s="80"/>
-      <c r="EK4" s="80"/>
-      <c r="EL4" s="80"/>
-      <c r="EM4" s="80"/>
-      <c r="EN4" s="80"/>
-      <c r="EO4" s="80"/>
-      <c r="EP4" s="80"/>
-      <c r="EQ4" s="81" t="s">
+      <c r="ED4" s="78"/>
+      <c r="EE4" s="78"/>
+      <c r="EF4" s="78"/>
+      <c r="EG4" s="78"/>
+      <c r="EH4" s="78"/>
+      <c r="EI4" s="78"/>
+      <c r="EJ4" s="78"/>
+      <c r="EK4" s="78"/>
+      <c r="EL4" s="78"/>
+      <c r="EM4" s="78"/>
+      <c r="EN4" s="78"/>
+      <c r="EO4" s="78"/>
+      <c r="EP4" s="78"/>
+      <c r="EQ4" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="81"/>
-      <c r="ES4" s="81"/>
-      <c r="ET4" s="81"/>
-      <c r="EU4" s="81"/>
-      <c r="EV4" s="81"/>
-      <c r="EW4" s="81"/>
-      <c r="EX4" s="81"/>
-      <c r="EY4" s="81"/>
-      <c r="EZ4" s="81"/>
-      <c r="FA4" s="81"/>
-      <c r="FB4" s="81"/>
-      <c r="FC4" s="81"/>
-      <c r="FD4" s="81"/>
-      <c r="FE4" s="82" t="s">
+      <c r="ER4" s="79"/>
+      <c r="ES4" s="79"/>
+      <c r="ET4" s="79"/>
+      <c r="EU4" s="79"/>
+      <c r="EV4" s="79"/>
+      <c r="EW4" s="79"/>
+      <c r="EX4" s="79"/>
+      <c r="EY4" s="79"/>
+      <c r="EZ4" s="79"/>
+      <c r="FA4" s="79"/>
+      <c r="FB4" s="79"/>
+      <c r="FC4" s="79"/>
+      <c r="FD4" s="79"/>
+      <c r="FE4" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="82"/>
-      <c r="FG4" s="82"/>
-      <c r="FH4" s="82"/>
-      <c r="FI4" s="82"/>
-      <c r="FJ4" s="82"/>
-      <c r="FK4" s="82"/>
-      <c r="FL4" s="82"/>
-      <c r="FM4" s="82"/>
-      <c r="FN4" s="82"/>
-      <c r="FO4" s="82"/>
-      <c r="FP4" s="82"/>
-      <c r="FQ4" s="82"/>
-      <c r="FR4" s="82"/>
-      <c r="FS4" s="83" t="s">
+      <c r="FF4" s="80"/>
+      <c r="FG4" s="80"/>
+      <c r="FH4" s="80"/>
+      <c r="FI4" s="80"/>
+      <c r="FJ4" s="80"/>
+      <c r="FK4" s="80"/>
+      <c r="FL4" s="80"/>
+      <c r="FM4" s="80"/>
+      <c r="FN4" s="80"/>
+      <c r="FO4" s="80"/>
+      <c r="FP4" s="80"/>
+      <c r="FQ4" s="80"/>
+      <c r="FR4" s="80"/>
+      <c r="FS4" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="83"/>
-      <c r="FU4" s="83"/>
-      <c r="FV4" s="83"/>
-      <c r="FW4" s="83"/>
-      <c r="FX4" s="83"/>
-      <c r="FY4" s="83"/>
-      <c r="FZ4" s="83"/>
-      <c r="GA4" s="83"/>
-      <c r="GB4" s="83"/>
-      <c r="GC4" s="83"/>
-      <c r="GD4" s="83"/>
-      <c r="GE4" s="83"/>
-      <c r="GF4" s="83"/>
-      <c r="GG4" s="73" t="s">
+      <c r="FT4" s="81"/>
+      <c r="FU4" s="81"/>
+      <c r="FV4" s="81"/>
+      <c r="FW4" s="81"/>
+      <c r="FX4" s="81"/>
+      <c r="FY4" s="81"/>
+      <c r="FZ4" s="81"/>
+      <c r="GA4" s="81"/>
+      <c r="GB4" s="81"/>
+      <c r="GC4" s="81"/>
+      <c r="GD4" s="81"/>
+      <c r="GE4" s="81"/>
+      <c r="GF4" s="81"/>
+      <c r="GG4" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="GH4" s="73"/>
-      <c r="GI4" s="73"/>
-      <c r="GJ4" s="73"/>
-      <c r="GK4" s="73"/>
-      <c r="GL4" s="73"/>
-      <c r="GM4" s="73"/>
-      <c r="GN4" s="73"/>
-      <c r="GO4" s="73"/>
-      <c r="GP4" s="73"/>
-      <c r="GQ4" s="73"/>
-      <c r="GR4" s="73"/>
-      <c r="GS4" s="73"/>
-      <c r="GT4" s="73"/>
-      <c r="GU4" s="73" t="s">
+      <c r="GH4" s="69"/>
+      <c r="GI4" s="69"/>
+      <c r="GJ4" s="69"/>
+      <c r="GK4" s="69"/>
+      <c r="GL4" s="69"/>
+      <c r="GM4" s="69"/>
+      <c r="GN4" s="69"/>
+      <c r="GO4" s="69"/>
+      <c r="GP4" s="69"/>
+      <c r="GQ4" s="69"/>
+      <c r="GR4" s="69"/>
+      <c r="GS4" s="69"/>
+      <c r="GT4" s="69"/>
+      <c r="GU4" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="GV4" s="73"/>
-      <c r="GW4" s="73"/>
-      <c r="GX4" s="73"/>
-      <c r="GY4" s="73"/>
-      <c r="GZ4" s="73"/>
-      <c r="HA4" s="73"/>
-      <c r="HB4" s="73"/>
-      <c r="HC4" s="73"/>
-      <c r="HD4" s="73"/>
-      <c r="HE4" s="73"/>
-      <c r="HF4" s="73"/>
-      <c r="HG4" s="73"/>
-      <c r="HH4" s="73"/>
-      <c r="HI4" s="73" t="s">
+      <c r="GV4" s="69"/>
+      <c r="GW4" s="69"/>
+      <c r="GX4" s="69"/>
+      <c r="GY4" s="69"/>
+      <c r="GZ4" s="69"/>
+      <c r="HA4" s="69"/>
+      <c r="HB4" s="69"/>
+      <c r="HC4" s="69"/>
+      <c r="HD4" s="69"/>
+      <c r="HE4" s="69"/>
+      <c r="HF4" s="69"/>
+      <c r="HG4" s="69"/>
+      <c r="HH4" s="69"/>
+      <c r="HI4" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="HJ4" s="73"/>
-      <c r="HK4" s="73"/>
-      <c r="HL4" s="73"/>
-      <c r="HM4" s="73"/>
-      <c r="HN4" s="73"/>
-      <c r="HO4" s="73"/>
-      <c r="HP4" s="73"/>
-      <c r="HQ4" s="73"/>
-      <c r="HR4" s="73"/>
-      <c r="HS4" s="73"/>
-      <c r="HT4" s="73"/>
-      <c r="HU4" s="73"/>
-      <c r="HV4" s="73"/>
-      <c r="HW4" s="90" t="s">
+      <c r="HJ4" s="69"/>
+      <c r="HK4" s="69"/>
+      <c r="HL4" s="69"/>
+      <c r="HM4" s="69"/>
+      <c r="HN4" s="69"/>
+      <c r="HO4" s="69"/>
+      <c r="HP4" s="69"/>
+      <c r="HQ4" s="69"/>
+      <c r="HR4" s="69"/>
+      <c r="HS4" s="69"/>
+      <c r="HT4" s="69"/>
+      <c r="HU4" s="69"/>
+      <c r="HV4" s="69"/>
+      <c r="HW4" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="90"/>
-      <c r="HY4" s="90"/>
-      <c r="HZ4" s="90"/>
-      <c r="IA4" s="90"/>
-      <c r="IB4" s="90"/>
-      <c r="IC4" s="90"/>
-      <c r="ID4" s="90"/>
-      <c r="IE4" s="90"/>
-      <c r="IF4" s="90"/>
-      <c r="IG4" s="90"/>
-      <c r="IH4" s="90"/>
-      <c r="II4" s="90"/>
-      <c r="IJ4" s="90"/>
-      <c r="IK4" s="90" t="s">
+      <c r="HX4" s="70"/>
+      <c r="HY4" s="70"/>
+      <c r="HZ4" s="70"/>
+      <c r="IA4" s="70"/>
+      <c r="IB4" s="70"/>
+      <c r="IC4" s="70"/>
+      <c r="ID4" s="70"/>
+      <c r="IE4" s="70"/>
+      <c r="IF4" s="70"/>
+      <c r="IG4" s="70"/>
+      <c r="IH4" s="70"/>
+      <c r="II4" s="70"/>
+      <c r="IJ4" s="70"/>
+      <c r="IK4" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="90"/>
-      <c r="IM4" s="90"/>
-      <c r="IN4" s="90"/>
-      <c r="IO4" s="90"/>
-      <c r="IP4" s="90"/>
-      <c r="IQ4" s="90"/>
-      <c r="IR4" s="90"/>
-      <c r="IS4" s="90"/>
-      <c r="IT4" s="90"/>
-      <c r="IU4" s="90"/>
-      <c r="IV4" s="90"/>
-      <c r="IW4" s="90"/>
-      <c r="IX4" s="90"/>
-      <c r="IY4" s="90" t="s">
+      <c r="IL4" s="70"/>
+      <c r="IM4" s="70"/>
+      <c r="IN4" s="70"/>
+      <c r="IO4" s="70"/>
+      <c r="IP4" s="70"/>
+      <c r="IQ4" s="70"/>
+      <c r="IR4" s="70"/>
+      <c r="IS4" s="70"/>
+      <c r="IT4" s="70"/>
+      <c r="IU4" s="70"/>
+      <c r="IV4" s="70"/>
+      <c r="IW4" s="70"/>
+      <c r="IX4" s="70"/>
+      <c r="IY4" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="90"/>
-      <c r="JA4" s="90"/>
-      <c r="JB4" s="90"/>
-      <c r="JC4" s="90"/>
-      <c r="JD4" s="90"/>
-      <c r="JE4" s="90"/>
-      <c r="JF4" s="90"/>
-      <c r="JG4" s="90"/>
-      <c r="JH4" s="90"/>
-      <c r="JI4" s="90"/>
-      <c r="JJ4" s="90"/>
-      <c r="JK4" s="90"/>
-      <c r="JL4" s="90"/>
-      <c r="JM4" s="91" t="s">
+      <c r="IZ4" s="70"/>
+      <c r="JA4" s="70"/>
+      <c r="JB4" s="70"/>
+      <c r="JC4" s="70"/>
+      <c r="JD4" s="70"/>
+      <c r="JE4" s="70"/>
+      <c r="JF4" s="70"/>
+      <c r="JG4" s="70"/>
+      <c r="JH4" s="70"/>
+      <c r="JI4" s="70"/>
+      <c r="JJ4" s="70"/>
+      <c r="JK4" s="70"/>
+      <c r="JL4" s="70"/>
+      <c r="JM4" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="91"/>
-      <c r="JO4" s="91"/>
-      <c r="JP4" s="91"/>
-      <c r="JQ4" s="91"/>
-      <c r="JR4" s="91"/>
-      <c r="JS4" s="91"/>
-      <c r="JT4" s="91"/>
-      <c r="JU4" s="91"/>
-      <c r="JV4" s="91"/>
-      <c r="JW4" s="91"/>
-      <c r="JX4" s="91"/>
-      <c r="JY4" s="91"/>
-      <c r="JZ4" s="88" t="s">
+      <c r="JN4" s="71"/>
+      <c r="JO4" s="71"/>
+      <c r="JP4" s="71"/>
+      <c r="JQ4" s="71"/>
+      <c r="JR4" s="71"/>
+      <c r="JS4" s="71"/>
+      <c r="JT4" s="71"/>
+      <c r="JU4" s="71"/>
+      <c r="JV4" s="71"/>
+      <c r="JW4" s="71"/>
+      <c r="JX4" s="71"/>
+      <c r="JY4" s="71"/>
+      <c r="JZ4" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="89"/>
-      <c r="KB4" s="89"/>
-      <c r="KC4" s="89"/>
-      <c r="KD4" s="89"/>
-      <c r="KE4" s="89"/>
-      <c r="KF4" s="89"/>
-      <c r="KG4" s="89"/>
-      <c r="KH4" s="84" t="s">
+      <c r="KA4" s="68"/>
+      <c r="KB4" s="68"/>
+      <c r="KC4" s="68"/>
+      <c r="KD4" s="68"/>
+      <c r="KE4" s="68"/>
+      <c r="KF4" s="68"/>
+      <c r="KG4" s="68"/>
+      <c r="KH4" s="63" t="s">
         <v>316</v>
       </c>
-      <c r="KI4" s="85"/>
-      <c r="KJ4" s="85"/>
+      <c r="KI4" s="64"/>
+      <c r="KJ4" s="64"/>
       <c r="KK4" s="46"/>
     </row>
     <row r="5" spans="1:299" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="66"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="69"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="69"/>
-      <c r="U5" s="70"/>
-      <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
-      <c r="X5" s="70"/>
-      <c r="Y5" s="70"/>
-      <c r="Z5" s="70"/>
-      <c r="AA5" s="70"/>
-      <c r="AB5" s="70"/>
-      <c r="AC5" s="71"/>
-      <c r="AD5" s="71"/>
-      <c r="AE5" s="71"/>
-      <c r="AF5" s="71"/>
-      <c r="AG5" s="71"/>
-      <c r="AH5" s="71"/>
-      <c r="AI5" s="71"/>
-      <c r="AJ5" s="72"/>
-      <c r="AK5" s="72"/>
-      <c r="AL5" s="72"/>
-      <c r="AM5" s="63"/>
-      <c r="AN5" s="63"/>
-      <c r="AO5" s="74"/>
-      <c r="AP5" s="74"/>
-      <c r="AQ5" s="74"/>
-      <c r="AR5" s="74"/>
-      <c r="AS5" s="75"/>
-      <c r="AT5" s="75"/>
-      <c r="AU5" s="75"/>
-      <c r="AV5" s="75"/>
-      <c r="AW5" s="75"/>
-      <c r="AX5" s="75"/>
-      <c r="AY5" s="75"/>
-      <c r="AZ5" s="75"/>
-      <c r="BA5" s="75"/>
-      <c r="BB5" s="75"/>
-      <c r="BC5" s="75"/>
-      <c r="BD5" s="75"/>
-      <c r="BE5" s="75"/>
-      <c r="BF5" s="75"/>
-      <c r="BG5" s="75"/>
-      <c r="BH5" s="75"/>
-      <c r="BI5" s="75"/>
-      <c r="BJ5" s="75"/>
+      <c r="A5" s="85"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="87"/>
+      <c r="L5" s="87"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="88"/>
+      <c r="R5" s="88"/>
+      <c r="S5" s="88"/>
+      <c r="T5" s="88"/>
+      <c r="U5" s="89"/>
+      <c r="V5" s="89"/>
+      <c r="W5" s="89"/>
+      <c r="X5" s="89"/>
+      <c r="Y5" s="89"/>
+      <c r="Z5" s="89"/>
+      <c r="AA5" s="89"/>
+      <c r="AB5" s="89"/>
+      <c r="AC5" s="90"/>
+      <c r="AD5" s="90"/>
+      <c r="AE5" s="90"/>
+      <c r="AF5" s="90"/>
+      <c r="AG5" s="90"/>
+      <c r="AH5" s="90"/>
+      <c r="AI5" s="90"/>
+      <c r="AJ5" s="91"/>
+      <c r="AK5" s="91"/>
+      <c r="AL5" s="91"/>
+      <c r="AM5" s="82"/>
+      <c r="AN5" s="82"/>
+      <c r="AO5" s="72"/>
+      <c r="AP5" s="72"/>
+      <c r="AQ5" s="72"/>
+      <c r="AR5" s="72"/>
+      <c r="AS5" s="73"/>
+      <c r="AT5" s="73"/>
+      <c r="AU5" s="73"/>
+      <c r="AV5" s="73"/>
+      <c r="AW5" s="73"/>
+      <c r="AX5" s="73"/>
+      <c r="AY5" s="73"/>
+      <c r="AZ5" s="73"/>
+      <c r="BA5" s="73"/>
+      <c r="BB5" s="73"/>
+      <c r="BC5" s="73"/>
+      <c r="BD5" s="73"/>
+      <c r="BE5" s="73"/>
+      <c r="BF5" s="73"/>
+      <c r="BG5" s="73"/>
+      <c r="BH5" s="73"/>
+      <c r="BI5" s="73"/>
+      <c r="BJ5" s="73"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -4064,34 +4064,34 @@
       <c r="JL5" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="JM5" s="91"/>
-      <c r="JN5" s="91"/>
-      <c r="JO5" s="91"/>
-      <c r="JP5" s="91"/>
-      <c r="JQ5" s="91"/>
-      <c r="JR5" s="91"/>
-      <c r="JS5" s="91"/>
-      <c r="JT5" s="91"/>
-      <c r="JU5" s="91"/>
-      <c r="JV5" s="91"/>
-      <c r="JW5" s="91"/>
-      <c r="JX5" s="91"/>
-      <c r="JY5" s="91"/>
-      <c r="JZ5" s="89" t="s">
+      <c r="JM5" s="71"/>
+      <c r="JN5" s="71"/>
+      <c r="JO5" s="71"/>
+      <c r="JP5" s="71"/>
+      <c r="JQ5" s="71"/>
+      <c r="JR5" s="71"/>
+      <c r="JS5" s="71"/>
+      <c r="JT5" s="71"/>
+      <c r="JU5" s="71"/>
+      <c r="JV5" s="71"/>
+      <c r="JW5" s="71"/>
+      <c r="JX5" s="71"/>
+      <c r="JY5" s="71"/>
+      <c r="JZ5" s="68" t="s">
         <v>342</v>
       </c>
-      <c r="KA5" s="89"/>
-      <c r="KB5" s="89"/>
-      <c r="KC5" s="89"/>
-      <c r="KD5" s="89" t="s">
+      <c r="KA5" s="68"/>
+      <c r="KB5" s="68"/>
+      <c r="KC5" s="68"/>
+      <c r="KD5" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="89"/>
-      <c r="KF5" s="89"/>
-      <c r="KG5" s="89"/>
-      <c r="KH5" s="86"/>
-      <c r="KI5" s="87"/>
-      <c r="KJ5" s="87"/>
+      <c r="KE5" s="68"/>
+      <c r="KF5" s="68"/>
+      <c r="KG5" s="68"/>
+      <c r="KH5" s="65"/>
+      <c r="KI5" s="66"/>
+      <c r="KJ5" s="66"/>
       <c r="KK5" s="46"/>
     </row>
     <row r="6" spans="1:299" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5427,16 +5427,16 @@
   </sheetData>
   <autoFilter ref="A6:KK6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="32">
-    <mergeCell ref="KH4:KJ5"/>
-    <mergeCell ref="JZ4:KG4"/>
-    <mergeCell ref="JZ5:KC5"/>
-    <mergeCell ref="KD5:KG5"/>
-    <mergeCell ref="GU4:HH4"/>
-    <mergeCell ref="HI4:HV4"/>
-    <mergeCell ref="HW4:IJ4"/>
-    <mergeCell ref="IK4:IX4"/>
-    <mergeCell ref="IY4:JL4"/>
-    <mergeCell ref="JM4:JY5"/>
+    <mergeCell ref="AM4:AN5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:D5"/>
+    <mergeCell ref="E4:J5"/>
+    <mergeCell ref="K4:O5"/>
+    <mergeCell ref="P4:T5"/>
+    <mergeCell ref="U4:AB5"/>
+    <mergeCell ref="AC4:AI5"/>
+    <mergeCell ref="AJ4:AL5"/>
     <mergeCell ref="GG4:GT4"/>
     <mergeCell ref="AO4:AR5"/>
     <mergeCell ref="AS4:BJ5"/>
@@ -5449,26 +5449,23 @@
     <mergeCell ref="EQ4:FD4"/>
     <mergeCell ref="FE4:FR4"/>
     <mergeCell ref="FS4:GF4"/>
-    <mergeCell ref="AM4:AN5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:D5"/>
-    <mergeCell ref="E4:J5"/>
-    <mergeCell ref="K4:O5"/>
-    <mergeCell ref="P4:T5"/>
-    <mergeCell ref="U4:AB5"/>
-    <mergeCell ref="AC4:AI5"/>
-    <mergeCell ref="AJ4:AL5"/>
+    <mergeCell ref="KH4:KJ5"/>
+    <mergeCell ref="JZ4:KG4"/>
+    <mergeCell ref="JZ5:KC5"/>
+    <mergeCell ref="KD5:KG5"/>
+    <mergeCell ref="GU4:HH4"/>
+    <mergeCell ref="HI4:HV4"/>
+    <mergeCell ref="HW4:IJ4"/>
+    <mergeCell ref="IK4:IX4"/>
+    <mergeCell ref="IY4:JL4"/>
+    <mergeCell ref="JM4:JY5"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>
   </conditionalFormatting>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>36526</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KK7" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>"NGSA, WEM, FCRM Operational Framework, Other, Unknown/TBC"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KI7" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete, No Delivery pre 2021 "</formula1>

</xml_diff>

<commit_message>
[PM-343] Correct dropdown values and remove spurious validation
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthall/Work/pafs/pafs_core/lib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DAC8F2-0DFE-7347-99E2-9CC799A05998}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25200" windowHeight="11980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25200" windowHeight="11980"/>
   </bookViews>
   <sheets>
-    <sheet name="Master local choices" sheetId="2" r:id="rId1"/>
+    <sheet name="Master local choices" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$KK$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,29 +33,29 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author>Registered User</author>
   </authors>
   <commentList>
-    <comment ref="CD6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="CD6" authorId="0">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <b val="1"/>
+            <color indexed="81"/>
+            <sz val="9"/>
           </rPr>
           <t>Registered User:</t>
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <color indexed="81"/>
+            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="343" count="343">
   <si>
     <t>FCRM1 - National Capital Programme</t>
   </si>
@@ -88,7 +87,7 @@
     <t>DESCRIPTIVE DETAILS</t>
   </si>
   <si>
-    <t>PARTNERSHIP FUNDING SUMMARY
+    <t xml:space="preserve">PARTNERSHIP FUNDING SUMMARY
 (Values to be taken from PF Calculator)</t>
   </si>
   <si>
@@ -98,51 +97,51 @@
     <t>ADDITIONAL DETAILS</t>
   </si>
   <si>
-    <t>PROJECT TOTALS
+    <t xml:space="preserve">PROJECT TOTALS
 (calculated from relevant columns)
 £ CASH</t>
   </si>
   <si>
-    <t>TOTAL PROJECT EXPENDITURE
+    <t xml:space="preserve">TOTAL PROJECT EXPENDITURE
  (calculated from FCRM GiA to be expended + Total Local Contributions Secured + Funding From Other EA Functions + Further Contributions Required)
 £ CASH</t>
   </si>
   <si>
-    <t>FCRM Grant in Aid TO BE EXPENDED ON PROJECT
+    <t xml:space="preserve">FCRM Grant in Aid TO BE EXPENDED ON PROJECT
 £ CASH</t>
   </si>
   <si>
-    <t>GROWTH FUND
+    <t xml:space="preserve">GROWTH FUND
  £ CASH</t>
   </si>
   <si>
-    <t>LOCAL LEVY SECURED
+    <t xml:space="preserve">LOCAL LEVY SECURED
  £ CASH</t>
   </si>
   <si>
-    <t>INTERNAL DRAINAGE BOARD PRECEPTS SECURED
+    <t xml:space="preserve">INTERNAL DRAINAGE BOARD PRECEPTS SECURED
  £ CASH</t>
   </si>
   <si>
-    <t>PUBLICLY FUNDED CONTRIBUTIONS SECURED
+    <t xml:space="preserve">PUBLICLY FUNDED CONTRIBUTIONS SECURED
 (Contract In Place, or In Negotiation)
  £ CASH</t>
   </si>
   <si>
-    <t>PRIVATELY FUNDED CONTRIBUTIONS SECURED
+    <t xml:space="preserve">PRIVATELY FUNDED CONTRIBUTIONS SECURED
 (Contract In Place, or In Negotiation)
  £ CASH</t>
   </si>
   <si>
-    <t>FUNDING CONTRIBUTIONS FROM OTHER ENVIRONMENT AGENCY FUNCTIONS/SOURCES
+    <t xml:space="preserve">FUNDING CONTRIBUTIONS FROM OTHER ENVIRONMENT AGENCY FUNCTIONS/SOURCES
 £ CASH</t>
   </si>
   <si>
-    <t>FURTHER CONTRIBUTIONS REQUIRED
+    <t xml:space="preserve">FURTHER CONTRIBUTIONS REQUIRED
  £ CASH</t>
   </si>
   <si>
-    <t>Outcome Measures
+    <t xml:space="preserve">Outcome Measures
  OM2 Delivery</t>
   </si>
   <si>
@@ -169,7 +168,7 @@
     <t>Environmental performance specification indicators</t>
   </si>
   <si>
-    <t>SCHEME OVERVIEW
+    <t xml:space="preserve">SCHEME OVERVIEW
 (calculated from relevant columns)</t>
   </si>
   <si>
@@ -397,7 +396,7 @@
     <t>OM4c - PROJECT TOTAL</t>
   </si>
   <si>
-    <t>TPE - PREVIOUS
+    <t xml:space="preserve">TPE - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -437,7 +436,7 @@
     <t>TPE - 2026/27</t>
   </si>
   <si>
-    <t>GiA - PREVIOUS
+    <t xml:space="preserve">GiA - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -477,7 +476,7 @@
     <t>GiA - 2026/27</t>
   </si>
   <si>
-    <t>Growth - PREVIOUS
+    <t xml:space="preserve">Growth - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -517,7 +516,7 @@
     <t>Growth - 2026/27</t>
   </si>
   <si>
-    <t>Local Levy - PREVIOUS
+    <t xml:space="preserve">Local Levy - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -557,7 +556,7 @@
     <t>Local Levy - 2026/27</t>
   </si>
   <si>
-    <t>IDB - PREVIOUS
+    <t xml:space="preserve">IDB - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -597,7 +596,7 @@
     <t>IDB - 2026/27</t>
   </si>
   <si>
-    <t>Public - PREVIOUS
+    <t xml:space="preserve">Public - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -637,7 +636,7 @@
     <t>Public - 2026/27</t>
   </si>
   <si>
-    <t>Private - PREVIOUS
+    <t xml:space="preserve">Private - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -677,7 +676,7 @@
     <t>Private - 2026/27</t>
   </si>
   <si>
-    <t>Other EA - PREVIOUS
+    <t xml:space="preserve">Other EA - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -717,7 +716,7 @@
     <t>Other EA - 2026/27</t>
   </si>
   <si>
-    <t>Further required - PREVIOUS
+    <t xml:space="preserve">Further required - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -757,7 +756,7 @@
     <t>Further required - 2026/27</t>
   </si>
   <si>
-    <t>OM2 - PREVIOUS
+    <t xml:space="preserve">OM2 - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -797,7 +796,7 @@
     <t>OM2 - 2026/27</t>
   </si>
   <si>
-    <t>OM2b - PREVIOUS
+    <t xml:space="preserve">OM2b - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -837,7 +836,7 @@
     <t>OM2b - 2026/27</t>
   </si>
   <si>
-    <t>OM2c - PREVIOUS
+    <t xml:space="preserve">OM2c - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -877,7 +876,7 @@
     <t>OM2c - 2026/27</t>
   </si>
   <si>
-    <t>OM3 - PREVIOUS
+    <t xml:space="preserve">OM3 - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -917,7 +916,7 @@
     <t>OM3 - 2026/27</t>
   </si>
   <si>
-    <t>OM3b - PREVIOUS
+    <t xml:space="preserve">OM3b - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -957,7 +956,7 @@
     <t>OM3b - 2026/27</t>
   </si>
   <si>
-    <t>OM3c - PREVIOUS
+    <t xml:space="preserve">OM3c - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -1050,20 +1049,20 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <b val="1"/>
+        <color rgb="FFFF0000"/>
+        <sz val="12"/>
       </rPr>
       <t>GROWTH</t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <b val="1"/>
+        <sz val="12"/>
       </rPr>
       <t xml:space="preserve"> 6 year total</t>
     </r>
@@ -1149,20 +1148,20 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <b val="1"/>
+        <color rgb="FFFF0000"/>
+        <sz val="12"/>
       </rPr>
       <t>GROWTH</t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <b val="1"/>
+        <sz val="12"/>
       </rPr>
       <t xml:space="preserve"> 20/21</t>
     </r>
@@ -1183,7 +1182,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -1191,115 +1190,115 @@
     <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     <numFmt numFmtId="168" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="12"/>
     </font>
     <font>
-      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="12"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="0"/>
+      <sz val="16"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
     <font>
-      <b/>
-      <sz val="22"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="22"/>
     </font>
     <font>
-      <b/>
-      <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="20"/>
     </font>
     <font>
-      <sz val="30"/>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="30"/>
     </font>
     <font>
-      <b/>
-      <sz val="22"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="22"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="14"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <b val="1"/>
+      <color indexed="81"/>
+      <sz val="9"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <color indexed="81"/>
+      <sz val="9"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FFFF0000"/>
+      <sz val="12"/>
     </font>
     <font>
-      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="11"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="27">
@@ -1359,7 +1358,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor theme="3" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1371,7 +1370,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.3499862666707358"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1449,13 +1448,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1515,15 +1514,15 @@
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1701,6 +1700,69 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1719,87 +1781,24 @@
     <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="%" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="% 2 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="%" xfId="3"/>
+    <cellStyle name="% 2 2 2" xfId="4"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Comma 2" xfId="9"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal_RCP" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2" xfId="8"/>
+    <cellStyle name="Normal 2 2" xfId="6"/>
+    <cellStyle name="Normal_RCP" xfId="5"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Percent 11" xfId="7" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Percent 11" xfId="7"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1813,7 +1812,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16" count="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1967,7 +1966,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1993,7 +1992,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -2028,7 +2027,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2071,7 +2070,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -2087,7 +2086,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
@@ -2102,7 +2101,7 @@
       <selection pane="bottomRight" activeCell="KH7" sqref="KH7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="24.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98.7109375" style="1" customWidth="1"/>
@@ -2129,11 +2128,11 @@
     <col min="300" max="16384" width="8.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:299" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:293" customFormat="false" ht="28.5" customHeight="1">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
+      <c r="B1" s="64"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
@@ -2426,11 +2425,11 @@
       <c r="KF1" s="23"/>
       <c r="KG1" s="23"/>
     </row>
-    <row r="2" spans="1:299" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="84" t="s">
+    <row r="2" spans="1:293" customFormat="false" ht="28.5" customHeight="1">
+      <c r="A2" s="65" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="84"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="23"/>
@@ -2723,7 +2722,7 @@
       <c r="KF2" s="37"/>
       <c r="KG2" s="37"/>
     </row>
-    <row r="3" spans="1:299" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:293" customFormat="false" ht="25.5" customHeight="1">
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="39"/>
@@ -3018,422 +3017,422 @@
       <c r="KF3" s="45"/>
       <c r="KG3" s="45"/>
     </row>
-    <row r="4" spans="1:299" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="85" t="s">
+    <row r="4" spans="1:297" customFormat="false" ht="46.5" customHeight="1">
+      <c r="A4" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="86" t="s">
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="87" t="s">
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="88" t="s">
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="89" t="s">
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="69"/>
+      <c r="T4" s="69"/>
+      <c r="U4" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="89"/>
-      <c r="W4" s="89"/>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="90" t="s">
+      <c r="V4" s="70"/>
+      <c r="W4" s="70"/>
+      <c r="X4" s="70"/>
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="70"/>
+      <c r="AA4" s="70"/>
+      <c r="AB4" s="70"/>
+      <c r="AC4" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="90"/>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="90"/>
-      <c r="AG4" s="90"/>
-      <c r="AH4" s="90"/>
-      <c r="AI4" s="90"/>
-      <c r="AJ4" s="91" t="s">
+      <c r="AD4" s="71"/>
+      <c r="AE4" s="71"/>
+      <c r="AF4" s="71"/>
+      <c r="AG4" s="71"/>
+      <c r="AH4" s="71"/>
+      <c r="AI4" s="71"/>
+      <c r="AJ4" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="91"/>
-      <c r="AL4" s="91"/>
-      <c r="AM4" s="82" t="s">
+      <c r="AK4" s="72"/>
+      <c r="AL4" s="72"/>
+      <c r="AM4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="82"/>
-      <c r="AO4" s="72"/>
-      <c r="AP4" s="72"/>
-      <c r="AQ4" s="72"/>
-      <c r="AR4" s="72"/>
-      <c r="AS4" s="73" t="s">
+      <c r="AN4" s="63"/>
+      <c r="AO4" s="74"/>
+      <c r="AP4" s="74"/>
+      <c r="AQ4" s="74"/>
+      <c r="AR4" s="74"/>
+      <c r="AS4" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="73"/>
-      <c r="AV4" s="73"/>
-      <c r="AW4" s="73"/>
-      <c r="AX4" s="73"/>
-      <c r="AY4" s="73"/>
-      <c r="AZ4" s="73"/>
-      <c r="BA4" s="73"/>
-      <c r="BB4" s="73"/>
-      <c r="BC4" s="73"/>
-      <c r="BD4" s="73"/>
-      <c r="BE4" s="73"/>
-      <c r="BF4" s="73"/>
-      <c r="BG4" s="73"/>
-      <c r="BH4" s="73"/>
-      <c r="BI4" s="73"/>
-      <c r="BJ4" s="73"/>
-      <c r="BK4" s="69" t="s">
+      <c r="AT4" s="75"/>
+      <c r="AU4" s="75"/>
+      <c r="AV4" s="75"/>
+      <c r="AW4" s="75"/>
+      <c r="AX4" s="75"/>
+      <c r="AY4" s="75"/>
+      <c r="AZ4" s="75"/>
+      <c r="BA4" s="75"/>
+      <c r="BB4" s="75"/>
+      <c r="BC4" s="75"/>
+      <c r="BD4" s="75"/>
+      <c r="BE4" s="75"/>
+      <c r="BF4" s="75"/>
+      <c r="BG4" s="75"/>
+      <c r="BH4" s="75"/>
+      <c r="BI4" s="75"/>
+      <c r="BJ4" s="75"/>
+      <c r="BK4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="BL4" s="69"/>
-      <c r="BM4" s="69"/>
-      <c r="BN4" s="69"/>
-      <c r="BO4" s="69"/>
-      <c r="BP4" s="69"/>
-      <c r="BQ4" s="69"/>
-      <c r="BR4" s="69"/>
-      <c r="BS4" s="69"/>
-      <c r="BT4" s="69"/>
-      <c r="BU4" s="69"/>
-      <c r="BV4" s="69"/>
-      <c r="BW4" s="69"/>
-      <c r="BX4" s="69"/>
-      <c r="BY4" s="74" t="s">
+      <c r="BL4" s="73"/>
+      <c r="BM4" s="73"/>
+      <c r="BN4" s="73"/>
+      <c r="BO4" s="73"/>
+      <c r="BP4" s="73"/>
+      <c r="BQ4" s="73"/>
+      <c r="BR4" s="73"/>
+      <c r="BS4" s="73"/>
+      <c r="BT4" s="73"/>
+      <c r="BU4" s="73"/>
+      <c r="BV4" s="73"/>
+      <c r="BW4" s="73"/>
+      <c r="BX4" s="73"/>
+      <c r="BY4" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="74"/>
-      <c r="CA4" s="74"/>
-      <c r="CB4" s="74"/>
-      <c r="CC4" s="74"/>
-      <c r="CD4" s="74"/>
-      <c r="CE4" s="74"/>
-      <c r="CF4" s="74"/>
-      <c r="CG4" s="74"/>
-      <c r="CH4" s="74"/>
-      <c r="CI4" s="74"/>
-      <c r="CJ4" s="74"/>
-      <c r="CK4" s="74"/>
-      <c r="CL4" s="74"/>
-      <c r="CM4" s="75" t="s">
+      <c r="BZ4" s="76"/>
+      <c r="CA4" s="76"/>
+      <c r="CB4" s="76"/>
+      <c r="CC4" s="76"/>
+      <c r="CD4" s="76"/>
+      <c r="CE4" s="76"/>
+      <c r="CF4" s="76"/>
+      <c r="CG4" s="76"/>
+      <c r="CH4" s="76"/>
+      <c r="CI4" s="76"/>
+      <c r="CJ4" s="76"/>
+      <c r="CK4" s="76"/>
+      <c r="CL4" s="76"/>
+      <c r="CM4" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="75"/>
-      <c r="CO4" s="75"/>
-      <c r="CP4" s="75"/>
-      <c r="CQ4" s="75"/>
-      <c r="CR4" s="75"/>
-      <c r="CS4" s="75"/>
-      <c r="CT4" s="75"/>
-      <c r="CU4" s="75"/>
-      <c r="CV4" s="75"/>
-      <c r="CW4" s="75"/>
-      <c r="CX4" s="75"/>
-      <c r="CY4" s="75"/>
-      <c r="CZ4" s="75"/>
-      <c r="DA4" s="76" t="s">
+      <c r="CN4" s="77"/>
+      <c r="CO4" s="77"/>
+      <c r="CP4" s="77"/>
+      <c r="CQ4" s="77"/>
+      <c r="CR4" s="77"/>
+      <c r="CS4" s="77"/>
+      <c r="CT4" s="77"/>
+      <c r="CU4" s="77"/>
+      <c r="CV4" s="77"/>
+      <c r="CW4" s="77"/>
+      <c r="CX4" s="77"/>
+      <c r="CY4" s="77"/>
+      <c r="CZ4" s="77"/>
+      <c r="DA4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="76"/>
-      <c r="DC4" s="76"/>
-      <c r="DD4" s="76"/>
-      <c r="DE4" s="76"/>
-      <c r="DF4" s="76"/>
-      <c r="DG4" s="76"/>
-      <c r="DH4" s="76"/>
-      <c r="DI4" s="76"/>
-      <c r="DJ4" s="76"/>
-      <c r="DK4" s="76"/>
-      <c r="DL4" s="76"/>
-      <c r="DM4" s="76"/>
-      <c r="DN4" s="76"/>
-      <c r="DO4" s="77" t="s">
+      <c r="DB4" s="78"/>
+      <c r="DC4" s="78"/>
+      <c r="DD4" s="78"/>
+      <c r="DE4" s="78"/>
+      <c r="DF4" s="78"/>
+      <c r="DG4" s="78"/>
+      <c r="DH4" s="78"/>
+      <c r="DI4" s="78"/>
+      <c r="DJ4" s="78"/>
+      <c r="DK4" s="78"/>
+      <c r="DL4" s="78"/>
+      <c r="DM4" s="78"/>
+      <c r="DN4" s="78"/>
+      <c r="DO4" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="77"/>
-      <c r="DQ4" s="77"/>
-      <c r="DR4" s="77"/>
-      <c r="DS4" s="77"/>
-      <c r="DT4" s="77"/>
-      <c r="DU4" s="77"/>
-      <c r="DV4" s="77"/>
-      <c r="DW4" s="77"/>
-      <c r="DX4" s="77"/>
-      <c r="DY4" s="77"/>
-      <c r="DZ4" s="77"/>
-      <c r="EA4" s="77"/>
-      <c r="EB4" s="77"/>
-      <c r="EC4" s="78" t="s">
+      <c r="DP4" s="79"/>
+      <c r="DQ4" s="79"/>
+      <c r="DR4" s="79"/>
+      <c r="DS4" s="79"/>
+      <c r="DT4" s="79"/>
+      <c r="DU4" s="79"/>
+      <c r="DV4" s="79"/>
+      <c r="DW4" s="79"/>
+      <c r="DX4" s="79"/>
+      <c r="DY4" s="79"/>
+      <c r="DZ4" s="79"/>
+      <c r="EA4" s="79"/>
+      <c r="EB4" s="79"/>
+      <c r="EC4" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="78"/>
-      <c r="EE4" s="78"/>
-      <c r="EF4" s="78"/>
-      <c r="EG4" s="78"/>
-      <c r="EH4" s="78"/>
-      <c r="EI4" s="78"/>
-      <c r="EJ4" s="78"/>
-      <c r="EK4" s="78"/>
-      <c r="EL4" s="78"/>
-      <c r="EM4" s="78"/>
-      <c r="EN4" s="78"/>
-      <c r="EO4" s="78"/>
-      <c r="EP4" s="78"/>
-      <c r="EQ4" s="79" t="s">
+      <c r="ED4" s="80"/>
+      <c r="EE4" s="80"/>
+      <c r="EF4" s="80"/>
+      <c r="EG4" s="80"/>
+      <c r="EH4" s="80"/>
+      <c r="EI4" s="80"/>
+      <c r="EJ4" s="80"/>
+      <c r="EK4" s="80"/>
+      <c r="EL4" s="80"/>
+      <c r="EM4" s="80"/>
+      <c r="EN4" s="80"/>
+      <c r="EO4" s="80"/>
+      <c r="EP4" s="80"/>
+      <c r="EQ4" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="79"/>
-      <c r="ES4" s="79"/>
-      <c r="ET4" s="79"/>
-      <c r="EU4" s="79"/>
-      <c r="EV4" s="79"/>
-      <c r="EW4" s="79"/>
-      <c r="EX4" s="79"/>
-      <c r="EY4" s="79"/>
-      <c r="EZ4" s="79"/>
-      <c r="FA4" s="79"/>
-      <c r="FB4" s="79"/>
-      <c r="FC4" s="79"/>
-      <c r="FD4" s="79"/>
-      <c r="FE4" s="80" t="s">
+      <c r="ER4" s="81"/>
+      <c r="ES4" s="81"/>
+      <c r="ET4" s="81"/>
+      <c r="EU4" s="81"/>
+      <c r="EV4" s="81"/>
+      <c r="EW4" s="81"/>
+      <c r="EX4" s="81"/>
+      <c r="EY4" s="81"/>
+      <c r="EZ4" s="81"/>
+      <c r="FA4" s="81"/>
+      <c r="FB4" s="81"/>
+      <c r="FC4" s="81"/>
+      <c r="FD4" s="81"/>
+      <c r="FE4" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="80"/>
-      <c r="FG4" s="80"/>
-      <c r="FH4" s="80"/>
-      <c r="FI4" s="80"/>
-      <c r="FJ4" s="80"/>
-      <c r="FK4" s="80"/>
-      <c r="FL4" s="80"/>
-      <c r="FM4" s="80"/>
-      <c r="FN4" s="80"/>
-      <c r="FO4" s="80"/>
-      <c r="FP4" s="80"/>
-      <c r="FQ4" s="80"/>
-      <c r="FR4" s="80"/>
-      <c r="FS4" s="81" t="s">
+      <c r="FF4" s="82"/>
+      <c r="FG4" s="82"/>
+      <c r="FH4" s="82"/>
+      <c r="FI4" s="82"/>
+      <c r="FJ4" s="82"/>
+      <c r="FK4" s="82"/>
+      <c r="FL4" s="82"/>
+      <c r="FM4" s="82"/>
+      <c r="FN4" s="82"/>
+      <c r="FO4" s="82"/>
+      <c r="FP4" s="82"/>
+      <c r="FQ4" s="82"/>
+      <c r="FR4" s="82"/>
+      <c r="FS4" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="81"/>
-      <c r="FU4" s="81"/>
-      <c r="FV4" s="81"/>
-      <c r="FW4" s="81"/>
-      <c r="FX4" s="81"/>
-      <c r="FY4" s="81"/>
-      <c r="FZ4" s="81"/>
-      <c r="GA4" s="81"/>
-      <c r="GB4" s="81"/>
-      <c r="GC4" s="81"/>
-      <c r="GD4" s="81"/>
-      <c r="GE4" s="81"/>
-      <c r="GF4" s="81"/>
-      <c r="GG4" s="69" t="s">
+      <c r="FT4" s="83"/>
+      <c r="FU4" s="83"/>
+      <c r="FV4" s="83"/>
+      <c r="FW4" s="83"/>
+      <c r="FX4" s="83"/>
+      <c r="FY4" s="83"/>
+      <c r="FZ4" s="83"/>
+      <c r="GA4" s="83"/>
+      <c r="GB4" s="83"/>
+      <c r="GC4" s="83"/>
+      <c r="GD4" s="83"/>
+      <c r="GE4" s="83"/>
+      <c r="GF4" s="83"/>
+      <c r="GG4" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="GH4" s="69"/>
-      <c r="GI4" s="69"/>
-      <c r="GJ4" s="69"/>
-      <c r="GK4" s="69"/>
-      <c r="GL4" s="69"/>
-      <c r="GM4" s="69"/>
-      <c r="GN4" s="69"/>
-      <c r="GO4" s="69"/>
-      <c r="GP4" s="69"/>
-      <c r="GQ4" s="69"/>
-      <c r="GR4" s="69"/>
-      <c r="GS4" s="69"/>
-      <c r="GT4" s="69"/>
-      <c r="GU4" s="69" t="s">
+      <c r="GH4" s="73"/>
+      <c r="GI4" s="73"/>
+      <c r="GJ4" s="73"/>
+      <c r="GK4" s="73"/>
+      <c r="GL4" s="73"/>
+      <c r="GM4" s="73"/>
+      <c r="GN4" s="73"/>
+      <c r="GO4" s="73"/>
+      <c r="GP4" s="73"/>
+      <c r="GQ4" s="73"/>
+      <c r="GR4" s="73"/>
+      <c r="GS4" s="73"/>
+      <c r="GT4" s="73"/>
+      <c r="GU4" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="GV4" s="69"/>
-      <c r="GW4" s="69"/>
-      <c r="GX4" s="69"/>
-      <c r="GY4" s="69"/>
-      <c r="GZ4" s="69"/>
-      <c r="HA4" s="69"/>
-      <c r="HB4" s="69"/>
-      <c r="HC4" s="69"/>
-      <c r="HD4" s="69"/>
-      <c r="HE4" s="69"/>
-      <c r="HF4" s="69"/>
-      <c r="HG4" s="69"/>
-      <c r="HH4" s="69"/>
-      <c r="HI4" s="69" t="s">
+      <c r="GV4" s="73"/>
+      <c r="GW4" s="73"/>
+      <c r="GX4" s="73"/>
+      <c r="GY4" s="73"/>
+      <c r="GZ4" s="73"/>
+      <c r="HA4" s="73"/>
+      <c r="HB4" s="73"/>
+      <c r="HC4" s="73"/>
+      <c r="HD4" s="73"/>
+      <c r="HE4" s="73"/>
+      <c r="HF4" s="73"/>
+      <c r="HG4" s="73"/>
+      <c r="HH4" s="73"/>
+      <c r="HI4" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="HJ4" s="69"/>
-      <c r="HK4" s="69"/>
-      <c r="HL4" s="69"/>
-      <c r="HM4" s="69"/>
-      <c r="HN4" s="69"/>
-      <c r="HO4" s="69"/>
-      <c r="HP4" s="69"/>
-      <c r="HQ4" s="69"/>
-      <c r="HR4" s="69"/>
-      <c r="HS4" s="69"/>
-      <c r="HT4" s="69"/>
-      <c r="HU4" s="69"/>
-      <c r="HV4" s="69"/>
-      <c r="HW4" s="70" t="s">
+      <c r="HJ4" s="73"/>
+      <c r="HK4" s="73"/>
+      <c r="HL4" s="73"/>
+      <c r="HM4" s="73"/>
+      <c r="HN4" s="73"/>
+      <c r="HO4" s="73"/>
+      <c r="HP4" s="73"/>
+      <c r="HQ4" s="73"/>
+      <c r="HR4" s="73"/>
+      <c r="HS4" s="73"/>
+      <c r="HT4" s="73"/>
+      <c r="HU4" s="73"/>
+      <c r="HV4" s="73"/>
+      <c r="HW4" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="70"/>
-      <c r="HY4" s="70"/>
-      <c r="HZ4" s="70"/>
-      <c r="IA4" s="70"/>
-      <c r="IB4" s="70"/>
-      <c r="IC4" s="70"/>
-      <c r="ID4" s="70"/>
-      <c r="IE4" s="70"/>
-      <c r="IF4" s="70"/>
-      <c r="IG4" s="70"/>
-      <c r="IH4" s="70"/>
-      <c r="II4" s="70"/>
-      <c r="IJ4" s="70"/>
-      <c r="IK4" s="70" t="s">
+      <c r="HX4" s="90"/>
+      <c r="HY4" s="90"/>
+      <c r="HZ4" s="90"/>
+      <c r="IA4" s="90"/>
+      <c r="IB4" s="90"/>
+      <c r="IC4" s="90"/>
+      <c r="ID4" s="90"/>
+      <c r="IE4" s="90"/>
+      <c r="IF4" s="90"/>
+      <c r="IG4" s="90"/>
+      <c r="IH4" s="90"/>
+      <c r="II4" s="90"/>
+      <c r="IJ4" s="90"/>
+      <c r="IK4" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="70"/>
-      <c r="IM4" s="70"/>
-      <c r="IN4" s="70"/>
-      <c r="IO4" s="70"/>
-      <c r="IP4" s="70"/>
-      <c r="IQ4" s="70"/>
-      <c r="IR4" s="70"/>
-      <c r="IS4" s="70"/>
-      <c r="IT4" s="70"/>
-      <c r="IU4" s="70"/>
-      <c r="IV4" s="70"/>
-      <c r="IW4" s="70"/>
-      <c r="IX4" s="70"/>
-      <c r="IY4" s="70" t="s">
+      <c r="IL4" s="90"/>
+      <c r="IM4" s="90"/>
+      <c r="IN4" s="90"/>
+      <c r="IO4" s="90"/>
+      <c r="IP4" s="90"/>
+      <c r="IQ4" s="90"/>
+      <c r="IR4" s="90"/>
+      <c r="IS4" s="90"/>
+      <c r="IT4" s="90"/>
+      <c r="IU4" s="90"/>
+      <c r="IV4" s="90"/>
+      <c r="IW4" s="90"/>
+      <c r="IX4" s="90"/>
+      <c r="IY4" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="70"/>
-      <c r="JA4" s="70"/>
-      <c r="JB4" s="70"/>
-      <c r="JC4" s="70"/>
-      <c r="JD4" s="70"/>
-      <c r="JE4" s="70"/>
-      <c r="JF4" s="70"/>
-      <c r="JG4" s="70"/>
-      <c r="JH4" s="70"/>
-      <c r="JI4" s="70"/>
-      <c r="JJ4" s="70"/>
-      <c r="JK4" s="70"/>
-      <c r="JL4" s="70"/>
-      <c r="JM4" s="71" t="s">
+      <c r="IZ4" s="90"/>
+      <c r="JA4" s="90"/>
+      <c r="JB4" s="90"/>
+      <c r="JC4" s="90"/>
+      <c r="JD4" s="90"/>
+      <c r="JE4" s="90"/>
+      <c r="JF4" s="90"/>
+      <c r="JG4" s="90"/>
+      <c r="JH4" s="90"/>
+      <c r="JI4" s="90"/>
+      <c r="JJ4" s="90"/>
+      <c r="JK4" s="90"/>
+      <c r="JL4" s="90"/>
+      <c r="JM4" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="71"/>
-      <c r="JO4" s="71"/>
-      <c r="JP4" s="71"/>
-      <c r="JQ4" s="71"/>
-      <c r="JR4" s="71"/>
-      <c r="JS4" s="71"/>
-      <c r="JT4" s="71"/>
-      <c r="JU4" s="71"/>
-      <c r="JV4" s="71"/>
-      <c r="JW4" s="71"/>
-      <c r="JX4" s="71"/>
-      <c r="JY4" s="71"/>
-      <c r="JZ4" s="67" t="s">
+      <c r="JN4" s="91"/>
+      <c r="JO4" s="91"/>
+      <c r="JP4" s="91"/>
+      <c r="JQ4" s="91"/>
+      <c r="JR4" s="91"/>
+      <c r="JS4" s="91"/>
+      <c r="JT4" s="91"/>
+      <c r="JU4" s="91"/>
+      <c r="JV4" s="91"/>
+      <c r="JW4" s="91"/>
+      <c r="JX4" s="91"/>
+      <c r="JY4" s="91"/>
+      <c r="JZ4" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="68"/>
-      <c r="KB4" s="68"/>
-      <c r="KC4" s="68"/>
-      <c r="KD4" s="68"/>
-      <c r="KE4" s="68"/>
-      <c r="KF4" s="68"/>
-      <c r="KG4" s="68"/>
-      <c r="KH4" s="63" t="s">
+      <c r="KA4" s="89"/>
+      <c r="KB4" s="89"/>
+      <c r="KC4" s="89"/>
+      <c r="KD4" s="89"/>
+      <c r="KE4" s="89"/>
+      <c r="KF4" s="89"/>
+      <c r="KG4" s="89"/>
+      <c r="KH4" s="84" t="s">
         <v>316</v>
       </c>
-      <c r="KI4" s="64"/>
-      <c r="KJ4" s="64"/>
+      <c r="KI4" s="85"/>
+      <c r="KJ4" s="85"/>
       <c r="KK4" s="46"/>
     </row>
-    <row r="5" spans="1:299" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="85"/>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="87"/>
-      <c r="M5" s="87"/>
-      <c r="N5" s="87"/>
-      <c r="O5" s="87"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="88"/>
-      <c r="T5" s="88"/>
-      <c r="U5" s="89"/>
-      <c r="V5" s="89"/>
-      <c r="W5" s="89"/>
-      <c r="X5" s="89"/>
-      <c r="Y5" s="89"/>
-      <c r="Z5" s="89"/>
-      <c r="AA5" s="89"/>
-      <c r="AB5" s="89"/>
-      <c r="AC5" s="90"/>
-      <c r="AD5" s="90"/>
-      <c r="AE5" s="90"/>
-      <c r="AF5" s="90"/>
-      <c r="AG5" s="90"/>
-      <c r="AH5" s="90"/>
-      <c r="AI5" s="90"/>
-      <c r="AJ5" s="91"/>
-      <c r="AK5" s="91"/>
-      <c r="AL5" s="91"/>
-      <c r="AM5" s="82"/>
-      <c r="AN5" s="82"/>
-      <c r="AO5" s="72"/>
-      <c r="AP5" s="72"/>
-      <c r="AQ5" s="72"/>
-      <c r="AR5" s="72"/>
-      <c r="AS5" s="73"/>
-      <c r="AT5" s="73"/>
-      <c r="AU5" s="73"/>
-      <c r="AV5" s="73"/>
-      <c r="AW5" s="73"/>
-      <c r="AX5" s="73"/>
-      <c r="AY5" s="73"/>
-      <c r="AZ5" s="73"/>
-      <c r="BA5" s="73"/>
-      <c r="BB5" s="73"/>
-      <c r="BC5" s="73"/>
-      <c r="BD5" s="73"/>
-      <c r="BE5" s="73"/>
-      <c r="BF5" s="73"/>
-      <c r="BG5" s="73"/>
-      <c r="BH5" s="73"/>
-      <c r="BI5" s="73"/>
-      <c r="BJ5" s="73"/>
+    <row r="5" spans="1:297" customFormat="false" ht="12" customHeight="1">
+      <c r="A5" s="66"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="70"/>
+      <c r="X5" s="70"/>
+      <c r="Y5" s="70"/>
+      <c r="Z5" s="70"/>
+      <c r="AA5" s="70"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="71"/>
+      <c r="AD5" s="71"/>
+      <c r="AE5" s="71"/>
+      <c r="AF5" s="71"/>
+      <c r="AG5" s="71"/>
+      <c r="AH5" s="71"/>
+      <c r="AI5" s="71"/>
+      <c r="AJ5" s="72"/>
+      <c r="AK5" s="72"/>
+      <c r="AL5" s="72"/>
+      <c r="AM5" s="63"/>
+      <c r="AN5" s="63"/>
+      <c r="AO5" s="74"/>
+      <c r="AP5" s="74"/>
+      <c r="AQ5" s="74"/>
+      <c r="AR5" s="74"/>
+      <c r="AS5" s="75"/>
+      <c r="AT5" s="75"/>
+      <c r="AU5" s="75"/>
+      <c r="AV5" s="75"/>
+      <c r="AW5" s="75"/>
+      <c r="AX5" s="75"/>
+      <c r="AY5" s="75"/>
+      <c r="AZ5" s="75"/>
+      <c r="BA5" s="75"/>
+      <c r="BB5" s="75"/>
+      <c r="BC5" s="75"/>
+      <c r="BD5" s="75"/>
+      <c r="BE5" s="75"/>
+      <c r="BF5" s="75"/>
+      <c r="BG5" s="75"/>
+      <c r="BH5" s="75"/>
+      <c r="BI5" s="75"/>
+      <c r="BJ5" s="75"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -4064,37 +4063,37 @@
       <c r="JL5" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="JM5" s="71"/>
-      <c r="JN5" s="71"/>
-      <c r="JO5" s="71"/>
-      <c r="JP5" s="71"/>
-      <c r="JQ5" s="71"/>
-      <c r="JR5" s="71"/>
-      <c r="JS5" s="71"/>
-      <c r="JT5" s="71"/>
-      <c r="JU5" s="71"/>
-      <c r="JV5" s="71"/>
-      <c r="JW5" s="71"/>
-      <c r="JX5" s="71"/>
-      <c r="JY5" s="71"/>
-      <c r="JZ5" s="68" t="s">
+      <c r="JM5" s="91"/>
+      <c r="JN5" s="91"/>
+      <c r="JO5" s="91"/>
+      <c r="JP5" s="91"/>
+      <c r="JQ5" s="91"/>
+      <c r="JR5" s="91"/>
+      <c r="JS5" s="91"/>
+      <c r="JT5" s="91"/>
+      <c r="JU5" s="91"/>
+      <c r="JV5" s="91"/>
+      <c r="JW5" s="91"/>
+      <c r="JX5" s="91"/>
+      <c r="JY5" s="91"/>
+      <c r="JZ5" s="89" t="s">
         <v>342</v>
       </c>
-      <c r="KA5" s="68"/>
-      <c r="KB5" s="68"/>
-      <c r="KC5" s="68"/>
-      <c r="KD5" s="68" t="s">
+      <c r="KA5" s="89"/>
+      <c r="KB5" s="89"/>
+      <c r="KC5" s="89"/>
+      <c r="KD5" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="68"/>
-      <c r="KF5" s="68"/>
-      <c r="KG5" s="68"/>
-      <c r="KH5" s="65"/>
-      <c r="KI5" s="66"/>
-      <c r="KJ5" s="66"/>
+      <c r="KE5" s="89"/>
+      <c r="KF5" s="89"/>
+      <c r="KG5" s="89"/>
+      <c r="KH5" s="86"/>
+      <c r="KI5" s="87"/>
+      <c r="KJ5" s="87"/>
       <c r="KK5" s="46"/>
     </row>
-    <row r="6" spans="1:299" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:299" customFormat="false" ht="81.75" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -4989,7 +4988,7 @@
       <c r="KL6" s="48"/>
       <c r="KM6" s="49"/>
     </row>
-    <row r="7" spans="1:299" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:297" customFormat="false" ht="15" customHeight="1">
       <c r="A7" s="50"/>
       <c r="B7" s="50"/>
       <c r="C7" s="50"/>
@@ -5425,18 +5424,18 @@
       <c r="KK7" s="47"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:KK6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A6:KK6"/>
   <mergeCells count="32">
-    <mergeCell ref="AM4:AN5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:D5"/>
-    <mergeCell ref="E4:J5"/>
-    <mergeCell ref="K4:O5"/>
-    <mergeCell ref="P4:T5"/>
-    <mergeCell ref="U4:AB5"/>
-    <mergeCell ref="AC4:AI5"/>
-    <mergeCell ref="AJ4:AL5"/>
+    <mergeCell ref="KH4:KJ5"/>
+    <mergeCell ref="JZ4:KG4"/>
+    <mergeCell ref="JZ5:KC5"/>
+    <mergeCell ref="KD5:KG5"/>
+    <mergeCell ref="GU4:HH4"/>
+    <mergeCell ref="HI4:HV4"/>
+    <mergeCell ref="HW4:IJ4"/>
+    <mergeCell ref="IK4:IX4"/>
+    <mergeCell ref="IY4:JL4"/>
+    <mergeCell ref="JM4:JY5"/>
     <mergeCell ref="GG4:GT4"/>
     <mergeCell ref="AO4:AR5"/>
     <mergeCell ref="AS4:BJ5"/>
@@ -5449,32 +5448,29 @@
     <mergeCell ref="EQ4:FD4"/>
     <mergeCell ref="FE4:FR4"/>
     <mergeCell ref="FS4:GF4"/>
-    <mergeCell ref="KH4:KJ5"/>
-    <mergeCell ref="JZ4:KG4"/>
-    <mergeCell ref="JZ5:KC5"/>
-    <mergeCell ref="KD5:KG5"/>
-    <mergeCell ref="GU4:HH4"/>
-    <mergeCell ref="HI4:HV4"/>
-    <mergeCell ref="HW4:IJ4"/>
-    <mergeCell ref="IK4:IX4"/>
-    <mergeCell ref="IY4:JL4"/>
-    <mergeCell ref="JM4:JY5"/>
+    <mergeCell ref="AM4:AN5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:D5"/>
+    <mergeCell ref="E4:J5"/>
+    <mergeCell ref="K4:O5"/>
+    <mergeCell ref="P4:T5"/>
+    <mergeCell ref="U4:AB5"/>
+    <mergeCell ref="AC4:AI5"/>
+    <mergeCell ref="AJ4:AL5"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>
   </conditionalFormatting>
-  <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR7" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR7">
       <formula1>36526</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KI7" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete, No Delivery pre 2021 "</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH6:KJ999996" xr:uid="{00000000-0002-0000-0000-000002000000}">
-      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete,"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH6:KJ999996">
+      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, N/A"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.7086614173228347" right="0.7086614173228347" top="0.7480314960629921" bottom="0.7480314960629921" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="10" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
[PM-343] Correct dropdown in rows KH-KJ (#238)
* [PM-343] Correct range on data validations

* Update fcerm1 spreadsheet template to correct data validation range so
all cells in the KH-KJ include the dropdown
* Remove redundant values for dropdown from sheet

* [PM-343] Remove spurious data validation from KK

* [PM-343] Correct dropdown values and remove spurious validation
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthall/Work/pafs/pafs_core/lib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84F3FAD-9F25-3A49-9B3B-4E25A0E35093}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25200" windowHeight="11980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25200" windowHeight="11980"/>
   </bookViews>
   <sheets>
-    <sheet name="Master local choices" sheetId="2" r:id="rId1"/>
+    <sheet name="Master local choices" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$KK$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,29 +33,29 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author>Registered User</author>
   </authors>
   <commentList>
-    <comment ref="CD6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="CD6" authorId="0">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <b val="1"/>
+            <color indexed="81"/>
+            <sz val="9"/>
           </rPr>
           <t>Registered User:</t>
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <color indexed="81"/>
+            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="343" count="343">
   <si>
     <t>FCRM1 - National Capital Programme</t>
   </si>
@@ -88,7 +87,7 @@
     <t>DESCRIPTIVE DETAILS</t>
   </si>
   <si>
-    <t>PARTNERSHIP FUNDING SUMMARY
+    <t xml:space="preserve">PARTNERSHIP FUNDING SUMMARY
 (Values to be taken from PF Calculator)</t>
   </si>
   <si>
@@ -98,51 +97,51 @@
     <t>ADDITIONAL DETAILS</t>
   </si>
   <si>
-    <t>PROJECT TOTALS
+    <t xml:space="preserve">PROJECT TOTALS
 (calculated from relevant columns)
 £ CASH</t>
   </si>
   <si>
-    <t>TOTAL PROJECT EXPENDITURE
+    <t xml:space="preserve">TOTAL PROJECT EXPENDITURE
  (calculated from FCRM GiA to be expended + Total Local Contributions Secured + Funding From Other EA Functions + Further Contributions Required)
 £ CASH</t>
   </si>
   <si>
-    <t>FCRM Grant in Aid TO BE EXPENDED ON PROJECT
+    <t xml:space="preserve">FCRM Grant in Aid TO BE EXPENDED ON PROJECT
 £ CASH</t>
   </si>
   <si>
-    <t>GROWTH FUND
+    <t xml:space="preserve">GROWTH FUND
  £ CASH</t>
   </si>
   <si>
-    <t>LOCAL LEVY SECURED
+    <t xml:space="preserve">LOCAL LEVY SECURED
  £ CASH</t>
   </si>
   <si>
-    <t>INTERNAL DRAINAGE BOARD PRECEPTS SECURED
+    <t xml:space="preserve">INTERNAL DRAINAGE BOARD PRECEPTS SECURED
  £ CASH</t>
   </si>
   <si>
-    <t>PUBLICLY FUNDED CONTRIBUTIONS SECURED
+    <t xml:space="preserve">PUBLICLY FUNDED CONTRIBUTIONS SECURED
 (Contract In Place, or In Negotiation)
  £ CASH</t>
   </si>
   <si>
-    <t>PRIVATELY FUNDED CONTRIBUTIONS SECURED
+    <t xml:space="preserve">PRIVATELY FUNDED CONTRIBUTIONS SECURED
 (Contract In Place, or In Negotiation)
  £ CASH</t>
   </si>
   <si>
-    <t>FUNDING CONTRIBUTIONS FROM OTHER ENVIRONMENT AGENCY FUNCTIONS/SOURCES
+    <t xml:space="preserve">FUNDING CONTRIBUTIONS FROM OTHER ENVIRONMENT AGENCY FUNCTIONS/SOURCES
 £ CASH</t>
   </si>
   <si>
-    <t>FURTHER CONTRIBUTIONS REQUIRED
+    <t xml:space="preserve">FURTHER CONTRIBUTIONS REQUIRED
  £ CASH</t>
   </si>
   <si>
-    <t>Outcome Measures
+    <t xml:space="preserve">Outcome Measures
  OM2 Delivery</t>
   </si>
   <si>
@@ -169,7 +168,7 @@
     <t>Environmental performance specification indicators</t>
   </si>
   <si>
-    <t>SCHEME OVERVIEW
+    <t xml:space="preserve">SCHEME OVERVIEW
 (calculated from relevant columns)</t>
   </si>
   <si>
@@ -397,7 +396,7 @@
     <t>OM4c - PROJECT TOTAL</t>
   </si>
   <si>
-    <t>TPE - PREVIOUS
+    <t xml:space="preserve">TPE - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -437,7 +436,7 @@
     <t>TPE - 2026/27</t>
   </si>
   <si>
-    <t>GiA - PREVIOUS
+    <t xml:space="preserve">GiA - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -477,7 +476,7 @@
     <t>GiA - 2026/27</t>
   </si>
   <si>
-    <t>Growth - PREVIOUS
+    <t xml:space="preserve">Growth - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -517,7 +516,7 @@
     <t>Growth - 2026/27</t>
   </si>
   <si>
-    <t>Local Levy - PREVIOUS
+    <t xml:space="preserve">Local Levy - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -557,7 +556,7 @@
     <t>Local Levy - 2026/27</t>
   </si>
   <si>
-    <t>IDB - PREVIOUS
+    <t xml:space="preserve">IDB - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -597,7 +596,7 @@
     <t>IDB - 2026/27</t>
   </si>
   <si>
-    <t>Public - PREVIOUS
+    <t xml:space="preserve">Public - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -637,7 +636,7 @@
     <t>Public - 2026/27</t>
   </si>
   <si>
-    <t>Private - PREVIOUS
+    <t xml:space="preserve">Private - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -677,7 +676,7 @@
     <t>Private - 2026/27</t>
   </si>
   <si>
-    <t>Other EA - PREVIOUS
+    <t xml:space="preserve">Other EA - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -717,7 +716,7 @@
     <t>Other EA - 2026/27</t>
   </si>
   <si>
-    <t>Further required - PREVIOUS
+    <t xml:space="preserve">Further required - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -757,7 +756,7 @@
     <t>Further required - 2026/27</t>
   </si>
   <si>
-    <t>OM2 - PREVIOUS
+    <t xml:space="preserve">OM2 - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -797,7 +796,7 @@
     <t>OM2 - 2026/27</t>
   </si>
   <si>
-    <t>OM2b - PREVIOUS
+    <t xml:space="preserve">OM2b - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -837,7 +836,7 @@
     <t>OM2b - 2026/27</t>
   </si>
   <si>
-    <t>OM2c - PREVIOUS
+    <t xml:space="preserve">OM2c - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -877,7 +876,7 @@
     <t>OM2c - 2026/27</t>
   </si>
   <si>
-    <t>OM3 - PREVIOUS
+    <t xml:space="preserve">OM3 - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -917,7 +916,7 @@
     <t>OM3 - 2026/27</t>
   </si>
   <si>
-    <t>OM3b - PREVIOUS
+    <t xml:space="preserve">OM3b - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -957,7 +956,7 @@
     <t>OM3b - 2026/27</t>
   </si>
   <si>
-    <t>OM3c - PREVIOUS
+    <t xml:space="preserve">OM3c - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -1050,20 +1049,20 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <b val="1"/>
+        <color rgb="FFFF0000"/>
+        <sz val="12"/>
       </rPr>
       <t>GROWTH</t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <b val="1"/>
+        <sz val="12"/>
       </rPr>
       <t xml:space="preserve"> 6 year total</t>
     </r>
@@ -1136,21 +1135,6 @@
   </si>
   <si>
     <t>Confidence in Securing Partnership Funding (all schemes including post-2021)</t>
-  </si>
-  <si>
-    <t>Confidence Assessment Picklist</t>
-  </si>
-  <si>
-    <t>3. Medium High</t>
-  </si>
-  <si>
-    <t>2. Medium Low</t>
-  </si>
-  <si>
-    <t>1. Low</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t/>
@@ -1164,20 +1148,20 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <b val="1"/>
+        <color rgb="FFFF0000"/>
+        <sz val="12"/>
       </rPr>
       <t>GROWTH</t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <b val="1"/>
+        <sz val="12"/>
       </rPr>
       <t xml:space="preserve"> 20/21</t>
     </r>
@@ -1193,15 +1177,12 @@
   </si>
   <si>
     <t>20/21</t>
-  </si>
-  <si>
-    <t>4. High</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -1211,113 +1192,113 @@
   </numFmts>
   <fonts count="18">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="12"/>
     </font>
     <font>
-      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="12"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="0"/>
+      <sz val="16"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
     <font>
-      <b/>
-      <sz val="22"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="22"/>
     </font>
     <font>
-      <b/>
-      <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="20"/>
     </font>
     <font>
-      <sz val="30"/>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="30"/>
     </font>
     <font>
-      <b/>
-      <sz val="22"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="22"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="14"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <b val="1"/>
+      <color indexed="81"/>
+      <sz val="9"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <color indexed="81"/>
+      <sz val="9"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FFFF0000"/>
+      <sz val="12"/>
     </font>
     <font>
-      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="11"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="27">
@@ -1377,7 +1358,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor theme="3" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1389,7 +1370,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.3499862666707358"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1467,13 +1448,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1533,17 +1514,17 @@
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1679,11 +1660,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1812,16 +1789,16 @@
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="%" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="% 2 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="%" xfId="3"/>
+    <cellStyle name="% 2 2 2" xfId="4"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Comma 2" xfId="9"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal_RCP" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2" xfId="8"/>
+    <cellStyle name="Normal 2 2" xfId="6"/>
+    <cellStyle name="Normal_RCP" xfId="5"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Percent 11" xfId="7" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Percent 11" xfId="7"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1835,7 +1812,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16" count="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1969,53 +1946,53 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="67000"/>
+                <a:satMod val="105000"/>
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:tint val="73000"/>
+                <a:satMod val="103000"/>
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="81000"/>
+                <a:satMod val="109000"/>
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="94000"/>
                 <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:shade val="100000"/>
                 <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:shade val="78000"/>
+                <a:satMod val="120000"/>
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -2050,7 +2027,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2073,16 +2050,16 @@
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
+                <a:shade val="98000"/>
                 <a:satMod val="150000"/>
-                <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
+                <a:shade val="90000"/>
                 <a:satMod val="130000"/>
-                <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
@@ -2093,7 +2070,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -2109,19 +2086,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:KN11"/>
+  <dimension ref="A1:KM7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="AZ9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="KG7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="KH7" sqref="KH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
@@ -2145,18 +2122,17 @@
     <col min="279" max="285" width="21" style="28" customWidth="1"/>
     <col min="286" max="293" width="21" style="6" customWidth="1"/>
     <col min="294" max="296" width="22.28515625" style="7" customWidth="1"/>
-    <col min="297" max="297" width="11" style="7" customWidth="1"/>
-    <col min="298" max="298" width="12.85546875" style="7" hidden="1" customWidth="1"/>
-    <col min="299" max="299" width="8.7109375" style="7"/>
-    <col min="300" max="300" width="11" style="7" customWidth="1"/>
-    <col min="301" max="16384" width="8.7109375" style="7"/>
+    <col min="297" max="297" width="17.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="298" max="298" width="8.7109375" style="7"/>
+    <col min="299" max="299" width="11" style="7" customWidth="1"/>
+    <col min="300" max="16384" width="8.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:300" ht="28.5" customHeight="1">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:293" customFormat="false" ht="28.5" customHeight="1">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="64"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
@@ -2449,11 +2425,11 @@
       <c r="KF1" s="23"/>
       <c r="KG1" s="23"/>
     </row>
-    <row r="2" spans="1:300" ht="28.5" customHeight="1">
-      <c r="A2" s="67" t="s">
-        <v>342</v>
-      </c>
-      <c r="B2" s="67"/>
+    <row r="2" spans="1:293" customFormat="false" ht="28.5" customHeight="1">
+      <c r="A2" s="65" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2" s="65"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="23"/>
@@ -2746,7 +2722,7 @@
       <c r="KF2" s="37"/>
       <c r="KG2" s="37"/>
     </row>
-    <row r="3" spans="1:300" ht="25.5" customHeight="1">
+    <row r="3" spans="1:293" customFormat="false" ht="25.5" customHeight="1">
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="39"/>
@@ -3041,422 +3017,422 @@
       <c r="KF3" s="45"/>
       <c r="KG3" s="45"/>
     </row>
-    <row r="4" spans="1:300" ht="46.5" customHeight="1">
-      <c r="A4" s="68" t="s">
+    <row r="4" spans="1:297" customFormat="false" ht="46.5" customHeight="1">
+      <c r="A4" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="69" t="s">
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="70" t="s">
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="70"/>
-      <c r="P4" s="71" t="s">
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="71"/>
-      <c r="S4" s="71"/>
-      <c r="T4" s="71"/>
-      <c r="U4" s="72" t="s">
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="69"/>
+      <c r="T4" s="69"/>
+      <c r="U4" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="72"/>
-      <c r="W4" s="72"/>
-      <c r="X4" s="72"/>
-      <c r="Y4" s="72"/>
-      <c r="Z4" s="72"/>
-      <c r="AA4" s="72"/>
-      <c r="AB4" s="72"/>
-      <c r="AC4" s="73" t="s">
+      <c r="V4" s="70"/>
+      <c r="W4" s="70"/>
+      <c r="X4" s="70"/>
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="70"/>
+      <c r="AA4" s="70"/>
+      <c r="AB4" s="70"/>
+      <c r="AC4" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="73"/>
-      <c r="AE4" s="73"/>
-      <c r="AF4" s="73"/>
-      <c r="AG4" s="73"/>
-      <c r="AH4" s="73"/>
-      <c r="AI4" s="73"/>
-      <c r="AJ4" s="74" t="s">
+      <c r="AD4" s="71"/>
+      <c r="AE4" s="71"/>
+      <c r="AF4" s="71"/>
+      <c r="AG4" s="71"/>
+      <c r="AH4" s="71"/>
+      <c r="AI4" s="71"/>
+      <c r="AJ4" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="74"/>
-      <c r="AL4" s="74"/>
-      <c r="AM4" s="65" t="s">
+      <c r="AK4" s="72"/>
+      <c r="AL4" s="72"/>
+      <c r="AM4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="65"/>
-      <c r="AO4" s="76"/>
-      <c r="AP4" s="76"/>
-      <c r="AQ4" s="76"/>
-      <c r="AR4" s="76"/>
-      <c r="AS4" s="77" t="s">
+      <c r="AN4" s="63"/>
+      <c r="AO4" s="74"/>
+      <c r="AP4" s="74"/>
+      <c r="AQ4" s="74"/>
+      <c r="AR4" s="74"/>
+      <c r="AS4" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="77"/>
-      <c r="AU4" s="77"/>
-      <c r="AV4" s="77"/>
-      <c r="AW4" s="77"/>
-      <c r="AX4" s="77"/>
-      <c r="AY4" s="77"/>
-      <c r="AZ4" s="77"/>
-      <c r="BA4" s="77"/>
-      <c r="BB4" s="77"/>
-      <c r="BC4" s="77"/>
-      <c r="BD4" s="77"/>
-      <c r="BE4" s="77"/>
-      <c r="BF4" s="77"/>
-      <c r="BG4" s="77"/>
-      <c r="BH4" s="77"/>
-      <c r="BI4" s="77"/>
-      <c r="BJ4" s="77"/>
-      <c r="BK4" s="75" t="s">
+      <c r="AT4" s="75"/>
+      <c r="AU4" s="75"/>
+      <c r="AV4" s="75"/>
+      <c r="AW4" s="75"/>
+      <c r="AX4" s="75"/>
+      <c r="AY4" s="75"/>
+      <c r="AZ4" s="75"/>
+      <c r="BA4" s="75"/>
+      <c r="BB4" s="75"/>
+      <c r="BC4" s="75"/>
+      <c r="BD4" s="75"/>
+      <c r="BE4" s="75"/>
+      <c r="BF4" s="75"/>
+      <c r="BG4" s="75"/>
+      <c r="BH4" s="75"/>
+      <c r="BI4" s="75"/>
+      <c r="BJ4" s="75"/>
+      <c r="BK4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="BL4" s="75"/>
-      <c r="BM4" s="75"/>
-      <c r="BN4" s="75"/>
-      <c r="BO4" s="75"/>
-      <c r="BP4" s="75"/>
-      <c r="BQ4" s="75"/>
-      <c r="BR4" s="75"/>
-      <c r="BS4" s="75"/>
-      <c r="BT4" s="75"/>
-      <c r="BU4" s="75"/>
-      <c r="BV4" s="75"/>
-      <c r="BW4" s="75"/>
-      <c r="BX4" s="75"/>
-      <c r="BY4" s="78" t="s">
+      <c r="BL4" s="73"/>
+      <c r="BM4" s="73"/>
+      <c r="BN4" s="73"/>
+      <c r="BO4" s="73"/>
+      <c r="BP4" s="73"/>
+      <c r="BQ4" s="73"/>
+      <c r="BR4" s="73"/>
+      <c r="BS4" s="73"/>
+      <c r="BT4" s="73"/>
+      <c r="BU4" s="73"/>
+      <c r="BV4" s="73"/>
+      <c r="BW4" s="73"/>
+      <c r="BX4" s="73"/>
+      <c r="BY4" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="78"/>
-      <c r="CA4" s="78"/>
-      <c r="CB4" s="78"/>
-      <c r="CC4" s="78"/>
-      <c r="CD4" s="78"/>
-      <c r="CE4" s="78"/>
-      <c r="CF4" s="78"/>
-      <c r="CG4" s="78"/>
-      <c r="CH4" s="78"/>
-      <c r="CI4" s="78"/>
-      <c r="CJ4" s="78"/>
-      <c r="CK4" s="78"/>
-      <c r="CL4" s="78"/>
-      <c r="CM4" s="79" t="s">
+      <c r="BZ4" s="76"/>
+      <c r="CA4" s="76"/>
+      <c r="CB4" s="76"/>
+      <c r="CC4" s="76"/>
+      <c r="CD4" s="76"/>
+      <c r="CE4" s="76"/>
+      <c r="CF4" s="76"/>
+      <c r="CG4" s="76"/>
+      <c r="CH4" s="76"/>
+      <c r="CI4" s="76"/>
+      <c r="CJ4" s="76"/>
+      <c r="CK4" s="76"/>
+      <c r="CL4" s="76"/>
+      <c r="CM4" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="79"/>
-      <c r="CO4" s="79"/>
-      <c r="CP4" s="79"/>
-      <c r="CQ4" s="79"/>
-      <c r="CR4" s="79"/>
-      <c r="CS4" s="79"/>
-      <c r="CT4" s="79"/>
-      <c r="CU4" s="79"/>
-      <c r="CV4" s="79"/>
-      <c r="CW4" s="79"/>
-      <c r="CX4" s="79"/>
-      <c r="CY4" s="79"/>
-      <c r="CZ4" s="79"/>
-      <c r="DA4" s="80" t="s">
+      <c r="CN4" s="77"/>
+      <c r="CO4" s="77"/>
+      <c r="CP4" s="77"/>
+      <c r="CQ4" s="77"/>
+      <c r="CR4" s="77"/>
+      <c r="CS4" s="77"/>
+      <c r="CT4" s="77"/>
+      <c r="CU4" s="77"/>
+      <c r="CV4" s="77"/>
+      <c r="CW4" s="77"/>
+      <c r="CX4" s="77"/>
+      <c r="CY4" s="77"/>
+      <c r="CZ4" s="77"/>
+      <c r="DA4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="80"/>
-      <c r="DC4" s="80"/>
-      <c r="DD4" s="80"/>
-      <c r="DE4" s="80"/>
-      <c r="DF4" s="80"/>
-      <c r="DG4" s="80"/>
-      <c r="DH4" s="80"/>
-      <c r="DI4" s="80"/>
-      <c r="DJ4" s="80"/>
-      <c r="DK4" s="80"/>
-      <c r="DL4" s="80"/>
-      <c r="DM4" s="80"/>
-      <c r="DN4" s="80"/>
-      <c r="DO4" s="81" t="s">
+      <c r="DB4" s="78"/>
+      <c r="DC4" s="78"/>
+      <c r="DD4" s="78"/>
+      <c r="DE4" s="78"/>
+      <c r="DF4" s="78"/>
+      <c r="DG4" s="78"/>
+      <c r="DH4" s="78"/>
+      <c r="DI4" s="78"/>
+      <c r="DJ4" s="78"/>
+      <c r="DK4" s="78"/>
+      <c r="DL4" s="78"/>
+      <c r="DM4" s="78"/>
+      <c r="DN4" s="78"/>
+      <c r="DO4" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="81"/>
-      <c r="DQ4" s="81"/>
-      <c r="DR4" s="81"/>
-      <c r="DS4" s="81"/>
-      <c r="DT4" s="81"/>
-      <c r="DU4" s="81"/>
-      <c r="DV4" s="81"/>
-      <c r="DW4" s="81"/>
-      <c r="DX4" s="81"/>
-      <c r="DY4" s="81"/>
-      <c r="DZ4" s="81"/>
-      <c r="EA4" s="81"/>
-      <c r="EB4" s="81"/>
-      <c r="EC4" s="82" t="s">
+      <c r="DP4" s="79"/>
+      <c r="DQ4" s="79"/>
+      <c r="DR4" s="79"/>
+      <c r="DS4" s="79"/>
+      <c r="DT4" s="79"/>
+      <c r="DU4" s="79"/>
+      <c r="DV4" s="79"/>
+      <c r="DW4" s="79"/>
+      <c r="DX4" s="79"/>
+      <c r="DY4" s="79"/>
+      <c r="DZ4" s="79"/>
+      <c r="EA4" s="79"/>
+      <c r="EB4" s="79"/>
+      <c r="EC4" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="82"/>
-      <c r="EE4" s="82"/>
-      <c r="EF4" s="82"/>
-      <c r="EG4" s="82"/>
-      <c r="EH4" s="82"/>
-      <c r="EI4" s="82"/>
-      <c r="EJ4" s="82"/>
-      <c r="EK4" s="82"/>
-      <c r="EL4" s="82"/>
-      <c r="EM4" s="82"/>
-      <c r="EN4" s="82"/>
-      <c r="EO4" s="82"/>
-      <c r="EP4" s="82"/>
-      <c r="EQ4" s="83" t="s">
+      <c r="ED4" s="80"/>
+      <c r="EE4" s="80"/>
+      <c r="EF4" s="80"/>
+      <c r="EG4" s="80"/>
+      <c r="EH4" s="80"/>
+      <c r="EI4" s="80"/>
+      <c r="EJ4" s="80"/>
+      <c r="EK4" s="80"/>
+      <c r="EL4" s="80"/>
+      <c r="EM4" s="80"/>
+      <c r="EN4" s="80"/>
+      <c r="EO4" s="80"/>
+      <c r="EP4" s="80"/>
+      <c r="EQ4" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="83"/>
-      <c r="ES4" s="83"/>
-      <c r="ET4" s="83"/>
-      <c r="EU4" s="83"/>
-      <c r="EV4" s="83"/>
-      <c r="EW4" s="83"/>
-      <c r="EX4" s="83"/>
-      <c r="EY4" s="83"/>
-      <c r="EZ4" s="83"/>
-      <c r="FA4" s="83"/>
-      <c r="FB4" s="83"/>
-      <c r="FC4" s="83"/>
-      <c r="FD4" s="83"/>
-      <c r="FE4" s="84" t="s">
+      <c r="ER4" s="81"/>
+      <c r="ES4" s="81"/>
+      <c r="ET4" s="81"/>
+      <c r="EU4" s="81"/>
+      <c r="EV4" s="81"/>
+      <c r="EW4" s="81"/>
+      <c r="EX4" s="81"/>
+      <c r="EY4" s="81"/>
+      <c r="EZ4" s="81"/>
+      <c r="FA4" s="81"/>
+      <c r="FB4" s="81"/>
+      <c r="FC4" s="81"/>
+      <c r="FD4" s="81"/>
+      <c r="FE4" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="84"/>
-      <c r="FG4" s="84"/>
-      <c r="FH4" s="84"/>
-      <c r="FI4" s="84"/>
-      <c r="FJ4" s="84"/>
-      <c r="FK4" s="84"/>
-      <c r="FL4" s="84"/>
-      <c r="FM4" s="84"/>
-      <c r="FN4" s="84"/>
-      <c r="FO4" s="84"/>
-      <c r="FP4" s="84"/>
-      <c r="FQ4" s="84"/>
-      <c r="FR4" s="84"/>
-      <c r="FS4" s="85" t="s">
+      <c r="FF4" s="82"/>
+      <c r="FG4" s="82"/>
+      <c r="FH4" s="82"/>
+      <c r="FI4" s="82"/>
+      <c r="FJ4" s="82"/>
+      <c r="FK4" s="82"/>
+      <c r="FL4" s="82"/>
+      <c r="FM4" s="82"/>
+      <c r="FN4" s="82"/>
+      <c r="FO4" s="82"/>
+      <c r="FP4" s="82"/>
+      <c r="FQ4" s="82"/>
+      <c r="FR4" s="82"/>
+      <c r="FS4" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="85"/>
-      <c r="FU4" s="85"/>
-      <c r="FV4" s="85"/>
-      <c r="FW4" s="85"/>
-      <c r="FX4" s="85"/>
-      <c r="FY4" s="85"/>
-      <c r="FZ4" s="85"/>
-      <c r="GA4" s="85"/>
-      <c r="GB4" s="85"/>
-      <c r="GC4" s="85"/>
-      <c r="GD4" s="85"/>
-      <c r="GE4" s="85"/>
-      <c r="GF4" s="85"/>
-      <c r="GG4" s="75" t="s">
+      <c r="FT4" s="83"/>
+      <c r="FU4" s="83"/>
+      <c r="FV4" s="83"/>
+      <c r="FW4" s="83"/>
+      <c r="FX4" s="83"/>
+      <c r="FY4" s="83"/>
+      <c r="FZ4" s="83"/>
+      <c r="GA4" s="83"/>
+      <c r="GB4" s="83"/>
+      <c r="GC4" s="83"/>
+      <c r="GD4" s="83"/>
+      <c r="GE4" s="83"/>
+      <c r="GF4" s="83"/>
+      <c r="GG4" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="GH4" s="75"/>
-      <c r="GI4" s="75"/>
-      <c r="GJ4" s="75"/>
-      <c r="GK4" s="75"/>
-      <c r="GL4" s="75"/>
-      <c r="GM4" s="75"/>
-      <c r="GN4" s="75"/>
-      <c r="GO4" s="75"/>
-      <c r="GP4" s="75"/>
-      <c r="GQ4" s="75"/>
-      <c r="GR4" s="75"/>
-      <c r="GS4" s="75"/>
-      <c r="GT4" s="75"/>
-      <c r="GU4" s="75" t="s">
+      <c r="GH4" s="73"/>
+      <c r="GI4" s="73"/>
+      <c r="GJ4" s="73"/>
+      <c r="GK4" s="73"/>
+      <c r="GL4" s="73"/>
+      <c r="GM4" s="73"/>
+      <c r="GN4" s="73"/>
+      <c r="GO4" s="73"/>
+      <c r="GP4" s="73"/>
+      <c r="GQ4" s="73"/>
+      <c r="GR4" s="73"/>
+      <c r="GS4" s="73"/>
+      <c r="GT4" s="73"/>
+      <c r="GU4" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="GV4" s="75"/>
-      <c r="GW4" s="75"/>
-      <c r="GX4" s="75"/>
-      <c r="GY4" s="75"/>
-      <c r="GZ4" s="75"/>
-      <c r="HA4" s="75"/>
-      <c r="HB4" s="75"/>
-      <c r="HC4" s="75"/>
-      <c r="HD4" s="75"/>
-      <c r="HE4" s="75"/>
-      <c r="HF4" s="75"/>
-      <c r="HG4" s="75"/>
-      <c r="HH4" s="75"/>
-      <c r="HI4" s="75" t="s">
+      <c r="GV4" s="73"/>
+      <c r="GW4" s="73"/>
+      <c r="GX4" s="73"/>
+      <c r="GY4" s="73"/>
+      <c r="GZ4" s="73"/>
+      <c r="HA4" s="73"/>
+      <c r="HB4" s="73"/>
+      <c r="HC4" s="73"/>
+      <c r="HD4" s="73"/>
+      <c r="HE4" s="73"/>
+      <c r="HF4" s="73"/>
+      <c r="HG4" s="73"/>
+      <c r="HH4" s="73"/>
+      <c r="HI4" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="HJ4" s="75"/>
-      <c r="HK4" s="75"/>
-      <c r="HL4" s="75"/>
-      <c r="HM4" s="75"/>
-      <c r="HN4" s="75"/>
-      <c r="HO4" s="75"/>
-      <c r="HP4" s="75"/>
-      <c r="HQ4" s="75"/>
-      <c r="HR4" s="75"/>
-      <c r="HS4" s="75"/>
-      <c r="HT4" s="75"/>
-      <c r="HU4" s="75"/>
-      <c r="HV4" s="75"/>
-      <c r="HW4" s="92" t="s">
+      <c r="HJ4" s="73"/>
+      <c r="HK4" s="73"/>
+      <c r="HL4" s="73"/>
+      <c r="HM4" s="73"/>
+      <c r="HN4" s="73"/>
+      <c r="HO4" s="73"/>
+      <c r="HP4" s="73"/>
+      <c r="HQ4" s="73"/>
+      <c r="HR4" s="73"/>
+      <c r="HS4" s="73"/>
+      <c r="HT4" s="73"/>
+      <c r="HU4" s="73"/>
+      <c r="HV4" s="73"/>
+      <c r="HW4" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="92"/>
-      <c r="HY4" s="92"/>
-      <c r="HZ4" s="92"/>
-      <c r="IA4" s="92"/>
-      <c r="IB4" s="92"/>
-      <c r="IC4" s="92"/>
-      <c r="ID4" s="92"/>
-      <c r="IE4" s="92"/>
-      <c r="IF4" s="92"/>
-      <c r="IG4" s="92"/>
-      <c r="IH4" s="92"/>
-      <c r="II4" s="92"/>
-      <c r="IJ4" s="92"/>
-      <c r="IK4" s="92" t="s">
+      <c r="HX4" s="90"/>
+      <c r="HY4" s="90"/>
+      <c r="HZ4" s="90"/>
+      <c r="IA4" s="90"/>
+      <c r="IB4" s="90"/>
+      <c r="IC4" s="90"/>
+      <c r="ID4" s="90"/>
+      <c r="IE4" s="90"/>
+      <c r="IF4" s="90"/>
+      <c r="IG4" s="90"/>
+      <c r="IH4" s="90"/>
+      <c r="II4" s="90"/>
+      <c r="IJ4" s="90"/>
+      <c r="IK4" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="92"/>
-      <c r="IM4" s="92"/>
-      <c r="IN4" s="92"/>
-      <c r="IO4" s="92"/>
-      <c r="IP4" s="92"/>
-      <c r="IQ4" s="92"/>
-      <c r="IR4" s="92"/>
-      <c r="IS4" s="92"/>
-      <c r="IT4" s="92"/>
-      <c r="IU4" s="92"/>
-      <c r="IV4" s="92"/>
-      <c r="IW4" s="92"/>
-      <c r="IX4" s="92"/>
-      <c r="IY4" s="92" t="s">
+      <c r="IL4" s="90"/>
+      <c r="IM4" s="90"/>
+      <c r="IN4" s="90"/>
+      <c r="IO4" s="90"/>
+      <c r="IP4" s="90"/>
+      <c r="IQ4" s="90"/>
+      <c r="IR4" s="90"/>
+      <c r="IS4" s="90"/>
+      <c r="IT4" s="90"/>
+      <c r="IU4" s="90"/>
+      <c r="IV4" s="90"/>
+      <c r="IW4" s="90"/>
+      <c r="IX4" s="90"/>
+      <c r="IY4" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="92"/>
-      <c r="JA4" s="92"/>
-      <c r="JB4" s="92"/>
-      <c r="JC4" s="92"/>
-      <c r="JD4" s="92"/>
-      <c r="JE4" s="92"/>
-      <c r="JF4" s="92"/>
-      <c r="JG4" s="92"/>
-      <c r="JH4" s="92"/>
-      <c r="JI4" s="92"/>
-      <c r="JJ4" s="92"/>
-      <c r="JK4" s="92"/>
-      <c r="JL4" s="92"/>
-      <c r="JM4" s="93" t="s">
+      <c r="IZ4" s="90"/>
+      <c r="JA4" s="90"/>
+      <c r="JB4" s="90"/>
+      <c r="JC4" s="90"/>
+      <c r="JD4" s="90"/>
+      <c r="JE4" s="90"/>
+      <c r="JF4" s="90"/>
+      <c r="JG4" s="90"/>
+      <c r="JH4" s="90"/>
+      <c r="JI4" s="90"/>
+      <c r="JJ4" s="90"/>
+      <c r="JK4" s="90"/>
+      <c r="JL4" s="90"/>
+      <c r="JM4" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="93"/>
-      <c r="JO4" s="93"/>
-      <c r="JP4" s="93"/>
-      <c r="JQ4" s="93"/>
-      <c r="JR4" s="93"/>
-      <c r="JS4" s="93"/>
-      <c r="JT4" s="93"/>
-      <c r="JU4" s="93"/>
-      <c r="JV4" s="93"/>
-      <c r="JW4" s="93"/>
-      <c r="JX4" s="93"/>
-      <c r="JY4" s="93"/>
-      <c r="JZ4" s="90" t="s">
+      <c r="JN4" s="91"/>
+      <c r="JO4" s="91"/>
+      <c r="JP4" s="91"/>
+      <c r="JQ4" s="91"/>
+      <c r="JR4" s="91"/>
+      <c r="JS4" s="91"/>
+      <c r="JT4" s="91"/>
+      <c r="JU4" s="91"/>
+      <c r="JV4" s="91"/>
+      <c r="JW4" s="91"/>
+      <c r="JX4" s="91"/>
+      <c r="JY4" s="91"/>
+      <c r="JZ4" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="91"/>
-      <c r="KB4" s="91"/>
-      <c r="KC4" s="91"/>
-      <c r="KD4" s="91"/>
-      <c r="KE4" s="91"/>
-      <c r="KF4" s="91"/>
-      <c r="KG4" s="91"/>
-      <c r="KH4" s="86" t="s">
+      <c r="KA4" s="89"/>
+      <c r="KB4" s="89"/>
+      <c r="KC4" s="89"/>
+      <c r="KD4" s="89"/>
+      <c r="KE4" s="89"/>
+      <c r="KF4" s="89"/>
+      <c r="KG4" s="89"/>
+      <c r="KH4" s="84" t="s">
         <v>316</v>
       </c>
-      <c r="KI4" s="87"/>
-      <c r="KJ4" s="87"/>
+      <c r="KI4" s="85"/>
+      <c r="KJ4" s="85"/>
       <c r="KK4" s="46"/>
     </row>
-    <row r="5" spans="1:300" ht="12" customHeight="1">
-      <c r="A5" s="68"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="71"/>
-      <c r="R5" s="71"/>
-      <c r="S5" s="71"/>
-      <c r="T5" s="71"/>
-      <c r="U5" s="72"/>
-      <c r="V5" s="72"/>
-      <c r="W5" s="72"/>
-      <c r="X5" s="72"/>
-      <c r="Y5" s="72"/>
-      <c r="Z5" s="72"/>
-      <c r="AA5" s="72"/>
-      <c r="AB5" s="72"/>
-      <c r="AC5" s="73"/>
-      <c r="AD5" s="73"/>
-      <c r="AE5" s="73"/>
-      <c r="AF5" s="73"/>
-      <c r="AG5" s="73"/>
-      <c r="AH5" s="73"/>
-      <c r="AI5" s="73"/>
-      <c r="AJ5" s="74"/>
-      <c r="AK5" s="74"/>
-      <c r="AL5" s="74"/>
-      <c r="AM5" s="65"/>
-      <c r="AN5" s="65"/>
-      <c r="AO5" s="76"/>
-      <c r="AP5" s="76"/>
-      <c r="AQ5" s="76"/>
-      <c r="AR5" s="76"/>
-      <c r="AS5" s="77"/>
-      <c r="AT5" s="77"/>
-      <c r="AU5" s="77"/>
-      <c r="AV5" s="77"/>
-      <c r="AW5" s="77"/>
-      <c r="AX5" s="77"/>
-      <c r="AY5" s="77"/>
-      <c r="AZ5" s="77"/>
-      <c r="BA5" s="77"/>
-      <c r="BB5" s="77"/>
-      <c r="BC5" s="77"/>
-      <c r="BD5" s="77"/>
-      <c r="BE5" s="77"/>
-      <c r="BF5" s="77"/>
-      <c r="BG5" s="77"/>
-      <c r="BH5" s="77"/>
-      <c r="BI5" s="77"/>
-      <c r="BJ5" s="77"/>
+    <row r="5" spans="1:297" customFormat="false" ht="12" customHeight="1">
+      <c r="A5" s="66"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="70"/>
+      <c r="X5" s="70"/>
+      <c r="Y5" s="70"/>
+      <c r="Z5" s="70"/>
+      <c r="AA5" s="70"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="71"/>
+      <c r="AD5" s="71"/>
+      <c r="AE5" s="71"/>
+      <c r="AF5" s="71"/>
+      <c r="AG5" s="71"/>
+      <c r="AH5" s="71"/>
+      <c r="AI5" s="71"/>
+      <c r="AJ5" s="72"/>
+      <c r="AK5" s="72"/>
+      <c r="AL5" s="72"/>
+      <c r="AM5" s="63"/>
+      <c r="AN5" s="63"/>
+      <c r="AO5" s="74"/>
+      <c r="AP5" s="74"/>
+      <c r="AQ5" s="74"/>
+      <c r="AR5" s="74"/>
+      <c r="AS5" s="75"/>
+      <c r="AT5" s="75"/>
+      <c r="AU5" s="75"/>
+      <c r="AV5" s="75"/>
+      <c r="AW5" s="75"/>
+      <c r="AX5" s="75"/>
+      <c r="AY5" s="75"/>
+      <c r="AZ5" s="75"/>
+      <c r="BA5" s="75"/>
+      <c r="BB5" s="75"/>
+      <c r="BC5" s="75"/>
+      <c r="BD5" s="75"/>
+      <c r="BE5" s="75"/>
+      <c r="BF5" s="75"/>
+      <c r="BG5" s="75"/>
+      <c r="BH5" s="75"/>
+      <c r="BI5" s="75"/>
+      <c r="BJ5" s="75"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -4087,37 +4063,37 @@
       <c r="JL5" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="JM5" s="93"/>
-      <c r="JN5" s="93"/>
-      <c r="JO5" s="93"/>
-      <c r="JP5" s="93"/>
-      <c r="JQ5" s="93"/>
-      <c r="JR5" s="93"/>
-      <c r="JS5" s="93"/>
-      <c r="JT5" s="93"/>
-      <c r="JU5" s="93"/>
-      <c r="JV5" s="93"/>
-      <c r="JW5" s="93"/>
-      <c r="JX5" s="93"/>
-      <c r="JY5" s="93"/>
-      <c r="JZ5" s="91" t="s">
-        <v>347</v>
-      </c>
-      <c r="KA5" s="91"/>
-      <c r="KB5" s="91"/>
-      <c r="KC5" s="91"/>
-      <c r="KD5" s="91" t="s">
+      <c r="JM5" s="91"/>
+      <c r="JN5" s="91"/>
+      <c r="JO5" s="91"/>
+      <c r="JP5" s="91"/>
+      <c r="JQ5" s="91"/>
+      <c r="JR5" s="91"/>
+      <c r="JS5" s="91"/>
+      <c r="JT5" s="91"/>
+      <c r="JU5" s="91"/>
+      <c r="JV5" s="91"/>
+      <c r="JW5" s="91"/>
+      <c r="JX5" s="91"/>
+      <c r="JY5" s="91"/>
+      <c r="JZ5" s="89" t="s">
+        <v>342</v>
+      </c>
+      <c r="KA5" s="89"/>
+      <c r="KB5" s="89"/>
+      <c r="KC5" s="89"/>
+      <c r="KD5" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="91"/>
-      <c r="KF5" s="91"/>
-      <c r="KG5" s="91"/>
-      <c r="KH5" s="88"/>
-      <c r="KI5" s="89"/>
-      <c r="KJ5" s="89"/>
+      <c r="KE5" s="89"/>
+      <c r="KF5" s="89"/>
+      <c r="KG5" s="89"/>
+      <c r="KH5" s="86"/>
+      <c r="KI5" s="87"/>
+      <c r="KJ5" s="87"/>
       <c r="KK5" s="46"/>
     </row>
-    <row r="6" spans="1:300" ht="81.75" customHeight="1">
+    <row r="6" spans="1:299" customFormat="false" ht="81.75" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -4974,16 +4950,16 @@
         <v>308</v>
       </c>
       <c r="JZ6" s="22" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="KA6" s="29" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="KB6" s="22" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="KC6" s="22" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="KD6" s="22" t="s">
         <v>309</v>
@@ -5009,1660 +4985,446 @@
       <c r="KK6" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="KL6" s="49" t="s">
+      <c r="KL6" s="48"/>
+      <c r="KM6" s="49"/>
+    </row>
+    <row r="7" spans="1:297" customFormat="false" ht="15" customHeight="1">
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50" t="s">
         <v>336</v>
       </c>
-      <c r="KM6" s="50"/>
-      <c r="KN6" s="51"/>
-    </row>
-    <row r="7" spans="1:300" ht="15" customHeight="1">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52" t="s">
-        <v>341</v>
-      </c>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="54" t="s">
-        <v>341</v>
-      </c>
-      <c r="S7" s="54" t="s">
-        <v>341</v>
-      </c>
-      <c r="T7" s="54"/>
-      <c r="U7" s="54"/>
-      <c r="V7" s="54"/>
-      <c r="W7" s="54"/>
-      <c r="X7" s="55" t="s">
-        <v>341</v>
-      </c>
-      <c r="Y7" s="55" t="s">
-        <v>341</v>
-      </c>
-      <c r="Z7" s="54"/>
-      <c r="AA7" s="54"/>
-      <c r="AB7" s="55"/>
-      <c r="AC7" s="56"/>
-      <c r="AD7" s="57"/>
-      <c r="AE7" s="57"/>
-      <c r="AF7" s="58"/>
-      <c r="AG7" s="58"/>
-      <c r="AH7" s="59"/>
-      <c r="AI7" s="58"/>
-      <c r="AJ7" s="53" t="s">
-        <v>341</v>
-      </c>
-      <c r="AK7" s="53" t="s">
-        <v>341</v>
-      </c>
-      <c r="AL7" s="53" t="s">
-        <v>341</v>
-      </c>
-      <c r="AM7" s="54"/>
-      <c r="AN7" s="60"/>
-      <c r="AO7" s="61"/>
-      <c r="AP7" s="61"/>
-      <c r="AQ7" s="61"/>
-      <c r="AR7" s="61"/>
-      <c r="AS7" s="62">
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="52" t="s">
+        <v>336</v>
+      </c>
+      <c r="S7" s="52" t="s">
+        <v>336</v>
+      </c>
+      <c r="T7" s="52"/>
+      <c r="U7" s="52"/>
+      <c r="V7" s="52"/>
+      <c r="W7" s="52"/>
+      <c r="X7" s="53" t="s">
+        <v>336</v>
+      </c>
+      <c r="Y7" s="53" t="s">
+        <v>336</v>
+      </c>
+      <c r="Z7" s="52"/>
+      <c r="AA7" s="52"/>
+      <c r="AB7" s="53"/>
+      <c r="AC7" s="54"/>
+      <c r="AD7" s="55"/>
+      <c r="AE7" s="55"/>
+      <c r="AF7" s="56"/>
+      <c r="AG7" s="56"/>
+      <c r="AH7" s="57"/>
+      <c r="AI7" s="56"/>
+      <c r="AJ7" s="51" t="s">
+        <v>336</v>
+      </c>
+      <c r="AK7" s="51" t="s">
+        <v>336</v>
+      </c>
+      <c r="AL7" s="51" t="s">
+        <v>336</v>
+      </c>
+      <c r="AM7" s="52"/>
+      <c r="AN7" s="58"/>
+      <c r="AO7" s="59"/>
+      <c r="AP7" s="59"/>
+      <c r="AQ7" s="59"/>
+      <c r="AR7" s="59"/>
+      <c r="AS7" s="60">
         <f>SUM(BK7:BX7)</f>
         <v>0</v>
       </c>
-      <c r="AT7" s="63">
+      <c r="AT7" s="61">
         <f>SUM(BY7:CL7)</f>
         <v>0</v>
       </c>
-      <c r="AU7" s="63">
+      <c r="AU7" s="61">
         <f>SUM(CM7:CZ7)</f>
         <v>0</v>
       </c>
-      <c r="AV7" s="63">
+      <c r="AV7" s="61">
         <f>SUM(DA7:DN7)</f>
         <v>0</v>
       </c>
-      <c r="AW7" s="63">
+      <c r="AW7" s="61">
         <f>SUM(DO7:EB7)</f>
         <v>0</v>
       </c>
-      <c r="AX7" s="63">
+      <c r="AX7" s="61">
         <f>SUM(EC7:EP7)</f>
         <v>0</v>
       </c>
-      <c r="AY7" s="63">
+      <c r="AY7" s="61">
         <f>SUM(EQ7:FD7)</f>
         <v>0</v>
       </c>
-      <c r="AZ7" s="63">
+      <c r="AZ7" s="61">
         <f>SUM(FE7:FR7)</f>
         <v>0</v>
       </c>
-      <c r="BA7" s="63">
+      <c r="BA7" s="61">
         <f>SUM(FS7:GF7)</f>
         <v>0</v>
       </c>
-      <c r="BB7" s="63">
+      <c r="BB7" s="61">
         <f>SUM(GG7:GT7)</f>
         <v>0</v>
       </c>
-      <c r="BC7" s="63">
+      <c r="BC7" s="61">
         <f>SUM(GU7:HH7)</f>
         <v>0</v>
       </c>
-      <c r="BD7" s="63">
+      <c r="BD7" s="61">
         <f>SUM(HI7:HV7)</f>
         <v>0</v>
       </c>
-      <c r="BE7" s="63">
+      <c r="BE7" s="61">
         <f>SUM(HW7:IJ7)</f>
         <v>0</v>
       </c>
-      <c r="BF7" s="63">
+      <c r="BF7" s="61">
         <f>SUM(IK7:IX7)</f>
         <v>0</v>
       </c>
-      <c r="BG7" s="63">
+      <c r="BG7" s="61">
         <f>SUM(IY7:JL7)</f>
         <v>0</v>
       </c>
-      <c r="BH7" s="63">
+      <c r="BH7" s="61">
         <f t="shared" ref="BH7" si="0">JM7</f>
         <v>0</v>
       </c>
-      <c r="BI7" s="63">
+      <c r="BI7" s="61">
         <f>JN7</f>
         <v>0</v>
       </c>
-      <c r="BJ7" s="63">
+      <c r="BJ7" s="61">
         <f>JO7</f>
         <v>0</v>
       </c>
-      <c r="BK7" s="63">
+      <c r="BK7" s="61">
         <f t="shared" ref="BK7:BX7" si="1">BY7+CM7+DA7+DO7+EC7+EQ7+FE7+FS7</f>
         <v>0</v>
       </c>
-      <c r="BL7" s="63">
+      <c r="BL7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BM7" s="63">
+      <c r="BM7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BN7" s="63">
+      <c r="BN7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BO7" s="63">
+      <c r="BO7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BP7" s="63">
+      <c r="BP7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BQ7" s="63">
+      <c r="BQ7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BR7" s="63">
+      <c r="BR7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BS7" s="63">
+      <c r="BS7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BT7" s="63">
+      <c r="BT7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BU7" s="63">
+      <c r="BU7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BV7" s="63">
+      <c r="BV7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BW7" s="63">
+      <c r="BW7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BX7" s="63">
+      <c r="BX7" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BY7" s="58"/>
-      <c r="BZ7" s="58"/>
-      <c r="CA7" s="58"/>
-      <c r="CB7" s="58"/>
-      <c r="CC7" s="58"/>
-      <c r="CD7" s="58"/>
-      <c r="CE7" s="58"/>
-      <c r="CF7" s="58"/>
-      <c r="CG7" s="58"/>
-      <c r="CH7" s="58"/>
-      <c r="CI7" s="58"/>
-      <c r="CJ7" s="58"/>
-      <c r="CK7" s="58"/>
-      <c r="CL7" s="58"/>
-      <c r="CM7" s="58"/>
-      <c r="CN7" s="58"/>
-      <c r="CO7" s="58"/>
-      <c r="CP7" s="58"/>
-      <c r="CQ7" s="58"/>
-      <c r="CR7" s="58"/>
-      <c r="CS7" s="58"/>
-      <c r="CT7" s="58"/>
-      <c r="CU7" s="58"/>
-      <c r="CV7" s="58"/>
-      <c r="CW7" s="58"/>
-      <c r="CX7" s="58"/>
-      <c r="CY7" s="58"/>
-      <c r="CZ7" s="58"/>
-      <c r="DA7" s="58"/>
-      <c r="DB7" s="58"/>
-      <c r="DC7" s="58"/>
-      <c r="DD7" s="58"/>
-      <c r="DE7" s="58"/>
-      <c r="DF7" s="58"/>
-      <c r="DG7" s="58"/>
-      <c r="DH7" s="58"/>
-      <c r="DI7" s="58"/>
-      <c r="DJ7" s="58"/>
-      <c r="DK7" s="58"/>
-      <c r="DL7" s="58"/>
-      <c r="DM7" s="58"/>
-      <c r="DN7" s="58"/>
-      <c r="DO7" s="58"/>
-      <c r="DP7" s="58"/>
-      <c r="DQ7" s="58"/>
-      <c r="DR7" s="58"/>
-      <c r="DS7" s="58"/>
-      <c r="DT7" s="58"/>
-      <c r="DU7" s="58"/>
-      <c r="DV7" s="58"/>
-      <c r="DW7" s="58"/>
-      <c r="DX7" s="58"/>
-      <c r="DY7" s="58"/>
-      <c r="DZ7" s="58"/>
-      <c r="EA7" s="58"/>
-      <c r="EB7" s="58"/>
-      <c r="EC7" s="58"/>
-      <c r="ED7" s="58"/>
-      <c r="EE7" s="58"/>
-      <c r="EF7" s="58"/>
-      <c r="EG7" s="58"/>
-      <c r="EH7" s="58"/>
-      <c r="EI7" s="58"/>
-      <c r="EJ7" s="58"/>
-      <c r="EK7" s="58"/>
-      <c r="EL7" s="58"/>
-      <c r="EM7" s="58"/>
-      <c r="EN7" s="58"/>
-      <c r="EO7" s="58"/>
-      <c r="EP7" s="58"/>
-      <c r="EQ7" s="58"/>
-      <c r="ER7" s="58"/>
-      <c r="ES7" s="58"/>
-      <c r="ET7" s="58"/>
-      <c r="EU7" s="58"/>
-      <c r="EV7" s="58"/>
-      <c r="EW7" s="58"/>
-      <c r="EX7" s="58"/>
-      <c r="EY7" s="58"/>
-      <c r="EZ7" s="58"/>
-      <c r="FA7" s="58"/>
-      <c r="FB7" s="58"/>
-      <c r="FC7" s="58"/>
-      <c r="FD7" s="58"/>
-      <c r="FE7" s="58"/>
-      <c r="FF7" s="58"/>
-      <c r="FG7" s="58"/>
-      <c r="FH7" s="58"/>
-      <c r="FI7" s="58"/>
-      <c r="FJ7" s="58"/>
-      <c r="FK7" s="58"/>
-      <c r="FL7" s="58"/>
-      <c r="FM7" s="58"/>
-      <c r="FN7" s="58"/>
-      <c r="FO7" s="58"/>
-      <c r="FP7" s="58"/>
-      <c r="FQ7" s="58"/>
-      <c r="FR7" s="58"/>
-      <c r="FS7" s="58"/>
-      <c r="FT7" s="58"/>
-      <c r="FU7" s="58"/>
-      <c r="FV7" s="58"/>
-      <c r="FW7" s="58"/>
-      <c r="FX7" s="58"/>
-      <c r="FY7" s="58"/>
-      <c r="FZ7" s="58"/>
-      <c r="GA7" s="58"/>
-      <c r="GB7" s="58"/>
-      <c r="GC7" s="58"/>
-      <c r="GD7" s="58"/>
-      <c r="GE7" s="58"/>
-      <c r="GF7" s="58"/>
-      <c r="GG7" s="58"/>
-      <c r="GH7" s="58"/>
-      <c r="GI7" s="58"/>
-      <c r="GJ7" s="58"/>
-      <c r="GK7" s="58"/>
-      <c r="GL7" s="58"/>
-      <c r="GM7" s="58"/>
-      <c r="GN7" s="58"/>
-      <c r="GO7" s="58"/>
-      <c r="GP7" s="58"/>
-      <c r="GQ7" s="58"/>
-      <c r="GR7" s="58"/>
-      <c r="GS7" s="58"/>
-      <c r="GT7" s="58"/>
-      <c r="GU7" s="58"/>
-      <c r="GV7" s="58"/>
-      <c r="GW7" s="58"/>
-      <c r="GX7" s="58"/>
-      <c r="GY7" s="58"/>
-      <c r="GZ7" s="58"/>
-      <c r="HA7" s="58"/>
-      <c r="HB7" s="58"/>
-      <c r="HC7" s="58"/>
-      <c r="HD7" s="58"/>
-      <c r="HE7" s="58"/>
-      <c r="HF7" s="58"/>
-      <c r="HG7" s="58"/>
-      <c r="HH7" s="58"/>
-      <c r="HI7" s="58"/>
-      <c r="HJ7" s="58"/>
-      <c r="HK7" s="58"/>
-      <c r="HL7" s="58"/>
-      <c r="HM7" s="58"/>
-      <c r="HN7" s="58"/>
-      <c r="HO7" s="58"/>
-      <c r="HP7" s="58"/>
-      <c r="HQ7" s="58"/>
-      <c r="HR7" s="58"/>
-      <c r="HS7" s="58"/>
-      <c r="HT7" s="58"/>
-      <c r="HU7" s="58"/>
-      <c r="HV7" s="58"/>
-      <c r="HW7" s="58"/>
-      <c r="HX7" s="58"/>
-      <c r="HY7" s="58"/>
-      <c r="HZ7" s="58"/>
-      <c r="IA7" s="58"/>
-      <c r="IB7" s="58"/>
-      <c r="IC7" s="58"/>
-      <c r="ID7" s="58"/>
-      <c r="IE7" s="58"/>
-      <c r="IF7" s="58"/>
-      <c r="IG7" s="58"/>
-      <c r="IH7" s="58"/>
-      <c r="II7" s="58"/>
-      <c r="IJ7" s="58"/>
-      <c r="IK7" s="58"/>
-      <c r="IL7" s="58"/>
-      <c r="IM7" s="58"/>
-      <c r="IN7" s="58"/>
-      <c r="IO7" s="58"/>
-      <c r="IP7" s="58"/>
-      <c r="IQ7" s="58"/>
-      <c r="IR7" s="58"/>
-      <c r="IS7" s="58"/>
-      <c r="IT7" s="58"/>
-      <c r="IU7" s="58"/>
-      <c r="IV7" s="58"/>
-      <c r="IW7" s="58"/>
-      <c r="IX7" s="58"/>
-      <c r="IY7" s="58"/>
-      <c r="IZ7" s="58"/>
-      <c r="JA7" s="58"/>
-      <c r="JB7" s="58"/>
-      <c r="JC7" s="58"/>
-      <c r="JD7" s="58"/>
-      <c r="JE7" s="58"/>
-      <c r="JF7" s="58"/>
-      <c r="JG7" s="58"/>
-      <c r="JH7" s="58"/>
-      <c r="JI7" s="58"/>
-      <c r="JJ7" s="58"/>
-      <c r="JK7" s="58"/>
-      <c r="JL7" s="58"/>
-      <c r="JM7" s="58"/>
-      <c r="JN7" s="58"/>
-      <c r="JO7" s="58"/>
-      <c r="JP7" s="53"/>
-      <c r="JQ7" s="53"/>
-      <c r="JR7" s="53"/>
-      <c r="JS7" s="64"/>
-      <c r="JT7" s="64"/>
-      <c r="JU7" s="64"/>
-      <c r="JV7" s="64"/>
-      <c r="JW7" s="64"/>
-      <c r="JX7" s="64"/>
-      <c r="JY7" s="64"/>
-      <c r="JZ7" s="63">
+      <c r="BY7" s="56"/>
+      <c r="BZ7" s="56"/>
+      <c r="CA7" s="56"/>
+      <c r="CB7" s="56"/>
+      <c r="CC7" s="56"/>
+      <c r="CD7" s="56"/>
+      <c r="CE7" s="56"/>
+      <c r="CF7" s="56"/>
+      <c r="CG7" s="56"/>
+      <c r="CH7" s="56"/>
+      <c r="CI7" s="56"/>
+      <c r="CJ7" s="56"/>
+      <c r="CK7" s="56"/>
+      <c r="CL7" s="56"/>
+      <c r="CM7" s="56"/>
+      <c r="CN7" s="56"/>
+      <c r="CO7" s="56"/>
+      <c r="CP7" s="56"/>
+      <c r="CQ7" s="56"/>
+      <c r="CR7" s="56"/>
+      <c r="CS7" s="56"/>
+      <c r="CT7" s="56"/>
+      <c r="CU7" s="56"/>
+      <c r="CV7" s="56"/>
+      <c r="CW7" s="56"/>
+      <c r="CX7" s="56"/>
+      <c r="CY7" s="56"/>
+      <c r="CZ7" s="56"/>
+      <c r="DA7" s="56"/>
+      <c r="DB7" s="56"/>
+      <c r="DC7" s="56"/>
+      <c r="DD7" s="56"/>
+      <c r="DE7" s="56"/>
+      <c r="DF7" s="56"/>
+      <c r="DG7" s="56"/>
+      <c r="DH7" s="56"/>
+      <c r="DI7" s="56"/>
+      <c r="DJ7" s="56"/>
+      <c r="DK7" s="56"/>
+      <c r="DL7" s="56"/>
+      <c r="DM7" s="56"/>
+      <c r="DN7" s="56"/>
+      <c r="DO7" s="56"/>
+      <c r="DP7" s="56"/>
+      <c r="DQ7" s="56"/>
+      <c r="DR7" s="56"/>
+      <c r="DS7" s="56"/>
+      <c r="DT7" s="56"/>
+      <c r="DU7" s="56"/>
+      <c r="DV7" s="56"/>
+      <c r="DW7" s="56"/>
+      <c r="DX7" s="56"/>
+      <c r="DY7" s="56"/>
+      <c r="DZ7" s="56"/>
+      <c r="EA7" s="56"/>
+      <c r="EB7" s="56"/>
+      <c r="EC7" s="56"/>
+      <c r="ED7" s="56"/>
+      <c r="EE7" s="56"/>
+      <c r="EF7" s="56"/>
+      <c r="EG7" s="56"/>
+      <c r="EH7" s="56"/>
+      <c r="EI7" s="56"/>
+      <c r="EJ7" s="56"/>
+      <c r="EK7" s="56"/>
+      <c r="EL7" s="56"/>
+      <c r="EM7" s="56"/>
+      <c r="EN7" s="56"/>
+      <c r="EO7" s="56"/>
+      <c r="EP7" s="56"/>
+      <c r="EQ7" s="56"/>
+      <c r="ER7" s="56"/>
+      <c r="ES7" s="56"/>
+      <c r="ET7" s="56"/>
+      <c r="EU7" s="56"/>
+      <c r="EV7" s="56"/>
+      <c r="EW7" s="56"/>
+      <c r="EX7" s="56"/>
+      <c r="EY7" s="56"/>
+      <c r="EZ7" s="56"/>
+      <c r="FA7" s="56"/>
+      <c r="FB7" s="56"/>
+      <c r="FC7" s="56"/>
+      <c r="FD7" s="56"/>
+      <c r="FE7" s="56"/>
+      <c r="FF7" s="56"/>
+      <c r="FG7" s="56"/>
+      <c r="FH7" s="56"/>
+      <c r="FI7" s="56"/>
+      <c r="FJ7" s="56"/>
+      <c r="FK7" s="56"/>
+      <c r="FL7" s="56"/>
+      <c r="FM7" s="56"/>
+      <c r="FN7" s="56"/>
+      <c r="FO7" s="56"/>
+      <c r="FP7" s="56"/>
+      <c r="FQ7" s="56"/>
+      <c r="FR7" s="56"/>
+      <c r="FS7" s="56"/>
+      <c r="FT7" s="56"/>
+      <c r="FU7" s="56"/>
+      <c r="FV7" s="56"/>
+      <c r="FW7" s="56"/>
+      <c r="FX7" s="56"/>
+      <c r="FY7" s="56"/>
+      <c r="FZ7" s="56"/>
+      <c r="GA7" s="56"/>
+      <c r="GB7" s="56"/>
+      <c r="GC7" s="56"/>
+      <c r="GD7" s="56"/>
+      <c r="GE7" s="56"/>
+      <c r="GF7" s="56"/>
+      <c r="GG7" s="56"/>
+      <c r="GH7" s="56"/>
+      <c r="GI7" s="56"/>
+      <c r="GJ7" s="56"/>
+      <c r="GK7" s="56"/>
+      <c r="GL7" s="56"/>
+      <c r="GM7" s="56"/>
+      <c r="GN7" s="56"/>
+      <c r="GO7" s="56"/>
+      <c r="GP7" s="56"/>
+      <c r="GQ7" s="56"/>
+      <c r="GR7" s="56"/>
+      <c r="GS7" s="56"/>
+      <c r="GT7" s="56"/>
+      <c r="GU7" s="56"/>
+      <c r="GV7" s="56"/>
+      <c r="GW7" s="56"/>
+      <c r="GX7" s="56"/>
+      <c r="GY7" s="56"/>
+      <c r="GZ7" s="56"/>
+      <c r="HA7" s="56"/>
+      <c r="HB7" s="56"/>
+      <c r="HC7" s="56"/>
+      <c r="HD7" s="56"/>
+      <c r="HE7" s="56"/>
+      <c r="HF7" s="56"/>
+      <c r="HG7" s="56"/>
+      <c r="HH7" s="56"/>
+      <c r="HI7" s="56"/>
+      <c r="HJ7" s="56"/>
+      <c r="HK7" s="56"/>
+      <c r="HL7" s="56"/>
+      <c r="HM7" s="56"/>
+      <c r="HN7" s="56"/>
+      <c r="HO7" s="56"/>
+      <c r="HP7" s="56"/>
+      <c r="HQ7" s="56"/>
+      <c r="HR7" s="56"/>
+      <c r="HS7" s="56"/>
+      <c r="HT7" s="56"/>
+      <c r="HU7" s="56"/>
+      <c r="HV7" s="56"/>
+      <c r="HW7" s="56"/>
+      <c r="HX7" s="56"/>
+      <c r="HY7" s="56"/>
+      <c r="HZ7" s="56"/>
+      <c r="IA7" s="56"/>
+      <c r="IB7" s="56"/>
+      <c r="IC7" s="56"/>
+      <c r="ID7" s="56"/>
+      <c r="IE7" s="56"/>
+      <c r="IF7" s="56"/>
+      <c r="IG7" s="56"/>
+      <c r="IH7" s="56"/>
+      <c r="II7" s="56"/>
+      <c r="IJ7" s="56"/>
+      <c r="IK7" s="56"/>
+      <c r="IL7" s="56"/>
+      <c r="IM7" s="56"/>
+      <c r="IN7" s="56"/>
+      <c r="IO7" s="56"/>
+      <c r="IP7" s="56"/>
+      <c r="IQ7" s="56"/>
+      <c r="IR7" s="56"/>
+      <c r="IS7" s="56"/>
+      <c r="IT7" s="56"/>
+      <c r="IU7" s="56"/>
+      <c r="IV7" s="56"/>
+      <c r="IW7" s="56"/>
+      <c r="IX7" s="56"/>
+      <c r="IY7" s="56"/>
+      <c r="IZ7" s="56"/>
+      <c r="JA7" s="56"/>
+      <c r="JB7" s="56"/>
+      <c r="JC7" s="56"/>
+      <c r="JD7" s="56"/>
+      <c r="JE7" s="56"/>
+      <c r="JF7" s="56"/>
+      <c r="JG7" s="56"/>
+      <c r="JH7" s="56"/>
+      <c r="JI7" s="56"/>
+      <c r="JJ7" s="56"/>
+      <c r="JK7" s="56"/>
+      <c r="JL7" s="56"/>
+      <c r="JM7" s="56"/>
+      <c r="JN7" s="56"/>
+      <c r="JO7" s="56"/>
+      <c r="JP7" s="51"/>
+      <c r="JQ7" s="51"/>
+      <c r="JR7" s="51"/>
+      <c r="JS7" s="62"/>
+      <c r="JT7" s="62"/>
+      <c r="JU7" s="62"/>
+      <c r="JV7" s="62"/>
+      <c r="JW7" s="62"/>
+      <c r="JX7" s="62"/>
+      <c r="JY7" s="62"/>
+      <c r="JZ7" s="61">
         <f>BQ7</f>
         <v>0</v>
       </c>
-      <c r="KA7" s="63">
+      <c r="KA7" s="61">
         <f>CE7+CS7</f>
         <v>0</v>
       </c>
-      <c r="KB7" s="63">
+      <c r="KB7" s="61">
         <f>DG7+DU7+EI7+EW7+FK7+FY7</f>
         <v>0</v>
       </c>
-      <c r="KC7" s="63">
+      <c r="KC7" s="61">
         <f>GM7+IC7</f>
         <v>0</v>
       </c>
-      <c r="KD7" s="63">
+      <c r="KD7" s="61">
         <f>SUM(BL7:BQ7)</f>
         <v>0</v>
       </c>
-      <c r="KE7" s="63">
+      <c r="KE7" s="61">
         <f>SUM(CN7:CS7)+SUM(BZ7:CE7)</f>
         <v>0</v>
       </c>
-      <c r="KF7" s="63">
+      <c r="KF7" s="61">
         <f>SUM(DB7:DG7)+SUM(DP7:DU7)+SUM(ED7:EI7)+SUM(ER7:EW7)+SUM(FF7:FK7)+SUM(FT7:FY7)</f>
         <v>0</v>
       </c>
-      <c r="KG7" s="63">
+      <c r="KG7" s="61">
         <f>SUM(GH7:GM7)+SUM(HX7:IC7)</f>
         <v>0</v>
       </c>
-      <c r="KH7" s="48"/>
-      <c r="KI7" s="48"/>
-      <c r="KJ7" s="48"/>
-      <c r="KK7" s="48"/>
-      <c r="KL7" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="8" spans="1:300">
-      <c r="A8" s="25"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="26"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="26"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="26"/>
-      <c r="AE8" s="26"/>
-      <c r="AF8" s="23"/>
-      <c r="AG8" s="23"/>
-      <c r="AH8" s="23"/>
-      <c r="AI8" s="23"/>
-      <c r="AJ8" s="23"/>
-      <c r="AK8" s="23"/>
-      <c r="AL8" s="23"/>
-      <c r="AM8" s="23"/>
-      <c r="AN8" s="27"/>
-      <c r="AO8" s="27"/>
-      <c r="AP8" s="27"/>
-      <c r="AQ8" s="27"/>
-      <c r="AR8" s="27"/>
-      <c r="AS8" s="23"/>
-      <c r="AT8" s="23"/>
-      <c r="AU8" s="23"/>
-      <c r="AV8" s="23"/>
-      <c r="AW8" s="23"/>
-      <c r="AX8" s="23"/>
-      <c r="AY8" s="23"/>
-      <c r="AZ8" s="23"/>
-      <c r="BA8" s="23"/>
-      <c r="BB8" s="23"/>
-      <c r="BC8" s="23"/>
-      <c r="BD8" s="23"/>
-      <c r="BE8" s="23"/>
-      <c r="BF8" s="23"/>
-      <c r="BG8" s="23"/>
-      <c r="BH8" s="23"/>
-      <c r="BI8" s="23"/>
-      <c r="BJ8" s="23"/>
-      <c r="BK8" s="23"/>
-      <c r="BL8" s="23"/>
-      <c r="BM8" s="23"/>
-      <c r="BN8" s="23"/>
-      <c r="BO8" s="23"/>
-      <c r="BP8" s="23"/>
-      <c r="BQ8" s="23"/>
-      <c r="BR8" s="23"/>
-      <c r="BS8" s="23"/>
-      <c r="BT8" s="23"/>
-      <c r="BU8" s="23"/>
-      <c r="BV8" s="23"/>
-      <c r="BW8" s="23"/>
-      <c r="BX8" s="23"/>
-      <c r="BY8" s="23"/>
-      <c r="BZ8" s="23"/>
-      <c r="CA8" s="23"/>
-      <c r="CB8" s="23"/>
-      <c r="CC8" s="23"/>
-      <c r="CD8" s="23"/>
-      <c r="CE8" s="23"/>
-      <c r="CF8" s="23"/>
-      <c r="CG8" s="23"/>
-      <c r="CH8" s="23"/>
-      <c r="CI8" s="23"/>
-      <c r="CJ8" s="23"/>
-      <c r="CK8" s="23"/>
-      <c r="CL8" s="23"/>
-      <c r="CM8" s="23"/>
-      <c r="CN8" s="23"/>
-      <c r="CO8" s="23"/>
-      <c r="CP8" s="23"/>
-      <c r="CQ8" s="23"/>
-      <c r="CR8" s="23"/>
-      <c r="CS8" s="23"/>
-      <c r="CT8" s="23"/>
-      <c r="CU8" s="23"/>
-      <c r="CV8" s="23"/>
-      <c r="CW8" s="23"/>
-      <c r="CX8" s="23"/>
-      <c r="CY8" s="23"/>
-      <c r="CZ8" s="23"/>
-      <c r="DA8" s="23"/>
-      <c r="DB8" s="23"/>
-      <c r="DC8" s="23"/>
-      <c r="DD8" s="23"/>
-      <c r="DE8" s="23"/>
-      <c r="DF8" s="23"/>
-      <c r="DG8" s="23"/>
-      <c r="DH8" s="23"/>
-      <c r="DI8" s="23"/>
-      <c r="DJ8" s="23"/>
-      <c r="DK8" s="23"/>
-      <c r="DL8" s="23"/>
-      <c r="DM8" s="23"/>
-      <c r="DN8" s="23"/>
-      <c r="DO8" s="23"/>
-      <c r="DP8" s="23"/>
-      <c r="DQ8" s="23"/>
-      <c r="DR8" s="23"/>
-      <c r="DS8" s="23"/>
-      <c r="DT8" s="23"/>
-      <c r="DU8" s="23"/>
-      <c r="DV8" s="23"/>
-      <c r="DW8" s="23"/>
-      <c r="DX8" s="23"/>
-      <c r="DY8" s="23"/>
-      <c r="DZ8" s="23"/>
-      <c r="EA8" s="23"/>
-      <c r="EB8" s="23"/>
-      <c r="EC8" s="23"/>
-      <c r="ED8" s="23"/>
-      <c r="EE8" s="23"/>
-      <c r="EF8" s="23"/>
-      <c r="EG8" s="23"/>
-      <c r="EH8" s="23"/>
-      <c r="EI8" s="23"/>
-      <c r="EJ8" s="23"/>
-      <c r="EK8" s="23"/>
-      <c r="EL8" s="23"/>
-      <c r="EM8" s="23"/>
-      <c r="EN8" s="23"/>
-      <c r="EO8" s="23"/>
-      <c r="EP8" s="23"/>
-      <c r="EQ8" s="23"/>
-      <c r="ER8" s="23"/>
-      <c r="ES8" s="23"/>
-      <c r="ET8" s="23"/>
-      <c r="EU8" s="23"/>
-      <c r="EV8" s="23"/>
-      <c r="EW8" s="23"/>
-      <c r="EX8" s="23"/>
-      <c r="EY8" s="23"/>
-      <c r="EZ8" s="23"/>
-      <c r="FA8" s="23"/>
-      <c r="FB8" s="23"/>
-      <c r="FC8" s="23"/>
-      <c r="FD8" s="23"/>
-      <c r="FE8" s="23"/>
-      <c r="FF8" s="23"/>
-      <c r="FG8" s="23"/>
-      <c r="FH8" s="23"/>
-      <c r="FI8" s="23"/>
-      <c r="FJ8" s="23"/>
-      <c r="FK8" s="23"/>
-      <c r="FL8" s="23"/>
-      <c r="FM8" s="23"/>
-      <c r="FN8" s="23"/>
-      <c r="FO8" s="23"/>
-      <c r="FP8" s="23"/>
-      <c r="FQ8" s="23"/>
-      <c r="FR8" s="23"/>
-      <c r="FS8" s="23"/>
-      <c r="FT8" s="23"/>
-      <c r="FU8" s="23"/>
-      <c r="FV8" s="23"/>
-      <c r="FW8" s="23"/>
-      <c r="FX8" s="23"/>
-      <c r="FY8" s="23"/>
-      <c r="FZ8" s="23"/>
-      <c r="GA8" s="23"/>
-      <c r="GB8" s="23"/>
-      <c r="GC8" s="23"/>
-      <c r="GD8" s="23"/>
-      <c r="GE8" s="23"/>
-      <c r="GF8" s="23"/>
-      <c r="GG8" s="23"/>
-      <c r="GH8" s="23"/>
-      <c r="GI8" s="23"/>
-      <c r="GJ8" s="23"/>
-      <c r="GK8" s="23"/>
-      <c r="GL8" s="23"/>
-      <c r="GM8" s="23"/>
-      <c r="GN8" s="23"/>
-      <c r="GO8" s="23"/>
-      <c r="GP8" s="23"/>
-      <c r="GQ8" s="23"/>
-      <c r="GR8" s="23"/>
-      <c r="GS8" s="23"/>
-      <c r="GT8" s="23"/>
-      <c r="GU8" s="23"/>
-      <c r="GV8" s="23"/>
-      <c r="GW8" s="23"/>
-      <c r="GX8" s="23"/>
-      <c r="GY8" s="23"/>
-      <c r="GZ8" s="23"/>
-      <c r="HA8" s="23"/>
-      <c r="HB8" s="23"/>
-      <c r="HC8" s="23"/>
-      <c r="HD8" s="23"/>
-      <c r="HE8" s="23"/>
-      <c r="HF8" s="23"/>
-      <c r="HG8" s="23"/>
-      <c r="HH8" s="23"/>
-      <c r="HI8" s="23"/>
-      <c r="HJ8" s="23"/>
-      <c r="HK8" s="23"/>
-      <c r="HL8" s="23"/>
-      <c r="HM8" s="23"/>
-      <c r="HN8" s="23"/>
-      <c r="HO8" s="23"/>
-      <c r="HP8" s="23"/>
-      <c r="HQ8" s="23"/>
-      <c r="HR8" s="23"/>
-      <c r="HS8" s="23"/>
-      <c r="HT8" s="23"/>
-      <c r="HU8" s="23"/>
-      <c r="HV8" s="23"/>
-      <c r="HW8" s="23"/>
-      <c r="HX8" s="23"/>
-      <c r="HY8" s="23"/>
-      <c r="HZ8" s="23"/>
-      <c r="IA8" s="23"/>
-      <c r="IB8" s="23"/>
-      <c r="IC8" s="23"/>
-      <c r="ID8" s="23"/>
-      <c r="IE8" s="23"/>
-      <c r="IF8" s="23"/>
-      <c r="IG8" s="23"/>
-      <c r="IH8" s="23"/>
-      <c r="II8" s="23"/>
-      <c r="IJ8" s="23"/>
-      <c r="IK8" s="23"/>
-      <c r="IL8" s="23"/>
-      <c r="IM8" s="23"/>
-      <c r="IN8" s="23"/>
-      <c r="IO8" s="23"/>
-      <c r="IP8" s="23"/>
-      <c r="IQ8" s="23"/>
-      <c r="IR8" s="23"/>
-      <c r="IS8" s="23"/>
-      <c r="IT8" s="23"/>
-      <c r="IU8" s="23"/>
-      <c r="IV8" s="23"/>
-      <c r="IW8" s="23"/>
-      <c r="IX8" s="23"/>
-      <c r="IY8" s="23"/>
-      <c r="IZ8" s="23"/>
-      <c r="JA8" s="23"/>
-      <c r="JB8" s="23"/>
-      <c r="JC8" s="23"/>
-      <c r="JD8" s="23"/>
-      <c r="JE8" s="23"/>
-      <c r="JF8" s="23"/>
-      <c r="JG8" s="23"/>
-      <c r="JH8" s="23"/>
-      <c r="JI8" s="23"/>
-      <c r="JJ8" s="23"/>
-      <c r="JK8" s="23"/>
-      <c r="JL8" s="23"/>
-      <c r="JM8" s="23"/>
-      <c r="JN8" s="23"/>
-      <c r="JO8" s="23"/>
-      <c r="JP8" s="23"/>
-      <c r="JQ8" s="23"/>
-      <c r="JR8" s="23"/>
-      <c r="JS8" s="47"/>
-      <c r="JT8" s="47"/>
-      <c r="JU8" s="47"/>
-      <c r="JV8" s="47"/>
-      <c r="JW8" s="47"/>
-      <c r="JX8" s="47"/>
-      <c r="JY8" s="47"/>
-      <c r="JZ8" s="23"/>
-      <c r="KA8" s="23"/>
-      <c r="KB8" s="23"/>
-      <c r="KC8" s="23"/>
-      <c r="KD8" s="23"/>
-      <c r="KE8" s="23"/>
-      <c r="KF8" s="23"/>
-      <c r="KG8" s="23"/>
-      <c r="KH8" s="48"/>
-      <c r="KI8" s="48"/>
-      <c r="KJ8" s="48"/>
-      <c r="KK8" s="48"/>
-      <c r="KL8" s="48" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="9" spans="1:300">
-      <c r="A9" s="25"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="26"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="23"/>
-      <c r="AD9" s="26"/>
-      <c r="AE9" s="26"/>
-      <c r="AF9" s="23"/>
-      <c r="AG9" s="23"/>
-      <c r="AH9" s="23"/>
-      <c r="AI9" s="23"/>
-      <c r="AJ9" s="23"/>
-      <c r="AK9" s="23"/>
-      <c r="AL9" s="23"/>
-      <c r="AM9" s="23"/>
-      <c r="AN9" s="27"/>
-      <c r="AO9" s="27"/>
-      <c r="AP9" s="27"/>
-      <c r="AQ9" s="27"/>
-      <c r="AR9" s="27"/>
-      <c r="AS9" s="23"/>
-      <c r="AT9" s="23"/>
-      <c r="AU9" s="23"/>
-      <c r="AV9" s="23"/>
-      <c r="AW9" s="23"/>
-      <c r="AX9" s="23"/>
-      <c r="AY9" s="23"/>
-      <c r="AZ9" s="23"/>
-      <c r="BA9" s="23"/>
-      <c r="BB9" s="23"/>
-      <c r="BC9" s="23"/>
-      <c r="BD9" s="23"/>
-      <c r="BE9" s="23"/>
-      <c r="BF9" s="23"/>
-      <c r="BG9" s="23"/>
-      <c r="BH9" s="23"/>
-      <c r="BI9" s="23"/>
-      <c r="BJ9" s="23"/>
-      <c r="BK9" s="23"/>
-      <c r="BL9" s="23"/>
-      <c r="BM9" s="23"/>
-      <c r="BN9" s="23"/>
-      <c r="BO9" s="23"/>
-      <c r="BP9" s="23"/>
-      <c r="BQ9" s="23"/>
-      <c r="BR9" s="23"/>
-      <c r="BS9" s="23"/>
-      <c r="BT9" s="23"/>
-      <c r="BU9" s="23"/>
-      <c r="BV9" s="23"/>
-      <c r="BW9" s="23"/>
-      <c r="BX9" s="23"/>
-      <c r="BY9" s="23"/>
-      <c r="BZ9" s="23"/>
-      <c r="CA9" s="23"/>
-      <c r="CB9" s="23"/>
-      <c r="CC9" s="23"/>
-      <c r="CD9" s="23"/>
-      <c r="CE9" s="23"/>
-      <c r="CF9" s="23"/>
-      <c r="CG9" s="23"/>
-      <c r="CH9" s="23"/>
-      <c r="CI9" s="23"/>
-      <c r="CJ9" s="23"/>
-      <c r="CK9" s="23"/>
-      <c r="CL9" s="23"/>
-      <c r="CM9" s="23"/>
-      <c r="CN9" s="23"/>
-      <c r="CO9" s="23"/>
-      <c r="CP9" s="23"/>
-      <c r="CQ9" s="23"/>
-      <c r="CR9" s="23"/>
-      <c r="CS9" s="23"/>
-      <c r="CT9" s="23"/>
-      <c r="CU9" s="23"/>
-      <c r="CV9" s="23"/>
-      <c r="CW9" s="23"/>
-      <c r="CX9" s="23"/>
-      <c r="CY9" s="23"/>
-      <c r="CZ9" s="23"/>
-      <c r="DA9" s="23"/>
-      <c r="DB9" s="23"/>
-      <c r="DC9" s="23"/>
-      <c r="DD9" s="23"/>
-      <c r="DE9" s="23"/>
-      <c r="DF9" s="23"/>
-      <c r="DG9" s="23"/>
-      <c r="DH9" s="23"/>
-      <c r="DI9" s="23"/>
-      <c r="DJ9" s="23"/>
-      <c r="DK9" s="23"/>
-      <c r="DL9" s="23"/>
-      <c r="DM9" s="23"/>
-      <c r="DN9" s="23"/>
-      <c r="DO9" s="23"/>
-      <c r="DP9" s="23"/>
-      <c r="DQ9" s="23"/>
-      <c r="DR9" s="23"/>
-      <c r="DS9" s="23"/>
-      <c r="DT9" s="23"/>
-      <c r="DU9" s="23"/>
-      <c r="DV9" s="23"/>
-      <c r="DW9" s="23"/>
-      <c r="DX9" s="23"/>
-      <c r="DY9" s="23"/>
-      <c r="DZ9" s="23"/>
-      <c r="EA9" s="23"/>
-      <c r="EB9" s="23"/>
-      <c r="EC9" s="23"/>
-      <c r="ED9" s="23"/>
-      <c r="EE9" s="23"/>
-      <c r="EF9" s="23"/>
-      <c r="EG9" s="23"/>
-      <c r="EH9" s="23"/>
-      <c r="EI9" s="23"/>
-      <c r="EJ9" s="23"/>
-      <c r="EK9" s="23"/>
-      <c r="EL9" s="23"/>
-      <c r="EM9" s="23"/>
-      <c r="EN9" s="23"/>
-      <c r="EO9" s="23"/>
-      <c r="EP9" s="23"/>
-      <c r="EQ9" s="23"/>
-      <c r="ER9" s="23"/>
-      <c r="ES9" s="23"/>
-      <c r="ET9" s="23"/>
-      <c r="EU9" s="23"/>
-      <c r="EV9" s="23"/>
-      <c r="EW9" s="23"/>
-      <c r="EX9" s="23"/>
-      <c r="EY9" s="23"/>
-      <c r="EZ9" s="23"/>
-      <c r="FA9" s="23"/>
-      <c r="FB9" s="23"/>
-      <c r="FC9" s="23"/>
-      <c r="FD9" s="23"/>
-      <c r="FE9" s="23"/>
-      <c r="FF9" s="23"/>
-      <c r="FG9" s="23"/>
-      <c r="FH9" s="23"/>
-      <c r="FI9" s="23"/>
-      <c r="FJ9" s="23"/>
-      <c r="FK9" s="23"/>
-      <c r="FL9" s="23"/>
-      <c r="FM9" s="23"/>
-      <c r="FN9" s="23"/>
-      <c r="FO9" s="23"/>
-      <c r="FP9" s="23"/>
-      <c r="FQ9" s="23"/>
-      <c r="FR9" s="23"/>
-      <c r="FS9" s="23"/>
-      <c r="FT9" s="23"/>
-      <c r="FU9" s="23"/>
-      <c r="FV9" s="23"/>
-      <c r="FW9" s="23"/>
-      <c r="FX9" s="23"/>
-      <c r="FY9" s="23"/>
-      <c r="FZ9" s="23"/>
-      <c r="GA9" s="23"/>
-      <c r="GB9" s="23"/>
-      <c r="GC9" s="23"/>
-      <c r="GD9" s="23"/>
-      <c r="GE9" s="23"/>
-      <c r="GF9" s="23"/>
-      <c r="GG9" s="23"/>
-      <c r="GH9" s="23"/>
-      <c r="GI9" s="23"/>
-      <c r="GJ9" s="23"/>
-      <c r="GK9" s="23"/>
-      <c r="GL9" s="23"/>
-      <c r="GM9" s="23"/>
-      <c r="GN9" s="23"/>
-      <c r="GO9" s="23"/>
-      <c r="GP9" s="23"/>
-      <c r="GQ9" s="23"/>
-      <c r="GR9" s="23"/>
-      <c r="GS9" s="23"/>
-      <c r="GT9" s="23"/>
-      <c r="GU9" s="23"/>
-      <c r="GV9" s="23"/>
-      <c r="GW9" s="23"/>
-      <c r="GX9" s="23"/>
-      <c r="GY9" s="23"/>
-      <c r="GZ9" s="23"/>
-      <c r="HA9" s="23"/>
-      <c r="HB9" s="23"/>
-      <c r="HC9" s="23"/>
-      <c r="HD9" s="23"/>
-      <c r="HE9" s="23"/>
-      <c r="HF9" s="23"/>
-      <c r="HG9" s="23"/>
-      <c r="HH9" s="23"/>
-      <c r="HI9" s="23"/>
-      <c r="HJ9" s="23"/>
-      <c r="HK9" s="23"/>
-      <c r="HL9" s="23"/>
-      <c r="HM9" s="23"/>
-      <c r="HN9" s="23"/>
-      <c r="HO9" s="23"/>
-      <c r="HP9" s="23"/>
-      <c r="HQ9" s="23"/>
-      <c r="HR9" s="23"/>
-      <c r="HS9" s="23"/>
-      <c r="HT9" s="23"/>
-      <c r="HU9" s="23"/>
-      <c r="HV9" s="23"/>
-      <c r="HW9" s="23"/>
-      <c r="HX9" s="23"/>
-      <c r="HY9" s="23"/>
-      <c r="HZ9" s="23"/>
-      <c r="IA9" s="23"/>
-      <c r="IB9" s="23"/>
-      <c r="IC9" s="23"/>
-      <c r="ID9" s="23"/>
-      <c r="IE9" s="23"/>
-      <c r="IF9" s="23"/>
-      <c r="IG9" s="23"/>
-      <c r="IH9" s="23"/>
-      <c r="II9" s="23"/>
-      <c r="IJ9" s="23"/>
-      <c r="IK9" s="23"/>
-      <c r="IL9" s="23"/>
-      <c r="IM9" s="23"/>
-      <c r="IN9" s="23"/>
-      <c r="IO9" s="23"/>
-      <c r="IP9" s="23"/>
-      <c r="IQ9" s="23"/>
-      <c r="IR9" s="23"/>
-      <c r="IS9" s="23"/>
-      <c r="IT9" s="23"/>
-      <c r="IU9" s="23"/>
-      <c r="IV9" s="23"/>
-      <c r="IW9" s="23"/>
-      <c r="IX9" s="23"/>
-      <c r="IY9" s="23"/>
-      <c r="IZ9" s="23"/>
-      <c r="JA9" s="23"/>
-      <c r="JB9" s="23"/>
-      <c r="JC9" s="23"/>
-      <c r="JD9" s="23"/>
-      <c r="JE9" s="23"/>
-      <c r="JF9" s="23"/>
-      <c r="JG9" s="23"/>
-      <c r="JH9" s="23"/>
-      <c r="JI9" s="23"/>
-      <c r="JJ9" s="23"/>
-      <c r="JK9" s="23"/>
-      <c r="JL9" s="23"/>
-      <c r="JM9" s="23"/>
-      <c r="JN9" s="23"/>
-      <c r="JO9" s="23"/>
-      <c r="JP9" s="23"/>
-      <c r="JQ9" s="23"/>
-      <c r="JR9" s="23"/>
-      <c r="JS9" s="47"/>
-      <c r="JT9" s="47"/>
-      <c r="JU9" s="47"/>
-      <c r="JV9" s="47"/>
-      <c r="JW9" s="47"/>
-      <c r="JX9" s="47"/>
-      <c r="JY9" s="47"/>
-      <c r="JZ9" s="23"/>
-      <c r="KA9" s="23"/>
-      <c r="KB9" s="23"/>
-      <c r="KC9" s="23"/>
-      <c r="KD9" s="23"/>
-      <c r="KE9" s="23"/>
-      <c r="KF9" s="23"/>
-      <c r="KG9" s="23"/>
-      <c r="KH9" s="48"/>
-      <c r="KI9" s="48"/>
-      <c r="KJ9" s="48"/>
-      <c r="KK9" s="48"/>
-      <c r="KL9" s="48" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="10" spans="1:300">
-      <c r="A10" s="25"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="26"/>
-      <c r="Y10" s="26"/>
-      <c r="Z10" s="23"/>
-      <c r="AA10" s="23"/>
-      <c r="AB10" s="26"/>
-      <c r="AC10" s="23"/>
-      <c r="AD10" s="26"/>
-      <c r="AE10" s="26"/>
-      <c r="AF10" s="23"/>
-      <c r="AG10" s="23"/>
-      <c r="AH10" s="23"/>
-      <c r="AI10" s="23"/>
-      <c r="AJ10" s="23"/>
-      <c r="AK10" s="23"/>
-      <c r="AL10" s="23"/>
-      <c r="AM10" s="23"/>
-      <c r="AN10" s="27"/>
-      <c r="AO10" s="27"/>
-      <c r="AP10" s="27"/>
-      <c r="AQ10" s="27"/>
-      <c r="AR10" s="27"/>
-      <c r="AS10" s="23"/>
-      <c r="AT10" s="23"/>
-      <c r="AU10" s="23"/>
-      <c r="AV10" s="23"/>
-      <c r="AW10" s="23"/>
-      <c r="AX10" s="23"/>
-      <c r="AY10" s="23"/>
-      <c r="AZ10" s="23"/>
-      <c r="BA10" s="23"/>
-      <c r="BB10" s="23"/>
-      <c r="BC10" s="23"/>
-      <c r="BD10" s="23"/>
-      <c r="BE10" s="23"/>
-      <c r="BF10" s="23"/>
-      <c r="BG10" s="23"/>
-      <c r="BH10" s="23"/>
-      <c r="BI10" s="23"/>
-      <c r="BJ10" s="23"/>
-      <c r="BK10" s="23"/>
-      <c r="BL10" s="23"/>
-      <c r="BM10" s="23"/>
-      <c r="BN10" s="23"/>
-      <c r="BO10" s="23"/>
-      <c r="BP10" s="23"/>
-      <c r="BQ10" s="23"/>
-      <c r="BR10" s="23"/>
-      <c r="BS10" s="23"/>
-      <c r="BT10" s="23"/>
-      <c r="BU10" s="23"/>
-      <c r="BV10" s="23"/>
-      <c r="BW10" s="23"/>
-      <c r="BX10" s="23"/>
-      <c r="BY10" s="23"/>
-      <c r="BZ10" s="23"/>
-      <c r="CA10" s="23"/>
-      <c r="CB10" s="23"/>
-      <c r="CC10" s="23"/>
-      <c r="CD10" s="23"/>
-      <c r="CE10" s="23"/>
-      <c r="CF10" s="23"/>
-      <c r="CG10" s="23"/>
-      <c r="CH10" s="23"/>
-      <c r="CI10" s="23"/>
-      <c r="CJ10" s="23"/>
-      <c r="CK10" s="23"/>
-      <c r="CL10" s="23"/>
-      <c r="CM10" s="23"/>
-      <c r="CN10" s="23"/>
-      <c r="CO10" s="23"/>
-      <c r="CP10" s="23"/>
-      <c r="CQ10" s="23"/>
-      <c r="CR10" s="23"/>
-      <c r="CS10" s="23"/>
-      <c r="CT10" s="23"/>
-      <c r="CU10" s="23"/>
-      <c r="CV10" s="23"/>
-      <c r="CW10" s="23"/>
-      <c r="CX10" s="23"/>
-      <c r="CY10" s="23"/>
-      <c r="CZ10" s="23"/>
-      <c r="DA10" s="23"/>
-      <c r="DB10" s="23"/>
-      <c r="DC10" s="23"/>
-      <c r="DD10" s="23"/>
-      <c r="DE10" s="23"/>
-      <c r="DF10" s="23"/>
-      <c r="DG10" s="23"/>
-      <c r="DH10" s="23"/>
-      <c r="DI10" s="23"/>
-      <c r="DJ10" s="23"/>
-      <c r="DK10" s="23"/>
-      <c r="DL10" s="23"/>
-      <c r="DM10" s="23"/>
-      <c r="DN10" s="23"/>
-      <c r="DO10" s="23"/>
-      <c r="DP10" s="23"/>
-      <c r="DQ10" s="23"/>
-      <c r="DR10" s="23"/>
-      <c r="DS10" s="23"/>
-      <c r="DT10" s="23"/>
-      <c r="DU10" s="23"/>
-      <c r="DV10" s="23"/>
-      <c r="DW10" s="23"/>
-      <c r="DX10" s="23"/>
-      <c r="DY10" s="23"/>
-      <c r="DZ10" s="23"/>
-      <c r="EA10" s="23"/>
-      <c r="EB10" s="23"/>
-      <c r="EC10" s="23"/>
-      <c r="ED10" s="23"/>
-      <c r="EE10" s="23"/>
-      <c r="EF10" s="23"/>
-      <c r="EG10" s="23"/>
-      <c r="EH10" s="23"/>
-      <c r="EI10" s="23"/>
-      <c r="EJ10" s="23"/>
-      <c r="EK10" s="23"/>
-      <c r="EL10" s="23"/>
-      <c r="EM10" s="23"/>
-      <c r="EN10" s="23"/>
-      <c r="EO10" s="23"/>
-      <c r="EP10" s="23"/>
-      <c r="EQ10" s="23"/>
-      <c r="ER10" s="23"/>
-      <c r="ES10" s="23"/>
-      <c r="ET10" s="23"/>
-      <c r="EU10" s="23"/>
-      <c r="EV10" s="23"/>
-      <c r="EW10" s="23"/>
-      <c r="EX10" s="23"/>
-      <c r="EY10" s="23"/>
-      <c r="EZ10" s="23"/>
-      <c r="FA10" s="23"/>
-      <c r="FB10" s="23"/>
-      <c r="FC10" s="23"/>
-      <c r="FD10" s="23"/>
-      <c r="FE10" s="23"/>
-      <c r="FF10" s="23"/>
-      <c r="FG10" s="23"/>
-      <c r="FH10" s="23"/>
-      <c r="FI10" s="23"/>
-      <c r="FJ10" s="23"/>
-      <c r="FK10" s="23"/>
-      <c r="FL10" s="23"/>
-      <c r="FM10" s="23"/>
-      <c r="FN10" s="23"/>
-      <c r="FO10" s="23"/>
-      <c r="FP10" s="23"/>
-      <c r="FQ10" s="23"/>
-      <c r="FR10" s="23"/>
-      <c r="FS10" s="23"/>
-      <c r="FT10" s="23"/>
-      <c r="FU10" s="23"/>
-      <c r="FV10" s="23"/>
-      <c r="FW10" s="23"/>
-      <c r="FX10" s="23"/>
-      <c r="FY10" s="23"/>
-      <c r="FZ10" s="23"/>
-      <c r="GA10" s="23"/>
-      <c r="GB10" s="23"/>
-      <c r="GC10" s="23"/>
-      <c r="GD10" s="23"/>
-      <c r="GE10" s="23"/>
-      <c r="GF10" s="23"/>
-      <c r="GG10" s="23"/>
-      <c r="GH10" s="23"/>
-      <c r="GI10" s="23"/>
-      <c r="GJ10" s="23"/>
-      <c r="GK10" s="23"/>
-      <c r="GL10" s="23"/>
-      <c r="GM10" s="23"/>
-      <c r="GN10" s="23"/>
-      <c r="GO10" s="23"/>
-      <c r="GP10" s="23"/>
-      <c r="GQ10" s="23"/>
-      <c r="GR10" s="23"/>
-      <c r="GS10" s="23"/>
-      <c r="GT10" s="23"/>
-      <c r="GU10" s="23"/>
-      <c r="GV10" s="23"/>
-      <c r="GW10" s="23"/>
-      <c r="GX10" s="23"/>
-      <c r="GY10" s="23"/>
-      <c r="GZ10" s="23"/>
-      <c r="HA10" s="23"/>
-      <c r="HB10" s="23"/>
-      <c r="HC10" s="23"/>
-      <c r="HD10" s="23"/>
-      <c r="HE10" s="23"/>
-      <c r="HF10" s="23"/>
-      <c r="HG10" s="23"/>
-      <c r="HH10" s="23"/>
-      <c r="HI10" s="23"/>
-      <c r="HJ10" s="23"/>
-      <c r="HK10" s="23"/>
-      <c r="HL10" s="23"/>
-      <c r="HM10" s="23"/>
-      <c r="HN10" s="23"/>
-      <c r="HO10" s="23"/>
-      <c r="HP10" s="23"/>
-      <c r="HQ10" s="23"/>
-      <c r="HR10" s="23"/>
-      <c r="HS10" s="23"/>
-      <c r="HT10" s="23"/>
-      <c r="HU10" s="23"/>
-      <c r="HV10" s="23"/>
-      <c r="HW10" s="23"/>
-      <c r="HX10" s="23"/>
-      <c r="HY10" s="23"/>
-      <c r="HZ10" s="23"/>
-      <c r="IA10" s="23"/>
-      <c r="IB10" s="23"/>
-      <c r="IC10" s="23"/>
-      <c r="ID10" s="23"/>
-      <c r="IE10" s="23"/>
-      <c r="IF10" s="23"/>
-      <c r="IG10" s="23"/>
-      <c r="IH10" s="23"/>
-      <c r="II10" s="23"/>
-      <c r="IJ10" s="23"/>
-      <c r="IK10" s="23"/>
-      <c r="IL10" s="23"/>
-      <c r="IM10" s="23"/>
-      <c r="IN10" s="23"/>
-      <c r="IO10" s="23"/>
-      <c r="IP10" s="23"/>
-      <c r="IQ10" s="23"/>
-      <c r="IR10" s="23"/>
-      <c r="IS10" s="23"/>
-      <c r="IT10" s="23"/>
-      <c r="IU10" s="23"/>
-      <c r="IV10" s="23"/>
-      <c r="IW10" s="23"/>
-      <c r="IX10" s="23"/>
-      <c r="IY10" s="23"/>
-      <c r="IZ10" s="23"/>
-      <c r="JA10" s="23"/>
-      <c r="JB10" s="23"/>
-      <c r="JC10" s="23"/>
-      <c r="JD10" s="23"/>
-      <c r="JE10" s="23"/>
-      <c r="JF10" s="23"/>
-      <c r="JG10" s="23"/>
-      <c r="JH10" s="23"/>
-      <c r="JI10" s="23"/>
-      <c r="JJ10" s="23"/>
-      <c r="JK10" s="23"/>
-      <c r="JL10" s="23"/>
-      <c r="JM10" s="23"/>
-      <c r="JN10" s="23"/>
-      <c r="JO10" s="23"/>
-      <c r="JP10" s="23"/>
-      <c r="JQ10" s="23"/>
-      <c r="JR10" s="23"/>
-      <c r="JS10" s="47"/>
-      <c r="JT10" s="47"/>
-      <c r="JU10" s="47"/>
-      <c r="JV10" s="47"/>
-      <c r="JW10" s="47"/>
-      <c r="JX10" s="47"/>
-      <c r="JY10" s="47"/>
-      <c r="JZ10" s="23"/>
-      <c r="KA10" s="23"/>
-      <c r="KB10" s="23"/>
-      <c r="KC10" s="23"/>
-      <c r="KD10" s="23"/>
-      <c r="KE10" s="23"/>
-      <c r="KF10" s="23"/>
-      <c r="KG10" s="23"/>
-      <c r="KH10" s="48"/>
-      <c r="KI10" s="48"/>
-      <c r="KJ10" s="48"/>
-      <c r="KK10" s="48"/>
-      <c r="KL10" s="48" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="11" spans="1:300">
-      <c r="A11" s="25"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="26"/>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="26"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="26"/>
-      <c r="AE11" s="26"/>
-      <c r="AF11" s="23"/>
-      <c r="AG11" s="23"/>
-      <c r="AH11" s="23"/>
-      <c r="AI11" s="23"/>
-      <c r="AJ11" s="23"/>
-      <c r="AK11" s="23"/>
-      <c r="AL11" s="23"/>
-      <c r="AM11" s="23"/>
-      <c r="AN11" s="27"/>
-      <c r="AO11" s="27"/>
-      <c r="AP11" s="27"/>
-      <c r="AQ11" s="27"/>
-      <c r="AR11" s="27"/>
-      <c r="AS11" s="23"/>
-      <c r="AT11" s="23"/>
-      <c r="AU11" s="23"/>
-      <c r="AV11" s="23"/>
-      <c r="AW11" s="23"/>
-      <c r="AX11" s="23"/>
-      <c r="AY11" s="23"/>
-      <c r="AZ11" s="23"/>
-      <c r="BA11" s="23"/>
-      <c r="BB11" s="23"/>
-      <c r="BC11" s="23"/>
-      <c r="BD11" s="23"/>
-      <c r="BE11" s="23"/>
-      <c r="BF11" s="23"/>
-      <c r="BG11" s="23"/>
-      <c r="BH11" s="23"/>
-      <c r="BI11" s="23"/>
-      <c r="BJ11" s="23"/>
-      <c r="BK11" s="23"/>
-      <c r="BL11" s="23"/>
-      <c r="BM11" s="23"/>
-      <c r="BN11" s="23"/>
-      <c r="BO11" s="23"/>
-      <c r="BP11" s="23"/>
-      <c r="BQ11" s="23"/>
-      <c r="BR11" s="23"/>
-      <c r="BS11" s="23"/>
-      <c r="BT11" s="23"/>
-      <c r="BU11" s="23"/>
-      <c r="BV11" s="23"/>
-      <c r="BW11" s="23"/>
-      <c r="BX11" s="23"/>
-      <c r="BY11" s="23"/>
-      <c r="BZ11" s="23"/>
-      <c r="CA11" s="23"/>
-      <c r="CB11" s="23"/>
-      <c r="CC11" s="23"/>
-      <c r="CD11" s="23"/>
-      <c r="CE11" s="23"/>
-      <c r="CF11" s="23"/>
-      <c r="CG11" s="23"/>
-      <c r="CH11" s="23"/>
-      <c r="CI11" s="23"/>
-      <c r="CJ11" s="23"/>
-      <c r="CK11" s="23"/>
-      <c r="CL11" s="23"/>
-      <c r="CM11" s="23"/>
-      <c r="CN11" s="23"/>
-      <c r="CO11" s="23"/>
-      <c r="CP11" s="23"/>
-      <c r="CQ11" s="23"/>
-      <c r="CR11" s="23"/>
-      <c r="CS11" s="23"/>
-      <c r="CT11" s="23"/>
-      <c r="CU11" s="23"/>
-      <c r="CV11" s="23"/>
-      <c r="CW11" s="23"/>
-      <c r="CX11" s="23"/>
-      <c r="CY11" s="23"/>
-      <c r="CZ11" s="23"/>
-      <c r="DA11" s="23"/>
-      <c r="DB11" s="23"/>
-      <c r="DC11" s="23"/>
-      <c r="DD11" s="23"/>
-      <c r="DE11" s="23"/>
-      <c r="DF11" s="23"/>
-      <c r="DG11" s="23"/>
-      <c r="DH11" s="23"/>
-      <c r="DI11" s="23"/>
-      <c r="DJ11" s="23"/>
-      <c r="DK11" s="23"/>
-      <c r="DL11" s="23"/>
-      <c r="DM11" s="23"/>
-      <c r="DN11" s="23"/>
-      <c r="DO11" s="23"/>
-      <c r="DP11" s="23"/>
-      <c r="DQ11" s="23"/>
-      <c r="DR11" s="23"/>
-      <c r="DS11" s="23"/>
-      <c r="DT11" s="23"/>
-      <c r="DU11" s="23"/>
-      <c r="DV11" s="23"/>
-      <c r="DW11" s="23"/>
-      <c r="DX11" s="23"/>
-      <c r="DY11" s="23"/>
-      <c r="DZ11" s="23"/>
-      <c r="EA11" s="23"/>
-      <c r="EB11" s="23"/>
-      <c r="EC11" s="23"/>
-      <c r="ED11" s="23"/>
-      <c r="EE11" s="23"/>
-      <c r="EF11" s="23"/>
-      <c r="EG11" s="23"/>
-      <c r="EH11" s="23"/>
-      <c r="EI11" s="23"/>
-      <c r="EJ11" s="23"/>
-      <c r="EK11" s="23"/>
-      <c r="EL11" s="23"/>
-      <c r="EM11" s="23"/>
-      <c r="EN11" s="23"/>
-      <c r="EO11" s="23"/>
-      <c r="EP11" s="23"/>
-      <c r="EQ11" s="23"/>
-      <c r="ER11" s="23"/>
-      <c r="ES11" s="23"/>
-      <c r="ET11" s="23"/>
-      <c r="EU11" s="23"/>
-      <c r="EV11" s="23"/>
-      <c r="EW11" s="23"/>
-      <c r="EX11" s="23"/>
-      <c r="EY11" s="23"/>
-      <c r="EZ11" s="23"/>
-      <c r="FA11" s="23"/>
-      <c r="FB11" s="23"/>
-      <c r="FC11" s="23"/>
-      <c r="FD11" s="23"/>
-      <c r="FE11" s="23"/>
-      <c r="FF11" s="23"/>
-      <c r="FG11" s="23"/>
-      <c r="FH11" s="23"/>
-      <c r="FI11" s="23"/>
-      <c r="FJ11" s="23"/>
-      <c r="FK11" s="23"/>
-      <c r="FL11" s="23"/>
-      <c r="FM11" s="23"/>
-      <c r="FN11" s="23"/>
-      <c r="FO11" s="23"/>
-      <c r="FP11" s="23"/>
-      <c r="FQ11" s="23"/>
-      <c r="FR11" s="23"/>
-      <c r="FS11" s="23"/>
-      <c r="FT11" s="23"/>
-      <c r="FU11" s="23"/>
-      <c r="FV11" s="23"/>
-      <c r="FW11" s="23"/>
-      <c r="FX11" s="23"/>
-      <c r="FY11" s="23"/>
-      <c r="FZ11" s="23"/>
-      <c r="GA11" s="23"/>
-      <c r="GB11" s="23"/>
-      <c r="GC11" s="23"/>
-      <c r="GD11" s="23"/>
-      <c r="GE11" s="23"/>
-      <c r="GF11" s="23"/>
-      <c r="GG11" s="23"/>
-      <c r="GH11" s="23"/>
-      <c r="GI11" s="23"/>
-      <c r="GJ11" s="23"/>
-      <c r="GK11" s="23"/>
-      <c r="GL11" s="23"/>
-      <c r="GM11" s="23"/>
-      <c r="GN11" s="23"/>
-      <c r="GO11" s="23"/>
-      <c r="GP11" s="23"/>
-      <c r="GQ11" s="23"/>
-      <c r="GR11" s="23"/>
-      <c r="GS11" s="23"/>
-      <c r="GT11" s="23"/>
-      <c r="GU11" s="23"/>
-      <c r="GV11" s="23"/>
-      <c r="GW11" s="23"/>
-      <c r="GX11" s="23"/>
-      <c r="GY11" s="23"/>
-      <c r="GZ11" s="23"/>
-      <c r="HA11" s="23"/>
-      <c r="HB11" s="23"/>
-      <c r="HC11" s="23"/>
-      <c r="HD11" s="23"/>
-      <c r="HE11" s="23"/>
-      <c r="HF11" s="23"/>
-      <c r="HG11" s="23"/>
-      <c r="HH11" s="23"/>
-      <c r="HI11" s="23"/>
-      <c r="HJ11" s="23"/>
-      <c r="HK11" s="23"/>
-      <c r="HL11" s="23"/>
-      <c r="HM11" s="23"/>
-      <c r="HN11" s="23"/>
-      <c r="HO11" s="23"/>
-      <c r="HP11" s="23"/>
-      <c r="HQ11" s="23"/>
-      <c r="HR11" s="23"/>
-      <c r="HS11" s="23"/>
-      <c r="HT11" s="23"/>
-      <c r="HU11" s="23"/>
-      <c r="HV11" s="23"/>
-      <c r="HW11" s="23"/>
-      <c r="HX11" s="23"/>
-      <c r="HY11" s="23"/>
-      <c r="HZ11" s="23"/>
-      <c r="IA11" s="23"/>
-      <c r="IB11" s="23"/>
-      <c r="IC11" s="23"/>
-      <c r="ID11" s="23"/>
-      <c r="IE11" s="23"/>
-      <c r="IF11" s="23"/>
-      <c r="IG11" s="23"/>
-      <c r="IH11" s="23"/>
-      <c r="II11" s="23"/>
-      <c r="IJ11" s="23"/>
-      <c r="IK11" s="23"/>
-      <c r="IL11" s="23"/>
-      <c r="IM11" s="23"/>
-      <c r="IN11" s="23"/>
-      <c r="IO11" s="23"/>
-      <c r="IP11" s="23"/>
-      <c r="IQ11" s="23"/>
-      <c r="IR11" s="23"/>
-      <c r="IS11" s="23"/>
-      <c r="IT11" s="23"/>
-      <c r="IU11" s="23"/>
-      <c r="IV11" s="23"/>
-      <c r="IW11" s="23"/>
-      <c r="IX11" s="23"/>
-      <c r="IY11" s="23"/>
-      <c r="IZ11" s="23"/>
-      <c r="JA11" s="23"/>
-      <c r="JB11" s="23"/>
-      <c r="JC11" s="23"/>
-      <c r="JD11" s="23"/>
-      <c r="JE11" s="23"/>
-      <c r="JF11" s="23"/>
-      <c r="JG11" s="23"/>
-      <c r="JH11" s="23"/>
-      <c r="JI11" s="23"/>
-      <c r="JJ11" s="23"/>
-      <c r="JK11" s="23"/>
-      <c r="JL11" s="23"/>
-      <c r="JM11" s="23"/>
-      <c r="JN11" s="23"/>
-      <c r="JO11" s="23"/>
-      <c r="JP11" s="23"/>
-      <c r="JQ11" s="23"/>
-      <c r="JR11" s="23"/>
-      <c r="JS11" s="47"/>
-      <c r="JT11" s="47"/>
-      <c r="JU11" s="47"/>
-      <c r="JV11" s="47"/>
-      <c r="JW11" s="47"/>
-      <c r="JX11" s="47"/>
-      <c r="JY11" s="47"/>
-      <c r="JZ11" s="23"/>
-      <c r="KA11" s="23"/>
-      <c r="KB11" s="23"/>
-      <c r="KC11" s="23"/>
-      <c r="KD11" s="23"/>
-      <c r="KE11" s="23"/>
-      <c r="KF11" s="23"/>
-      <c r="KG11" s="23"/>
-      <c r="KH11" s="48"/>
-      <c r="KI11" s="48"/>
-      <c r="KJ11" s="48"/>
-      <c r="KK11" s="48"/>
-      <c r="KL11" s="48" t="s">
-        <v>340</v>
-      </c>
+      <c r="KH7" s="47"/>
+      <c r="KI7" s="47"/>
+      <c r="KJ7" s="47"/>
+      <c r="KK7" s="47"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:KK6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A6:KK6"/>
   <mergeCells count="32">
     <mergeCell ref="KH4:KJ5"/>
     <mergeCell ref="JZ4:KG4"/>
@@ -6700,24 +5462,15 @@
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>
   </conditionalFormatting>
-  <dataValidations count="5">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR7" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR7">
       <formula1>36526</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH8:KJ11" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>$KL$7:$KL$11</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH7 KJ7" xr:uid="{00000000-0002-0000-0000-000002000000}">
-      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete,"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KK7" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>"NGSA, WEM, FCRM Operational Framework, Other, Unknown/TBC"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KI7" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete, No Delivery pre 2021 "</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH6:KJ999996">
+      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, N/A"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.7086614173228347" right="0.7086614173228347" top="0.7480314960629921" bottom="0.7480314960629921" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="10" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
[PM-577] Add carbon to the FCRM1
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -1,31 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthall/Work/pafs/pafs_core/lib/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16230ADF-9386-8C4D-81CA-AC41D44E0D83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25200" windowHeight="11980"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Master local choices" sheetId="2" r:id="rId5"/>
+    <sheet name="Master local choices" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$KK$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,29 +36,29 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Registered User</author>
   </authors>
   <commentList>
-    <comment ref="CD6" authorId="0">
+    <comment ref="CD6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <b val="1"/>
-            <color indexed="81"/>
-            <sz val="9"/>
           </rPr>
           <t>Registered User:</t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <color indexed="81"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -67,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="343" count="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="346">
   <si>
     <t>FCRM1 - National Capital Programme</t>
   </si>
@@ -87,7 +90,7 @@
     <t>DESCRIPTIVE DETAILS</t>
   </si>
   <si>
-    <t xml:space="preserve">PARTNERSHIP FUNDING SUMMARY
+    <t>PARTNERSHIP FUNDING SUMMARY
 (Values to be taken from PF Calculator)</t>
   </si>
   <si>
@@ -97,51 +100,51 @@
     <t>ADDITIONAL DETAILS</t>
   </si>
   <si>
-    <t xml:space="preserve">PROJECT TOTALS
+    <t>PROJECT TOTALS
 (calculated from relevant columns)
 £ CASH</t>
   </si>
   <si>
-    <t xml:space="preserve">TOTAL PROJECT EXPENDITURE
+    <t>TOTAL PROJECT EXPENDITURE
  (calculated from FCRM GiA to be expended + Total Local Contributions Secured + Funding From Other EA Functions + Further Contributions Required)
 £ CASH</t>
   </si>
   <si>
-    <t xml:space="preserve">FCRM Grant in Aid TO BE EXPENDED ON PROJECT
+    <t>FCRM Grant in Aid TO BE EXPENDED ON PROJECT
 £ CASH</t>
   </si>
   <si>
-    <t xml:space="preserve">GROWTH FUND
+    <t>GROWTH FUND
  £ CASH</t>
   </si>
   <si>
-    <t xml:space="preserve">LOCAL LEVY SECURED
+    <t>LOCAL LEVY SECURED
  £ CASH</t>
   </si>
   <si>
-    <t xml:space="preserve">INTERNAL DRAINAGE BOARD PRECEPTS SECURED
+    <t>INTERNAL DRAINAGE BOARD PRECEPTS SECURED
  £ CASH</t>
   </si>
   <si>
-    <t xml:space="preserve">PUBLICLY FUNDED CONTRIBUTIONS SECURED
+    <t>PUBLICLY FUNDED CONTRIBUTIONS SECURED
 (Contract In Place, or In Negotiation)
  £ CASH</t>
   </si>
   <si>
-    <t xml:space="preserve">PRIVATELY FUNDED CONTRIBUTIONS SECURED
+    <t>PRIVATELY FUNDED CONTRIBUTIONS SECURED
 (Contract In Place, or In Negotiation)
  £ CASH</t>
   </si>
   <si>
-    <t xml:space="preserve">FUNDING CONTRIBUTIONS FROM OTHER ENVIRONMENT AGENCY FUNCTIONS/SOURCES
+    <t>FUNDING CONTRIBUTIONS FROM OTHER ENVIRONMENT AGENCY FUNCTIONS/SOURCES
 £ CASH</t>
   </si>
   <si>
-    <t xml:space="preserve">FURTHER CONTRIBUTIONS REQUIRED
+    <t>FURTHER CONTRIBUTIONS REQUIRED
  £ CASH</t>
   </si>
   <si>
-    <t xml:space="preserve">Outcome Measures
+    <t>Outcome Measures
  OM2 Delivery</t>
   </si>
   <si>
@@ -168,7 +171,7 @@
     <t>Environmental performance specification indicators</t>
   </si>
   <si>
-    <t xml:space="preserve">SCHEME OVERVIEW
+    <t>SCHEME OVERVIEW
 (calculated from relevant columns)</t>
   </si>
   <si>
@@ -396,7 +399,7 @@
     <t>OM4c - PROJECT TOTAL</t>
   </si>
   <si>
-    <t xml:space="preserve">TPE - PREVIOUS
+    <t>TPE - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -436,7 +439,7 @@
     <t>TPE - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">GiA - PREVIOUS
+    <t>GiA - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -476,7 +479,7 @@
     <t>GiA - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">Growth - PREVIOUS
+    <t>Growth - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -516,7 +519,7 @@
     <t>Growth - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">Local Levy - PREVIOUS
+    <t>Local Levy - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -556,7 +559,7 @@
     <t>Local Levy - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">IDB - PREVIOUS
+    <t>IDB - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -596,7 +599,7 @@
     <t>IDB - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">Public - PREVIOUS
+    <t>Public - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -636,7 +639,7 @@
     <t>Public - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">Private - PREVIOUS
+    <t>Private - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -676,7 +679,7 @@
     <t>Private - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">Other EA - PREVIOUS
+    <t>Other EA - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -716,7 +719,7 @@
     <t>Other EA - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">Further required - PREVIOUS
+    <t>Further required - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -756,7 +759,7 @@
     <t>Further required - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">OM2 - PREVIOUS
+    <t>OM2 - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -796,7 +799,7 @@
     <t>OM2 - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">OM2b - PREVIOUS
+    <t>OM2b - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -836,7 +839,7 @@
     <t>OM2b - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">OM2c - PREVIOUS
+    <t>OM2c - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -876,7 +879,7 @@
     <t>OM2c - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">OM3 - PREVIOUS
+    <t>OM3 - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -916,7 +919,7 @@
     <t>OM3 - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">OM3b - PREVIOUS
+    <t>OM3b - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -956,7 +959,7 @@
     <t>OM3b - 2026/27</t>
   </si>
   <si>
-    <t xml:space="preserve">OM3c - PREVIOUS
+    <t>OM3c - PREVIOUS
 YEARS</t>
   </si>
   <si>
@@ -1049,20 +1052,20 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFFF0000"/>
-        <sz val="12"/>
       </rPr>
       <t>GROWTH</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <b val="1"/>
-        <sz val="12"/>
       </rPr>
       <t xml:space="preserve"> 6 year total</t>
     </r>
@@ -1148,20 +1151,20 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <b val="1"/>
-        <color rgb="FFFF0000"/>
-        <sz val="12"/>
       </rPr>
       <t>GROWTH</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <b val="1"/>
-        <sz val="12"/>
       </rPr>
       <t xml:space="preserve"> 20/21</t>
     </r>
@@ -1177,12 +1180,21 @@
   </si>
   <si>
     <t>20/21</t>
+  </si>
+  <si>
+    <t>Carbon Assessment</t>
+  </si>
+  <si>
+    <t>Capital Carbon</t>
+  </si>
+  <si>
+    <t>Lifecycle Carbon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -1190,115 +1202,115 @@
     <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     <numFmt numFmtId="168" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color rgb="FFFF0000"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="12"/>
     </font>
     <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="0"/>
-      <sz val="16"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <sz val="12"/>
     </font>
     <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="22"/>
     </font>
     <font>
+      <b/>
+      <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <sz val="20"/>
     </font>
     <font>
+      <sz val="30"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="30"/>
     </font>
     <font>
+      <b/>
+      <sz val="22"/>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <sz val="22"/>
     </font>
     <font>
+      <b/>
+      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <sz val="14"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <b val="1"/>
-      <color indexed="81"/>
-      <sz val="9"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <color indexed="81"/>
-      <sz val="9"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <b val="1"/>
-      <color rgb="FFFF0000"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="27">
@@ -1358,7 +1370,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.3999755851924192"/>
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1370,7 +1382,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.3499862666707358"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1448,18 +1460,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.3999755851924192"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.3999755851924192"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1488,15 +1500,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1511,20 +1514,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1661,7 +1719,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1700,6 +1757,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1730,75 +1838,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="%" xfId="3"/>
-    <cellStyle name="% 2 2 2" xfId="4"/>
+    <cellStyle name="%" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% 2 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="9"/>
+    <cellStyle name="Comma 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="8"/>
-    <cellStyle name="Normal 2 2" xfId="6"/>
-    <cellStyle name="Normal_RCP" xfId="5"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Percent 11" xfId="7"/>
+    <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal_RCP" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent 11" xfId="7" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1812,7 +1876,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16" count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1966,7 +2030,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1992,7 +2056,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -2027,7 +2091,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2070,7 +2134,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -2086,22 +2150,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:KM7"/>
+  <dimension ref="A1:KM32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="KG7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="KD7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="KH7" sqref="KH7"/>
+      <selection pane="bottomRight" activeCell="KJ29" sqref="KJ29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98.7109375" style="1" customWidth="1"/>
@@ -2123,16 +2187,16 @@
     <col min="286" max="293" width="21" style="6" customWidth="1"/>
     <col min="294" max="296" width="22.28515625" style="7" customWidth="1"/>
     <col min="297" max="297" width="17.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="298" max="298" width="8.7109375" style="7"/>
-    <col min="299" max="299" width="11" style="7" customWidth="1"/>
+    <col min="298" max="298" width="19.7109375" style="7" customWidth="1"/>
+    <col min="299" max="299" width="21.5703125" style="7" customWidth="1"/>
     <col min="300" max="16384" width="8.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:293" customFormat="false" ht="28.5" customHeight="1">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:299" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
+      <c r="B1" s="80"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
@@ -2424,12 +2488,18 @@
       <c r="KE1" s="23"/>
       <c r="KF1" s="23"/>
       <c r="KG1" s="23"/>
+      <c r="KH1" s="47"/>
+      <c r="KI1" s="47"/>
+      <c r="KJ1" s="47"/>
+      <c r="KK1" s="47"/>
+      <c r="KL1" s="47"/>
+      <c r="KM1" s="47"/>
     </row>
-    <row r="2" spans="1:293" customFormat="false" ht="28.5" customHeight="1">
-      <c r="A2" s="65" t="s">
+    <row r="2" spans="1:299" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="81" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="81"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="23"/>
@@ -2721,8 +2791,14 @@
       <c r="KE2" s="37"/>
       <c r="KF2" s="37"/>
       <c r="KG2" s="37"/>
+      <c r="KH2" s="47"/>
+      <c r="KI2" s="47"/>
+      <c r="KJ2" s="47"/>
+      <c r="KK2" s="47"/>
+      <c r="KL2" s="47"/>
+      <c r="KM2" s="47"/>
     </row>
-    <row r="3" spans="1:293" customFormat="false" ht="25.5" customHeight="1">
+    <row r="3" spans="1:299" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="39"/>
@@ -3016,423 +3092,433 @@
       <c r="KE3" s="45"/>
       <c r="KF3" s="45"/>
       <c r="KG3" s="45"/>
+      <c r="KH3" s="47"/>
+      <c r="KI3" s="47"/>
+      <c r="KJ3" s="47"/>
+      <c r="KK3" s="47"/>
+      <c r="KL3" s="47"/>
+      <c r="KM3" s="47"/>
     </row>
-    <row r="4" spans="1:297" customFormat="false" ht="46.5" customHeight="1">
-      <c r="A4" s="66" t="s">
+    <row r="4" spans="1:299" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="67" t="s">
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="68" t="s">
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="69" t="s">
+      <c r="L4" s="84"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="70" t="s">
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="70"/>
-      <c r="W4" s="70"/>
-      <c r="X4" s="70"/>
-      <c r="Y4" s="70"/>
-      <c r="Z4" s="70"/>
-      <c r="AA4" s="70"/>
-      <c r="AB4" s="70"/>
-      <c r="AC4" s="71" t="s">
+      <c r="V4" s="86"/>
+      <c r="W4" s="86"/>
+      <c r="X4" s="86"/>
+      <c r="Y4" s="86"/>
+      <c r="Z4" s="86"/>
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="86"/>
+      <c r="AC4" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="71"/>
-      <c r="AE4" s="71"/>
-      <c r="AF4" s="71"/>
-      <c r="AG4" s="71"/>
-      <c r="AH4" s="71"/>
-      <c r="AI4" s="71"/>
-      <c r="AJ4" s="72" t="s">
+      <c r="AD4" s="87"/>
+      <c r="AE4" s="87"/>
+      <c r="AF4" s="87"/>
+      <c r="AG4" s="87"/>
+      <c r="AH4" s="87"/>
+      <c r="AI4" s="87"/>
+      <c r="AJ4" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="72"/>
-      <c r="AL4" s="72"/>
-      <c r="AM4" s="63" t="s">
+      <c r="AK4" s="88"/>
+      <c r="AL4" s="88"/>
+      <c r="AM4" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="63"/>
-      <c r="AO4" s="74"/>
-      <c r="AP4" s="74"/>
-      <c r="AQ4" s="74"/>
-      <c r="AR4" s="74"/>
-      <c r="AS4" s="75" t="s">
+      <c r="AN4" s="79"/>
+      <c r="AO4" s="69"/>
+      <c r="AP4" s="69"/>
+      <c r="AQ4" s="69"/>
+      <c r="AR4" s="69"/>
+      <c r="AS4" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="75"/>
-      <c r="AU4" s="75"/>
-      <c r="AV4" s="75"/>
-      <c r="AW4" s="75"/>
-      <c r="AX4" s="75"/>
-      <c r="AY4" s="75"/>
-      <c r="AZ4" s="75"/>
-      <c r="BA4" s="75"/>
-      <c r="BB4" s="75"/>
-      <c r="BC4" s="75"/>
-      <c r="BD4" s="75"/>
-      <c r="BE4" s="75"/>
-      <c r="BF4" s="75"/>
-      <c r="BG4" s="75"/>
-      <c r="BH4" s="75"/>
-      <c r="BI4" s="75"/>
-      <c r="BJ4" s="75"/>
-      <c r="BK4" s="73" t="s">
+      <c r="AT4" s="70"/>
+      <c r="AU4" s="70"/>
+      <c r="AV4" s="70"/>
+      <c r="AW4" s="70"/>
+      <c r="AX4" s="70"/>
+      <c r="AY4" s="70"/>
+      <c r="AZ4" s="70"/>
+      <c r="BA4" s="70"/>
+      <c r="BB4" s="70"/>
+      <c r="BC4" s="70"/>
+      <c r="BD4" s="70"/>
+      <c r="BE4" s="70"/>
+      <c r="BF4" s="70"/>
+      <c r="BG4" s="70"/>
+      <c r="BH4" s="70"/>
+      <c r="BI4" s="70"/>
+      <c r="BJ4" s="70"/>
+      <c r="BK4" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="BL4" s="73"/>
-      <c r="BM4" s="73"/>
-      <c r="BN4" s="73"/>
-      <c r="BO4" s="73"/>
-      <c r="BP4" s="73"/>
-      <c r="BQ4" s="73"/>
-      <c r="BR4" s="73"/>
-      <c r="BS4" s="73"/>
-      <c r="BT4" s="73"/>
-      <c r="BU4" s="73"/>
-      <c r="BV4" s="73"/>
-      <c r="BW4" s="73"/>
-      <c r="BX4" s="73"/>
-      <c r="BY4" s="76" t="s">
+      <c r="BL4" s="66"/>
+      <c r="BM4" s="66"/>
+      <c r="BN4" s="66"/>
+      <c r="BO4" s="66"/>
+      <c r="BP4" s="66"/>
+      <c r="BQ4" s="66"/>
+      <c r="BR4" s="66"/>
+      <c r="BS4" s="66"/>
+      <c r="BT4" s="66"/>
+      <c r="BU4" s="66"/>
+      <c r="BV4" s="66"/>
+      <c r="BW4" s="66"/>
+      <c r="BX4" s="66"/>
+      <c r="BY4" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="76"/>
-      <c r="CA4" s="76"/>
-      <c r="CB4" s="76"/>
-      <c r="CC4" s="76"/>
-      <c r="CD4" s="76"/>
-      <c r="CE4" s="76"/>
-      <c r="CF4" s="76"/>
-      <c r="CG4" s="76"/>
-      <c r="CH4" s="76"/>
-      <c r="CI4" s="76"/>
-      <c r="CJ4" s="76"/>
-      <c r="CK4" s="76"/>
-      <c r="CL4" s="76"/>
-      <c r="CM4" s="77" t="s">
+      <c r="BZ4" s="71"/>
+      <c r="CA4" s="71"/>
+      <c r="CB4" s="71"/>
+      <c r="CC4" s="71"/>
+      <c r="CD4" s="71"/>
+      <c r="CE4" s="71"/>
+      <c r="CF4" s="71"/>
+      <c r="CG4" s="71"/>
+      <c r="CH4" s="71"/>
+      <c r="CI4" s="71"/>
+      <c r="CJ4" s="71"/>
+      <c r="CK4" s="71"/>
+      <c r="CL4" s="71"/>
+      <c r="CM4" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="77"/>
-      <c r="CO4" s="77"/>
-      <c r="CP4" s="77"/>
-      <c r="CQ4" s="77"/>
-      <c r="CR4" s="77"/>
-      <c r="CS4" s="77"/>
-      <c r="CT4" s="77"/>
-      <c r="CU4" s="77"/>
-      <c r="CV4" s="77"/>
-      <c r="CW4" s="77"/>
-      <c r="CX4" s="77"/>
-      <c r="CY4" s="77"/>
-      <c r="CZ4" s="77"/>
-      <c r="DA4" s="78" t="s">
+      <c r="CN4" s="72"/>
+      <c r="CO4" s="72"/>
+      <c r="CP4" s="72"/>
+      <c r="CQ4" s="72"/>
+      <c r="CR4" s="72"/>
+      <c r="CS4" s="72"/>
+      <c r="CT4" s="72"/>
+      <c r="CU4" s="72"/>
+      <c r="CV4" s="72"/>
+      <c r="CW4" s="72"/>
+      <c r="CX4" s="72"/>
+      <c r="CY4" s="72"/>
+      <c r="CZ4" s="72"/>
+      <c r="DA4" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="78"/>
-      <c r="DC4" s="78"/>
-      <c r="DD4" s="78"/>
-      <c r="DE4" s="78"/>
-      <c r="DF4" s="78"/>
-      <c r="DG4" s="78"/>
-      <c r="DH4" s="78"/>
-      <c r="DI4" s="78"/>
-      <c r="DJ4" s="78"/>
-      <c r="DK4" s="78"/>
-      <c r="DL4" s="78"/>
-      <c r="DM4" s="78"/>
-      <c r="DN4" s="78"/>
-      <c r="DO4" s="79" t="s">
+      <c r="DB4" s="73"/>
+      <c r="DC4" s="73"/>
+      <c r="DD4" s="73"/>
+      <c r="DE4" s="73"/>
+      <c r="DF4" s="73"/>
+      <c r="DG4" s="73"/>
+      <c r="DH4" s="73"/>
+      <c r="DI4" s="73"/>
+      <c r="DJ4" s="73"/>
+      <c r="DK4" s="73"/>
+      <c r="DL4" s="73"/>
+      <c r="DM4" s="73"/>
+      <c r="DN4" s="73"/>
+      <c r="DO4" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="79"/>
-      <c r="DQ4" s="79"/>
-      <c r="DR4" s="79"/>
-      <c r="DS4" s="79"/>
-      <c r="DT4" s="79"/>
-      <c r="DU4" s="79"/>
-      <c r="DV4" s="79"/>
-      <c r="DW4" s="79"/>
-      <c r="DX4" s="79"/>
-      <c r="DY4" s="79"/>
-      <c r="DZ4" s="79"/>
-      <c r="EA4" s="79"/>
-      <c r="EB4" s="79"/>
-      <c r="EC4" s="80" t="s">
+      <c r="DP4" s="74"/>
+      <c r="DQ4" s="74"/>
+      <c r="DR4" s="74"/>
+      <c r="DS4" s="74"/>
+      <c r="DT4" s="74"/>
+      <c r="DU4" s="74"/>
+      <c r="DV4" s="74"/>
+      <c r="DW4" s="74"/>
+      <c r="DX4" s="74"/>
+      <c r="DY4" s="74"/>
+      <c r="DZ4" s="74"/>
+      <c r="EA4" s="74"/>
+      <c r="EB4" s="74"/>
+      <c r="EC4" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="80"/>
-      <c r="EE4" s="80"/>
-      <c r="EF4" s="80"/>
-      <c r="EG4" s="80"/>
-      <c r="EH4" s="80"/>
-      <c r="EI4" s="80"/>
-      <c r="EJ4" s="80"/>
-      <c r="EK4" s="80"/>
-      <c r="EL4" s="80"/>
-      <c r="EM4" s="80"/>
-      <c r="EN4" s="80"/>
-      <c r="EO4" s="80"/>
-      <c r="EP4" s="80"/>
-      <c r="EQ4" s="81" t="s">
+      <c r="ED4" s="75"/>
+      <c r="EE4" s="75"/>
+      <c r="EF4" s="75"/>
+      <c r="EG4" s="75"/>
+      <c r="EH4" s="75"/>
+      <c r="EI4" s="75"/>
+      <c r="EJ4" s="75"/>
+      <c r="EK4" s="75"/>
+      <c r="EL4" s="75"/>
+      <c r="EM4" s="75"/>
+      <c r="EN4" s="75"/>
+      <c r="EO4" s="75"/>
+      <c r="EP4" s="75"/>
+      <c r="EQ4" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="81"/>
-      <c r="ES4" s="81"/>
-      <c r="ET4" s="81"/>
-      <c r="EU4" s="81"/>
-      <c r="EV4" s="81"/>
-      <c r="EW4" s="81"/>
-      <c r="EX4" s="81"/>
-      <c r="EY4" s="81"/>
-      <c r="EZ4" s="81"/>
-      <c r="FA4" s="81"/>
-      <c r="FB4" s="81"/>
-      <c r="FC4" s="81"/>
-      <c r="FD4" s="81"/>
-      <c r="FE4" s="82" t="s">
+      <c r="ER4" s="76"/>
+      <c r="ES4" s="76"/>
+      <c r="ET4" s="76"/>
+      <c r="EU4" s="76"/>
+      <c r="EV4" s="76"/>
+      <c r="EW4" s="76"/>
+      <c r="EX4" s="76"/>
+      <c r="EY4" s="76"/>
+      <c r="EZ4" s="76"/>
+      <c r="FA4" s="76"/>
+      <c r="FB4" s="76"/>
+      <c r="FC4" s="76"/>
+      <c r="FD4" s="76"/>
+      <c r="FE4" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="82"/>
-      <c r="FG4" s="82"/>
-      <c r="FH4" s="82"/>
-      <c r="FI4" s="82"/>
-      <c r="FJ4" s="82"/>
-      <c r="FK4" s="82"/>
-      <c r="FL4" s="82"/>
-      <c r="FM4" s="82"/>
-      <c r="FN4" s="82"/>
-      <c r="FO4" s="82"/>
-      <c r="FP4" s="82"/>
-      <c r="FQ4" s="82"/>
-      <c r="FR4" s="82"/>
-      <c r="FS4" s="83" t="s">
+      <c r="FF4" s="77"/>
+      <c r="FG4" s="77"/>
+      <c r="FH4" s="77"/>
+      <c r="FI4" s="77"/>
+      <c r="FJ4" s="77"/>
+      <c r="FK4" s="77"/>
+      <c r="FL4" s="77"/>
+      <c r="FM4" s="77"/>
+      <c r="FN4" s="77"/>
+      <c r="FO4" s="77"/>
+      <c r="FP4" s="77"/>
+      <c r="FQ4" s="77"/>
+      <c r="FR4" s="77"/>
+      <c r="FS4" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="83"/>
-      <c r="FU4" s="83"/>
-      <c r="FV4" s="83"/>
-      <c r="FW4" s="83"/>
-      <c r="FX4" s="83"/>
-      <c r="FY4" s="83"/>
-      <c r="FZ4" s="83"/>
-      <c r="GA4" s="83"/>
-      <c r="GB4" s="83"/>
-      <c r="GC4" s="83"/>
-      <c r="GD4" s="83"/>
-      <c r="GE4" s="83"/>
-      <c r="GF4" s="83"/>
-      <c r="GG4" s="73" t="s">
+      <c r="FT4" s="78"/>
+      <c r="FU4" s="78"/>
+      <c r="FV4" s="78"/>
+      <c r="FW4" s="78"/>
+      <c r="FX4" s="78"/>
+      <c r="FY4" s="78"/>
+      <c r="FZ4" s="78"/>
+      <c r="GA4" s="78"/>
+      <c r="GB4" s="78"/>
+      <c r="GC4" s="78"/>
+      <c r="GD4" s="78"/>
+      <c r="GE4" s="78"/>
+      <c r="GF4" s="78"/>
+      <c r="GG4" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="GH4" s="73"/>
-      <c r="GI4" s="73"/>
-      <c r="GJ4" s="73"/>
-      <c r="GK4" s="73"/>
-      <c r="GL4" s="73"/>
-      <c r="GM4" s="73"/>
-      <c r="GN4" s="73"/>
-      <c r="GO4" s="73"/>
-      <c r="GP4" s="73"/>
-      <c r="GQ4" s="73"/>
-      <c r="GR4" s="73"/>
-      <c r="GS4" s="73"/>
-      <c r="GT4" s="73"/>
-      <c r="GU4" s="73" t="s">
+      <c r="GH4" s="66"/>
+      <c r="GI4" s="66"/>
+      <c r="GJ4" s="66"/>
+      <c r="GK4" s="66"/>
+      <c r="GL4" s="66"/>
+      <c r="GM4" s="66"/>
+      <c r="GN4" s="66"/>
+      <c r="GO4" s="66"/>
+      <c r="GP4" s="66"/>
+      <c r="GQ4" s="66"/>
+      <c r="GR4" s="66"/>
+      <c r="GS4" s="66"/>
+      <c r="GT4" s="66"/>
+      <c r="GU4" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="GV4" s="73"/>
-      <c r="GW4" s="73"/>
-      <c r="GX4" s="73"/>
-      <c r="GY4" s="73"/>
-      <c r="GZ4" s="73"/>
-      <c r="HA4" s="73"/>
-      <c r="HB4" s="73"/>
-      <c r="HC4" s="73"/>
-      <c r="HD4" s="73"/>
-      <c r="HE4" s="73"/>
-      <c r="HF4" s="73"/>
-      <c r="HG4" s="73"/>
-      <c r="HH4" s="73"/>
-      <c r="HI4" s="73" t="s">
+      <c r="GV4" s="66"/>
+      <c r="GW4" s="66"/>
+      <c r="GX4" s="66"/>
+      <c r="GY4" s="66"/>
+      <c r="GZ4" s="66"/>
+      <c r="HA4" s="66"/>
+      <c r="HB4" s="66"/>
+      <c r="HC4" s="66"/>
+      <c r="HD4" s="66"/>
+      <c r="HE4" s="66"/>
+      <c r="HF4" s="66"/>
+      <c r="HG4" s="66"/>
+      <c r="HH4" s="66"/>
+      <c r="HI4" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="HJ4" s="73"/>
-      <c r="HK4" s="73"/>
-      <c r="HL4" s="73"/>
-      <c r="HM4" s="73"/>
-      <c r="HN4" s="73"/>
-      <c r="HO4" s="73"/>
-      <c r="HP4" s="73"/>
-      <c r="HQ4" s="73"/>
-      <c r="HR4" s="73"/>
-      <c r="HS4" s="73"/>
-      <c r="HT4" s="73"/>
-      <c r="HU4" s="73"/>
-      <c r="HV4" s="73"/>
-      <c r="HW4" s="90" t="s">
+      <c r="HJ4" s="66"/>
+      <c r="HK4" s="66"/>
+      <c r="HL4" s="66"/>
+      <c r="HM4" s="66"/>
+      <c r="HN4" s="66"/>
+      <c r="HO4" s="66"/>
+      <c r="HP4" s="66"/>
+      <c r="HQ4" s="66"/>
+      <c r="HR4" s="66"/>
+      <c r="HS4" s="66"/>
+      <c r="HT4" s="66"/>
+      <c r="HU4" s="66"/>
+      <c r="HV4" s="66"/>
+      <c r="HW4" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="90"/>
-      <c r="HY4" s="90"/>
-      <c r="HZ4" s="90"/>
-      <c r="IA4" s="90"/>
-      <c r="IB4" s="90"/>
-      <c r="IC4" s="90"/>
-      <c r="ID4" s="90"/>
-      <c r="IE4" s="90"/>
-      <c r="IF4" s="90"/>
-      <c r="IG4" s="90"/>
-      <c r="IH4" s="90"/>
-      <c r="II4" s="90"/>
-      <c r="IJ4" s="90"/>
-      <c r="IK4" s="90" t="s">
+      <c r="HX4" s="67"/>
+      <c r="HY4" s="67"/>
+      <c r="HZ4" s="67"/>
+      <c r="IA4" s="67"/>
+      <c r="IB4" s="67"/>
+      <c r="IC4" s="67"/>
+      <c r="ID4" s="67"/>
+      <c r="IE4" s="67"/>
+      <c r="IF4" s="67"/>
+      <c r="IG4" s="67"/>
+      <c r="IH4" s="67"/>
+      <c r="II4" s="67"/>
+      <c r="IJ4" s="67"/>
+      <c r="IK4" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="90"/>
-      <c r="IM4" s="90"/>
-      <c r="IN4" s="90"/>
-      <c r="IO4" s="90"/>
-      <c r="IP4" s="90"/>
-      <c r="IQ4" s="90"/>
-      <c r="IR4" s="90"/>
-      <c r="IS4" s="90"/>
-      <c r="IT4" s="90"/>
-      <c r="IU4" s="90"/>
-      <c r="IV4" s="90"/>
-      <c r="IW4" s="90"/>
-      <c r="IX4" s="90"/>
-      <c r="IY4" s="90" t="s">
+      <c r="IL4" s="67"/>
+      <c r="IM4" s="67"/>
+      <c r="IN4" s="67"/>
+      <c r="IO4" s="67"/>
+      <c r="IP4" s="67"/>
+      <c r="IQ4" s="67"/>
+      <c r="IR4" s="67"/>
+      <c r="IS4" s="67"/>
+      <c r="IT4" s="67"/>
+      <c r="IU4" s="67"/>
+      <c r="IV4" s="67"/>
+      <c r="IW4" s="67"/>
+      <c r="IX4" s="67"/>
+      <c r="IY4" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="90"/>
-      <c r="JA4" s="90"/>
-      <c r="JB4" s="90"/>
-      <c r="JC4" s="90"/>
-      <c r="JD4" s="90"/>
-      <c r="JE4" s="90"/>
-      <c r="JF4" s="90"/>
-      <c r="JG4" s="90"/>
-      <c r="JH4" s="90"/>
-      <c r="JI4" s="90"/>
-      <c r="JJ4" s="90"/>
-      <c r="JK4" s="90"/>
-      <c r="JL4" s="90"/>
-      <c r="JM4" s="91" t="s">
+      <c r="IZ4" s="67"/>
+      <c r="JA4" s="67"/>
+      <c r="JB4" s="67"/>
+      <c r="JC4" s="67"/>
+      <c r="JD4" s="67"/>
+      <c r="JE4" s="67"/>
+      <c r="JF4" s="67"/>
+      <c r="JG4" s="67"/>
+      <c r="JH4" s="67"/>
+      <c r="JI4" s="67"/>
+      <c r="JJ4" s="67"/>
+      <c r="JK4" s="67"/>
+      <c r="JL4" s="67"/>
+      <c r="JM4" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="91"/>
-      <c r="JO4" s="91"/>
-      <c r="JP4" s="91"/>
-      <c r="JQ4" s="91"/>
-      <c r="JR4" s="91"/>
-      <c r="JS4" s="91"/>
-      <c r="JT4" s="91"/>
-      <c r="JU4" s="91"/>
-      <c r="JV4" s="91"/>
-      <c r="JW4" s="91"/>
-      <c r="JX4" s="91"/>
-      <c r="JY4" s="91"/>
-      <c r="JZ4" s="88" t="s">
+      <c r="JN4" s="68"/>
+      <c r="JO4" s="68"/>
+      <c r="JP4" s="68"/>
+      <c r="JQ4" s="68"/>
+      <c r="JR4" s="68"/>
+      <c r="JS4" s="68"/>
+      <c r="JT4" s="68"/>
+      <c r="JU4" s="68"/>
+      <c r="JV4" s="68"/>
+      <c r="JW4" s="68"/>
+      <c r="JX4" s="68"/>
+      <c r="JY4" s="68"/>
+      <c r="JZ4" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="89"/>
-      <c r="KB4" s="89"/>
-      <c r="KC4" s="89"/>
-      <c r="KD4" s="89"/>
-      <c r="KE4" s="89"/>
-      <c r="KF4" s="89"/>
-      <c r="KG4" s="89"/>
-      <c r="KH4" s="84" t="s">
+      <c r="KA4" s="65"/>
+      <c r="KB4" s="65"/>
+      <c r="KC4" s="65"/>
+      <c r="KD4" s="65"/>
+      <c r="KE4" s="65"/>
+      <c r="KF4" s="65"/>
+      <c r="KG4" s="65"/>
+      <c r="KH4" s="90" t="s">
         <v>316</v>
       </c>
-      <c r="KI4" s="85"/>
-      <c r="KJ4" s="85"/>
+      <c r="KI4" s="93"/>
+      <c r="KJ4" s="91"/>
       <c r="KK4" s="46"/>
+      <c r="KL4" s="90" t="s">
+        <v>343</v>
+      </c>
+      <c r="KM4" s="91"/>
     </row>
-    <row r="5" spans="1:297" customFormat="false" ht="12" customHeight="1">
-      <c r="A5" s="66"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="69"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="69"/>
-      <c r="U5" s="70"/>
-      <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
-      <c r="X5" s="70"/>
-      <c r="Y5" s="70"/>
-      <c r="Z5" s="70"/>
-      <c r="AA5" s="70"/>
-      <c r="AB5" s="70"/>
-      <c r="AC5" s="71"/>
-      <c r="AD5" s="71"/>
-      <c r="AE5" s="71"/>
-      <c r="AF5" s="71"/>
-      <c r="AG5" s="71"/>
-      <c r="AH5" s="71"/>
-      <c r="AI5" s="71"/>
-      <c r="AJ5" s="72"/>
-      <c r="AK5" s="72"/>
-      <c r="AL5" s="72"/>
-      <c r="AM5" s="63"/>
-      <c r="AN5" s="63"/>
-      <c r="AO5" s="74"/>
-      <c r="AP5" s="74"/>
-      <c r="AQ5" s="74"/>
-      <c r="AR5" s="74"/>
-      <c r="AS5" s="75"/>
-      <c r="AT5" s="75"/>
-      <c r="AU5" s="75"/>
-      <c r="AV5" s="75"/>
-      <c r="AW5" s="75"/>
-      <c r="AX5" s="75"/>
-      <c r="AY5" s="75"/>
-      <c r="AZ5" s="75"/>
-      <c r="BA5" s="75"/>
-      <c r="BB5" s="75"/>
-      <c r="BC5" s="75"/>
-      <c r="BD5" s="75"/>
-      <c r="BE5" s="75"/>
-      <c r="BF5" s="75"/>
-      <c r="BG5" s="75"/>
-      <c r="BH5" s="75"/>
-      <c r="BI5" s="75"/>
-      <c r="BJ5" s="75"/>
+    <row r="5" spans="1:299" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="82"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="85"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="85"/>
+      <c r="U5" s="86"/>
+      <c r="V5" s="86"/>
+      <c r="W5" s="86"/>
+      <c r="X5" s="86"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="86"/>
+      <c r="AA5" s="86"/>
+      <c r="AB5" s="86"/>
+      <c r="AC5" s="87"/>
+      <c r="AD5" s="87"/>
+      <c r="AE5" s="87"/>
+      <c r="AF5" s="87"/>
+      <c r="AG5" s="87"/>
+      <c r="AH5" s="87"/>
+      <c r="AI5" s="87"/>
+      <c r="AJ5" s="88"/>
+      <c r="AK5" s="88"/>
+      <c r="AL5" s="88"/>
+      <c r="AM5" s="79"/>
+      <c r="AN5" s="79"/>
+      <c r="AO5" s="69"/>
+      <c r="AP5" s="69"/>
+      <c r="AQ5" s="69"/>
+      <c r="AR5" s="69"/>
+      <c r="AS5" s="70"/>
+      <c r="AT5" s="70"/>
+      <c r="AU5" s="70"/>
+      <c r="AV5" s="70"/>
+      <c r="AW5" s="70"/>
+      <c r="AX5" s="70"/>
+      <c r="AY5" s="70"/>
+      <c r="AZ5" s="70"/>
+      <c r="BA5" s="70"/>
+      <c r="BB5" s="70"/>
+      <c r="BC5" s="70"/>
+      <c r="BD5" s="70"/>
+      <c r="BE5" s="70"/>
+      <c r="BF5" s="70"/>
+      <c r="BG5" s="70"/>
+      <c r="BH5" s="70"/>
+      <c r="BI5" s="70"/>
+      <c r="BJ5" s="70"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -4063,37 +4149,39 @@
       <c r="JL5" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="JM5" s="91"/>
-      <c r="JN5" s="91"/>
-      <c r="JO5" s="91"/>
-      <c r="JP5" s="91"/>
-      <c r="JQ5" s="91"/>
-      <c r="JR5" s="91"/>
-      <c r="JS5" s="91"/>
-      <c r="JT5" s="91"/>
-      <c r="JU5" s="91"/>
-      <c r="JV5" s="91"/>
-      <c r="JW5" s="91"/>
-      <c r="JX5" s="91"/>
-      <c r="JY5" s="91"/>
-      <c r="JZ5" s="89" t="s">
+      <c r="JM5" s="68"/>
+      <c r="JN5" s="68"/>
+      <c r="JO5" s="68"/>
+      <c r="JP5" s="68"/>
+      <c r="JQ5" s="68"/>
+      <c r="JR5" s="68"/>
+      <c r="JS5" s="68"/>
+      <c r="JT5" s="68"/>
+      <c r="JU5" s="68"/>
+      <c r="JV5" s="68"/>
+      <c r="JW5" s="68"/>
+      <c r="JX5" s="68"/>
+      <c r="JY5" s="68"/>
+      <c r="JZ5" s="65" t="s">
         <v>342</v>
       </c>
-      <c r="KA5" s="89"/>
-      <c r="KB5" s="89"/>
-      <c r="KC5" s="89"/>
-      <c r="KD5" s="89" t="s">
+      <c r="KA5" s="65"/>
+      <c r="KB5" s="65"/>
+      <c r="KC5" s="65"/>
+      <c r="KD5" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="89"/>
-      <c r="KF5" s="89"/>
-      <c r="KG5" s="89"/>
-      <c r="KH5" s="86"/>
-      <c r="KI5" s="87"/>
-      <c r="KJ5" s="87"/>
+      <c r="KE5" s="65"/>
+      <c r="KF5" s="65"/>
+      <c r="KG5" s="65"/>
+      <c r="KH5" s="62"/>
+      <c r="KI5" s="63"/>
+      <c r="KJ5" s="92"/>
       <c r="KK5" s="46"/>
+      <c r="KL5" s="62"/>
+      <c r="KM5" s="92"/>
     </row>
-    <row r="6" spans="1:299" customFormat="false" ht="81.75" customHeight="1">
+    <row r="6" spans="1:299" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -4985,436 +5073,440 @@
       <c r="KK6" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="KL6" s="48"/>
-      <c r="KM6" s="49"/>
+      <c r="KL6" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="KM6" s="22" t="s">
+        <v>345</v>
+      </c>
     </row>
-    <row r="7" spans="1:297" customFormat="false" ht="15" customHeight="1">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50" t="s">
+    <row r="7" spans="1:299" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49" t="s">
         <v>336</v>
       </c>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52" t="s">
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="51" t="s">
         <v>336</v>
       </c>
-      <c r="S7" s="52" t="s">
+      <c r="S7" s="51" t="s">
         <v>336</v>
       </c>
-      <c r="T7" s="52"/>
-      <c r="U7" s="52"/>
-      <c r="V7" s="52"/>
-      <c r="W7" s="52"/>
-      <c r="X7" s="53" t="s">
+      <c r="T7" s="51"/>
+      <c r="U7" s="51"/>
+      <c r="V7" s="51"/>
+      <c r="W7" s="51"/>
+      <c r="X7" s="52" t="s">
         <v>336</v>
       </c>
-      <c r="Y7" s="53" t="s">
+      <c r="Y7" s="52" t="s">
         <v>336</v>
       </c>
-      <c r="Z7" s="52"/>
-      <c r="AA7" s="52"/>
-      <c r="AB7" s="53"/>
-      <c r="AC7" s="54"/>
-      <c r="AD7" s="55"/>
-      <c r="AE7" s="55"/>
-      <c r="AF7" s="56"/>
-      <c r="AG7" s="56"/>
-      <c r="AH7" s="57"/>
-      <c r="AI7" s="56"/>
-      <c r="AJ7" s="51" t="s">
+      <c r="Z7" s="51"/>
+      <c r="AA7" s="51"/>
+      <c r="AB7" s="52"/>
+      <c r="AC7" s="53"/>
+      <c r="AD7" s="54"/>
+      <c r="AE7" s="54"/>
+      <c r="AF7" s="55"/>
+      <c r="AG7" s="55"/>
+      <c r="AH7" s="56"/>
+      <c r="AI7" s="55"/>
+      <c r="AJ7" s="50" t="s">
         <v>336</v>
       </c>
-      <c r="AK7" s="51" t="s">
+      <c r="AK7" s="50" t="s">
         <v>336</v>
       </c>
-      <c r="AL7" s="51" t="s">
+      <c r="AL7" s="50" t="s">
         <v>336</v>
       </c>
-      <c r="AM7" s="52"/>
-      <c r="AN7" s="58"/>
-      <c r="AO7" s="59"/>
-      <c r="AP7" s="59"/>
-      <c r="AQ7" s="59"/>
-      <c r="AR7" s="59"/>
-      <c r="AS7" s="60">
+      <c r="AM7" s="51"/>
+      <c r="AN7" s="57"/>
+      <c r="AO7" s="58"/>
+      <c r="AP7" s="58"/>
+      <c r="AQ7" s="58"/>
+      <c r="AR7" s="58"/>
+      <c r="AS7" s="59">
         <f>SUM(BK7:BX7)</f>
         <v>0</v>
       </c>
-      <c r="AT7" s="61">
+      <c r="AT7" s="60">
         <f>SUM(BY7:CL7)</f>
         <v>0</v>
       </c>
-      <c r="AU7" s="61">
+      <c r="AU7" s="60">
         <f>SUM(CM7:CZ7)</f>
         <v>0</v>
       </c>
-      <c r="AV7" s="61">
+      <c r="AV7" s="60">
         <f>SUM(DA7:DN7)</f>
         <v>0</v>
       </c>
-      <c r="AW7" s="61">
+      <c r="AW7" s="60">
         <f>SUM(DO7:EB7)</f>
         <v>0</v>
       </c>
-      <c r="AX7" s="61">
+      <c r="AX7" s="60">
         <f>SUM(EC7:EP7)</f>
         <v>0</v>
       </c>
-      <c r="AY7" s="61">
+      <c r="AY7" s="60">
         <f>SUM(EQ7:FD7)</f>
         <v>0</v>
       </c>
-      <c r="AZ7" s="61">
+      <c r="AZ7" s="60">
         <f>SUM(FE7:FR7)</f>
         <v>0</v>
       </c>
-      <c r="BA7" s="61">
+      <c r="BA7" s="60">
         <f>SUM(FS7:GF7)</f>
         <v>0</v>
       </c>
-      <c r="BB7" s="61">
+      <c r="BB7" s="60">
         <f>SUM(GG7:GT7)</f>
         <v>0</v>
       </c>
-      <c r="BC7" s="61">
+      <c r="BC7" s="60">
         <f>SUM(GU7:HH7)</f>
         <v>0</v>
       </c>
-      <c r="BD7" s="61">
+      <c r="BD7" s="60">
         <f>SUM(HI7:HV7)</f>
         <v>0</v>
       </c>
-      <c r="BE7" s="61">
+      <c r="BE7" s="60">
         <f>SUM(HW7:IJ7)</f>
         <v>0</v>
       </c>
-      <c r="BF7" s="61">
+      <c r="BF7" s="60">
         <f>SUM(IK7:IX7)</f>
         <v>0</v>
       </c>
-      <c r="BG7" s="61">
+      <c r="BG7" s="60">
         <f>SUM(IY7:JL7)</f>
         <v>0</v>
       </c>
-      <c r="BH7" s="61">
+      <c r="BH7" s="60">
         <f t="shared" ref="BH7" si="0">JM7</f>
         <v>0</v>
       </c>
-      <c r="BI7" s="61">
+      <c r="BI7" s="60">
         <f>JN7</f>
         <v>0</v>
       </c>
-      <c r="BJ7" s="61">
+      <c r="BJ7" s="60">
         <f>JO7</f>
         <v>0</v>
       </c>
-      <c r="BK7" s="61">
+      <c r="BK7" s="60">
         <f t="shared" ref="BK7:BX7" si="1">BY7+CM7+DA7+DO7+EC7+EQ7+FE7+FS7</f>
         <v>0</v>
       </c>
-      <c r="BL7" s="61">
+      <c r="BL7" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BM7" s="61">
+      <c r="BM7" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BN7" s="61">
+      <c r="BN7" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BO7" s="61">
+      <c r="BO7" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BP7" s="61">
+      <c r="BP7" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BQ7" s="61">
+      <c r="BQ7" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BR7" s="61">
+      <c r="BR7" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BS7" s="61">
+      <c r="BS7" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BT7" s="61">
+      <c r="BT7" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BU7" s="61">
+      <c r="BU7" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BV7" s="61">
+      <c r="BV7" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BW7" s="61">
+      <c r="BW7" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BX7" s="61">
+      <c r="BX7" s="60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="BY7" s="56"/>
-      <c r="BZ7" s="56"/>
-      <c r="CA7" s="56"/>
-      <c r="CB7" s="56"/>
-      <c r="CC7" s="56"/>
-      <c r="CD7" s="56"/>
-      <c r="CE7" s="56"/>
-      <c r="CF7" s="56"/>
-      <c r="CG7" s="56"/>
-      <c r="CH7" s="56"/>
-      <c r="CI7" s="56"/>
-      <c r="CJ7" s="56"/>
-      <c r="CK7" s="56"/>
-      <c r="CL7" s="56"/>
-      <c r="CM7" s="56"/>
-      <c r="CN7" s="56"/>
-      <c r="CO7" s="56"/>
-      <c r="CP7" s="56"/>
-      <c r="CQ7" s="56"/>
-      <c r="CR7" s="56"/>
-      <c r="CS7" s="56"/>
-      <c r="CT7" s="56"/>
-      <c r="CU7" s="56"/>
-      <c r="CV7" s="56"/>
-      <c r="CW7" s="56"/>
-      <c r="CX7" s="56"/>
-      <c r="CY7" s="56"/>
-      <c r="CZ7" s="56"/>
-      <c r="DA7" s="56"/>
-      <c r="DB7" s="56"/>
-      <c r="DC7" s="56"/>
-      <c r="DD7" s="56"/>
-      <c r="DE7" s="56"/>
-      <c r="DF7" s="56"/>
-      <c r="DG7" s="56"/>
-      <c r="DH7" s="56"/>
-      <c r="DI7" s="56"/>
-      <c r="DJ7" s="56"/>
-      <c r="DK7" s="56"/>
-      <c r="DL7" s="56"/>
-      <c r="DM7" s="56"/>
-      <c r="DN7" s="56"/>
-      <c r="DO7" s="56"/>
-      <c r="DP7" s="56"/>
-      <c r="DQ7" s="56"/>
-      <c r="DR7" s="56"/>
-      <c r="DS7" s="56"/>
-      <c r="DT7" s="56"/>
-      <c r="DU7" s="56"/>
-      <c r="DV7" s="56"/>
-      <c r="DW7" s="56"/>
-      <c r="DX7" s="56"/>
-      <c r="DY7" s="56"/>
-      <c r="DZ7" s="56"/>
-      <c r="EA7" s="56"/>
-      <c r="EB7" s="56"/>
-      <c r="EC7" s="56"/>
-      <c r="ED7" s="56"/>
-      <c r="EE7" s="56"/>
-      <c r="EF7" s="56"/>
-      <c r="EG7" s="56"/>
-      <c r="EH7" s="56"/>
-      <c r="EI7" s="56"/>
-      <c r="EJ7" s="56"/>
-      <c r="EK7" s="56"/>
-      <c r="EL7" s="56"/>
-      <c r="EM7" s="56"/>
-      <c r="EN7" s="56"/>
-      <c r="EO7" s="56"/>
-      <c r="EP7" s="56"/>
-      <c r="EQ7" s="56"/>
-      <c r="ER7" s="56"/>
-      <c r="ES7" s="56"/>
-      <c r="ET7" s="56"/>
-      <c r="EU7" s="56"/>
-      <c r="EV7" s="56"/>
-      <c r="EW7" s="56"/>
-      <c r="EX7" s="56"/>
-      <c r="EY7" s="56"/>
-      <c r="EZ7" s="56"/>
-      <c r="FA7" s="56"/>
-      <c r="FB7" s="56"/>
-      <c r="FC7" s="56"/>
-      <c r="FD7" s="56"/>
-      <c r="FE7" s="56"/>
-      <c r="FF7" s="56"/>
-      <c r="FG7" s="56"/>
-      <c r="FH7" s="56"/>
-      <c r="FI7" s="56"/>
-      <c r="FJ7" s="56"/>
-      <c r="FK7" s="56"/>
-      <c r="FL7" s="56"/>
-      <c r="FM7" s="56"/>
-      <c r="FN7" s="56"/>
-      <c r="FO7" s="56"/>
-      <c r="FP7" s="56"/>
-      <c r="FQ7" s="56"/>
-      <c r="FR7" s="56"/>
-      <c r="FS7" s="56"/>
-      <c r="FT7" s="56"/>
-      <c r="FU7" s="56"/>
-      <c r="FV7" s="56"/>
-      <c r="FW7" s="56"/>
-      <c r="FX7" s="56"/>
-      <c r="FY7" s="56"/>
-      <c r="FZ7" s="56"/>
-      <c r="GA7" s="56"/>
-      <c r="GB7" s="56"/>
-      <c r="GC7" s="56"/>
-      <c r="GD7" s="56"/>
-      <c r="GE7" s="56"/>
-      <c r="GF7" s="56"/>
-      <c r="GG7" s="56"/>
-      <c r="GH7" s="56"/>
-      <c r="GI7" s="56"/>
-      <c r="GJ7" s="56"/>
-      <c r="GK7" s="56"/>
-      <c r="GL7" s="56"/>
-      <c r="GM7" s="56"/>
-      <c r="GN7" s="56"/>
-      <c r="GO7" s="56"/>
-      <c r="GP7" s="56"/>
-      <c r="GQ7" s="56"/>
-      <c r="GR7" s="56"/>
-      <c r="GS7" s="56"/>
-      <c r="GT7" s="56"/>
-      <c r="GU7" s="56"/>
-      <c r="GV7" s="56"/>
-      <c r="GW7" s="56"/>
-      <c r="GX7" s="56"/>
-      <c r="GY7" s="56"/>
-      <c r="GZ7" s="56"/>
-      <c r="HA7" s="56"/>
-      <c r="HB7" s="56"/>
-      <c r="HC7" s="56"/>
-      <c r="HD7" s="56"/>
-      <c r="HE7" s="56"/>
-      <c r="HF7" s="56"/>
-      <c r="HG7" s="56"/>
-      <c r="HH7" s="56"/>
-      <c r="HI7" s="56"/>
-      <c r="HJ7" s="56"/>
-      <c r="HK7" s="56"/>
-      <c r="HL7" s="56"/>
-      <c r="HM7" s="56"/>
-      <c r="HN7" s="56"/>
-      <c r="HO7" s="56"/>
-      <c r="HP7" s="56"/>
-      <c r="HQ7" s="56"/>
-      <c r="HR7" s="56"/>
-      <c r="HS7" s="56"/>
-      <c r="HT7" s="56"/>
-      <c r="HU7" s="56"/>
-      <c r="HV7" s="56"/>
-      <c r="HW7" s="56"/>
-      <c r="HX7" s="56"/>
-      <c r="HY7" s="56"/>
-      <c r="HZ7" s="56"/>
-      <c r="IA7" s="56"/>
-      <c r="IB7" s="56"/>
-      <c r="IC7" s="56"/>
-      <c r="ID7" s="56"/>
-      <c r="IE7" s="56"/>
-      <c r="IF7" s="56"/>
-      <c r="IG7" s="56"/>
-      <c r="IH7" s="56"/>
-      <c r="II7" s="56"/>
-      <c r="IJ7" s="56"/>
-      <c r="IK7" s="56"/>
-      <c r="IL7" s="56"/>
-      <c r="IM7" s="56"/>
-      <c r="IN7" s="56"/>
-      <c r="IO7" s="56"/>
-      <c r="IP7" s="56"/>
-      <c r="IQ7" s="56"/>
-      <c r="IR7" s="56"/>
-      <c r="IS7" s="56"/>
-      <c r="IT7" s="56"/>
-      <c r="IU7" s="56"/>
-      <c r="IV7" s="56"/>
-      <c r="IW7" s="56"/>
-      <c r="IX7" s="56"/>
-      <c r="IY7" s="56"/>
-      <c r="IZ7" s="56"/>
-      <c r="JA7" s="56"/>
-      <c r="JB7" s="56"/>
-      <c r="JC7" s="56"/>
-      <c r="JD7" s="56"/>
-      <c r="JE7" s="56"/>
-      <c r="JF7" s="56"/>
-      <c r="JG7" s="56"/>
-      <c r="JH7" s="56"/>
-      <c r="JI7" s="56"/>
-      <c r="JJ7" s="56"/>
-      <c r="JK7" s="56"/>
-      <c r="JL7" s="56"/>
-      <c r="JM7" s="56"/>
-      <c r="JN7" s="56"/>
-      <c r="JO7" s="56"/>
-      <c r="JP7" s="51"/>
-      <c r="JQ7" s="51"/>
-      <c r="JR7" s="51"/>
-      <c r="JS7" s="62"/>
-      <c r="JT7" s="62"/>
-      <c r="JU7" s="62"/>
-      <c r="JV7" s="62"/>
-      <c r="JW7" s="62"/>
-      <c r="JX7" s="62"/>
-      <c r="JY7" s="62"/>
-      <c r="JZ7" s="61">
+      <c r="BY7" s="55"/>
+      <c r="BZ7" s="55"/>
+      <c r="CA7" s="55"/>
+      <c r="CB7" s="55"/>
+      <c r="CC7" s="55"/>
+      <c r="CD7" s="55"/>
+      <c r="CE7" s="55"/>
+      <c r="CF7" s="55"/>
+      <c r="CG7" s="55"/>
+      <c r="CH7" s="55"/>
+      <c r="CI7" s="55"/>
+      <c r="CJ7" s="55"/>
+      <c r="CK7" s="55"/>
+      <c r="CL7" s="55"/>
+      <c r="CM7" s="55"/>
+      <c r="CN7" s="55"/>
+      <c r="CO7" s="55"/>
+      <c r="CP7" s="55"/>
+      <c r="CQ7" s="55"/>
+      <c r="CR7" s="55"/>
+      <c r="CS7" s="55"/>
+      <c r="CT7" s="55"/>
+      <c r="CU7" s="55"/>
+      <c r="CV7" s="55"/>
+      <c r="CW7" s="55"/>
+      <c r="CX7" s="55"/>
+      <c r="CY7" s="55"/>
+      <c r="CZ7" s="55"/>
+      <c r="DA7" s="55"/>
+      <c r="DB7" s="55"/>
+      <c r="DC7" s="55"/>
+      <c r="DD7" s="55"/>
+      <c r="DE7" s="55"/>
+      <c r="DF7" s="55"/>
+      <c r="DG7" s="55"/>
+      <c r="DH7" s="55"/>
+      <c r="DI7" s="55"/>
+      <c r="DJ7" s="55"/>
+      <c r="DK7" s="55"/>
+      <c r="DL7" s="55"/>
+      <c r="DM7" s="55"/>
+      <c r="DN7" s="55"/>
+      <c r="DO7" s="55"/>
+      <c r="DP7" s="55"/>
+      <c r="DQ7" s="55"/>
+      <c r="DR7" s="55"/>
+      <c r="DS7" s="55"/>
+      <c r="DT7" s="55"/>
+      <c r="DU7" s="55"/>
+      <c r="DV7" s="55"/>
+      <c r="DW7" s="55"/>
+      <c r="DX7" s="55"/>
+      <c r="DY7" s="55"/>
+      <c r="DZ7" s="55"/>
+      <c r="EA7" s="55"/>
+      <c r="EB7" s="55"/>
+      <c r="EC7" s="55"/>
+      <c r="ED7" s="55"/>
+      <c r="EE7" s="55"/>
+      <c r="EF7" s="55"/>
+      <c r="EG7" s="55"/>
+      <c r="EH7" s="55"/>
+      <c r="EI7" s="55"/>
+      <c r="EJ7" s="55"/>
+      <c r="EK7" s="55"/>
+      <c r="EL7" s="55"/>
+      <c r="EM7" s="55"/>
+      <c r="EN7" s="55"/>
+      <c r="EO7" s="55"/>
+      <c r="EP7" s="55"/>
+      <c r="EQ7" s="55"/>
+      <c r="ER7" s="55"/>
+      <c r="ES7" s="55"/>
+      <c r="ET7" s="55"/>
+      <c r="EU7" s="55"/>
+      <c r="EV7" s="55"/>
+      <c r="EW7" s="55"/>
+      <c r="EX7" s="55"/>
+      <c r="EY7" s="55"/>
+      <c r="EZ7" s="55"/>
+      <c r="FA7" s="55"/>
+      <c r="FB7" s="55"/>
+      <c r="FC7" s="55"/>
+      <c r="FD7" s="55"/>
+      <c r="FE7" s="55"/>
+      <c r="FF7" s="55"/>
+      <c r="FG7" s="55"/>
+      <c r="FH7" s="55"/>
+      <c r="FI7" s="55"/>
+      <c r="FJ7" s="55"/>
+      <c r="FK7" s="55"/>
+      <c r="FL7" s="55"/>
+      <c r="FM7" s="55"/>
+      <c r="FN7" s="55"/>
+      <c r="FO7" s="55"/>
+      <c r="FP7" s="55"/>
+      <c r="FQ7" s="55"/>
+      <c r="FR7" s="55"/>
+      <c r="FS7" s="55"/>
+      <c r="FT7" s="55"/>
+      <c r="FU7" s="55"/>
+      <c r="FV7" s="55"/>
+      <c r="FW7" s="55"/>
+      <c r="FX7" s="55"/>
+      <c r="FY7" s="55"/>
+      <c r="FZ7" s="55"/>
+      <c r="GA7" s="55"/>
+      <c r="GB7" s="55"/>
+      <c r="GC7" s="55"/>
+      <c r="GD7" s="55"/>
+      <c r="GE7" s="55"/>
+      <c r="GF7" s="55"/>
+      <c r="GG7" s="55"/>
+      <c r="GH7" s="55"/>
+      <c r="GI7" s="55"/>
+      <c r="GJ7" s="55"/>
+      <c r="GK7" s="55"/>
+      <c r="GL7" s="55"/>
+      <c r="GM7" s="55"/>
+      <c r="GN7" s="55"/>
+      <c r="GO7" s="55"/>
+      <c r="GP7" s="55"/>
+      <c r="GQ7" s="55"/>
+      <c r="GR7" s="55"/>
+      <c r="GS7" s="55"/>
+      <c r="GT7" s="55"/>
+      <c r="GU7" s="55"/>
+      <c r="GV7" s="55"/>
+      <c r="GW7" s="55"/>
+      <c r="GX7" s="55"/>
+      <c r="GY7" s="55"/>
+      <c r="GZ7" s="55"/>
+      <c r="HA7" s="55"/>
+      <c r="HB7" s="55"/>
+      <c r="HC7" s="55"/>
+      <c r="HD7" s="55"/>
+      <c r="HE7" s="55"/>
+      <c r="HF7" s="55"/>
+      <c r="HG7" s="55"/>
+      <c r="HH7" s="55"/>
+      <c r="HI7" s="55"/>
+      <c r="HJ7" s="55"/>
+      <c r="HK7" s="55"/>
+      <c r="HL7" s="55"/>
+      <c r="HM7" s="55"/>
+      <c r="HN7" s="55"/>
+      <c r="HO7" s="55"/>
+      <c r="HP7" s="55"/>
+      <c r="HQ7" s="55"/>
+      <c r="HR7" s="55"/>
+      <c r="HS7" s="55"/>
+      <c r="HT7" s="55"/>
+      <c r="HU7" s="55"/>
+      <c r="HV7" s="55"/>
+      <c r="HW7" s="55"/>
+      <c r="HX7" s="55"/>
+      <c r="HY7" s="55"/>
+      <c r="HZ7" s="55"/>
+      <c r="IA7" s="55"/>
+      <c r="IB7" s="55"/>
+      <c r="IC7" s="55"/>
+      <c r="ID7" s="55"/>
+      <c r="IE7" s="55"/>
+      <c r="IF7" s="55"/>
+      <c r="IG7" s="55"/>
+      <c r="IH7" s="55"/>
+      <c r="II7" s="55"/>
+      <c r="IJ7" s="55"/>
+      <c r="IK7" s="55"/>
+      <c r="IL7" s="55"/>
+      <c r="IM7" s="55"/>
+      <c r="IN7" s="55"/>
+      <c r="IO7" s="55"/>
+      <c r="IP7" s="55"/>
+      <c r="IQ7" s="55"/>
+      <c r="IR7" s="55"/>
+      <c r="IS7" s="55"/>
+      <c r="IT7" s="55"/>
+      <c r="IU7" s="55"/>
+      <c r="IV7" s="55"/>
+      <c r="IW7" s="55"/>
+      <c r="IX7" s="55"/>
+      <c r="IY7" s="55"/>
+      <c r="IZ7" s="55"/>
+      <c r="JA7" s="55"/>
+      <c r="JB7" s="55"/>
+      <c r="JC7" s="55"/>
+      <c r="JD7" s="55"/>
+      <c r="JE7" s="55"/>
+      <c r="JF7" s="55"/>
+      <c r="JG7" s="55"/>
+      <c r="JH7" s="55"/>
+      <c r="JI7" s="55"/>
+      <c r="JJ7" s="55"/>
+      <c r="JK7" s="55"/>
+      <c r="JL7" s="55"/>
+      <c r="JM7" s="55"/>
+      <c r="JN7" s="55"/>
+      <c r="JO7" s="55"/>
+      <c r="JP7" s="50"/>
+      <c r="JQ7" s="50"/>
+      <c r="JR7" s="50"/>
+      <c r="JS7" s="61"/>
+      <c r="JT7" s="61"/>
+      <c r="JU7" s="61"/>
+      <c r="JV7" s="61"/>
+      <c r="JW7" s="61"/>
+      <c r="JX7" s="61"/>
+      <c r="JY7" s="61"/>
+      <c r="JZ7" s="60">
         <f>BQ7</f>
         <v>0</v>
       </c>
-      <c r="KA7" s="61">
+      <c r="KA7" s="60">
         <f>CE7+CS7</f>
         <v>0</v>
       </c>
-      <c r="KB7" s="61">
+      <c r="KB7" s="60">
         <f>DG7+DU7+EI7+EW7+FK7+FY7</f>
         <v>0</v>
       </c>
-      <c r="KC7" s="61">
+      <c r="KC7" s="60">
         <f>GM7+IC7</f>
         <v>0</v>
       </c>
-      <c r="KD7" s="61">
+      <c r="KD7" s="60">
         <f>SUM(BL7:BQ7)</f>
         <v>0</v>
       </c>
-      <c r="KE7" s="61">
+      <c r="KE7" s="60">
         <f>SUM(CN7:CS7)+SUM(BZ7:CE7)</f>
         <v>0</v>
       </c>
-      <c r="KF7" s="61">
+      <c r="KF7" s="60">
         <f>SUM(DB7:DG7)+SUM(DP7:DU7)+SUM(ED7:EI7)+SUM(ER7:EW7)+SUM(FF7:FK7)+SUM(FT7:FY7)</f>
         <v>0</v>
       </c>
-      <c r="KG7" s="61">
+      <c r="KG7" s="60">
         <f>SUM(GH7:GM7)+SUM(HX7:IC7)</f>
         <v>0</v>
       </c>
@@ -5422,20 +5514,26 @@
       <c r="KI7" s="47"/>
       <c r="KJ7" s="47"/>
       <c r="KK7" s="47"/>
+      <c r="KL7" s="89"/>
+      <c r="KM7" s="89"/>
+    </row>
+    <row r="32" spans="297:297" x14ac:dyDescent="0.2">
+      <c r="KK32" s="48"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:KK6"/>
-  <mergeCells count="32">
-    <mergeCell ref="KH4:KJ5"/>
-    <mergeCell ref="JZ4:KG4"/>
-    <mergeCell ref="JZ5:KC5"/>
-    <mergeCell ref="KD5:KG5"/>
-    <mergeCell ref="GU4:HH4"/>
-    <mergeCell ref="HI4:HV4"/>
-    <mergeCell ref="HW4:IJ4"/>
-    <mergeCell ref="IK4:IX4"/>
-    <mergeCell ref="IY4:JL4"/>
-    <mergeCell ref="JM4:JY5"/>
+  <autoFilter ref="A6:KK6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <mergeCells count="33">
+    <mergeCell ref="KL4:KM5"/>
+    <mergeCell ref="AM4:AN5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:D5"/>
+    <mergeCell ref="E4:J5"/>
+    <mergeCell ref="K4:O5"/>
+    <mergeCell ref="P4:T5"/>
+    <mergeCell ref="U4:AB5"/>
+    <mergeCell ref="AC4:AI5"/>
+    <mergeCell ref="AJ4:AL5"/>
     <mergeCell ref="GG4:GT4"/>
     <mergeCell ref="AO4:AR5"/>
     <mergeCell ref="AS4:BJ5"/>
@@ -5448,29 +5546,29 @@
     <mergeCell ref="EQ4:FD4"/>
     <mergeCell ref="FE4:FR4"/>
     <mergeCell ref="FS4:GF4"/>
-    <mergeCell ref="AM4:AN5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:D5"/>
-    <mergeCell ref="E4:J5"/>
-    <mergeCell ref="K4:O5"/>
-    <mergeCell ref="P4:T5"/>
-    <mergeCell ref="U4:AB5"/>
-    <mergeCell ref="AC4:AI5"/>
-    <mergeCell ref="AJ4:AL5"/>
+    <mergeCell ref="KH4:KJ5"/>
+    <mergeCell ref="JZ4:KG4"/>
+    <mergeCell ref="JZ5:KC5"/>
+    <mergeCell ref="KD5:KG5"/>
+    <mergeCell ref="GU4:HH4"/>
+    <mergeCell ref="HI4:HV4"/>
+    <mergeCell ref="HW4:IJ4"/>
+    <mergeCell ref="IK4:IX4"/>
+    <mergeCell ref="IY4:JL4"/>
+    <mergeCell ref="JM4:JY5"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR7">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>36526</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH6:KJ999996">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH6:KJ999996" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, N/A"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7086614173228347" right="0.7086614173228347" top="0.7480314960629921" bottom="0.7480314960629921" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="10" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>